<commit_message>
Sep 2021 LFS update
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R Projects\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA70EA1B-4886-4B84-A0E6-100F92CA5FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC9C0CA-8734-4DCB-AF8B-40F7555F326C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="2535" windowWidth="15540" windowHeight="11385" xr2:uid="{DAAD9588-C85E-4EED-B6EC-CB5916F347A0}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="407">
   <si>
     <t>https://psa.gov.ph/statistics/survey/labor-force/lfs-index</t>
   </si>
@@ -1249,6 +1249,15 @@
   </si>
   <si>
     <t>2021 Aug</t>
+  </si>
+  <si>
+    <t>2021 Sep</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/unemployment-rate-september-2021-estimated-89-percent</t>
   </si>
 </sst>
 </file>
@@ -1699,13 +1708,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E701CAE5-AC4C-469D-A332-E8EB78C28CD8}">
-  <dimension ref="A1:P137"/>
+  <dimension ref="A1:P138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D131" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A138" sqref="A138"/>
+      <selection pane="bottomRight" activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8395,6 +8404,60 @@
         <v>402</v>
       </c>
     </row>
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F138" s="7">
+        <f t="shared" ref="F138" si="167">K138/J138</f>
+        <v>0.6331402680682755</v>
+      </c>
+      <c r="G138" s="7">
+        <f t="shared" ref="G138" si="168">L138/K138</f>
+        <v>0.91107414110929519</v>
+      </c>
+      <c r="H138" s="7">
+        <f t="shared" ref="H138" si="169">M138/K138</f>
+        <v>8.8923768878039405E-2</v>
+      </c>
+      <c r="I138" s="7">
+        <f t="shared" ref="I138" si="170">O138/L138</f>
+        <v>0.14183172064470839</v>
+      </c>
+      <c r="J138" s="6">
+        <v>75570.3</v>
+      </c>
+      <c r="K138" s="6">
+        <v>47846.6</v>
+      </c>
+      <c r="L138" s="6">
+        <v>43591.8</v>
+      </c>
+      <c r="M138" s="6">
+        <v>4254.7</v>
+      </c>
+      <c r="N138" s="6">
+        <v>27723.7</v>
+      </c>
+      <c r="O138" s="6">
+        <v>6182.7</v>
+      </c>
+      <c r="P138" t="s">
+        <v>406</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -8403,7 +8466,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <ignoredErrors>
-    <ignoredError sqref="B133:B137" numberStoredAsText="1"/>
+    <ignoredError sqref="B133:B138" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -9212,13 +9275,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FB4BCC-316E-4750-80C1-EBE5B1C8F894}">
-  <dimension ref="A1:D132"/>
+  <dimension ref="A1:D133"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B111" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B129" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A133" sqref="A133"/>
+      <selection pane="bottomRight" activeCell="A134" sqref="A134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10543,6 +10606,14 @@
       </c>
       <c r="B132" t="s">
         <v>402</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B133" t="s">
+        <v>406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Monthly labor update - Feb 2022
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R Projects\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995ED890-3479-4D4A-8BD3-D9D0A5CAF823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA1E185-F42C-4296-A5C0-0D205D3C2D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{DAAD9588-C85E-4EED-B6EC-CB5916F347A0}"/>
+    <workbookView xWindow="4560" yWindow="2985" windowWidth="21600" windowHeight="11385" xr2:uid="{DAAD9588-C85E-4EED-B6EC-CB5916F347A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="415">
   <si>
     <t>https://psa.gov.ph/statistics/survey/labor-force/lfs-index</t>
   </si>
@@ -1273,6 +1273,15 @@
   </si>
   <si>
     <t>https://psa.gov.ph/content/unemployment-rate-november-2021-estimated-65-percent</t>
+  </si>
+  <si>
+    <t>2021 Dec</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/unemployment-rate-december-2021-estimated-66-percent</t>
   </si>
 </sst>
 </file>
@@ -1723,13 +1732,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E701CAE5-AC4C-469D-A332-E8EB78C28CD8}">
-  <dimension ref="A1:P140"/>
+  <dimension ref="A1:P141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D122" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G122" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A141" sqref="A141"/>
+      <selection pane="bottomRight" activeCell="P142" sqref="P142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8588,6 +8597,60 @@
       </c>
       <c r="P140" t="s">
         <v>411</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="D141" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F141" s="7">
+        <f t="shared" ref="F141" si="180">K141/J141</f>
+        <v>0.65087071040179934</v>
+      </c>
+      <c r="G141" s="7">
+        <f t="shared" ref="G141" si="181">L141/K141</f>
+        <v>0.93396177690068338</v>
+      </c>
+      <c r="H141" s="7">
+        <f t="shared" ref="H141" si="182">M141/K141</f>
+        <v>6.603822309931652E-2</v>
+      </c>
+      <c r="I141" s="7">
+        <f t="shared" ref="I141" si="183">O141/L141</f>
+        <v>0.14718701580346608</v>
+      </c>
+      <c r="J141" s="6">
+        <v>76123.301000000007</v>
+      </c>
+      <c r="K141" s="6">
+        <v>49546.427000000003</v>
+      </c>
+      <c r="L141" s="6">
+        <v>46274.468999999997</v>
+      </c>
+      <c r="M141" s="6">
+        <v>3271.9580000000001</v>
+      </c>
+      <c r="N141" s="6">
+        <v>26576.874</v>
+      </c>
+      <c r="O141" s="6">
+        <v>6811.0010000000002</v>
+      </c>
+      <c r="P141" t="s">
+        <v>414</v>
       </c>
     </row>
   </sheetData>
@@ -9407,13 +9470,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FB4BCC-316E-4750-80C1-EBE5B1C8F894}">
-  <dimension ref="A1:D135"/>
+  <dimension ref="A1:D136"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B129" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B111" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A136" sqref="A136"/>
+      <selection pane="bottomRight" activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10762,6 +10825,14 @@
       </c>
       <c r="B135" t="s">
         <v>411</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="B136" t="s">
+        <v>414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Monthly labor update - May 2022
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R Projects\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA1E185-F42C-4296-A5C0-0D205D3C2D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4382096-9507-4459-8E7D-E256B48A7703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="2985" windowWidth="21600" windowHeight="11385" xr2:uid="{DAAD9588-C85E-4EED-B6EC-CB5916F347A0}"/>
+    <workbookView xWindow="2475" yWindow="645" windowWidth="13305" windowHeight="11685" xr2:uid="{DAAD9588-C85E-4EED-B6EC-CB5916F347A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="425">
   <si>
     <t>https://psa.gov.ph/statistics/survey/labor-force/lfs-index</t>
   </si>
@@ -1282,6 +1282,36 @@
   </si>
   <si>
     <t>https://psa.gov.ph/content/unemployment-rate-december-2021-estimated-66-percent</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/statistics/survey/labor-and-employment/labor-force-survey/title/Unemployment%20Rate%20in%20January%202022%20is%20Estimated%20at%206.4%20Percent</t>
+  </si>
+  <si>
+    <t>2021 Annual</t>
+  </si>
+  <si>
+    <t>2022 Jan</t>
+  </si>
+  <si>
+    <t>2022 Feb</t>
+  </si>
+  <si>
+    <t>2022 Mar</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/statistics/survey/labor-and-employment/labor-force-survey/title/Unemployment%20Rate%20in%20February%202022%20is%20Estimated%20at%206.4%20Percent</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/statistics/survey/labor-and-employment/labor-force-survey/title/Employment%20Rate%20in%20March%202022%20is%20Estimated%20at%2094.2%20Percent</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/statistics/survey/labor-and-employment/labor-force-survey/title/Employment%20Situation%20in%20July%202021</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/statistics/survey/labor-and-employment/labor-force-survey/title/2021%20Annual%20Labor%20Market%20Statistics%20%28Preliminary%20Results%29</t>
   </si>
 </sst>
 </file>
@@ -1732,13 +1762,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E701CAE5-AC4C-469D-A332-E8EB78C28CD8}">
-  <dimension ref="A1:P141"/>
+  <dimension ref="A1:P145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G122" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D122" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P142" sqref="P142"/>
+      <selection pane="bottomRight" activeCell="A146" sqref="A146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8007,40 +8037,37 @@
       <c r="D130" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E130" s="1" t="s">
-        <v>386</v>
-      </c>
       <c r="F130" s="7">
         <f t="shared" ref="F130:F132" si="143">K130/J130</f>
-        <v>0.60483656806272623</v>
+        <v>0.60497894238306626</v>
       </c>
       <c r="G130" s="7">
         <f t="shared" ref="G130:G132" si="144">L130/K130</f>
-        <v>0.91254026791799014</v>
+        <v>0.91232551283921692</v>
       </c>
       <c r="H130" s="7">
         <f t="shared" ref="H130:H132" si="145">M130/K130</f>
-        <v>8.7459732082009883E-2</v>
+        <v>8.7674487160783132E-2</v>
       </c>
       <c r="I130" s="7">
         <f t="shared" ref="I130:I132" si="146">O130/L130</f>
         <v>0.15973415166687116</v>
       </c>
       <c r="J130" s="6">
-        <v>74732.578000000009</v>
+        <v>74732.577999999994</v>
       </c>
       <c r="K130" s="6">
-        <v>45200.995999999999</v>
+        <v>45211.635999999999</v>
       </c>
       <c r="L130" s="6">
         <v>41247.728999999999</v>
       </c>
       <c r="M130" s="6">
-        <v>3953.2670000000003</v>
+        <v>3963.9070000000002</v>
       </c>
       <c r="N130" s="6">
         <f>J130-K130</f>
-        <v>29531.582000000009</v>
+        <v>29520.941999999995</v>
       </c>
       <c r="O130" s="6">
         <v>6588.6710000000003</v>
@@ -8062,40 +8089,37 @@
       <c r="D131" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E131" s="1" t="s">
-        <v>386</v>
-      </c>
       <c r="F131" s="7">
         <f t="shared" si="143"/>
-        <v>0.6345663613663034</v>
+        <v>0.63457004753807755</v>
       </c>
       <c r="G131" s="7">
         <f t="shared" si="144"/>
-        <v>0.91154641006686743</v>
+        <v>0.91154694501078559</v>
       </c>
       <c r="H131" s="7">
         <f t="shared" si="145"/>
-        <v>8.8453589933132501E-2</v>
+        <v>8.8453076112589277E-2</v>
       </c>
       <c r="I131" s="7">
         <f t="shared" si="146"/>
-        <v>0.18191980918214748</v>
+        <v>0.18191864566352034</v>
       </c>
       <c r="J131" s="6">
         <v>74603.142999999996</v>
       </c>
       <c r="K131" s="6">
-        <v>47340.645000000004</v>
+        <v>47340.92</v>
       </c>
       <c r="L131" s="6">
-        <v>43153.195</v>
+        <v>43153.470999999998</v>
       </c>
       <c r="M131" s="6">
         <v>4187.45</v>
       </c>
       <c r="N131" s="6">
-        <f t="shared" ref="N131:N140" si="147">J131-K131</f>
-        <v>27262.497999999992</v>
+        <f t="shared" ref="N131:N142" si="147">J131-K131</f>
+        <v>27262.222999999998</v>
       </c>
       <c r="O131" s="6">
         <v>7850.4210000000003</v>
@@ -8117,9 +8141,6 @@
       <c r="D132" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E132" s="1" t="s">
-        <v>386</v>
-      </c>
       <c r="F132" s="7">
         <f t="shared" si="143"/>
         <v>0.65003878942966153</v>
@@ -8511,15 +8532,15 @@
       </c>
       <c r="G139" s="7">
         <f t="shared" ref="G139" si="173">L139/K139</f>
-        <v>0.92597236425100349</v>
+        <v>0.92597295584196071</v>
       </c>
       <c r="H139" s="7">
         <f t="shared" ref="H139" si="174">M139/K139</f>
-        <v>7.4028354109444333E-2</v>
+        <v>7.4029156982886118E-2</v>
       </c>
       <c r="I139" s="7">
         <f t="shared" ref="I139" si="175">O139/L139</f>
-        <v>0.16073418245567409</v>
+        <v>0.16073453611187802</v>
       </c>
       <c r="J139" s="6">
         <v>75569.596000000005</v>
@@ -8528,17 +8549,17 @@
         <v>47330</v>
       </c>
       <c r="L139" s="6">
-        <v>43826.271999999997</v>
+        <v>43826.3</v>
       </c>
       <c r="M139" s="6">
-        <v>3503.7620000000002</v>
+        <v>3503.8</v>
       </c>
       <c r="N139" s="6">
         <f t="shared" si="147"/>
         <v>28239.596000000005</v>
       </c>
       <c r="O139" s="6">
-        <v>7044.38</v>
+        <v>7044.4</v>
       </c>
       <c r="P139" t="s">
         <v>408</v>
@@ -8616,19 +8637,19 @@
         <v>386</v>
       </c>
       <c r="F141" s="7">
-        <f t="shared" ref="F141" si="180">K141/J141</f>
+        <f t="shared" ref="F141:F142" si="180">K141/J141</f>
         <v>0.65087071040179934</v>
       </c>
       <c r="G141" s="7">
-        <f t="shared" ref="G141" si="181">L141/K141</f>
+        <f t="shared" ref="G141:G142" si="181">L141/K141</f>
         <v>0.93396177690068338</v>
       </c>
       <c r="H141" s="7">
-        <f t="shared" ref="H141" si="182">M141/K141</f>
+        <f t="shared" ref="H141:H142" si="182">M141/K141</f>
         <v>6.603822309931652E-2</v>
       </c>
       <c r="I141" s="7">
-        <f t="shared" ref="I141" si="183">O141/L141</f>
+        <f t="shared" ref="I141:I142" si="183">O141/L141</f>
         <v>0.14718701580346608</v>
       </c>
       <c r="J141" s="6">
@@ -8644,13 +8665,234 @@
         <v>3271.9580000000001</v>
       </c>
       <c r="N141" s="6">
-        <v>26576.874</v>
+        <f t="shared" si="147"/>
+        <v>26576.874000000003</v>
       </c>
       <c r="O141" s="6">
         <v>6811.0010000000002</v>
       </c>
       <c r="P141" t="s">
         <v>414</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F142" s="7">
+        <f t="shared" si="180"/>
+        <v>0.63346515961840855</v>
+      </c>
+      <c r="G142" s="7">
+        <f t="shared" si="181"/>
+        <v>0.92218769100179576</v>
+      </c>
+      <c r="H142" s="7">
+        <f t="shared" si="182"/>
+        <v>7.781231423920712E-2</v>
+      </c>
+      <c r="I142" s="7">
+        <f t="shared" si="183"/>
+        <v>0.15919453293482841</v>
+      </c>
+      <c r="J142" s="6">
+        <v>75301.370999999999</v>
+      </c>
+      <c r="K142" s="6">
+        <v>47700.794999999998</v>
+      </c>
+      <c r="L142" s="6">
+        <v>43989.086000000003</v>
+      </c>
+      <c r="M142" s="6">
+        <v>3711.7092499999999</v>
+      </c>
+      <c r="N142" s="6">
+        <f t="shared" si="147"/>
+        <v>27600.576000000001</v>
+      </c>
+      <c r="O142" s="6">
+        <v>7002.8220000000001</v>
+      </c>
+      <c r="P142" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="D143" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F143" s="7">
+        <f t="shared" ref="F143" si="184">K143/J143</f>
+        <v>0.60535990020885577</v>
+      </c>
+      <c r="G143" s="7">
+        <f t="shared" ref="G143" si="185">L143/K143</f>
+        <v>0.93632554233523335</v>
+      </c>
+      <c r="H143" s="7">
+        <f t="shared" ref="H143" si="186">M143/K143</f>
+        <v>6.3674457664766593E-2</v>
+      </c>
+      <c r="I143" s="7">
+        <f t="shared" ref="I143" si="187">O143/L143</f>
+        <v>0.14869538765410792</v>
+      </c>
+      <c r="J143" s="6">
+        <v>75894.509999999995</v>
+      </c>
+      <c r="K143" s="6">
+        <v>45943.493000000002</v>
+      </c>
+      <c r="L143" s="6">
+        <v>43018.065999999999</v>
+      </c>
+      <c r="M143" s="6">
+        <v>2925.4270000000001</v>
+      </c>
+      <c r="N143" s="6">
+        <f>J143-K143</f>
+        <v>29951.016999999993</v>
+      </c>
+      <c r="O143" s="6">
+        <v>6396.5879999999997</v>
+      </c>
+      <c r="P143" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="D144" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F144" s="7">
+        <f t="shared" ref="F144" si="188">K144/J144</f>
+        <v>0.63826219480167501</v>
+      </c>
+      <c r="G144" s="7">
+        <f t="shared" ref="G144" si="189">L144/K144</f>
+        <v>0.93568617546624733</v>
+      </c>
+      <c r="H144" s="7">
+        <f t="shared" ref="H144" si="190">M144/K144</f>
+        <v>6.4313824533752645E-2</v>
+      </c>
+      <c r="I144" s="7">
+        <f t="shared" ref="I144" si="191">O144/L144</f>
+        <v>0.14032389252916841</v>
+      </c>
+      <c r="J144" s="6">
+        <v>76153.759999999995</v>
+      </c>
+      <c r="K144" s="6">
+        <v>48606.065999999999</v>
+      </c>
+      <c r="L144" s="6">
+        <v>45480.023999999998</v>
+      </c>
+      <c r="M144" s="6">
+        <v>3126.0419999999999</v>
+      </c>
+      <c r="N144" s="6">
+        <f>J144-K144</f>
+        <v>27547.693999999996</v>
+      </c>
+      <c r="O144" s="6">
+        <v>6381.9340000000002</v>
+      </c>
+      <c r="P144" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="D145" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F145" s="7">
+        <f t="shared" ref="F145" si="192">K145/J145</f>
+        <v>0.65371628089860889</v>
+      </c>
+      <c r="G145" s="7">
+        <f t="shared" ref="G145" si="193">L145/K145</f>
+        <v>0.94232932300839312</v>
+      </c>
+      <c r="H145" s="7">
+        <f t="shared" ref="H145" si="194">M145/K145</f>
+        <v>5.7670676991606946E-2</v>
+      </c>
+      <c r="I145" s="7">
+        <f t="shared" ref="I145" si="195">O145/L145</f>
+        <v>0.15799248754088102</v>
+      </c>
+      <c r="J145" s="6">
+        <v>76256.183999999994</v>
+      </c>
+      <c r="K145" s="6">
+        <v>49849.909</v>
+      </c>
+      <c r="L145" s="6">
+        <v>46975.031000000003</v>
+      </c>
+      <c r="M145" s="6">
+        <v>2874.8780000000002</v>
+      </c>
+      <c r="N145" s="6">
+        <f>J145-K145</f>
+        <v>26406.274999999994</v>
+      </c>
+      <c r="O145" s="6">
+        <v>7421.7020000000002</v>
+      </c>
+      <c r="P145" t="s">
+        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -9470,13 +9712,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FB4BCC-316E-4750-80C1-EBE5B1C8F894}">
-  <dimension ref="A1:D136"/>
+  <dimension ref="A1:D140"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B111" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B125" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A137" sqref="A137"/>
+      <selection pane="bottomRight" activeCell="B137" sqref="B137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10771,7 +11013,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>391</v>
       </c>
@@ -10779,7 +11021,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>394</v>
       </c>
@@ -10787,15 +11029,18 @@
         <v>395</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>398</v>
       </c>
       <c r="B131" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D131" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>403</v>
       </c>
@@ -10803,7 +11048,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>404</v>
       </c>
@@ -10811,7 +11056,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>407</v>
       </c>
@@ -10819,7 +11064,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>409</v>
       </c>
@@ -10827,12 +11072,44 @@
         <v>411</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>412</v>
       </c>
       <c r="B136" t="s">
         <v>414</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="B137" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="B138" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B139" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="B140" t="s">
+        <v>422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Monthly labor update - June 2022
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R Projects\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4382096-9507-4459-8E7D-E256B48A7703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83162ED-5E05-4AD8-9319-9ED7EF4F68F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2475" yWindow="645" windowWidth="13305" windowHeight="11685" xr2:uid="{DAAD9588-C85E-4EED-B6EC-CB5916F347A0}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{DAAD9588-C85E-4EED-B6EC-CB5916F347A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="427">
   <si>
     <t>https://psa.gov.ph/statistics/survey/labor-force/lfs-index</t>
   </si>
@@ -1312,6 +1312,12 @@
   </si>
   <si>
     <t>https://psa.gov.ph/statistics/survey/labor-and-employment/labor-force-survey/title/2021%20Annual%20Labor%20Market%20Statistics%20%28Preliminary%20Results%29</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/employment-rate-april-2022-estimated-943-percent</t>
+  </si>
+  <si>
+    <t>2022 Apr</t>
   </si>
 </sst>
 </file>
@@ -1762,13 +1768,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E701CAE5-AC4C-469D-A332-E8EB78C28CD8}">
-  <dimension ref="A1:P145"/>
+  <dimension ref="A1:P146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D122" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A146" sqref="A146"/>
+      <selection pane="bottomRight" activeCell="A147" sqref="A147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8193,43 +8199,40 @@
       <c r="D133" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E133" s="1" t="s">
-        <v>386</v>
-      </c>
       <c r="F133" s="7">
         <f t="shared" ref="F133" si="148">K133/J133</f>
-        <v>0.6323427528672978</v>
+        <v>0.63233959377229831</v>
       </c>
       <c r="G133" s="7">
         <f t="shared" ref="G133" si="149">L133/K133</f>
-        <v>0.91271547296240896</v>
+        <v>0.91271602770276217</v>
       </c>
       <c r="H133" s="7">
         <f t="shared" ref="H133" si="150">M133/K133</f>
-        <v>8.728452703759107E-2</v>
+        <v>8.7283972297237791E-2</v>
       </c>
       <c r="I133" s="7">
         <f t="shared" ref="I133" si="151">O133/L133</f>
-        <v>0.17224755317298324</v>
+        <v>0.17223960201131672</v>
       </c>
       <c r="J133" s="6">
-        <v>74970.588000000003</v>
+        <v>74970.514999999999</v>
       </c>
       <c r="K133" s="6">
-        <v>47407.108</v>
+        <v>47406.824999999997</v>
       </c>
       <c r="L133" s="6">
-        <v>43269.201000000001</v>
+        <v>43268.968999999997</v>
       </c>
       <c r="M133" s="6">
-        <v>4137.9070000000002</v>
+        <v>4137.8559999999998</v>
       </c>
       <c r="N133" s="6">
         <f t="shared" si="147"/>
-        <v>27563.480000000003</v>
+        <v>27563.690000000002</v>
       </c>
       <c r="O133" s="6">
-        <v>7453.0140000000001</v>
+        <v>7452.63</v>
       </c>
       <c r="P133" t="s">
         <v>389</v>
@@ -8893,6 +8896,61 @@
       </c>
       <c r="P145" t="s">
         <v>422</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D146" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F146" s="7">
+        <f t="shared" ref="F146" si="196">K146/J146</f>
+        <v>0.63363855623736731</v>
+      </c>
+      <c r="G146" s="7">
+        <f t="shared" ref="G146" si="197">L146/K146</f>
+        <v>0.94292277756557008</v>
+      </c>
+      <c r="H146" s="7">
+        <f t="shared" ref="H146" si="198">M146/K146</f>
+        <v>5.7077222434429822E-2</v>
+      </c>
+      <c r="I146" s="7">
+        <f t="shared" ref="I146" si="199">O146/L146</f>
+        <v>0.14022888931866281</v>
+      </c>
+      <c r="J146" s="6">
+        <v>76373.801000000007</v>
+      </c>
+      <c r="K146" s="6">
+        <v>48393.385000000002</v>
+      </c>
+      <c r="L146" s="6">
+        <v>45631.224999999999</v>
+      </c>
+      <c r="M146" s="6">
+        <v>2762.16</v>
+      </c>
+      <c r="N146" s="6">
+        <f>J146-K146</f>
+        <v>27980.416000000005</v>
+      </c>
+      <c r="O146" s="6">
+        <v>6398.8159999999998</v>
+      </c>
+      <c r="P146" t="s">
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -9712,13 +9770,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FB4BCC-316E-4750-80C1-EBE5B1C8F894}">
-  <dimension ref="A1:D140"/>
+  <dimension ref="A1:D141"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B125" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B137" sqref="B137"/>
+      <selection pane="bottomRight" activeCell="A142" sqref="A142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11110,6 +11168,14 @@
       </c>
       <c r="B140" t="s">
         <v>422</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B141" t="s">
+        <v>425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Monthly labor update - July 2022
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R Projects\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83162ED-5E05-4AD8-9319-9ED7EF4F68F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F56F48-F46D-43EA-8EE7-422FB4763235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{DAAD9588-C85E-4EED-B6EC-CB5916F347A0}"/>
+    <workbookView xWindow="480" yWindow="1860" windowWidth="15330" windowHeight="10350" xr2:uid="{DAAD9588-C85E-4EED-B6EC-CB5916F347A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="429">
   <si>
     <t>https://psa.gov.ph/statistics/survey/labor-force/lfs-index</t>
   </si>
@@ -1318,6 +1318,12 @@
   </si>
   <si>
     <t>2022 Apr</t>
+  </si>
+  <si>
+    <t>2022 May</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/employment-rate-may-2022-estimated-940-percent</t>
   </si>
 </sst>
 </file>
@@ -1768,13 +1774,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E701CAE5-AC4C-469D-A332-E8EB78C28CD8}">
-  <dimension ref="A1:P146"/>
+  <dimension ref="A1:P147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D122" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F130" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A147" sqref="A147"/>
+      <selection pane="bottomRight" activeCell="A148" sqref="A148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8251,43 +8257,40 @@
       <c r="D134" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E134" s="1" t="s">
-        <v>386</v>
-      </c>
       <c r="F134" s="7">
         <f t="shared" ref="F134" si="152">K134/J134</f>
-        <v>0.64557037474745804</v>
+        <v>0.6457080371496432</v>
       </c>
       <c r="G134" s="7">
         <f t="shared" ref="G134" si="153">L134/K134</f>
-        <v>0.92300115619049261</v>
+        <v>0.92283120237813099</v>
       </c>
       <c r="H134" s="7">
         <f t="shared" ref="H134" si="154">M134/K134</f>
-        <v>7.6998864450974439E-2</v>
+        <v>7.7168797621869012E-2</v>
       </c>
       <c r="I134" s="7">
         <f t="shared" ref="I134" si="155">O134/L134</f>
-        <v>0.12281109592634562</v>
+        <v>0.1228153867653205</v>
       </c>
       <c r="J134" s="6">
-        <v>75043.978000000003</v>
+        <v>75043.520000000004</v>
       </c>
       <c r="K134" s="6">
-        <v>48446.169000000002</v>
+        <v>48456.203999999998</v>
       </c>
       <c r="L134" s="6">
-        <v>44715.87</v>
+        <v>44716.896999999997</v>
       </c>
       <c r="M134" s="6">
-        <v>3730.3</v>
+        <v>3739.3069999999998</v>
       </c>
       <c r="N134" s="6">
         <f t="shared" si="147"/>
-        <v>26597.809000000001</v>
+        <v>26587.316000000006</v>
       </c>
       <c r="O134" s="6">
-        <v>5491.6050000000005</v>
+        <v>5491.9229999999998</v>
       </c>
       <c r="P134" t="s">
         <v>396</v>
@@ -8915,19 +8918,19 @@
         <v>386</v>
       </c>
       <c r="F146" s="7">
-        <f t="shared" ref="F146" si="196">K146/J146</f>
+        <f t="shared" ref="F146:F147" si="196">K146/J146</f>
         <v>0.63363855623736731</v>
       </c>
       <c r="G146" s="7">
-        <f t="shared" ref="G146" si="197">L146/K146</f>
+        <f t="shared" ref="G146:G147" si="197">L146/K146</f>
         <v>0.94292277756557008</v>
       </c>
       <c r="H146" s="7">
-        <f t="shared" ref="H146" si="198">M146/K146</f>
+        <f t="shared" ref="H146:H147" si="198">M146/K146</f>
         <v>5.7077222434429822E-2</v>
       </c>
       <c r="I146" s="7">
-        <f t="shared" ref="I146" si="199">O146/L146</f>
+        <f t="shared" ref="I146:I147" si="199">O146/L146</f>
         <v>0.14022888931866281</v>
       </c>
       <c r="J146" s="6">
@@ -8951,6 +8954,61 @@
       </c>
       <c r="P146" t="s">
         <v>425</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D147" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F147" s="7">
+        <f t="shared" si="196"/>
+        <v>0.64040035214677771</v>
+      </c>
+      <c r="G147" s="7">
+        <f t="shared" si="197"/>
+        <v>0.9402713798018536</v>
+      </c>
+      <c r="H147" s="7">
+        <f t="shared" si="198"/>
+        <v>5.9728620198146364E-2</v>
+      </c>
+      <c r="I147" s="7">
+        <f t="shared" si="199"/>
+        <v>0.1446923174621802</v>
+      </c>
+      <c r="J147" s="6">
+        <v>76531.724000000002</v>
+      </c>
+      <c r="K147" s="6">
+        <v>49010.942999999999</v>
+      </c>
+      <c r="L147" s="6">
+        <v>46083.587</v>
+      </c>
+      <c r="M147" s="6">
+        <v>2927.3560000000002</v>
+      </c>
+      <c r="N147" s="6">
+        <f>J147-K147</f>
+        <v>27520.781000000003</v>
+      </c>
+      <c r="O147" s="6">
+        <v>6667.9409999999998</v>
+      </c>
+      <c r="P147" t="s">
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -9770,13 +9828,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FB4BCC-316E-4750-80C1-EBE5B1C8F894}">
-  <dimension ref="A1:D141"/>
+  <dimension ref="A1:D142"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B125" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A142" sqref="A142"/>
+      <selection pane="bottomRight" activeCell="B142" sqref="B142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11176,6 +11234,14 @@
       </c>
       <c r="B141" t="s">
         <v>425</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="B142" t="s">
+        <v>428</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Monthly labor update - August 2022
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R Projects\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F56F48-F46D-43EA-8EE7-422FB4763235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFB7B19-4C11-4D0B-AFBC-A2F59FD00C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1860" windowWidth="15330" windowHeight="10350" xr2:uid="{DAAD9588-C85E-4EED-B6EC-CB5916F347A0}"/>
+    <workbookView xWindow="12165" yWindow="5130" windowWidth="14325" windowHeight="8790" xr2:uid="{DAAD9588-C85E-4EED-B6EC-CB5916F347A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="432">
   <si>
     <t>https://psa.gov.ph/statistics/survey/labor-force/lfs-index</t>
   </si>
@@ -1324,6 +1324,15 @@
   </si>
   <si>
     <t>https://psa.gov.ph/content/employment-rate-may-2022-estimated-940-percent</t>
+  </si>
+  <si>
+    <t>2022 June`</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/employment-rate-june-2022-estimated-940</t>
+  </si>
+  <si>
+    <t>2022 Jun</t>
   </si>
 </sst>
 </file>
@@ -1774,13 +1783,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E701CAE5-AC4C-469D-A332-E8EB78C28CD8}">
-  <dimension ref="A1:P147"/>
+  <dimension ref="A1:P148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F130" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D135" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A148" sqref="A148"/>
+      <selection pane="bottomRight" activeCell="A149" sqref="A149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8309,43 +8318,39 @@
       <c r="D135" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="E135" s="1" t="s">
-        <v>386</v>
-      </c>
       <c r="F135" s="7">
         <f t="shared" ref="F135" si="156">K135/J135</f>
-        <v>0.65042469049675899</v>
+        <v>0.65050855094211091</v>
       </c>
       <c r="G135" s="7">
         <f t="shared" ref="G135" si="157">L135/K135</f>
-        <v>0.9229250764382293</v>
+        <v>0.9228100076034792</v>
       </c>
       <c r="H135" s="7">
         <f t="shared" ref="H135" si="158">M135/K135</f>
-        <v>7.7074923561770758E-2</v>
+        <v>7.7190012869001109E-2</v>
       </c>
       <c r="I135" s="7">
         <f t="shared" ref="I135" si="159">O135/L135</f>
-        <v>0.14219350306093503</v>
+        <v>0.14219855769967776</v>
       </c>
       <c r="J135" s="6">
-        <v>75089.036000000007</v>
+        <v>75089.035999999993</v>
       </c>
       <c r="K135" s="6">
-        <v>48839.762999999999</v>
+        <v>48846.06</v>
       </c>
       <c r="L135" s="6">
-        <v>45075.442000000003</v>
+        <v>45075.633000000002</v>
       </c>
       <c r="M135" s="6">
-        <v>3764.3209999999999</v>
+        <v>3770.4279999999999</v>
       </c>
       <c r="N135" s="6">
-        <f t="shared" si="147"/>
-        <v>26249.273000000008</v>
+        <v>26242.974999999999</v>
       </c>
       <c r="O135" s="6">
-        <v>6409.4350000000004</v>
+        <v>6409.69</v>
       </c>
       <c r="P135" t="s">
         <v>395</v>
@@ -9009,6 +9014,60 @@
       </c>
       <c r="P147" t="s">
         <v>428</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="D148" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="F148" s="7">
+        <f t="shared" ref="F148" si="200">K148/J148</f>
+        <v>0.64778131062774802</v>
+      </c>
+      <c r="G148" s="7">
+        <f t="shared" ref="G148" si="201">L148/K148</f>
+        <v>0.93969828003058808</v>
+      </c>
+      <c r="H148" s="7">
+        <f t="shared" ref="H148" si="202">M148/K148</f>
+        <v>6.0301719969411922E-2</v>
+      </c>
+      <c r="I148" s="7">
+        <f t="shared" ref="I148" si="203">O148/L148</f>
+        <v>0.12636794890817246</v>
+      </c>
+      <c r="J148" s="6">
+        <v>76540.345000000001</v>
+      </c>
+      <c r="K148" s="6">
+        <v>49581.404999999999</v>
+      </c>
+      <c r="L148" s="6">
+        <v>46591.561000000002</v>
+      </c>
+      <c r="M148" s="6">
+        <v>2989.8440000000001</v>
+      </c>
+      <c r="N148" s="6">
+        <v>26958.94</v>
+      </c>
+      <c r="O148" s="6">
+        <v>5887.68</v>
+      </c>
+      <c r="P148" t="s">
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -9828,13 +9887,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FB4BCC-316E-4750-80C1-EBE5B1C8F894}">
-  <dimension ref="A1:D142"/>
+  <dimension ref="A1:D143"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B125" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B142" sqref="B142"/>
+      <selection pane="bottomRight" activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11242,6 +11301,14 @@
       </c>
       <c r="B142" t="s">
         <v>428</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="B143" t="s">
+        <v>430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Monthly labor update - December 2022
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R-Projects\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5536927F-681A-4D13-9805-E230A607FEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBF9EDD-8DFF-450C-B043-41C3C4CB3520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13035" yWindow="2925" windowWidth="13380" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1552" uniqueCount="615">
   <si>
     <t>LFS Round</t>
   </si>
@@ -1875,6 +1875,12 @@
   </si>
   <si>
     <t>https://psa.gov.ph/content/unemployment-rate-november-2022-estimated-42-percent</t>
+  </si>
+  <si>
+    <t>2022 Dec</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/unemployment-rate-december-2022-estimated-43-percent</t>
   </si>
 </sst>
 </file>
@@ -2216,13 +2222,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P258"/>
+  <dimension ref="A1:P259"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D222" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A259" sqref="A259"/>
+      <selection pane="bottomRight" activeCell="A260" sqref="A260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13223,20 +13229,17 @@
       <c r="D246" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E246" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F246" s="3">
         <f t="shared" si="23"/>
-        <v>0.65087071040179934</v>
+        <v>0.65102498642301387</v>
       </c>
       <c r="G246" s="3">
         <f t="shared" si="24"/>
-        <v>0.93396177690068338</v>
+        <v>0.9337404522051469</v>
       </c>
       <c r="H246" s="3">
         <f t="shared" si="25"/>
-        <v>6.603822309931652E-2</v>
+        <v>6.6259547794853046E-2</v>
       </c>
       <c r="I246" s="3">
         <f t="shared" si="26"/>
@@ -13246,17 +13249,17 @@
         <v>76123.301000000007</v>
       </c>
       <c r="K246" s="2">
-        <v>49546.427000000003</v>
+        <v>49558.171000000002</v>
       </c>
       <c r="L246" s="2">
         <v>46274.468999999997</v>
       </c>
       <c r="M246" s="2">
-        <v>3271.9580000000001</v>
+        <v>3283.7020000000002</v>
       </c>
       <c r="N246" s="2">
         <f t="shared" si="27"/>
-        <v>26576.874000000003</v>
+        <v>26565.130000000005</v>
       </c>
       <c r="O246" s="2">
         <v>6811.0010000000002</v>
@@ -13923,6 +13926,61 @@
       </c>
       <c r="P258" t="s">
         <v>612</v>
+      </c>
+    </row>
+    <row r="259" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A259" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="D259" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E259" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F259" s="3">
+        <f>K259/J259</f>
+        <v>0.66390214884369403</v>
+      </c>
+      <c r="G259" s="3">
+        <f>L259/K259</f>
+        <v>0.95666600288938342</v>
+      </c>
+      <c r="H259" s="3">
+        <f>M259/K259</f>
+        <v>4.3333997110616529E-2</v>
+      </c>
+      <c r="I259" s="3">
+        <f>O259/L259</f>
+        <v>0.12645847609010394</v>
+      </c>
+      <c r="J259" s="2">
+        <v>77152.936000000002</v>
+      </c>
+      <c r="K259" s="2">
+        <v>51222</v>
+      </c>
+      <c r="L259" s="2">
+        <v>49002.345999999998</v>
+      </c>
+      <c r="M259" s="2">
+        <v>2219.654</v>
+      </c>
+      <c r="N259" s="2">
+        <f>J259-K259</f>
+        <v>25930.936000000002</v>
+      </c>
+      <c r="O259" s="2">
+        <v>6196.7619999999997</v>
+      </c>
+      <c r="P259" t="s">
+        <v>614</v>
       </c>
     </row>
   </sheetData>
@@ -14736,14 +14794,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D149"/>
+  <dimension ref="A1:D150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="5" topLeftCell="B116" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B147" sqref="B147"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B149" sqref="B149"/>
+      <selection pane="bottomRight" activeCell="A151" sqref="A151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16207,6 +16265,14 @@
       </c>
       <c r="B149" t="s">
         <v>612</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="B150" t="s">
+        <v>614</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Monthly labor update - January 2023
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R-Projects\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBF9EDD-8DFF-450C-B043-41C3C4CB3520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47587AE-2CD8-4955-BB7C-695E6D847BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1552" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="631">
   <si>
     <t>LFS Round</t>
   </si>
@@ -1881,6 +1881,54 @@
   </si>
   <si>
     <t>https://psa.gov.ph/content/unemployment-rate-december-2022-estimated-43-percent</t>
+  </si>
+  <si>
+    <t>2022 Annual</t>
+  </si>
+  <si>
+    <t>2023 Jan</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>2023 Feb</t>
+  </si>
+  <si>
+    <t>2023 Mar</t>
+  </si>
+  <si>
+    <t>2023 Apr</t>
+  </si>
+  <si>
+    <t>2023 May</t>
+  </si>
+  <si>
+    <t>2023 Jun</t>
+  </si>
+  <si>
+    <t>2023 Jul</t>
+  </si>
+  <si>
+    <t>2023 Aug</t>
+  </si>
+  <si>
+    <t>2023 Sep</t>
+  </si>
+  <si>
+    <t>2023 Oct</t>
+  </si>
+  <si>
+    <t>2023 Nov</t>
+  </si>
+  <si>
+    <t>2023 Dec</t>
+  </si>
+  <si>
+    <t>2023 Annual</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/statistics/survey/labor-and-employment/labor-force-survey/title/Unemployment%20Rate%20in%20January%202023%20is%20Estimated%20at%204.8%20Percent</t>
   </si>
 </sst>
 </file>
@@ -2222,13 +2270,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P259"/>
+  <dimension ref="A1:P273"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D222" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F240" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A260" sqref="A260"/>
+      <selection pane="bottomRight" activeCell="F262" sqref="F262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13273,7 +13321,7 @@
         <v>460</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>461</v>
+        <v>436</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>28</v>
@@ -13336,43 +13384,40 @@
       <c r="D248" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E248" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F248" s="3">
         <f t="shared" si="23"/>
-        <v>0.60535990020885577</v>
+        <v>0.60537273189677987</v>
       </c>
       <c r="G248" s="3">
         <f t="shared" si="24"/>
-        <v>0.93632554233523335</v>
+        <v>0.93611945522190365</v>
       </c>
       <c r="H248" s="3">
         <f t="shared" si="25"/>
-        <v>6.3674457664766593E-2</v>
+        <v>6.3880544778096363E-2</v>
       </c>
       <c r="I248" s="3">
         <f t="shared" si="26"/>
-        <v>0.14869538765410792</v>
+        <v>0.14863257413303863</v>
       </c>
       <c r="J248" s="2">
-        <v>75894.509999999995</v>
+        <v>76347.826000000001</v>
       </c>
       <c r="K248" s="2">
-        <v>45943.493000000002</v>
+        <v>46218.892</v>
       </c>
       <c r="L248" s="2">
-        <v>43018.065999999999</v>
+        <v>43266.404000000002</v>
       </c>
       <c r="M248" s="2">
-        <v>2925.4270000000001</v>
+        <v>2952.4879999999998</v>
       </c>
       <c r="N248" s="2">
         <f t="shared" si="27"/>
-        <v>29951.016999999993</v>
+        <v>30128.934000000001</v>
       </c>
       <c r="O248" s="2">
-        <v>6396.5879999999997</v>
+        <v>6430.7969999999996</v>
       </c>
       <c r="P248" t="s">
         <v>464</v>
@@ -13835,11 +13880,11 @@
         <v>425</v>
       </c>
       <c r="F257" s="3">
-        <f>K257/J257</f>
+        <f t="shared" ref="F257:G259" si="28">K257/J257</f>
         <v>0.64150515020588861</v>
       </c>
       <c r="G257" s="3">
-        <f>L257/K257</f>
+        <f t="shared" si="28"/>
         <v>0.95457810864448256</v>
       </c>
       <c r="H257" s="3">
@@ -13890,11 +13935,11 @@
         <v>425</v>
       </c>
       <c r="F258" s="3">
-        <f>K258/J258</f>
+        <f t="shared" si="28"/>
         <v>0.67455240427974039</v>
       </c>
       <c r="G258" s="3">
-        <f>L258/K258</f>
+        <f t="shared" si="28"/>
         <v>0.95804382818007605</v>
       </c>
       <c r="H258" s="3">
@@ -13945,11 +13990,11 @@
         <v>425</v>
       </c>
       <c r="F259" s="3">
-        <f>K259/J259</f>
+        <f t="shared" si="28"/>
         <v>0.66390214884369403</v>
       </c>
       <c r="G259" s="3">
-        <f>L259/K259</f>
+        <f t="shared" si="28"/>
         <v>0.95666600288938342</v>
       </c>
       <c r="H259" s="3">
@@ -13981,6 +14026,282 @@
       </c>
       <c r="P259" t="s">
         <v>614</v>
+      </c>
+    </row>
+    <row r="260" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A260" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="B260" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D260" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E260" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="261" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A261" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D261" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F261" s="3">
+        <f t="shared" ref="F261" si="29">K261/J261</f>
+        <v>0.6448960129797745</v>
+      </c>
+      <c r="G261" s="3">
+        <f t="shared" ref="G261" si="30">L261/K261</f>
+        <v>0.95227963685377781</v>
+      </c>
+      <c r="H261" s="3">
+        <f>M261/K261</f>
+        <v>4.7720383257059969E-2</v>
+      </c>
+      <c r="I261" s="3">
+        <f>O261/L261</f>
+        <v>0.14053252516574691</v>
+      </c>
+      <c r="J261" s="2">
+        <v>77104.574999999997</v>
+      </c>
+      <c r="K261" s="2">
+        <v>49724.432999999997</v>
+      </c>
+      <c r="L261" s="2">
+        <v>47351.565000000002</v>
+      </c>
+      <c r="M261" s="2">
+        <v>2372.8690000000001</v>
+      </c>
+      <c r="N261" s="2">
+        <f>J261-K261</f>
+        <v>27380.142</v>
+      </c>
+      <c r="O261" s="2">
+        <v>6654.4350000000004</v>
+      </c>
+      <c r="P261" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="262" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A262" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="D262" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E262" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="263" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A263" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D263" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E263" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="264" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A264" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="B264" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D264" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E264" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="265" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A265" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D265" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E265" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="266" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A266" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="B266" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="D266" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E266" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="267" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A267" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D267" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E267" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="268" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A268" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="B268" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D268" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E268" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="269" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A269" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D269" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E269" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="270" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A270" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="B270" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D270" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E270" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="271" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A271" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D271" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E271" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="272" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A272" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="B272" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="D272" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A273" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="C273" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D273" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E273" s="1" t="s">
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -14794,14 +15115,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D150"/>
+  <dimension ref="A1:D164"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B116" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B132" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B147" sqref="B147"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A151" sqref="A151"/>
+      <selection pane="bottomRight" activeCell="C152" sqref="C152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16273,6 +16594,79 @@
       </c>
       <c r="B150" t="s">
         <v>614</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="B152" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>629</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Monthly labor update - February 2023
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R-Projects\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47587AE-2CD8-4955-BB7C-695E6D847BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B659CE4-F2AB-4838-AEC8-84CB2B687AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1639" uniqueCount="632">
   <si>
     <t>LFS Round</t>
   </si>
@@ -1929,6 +1929,9 @@
   </si>
   <si>
     <t>https://psa.gov.ph/statistics/survey/labor-and-employment/labor-force-survey/title/Unemployment%20Rate%20in%20January%202023%20is%20Estimated%20at%204.8%20Percent</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/employment-rate-february-2023-estimated-952-percent</t>
   </si>
 </sst>
 </file>
@@ -2276,7 +2279,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="F240" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F262" sqref="F262"/>
+      <selection pane="bottomRight" activeCell="F263" sqref="F263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14062,11 +14065,11 @@
         <v>425</v>
       </c>
       <c r="F261" s="3">
-        <f t="shared" ref="F261" si="29">K261/J261</f>
+        <f t="shared" ref="F261:F262" si="29">K261/J261</f>
         <v>0.6448960129797745</v>
       </c>
       <c r="G261" s="3">
-        <f t="shared" ref="G261" si="30">L261/K261</f>
+        <f t="shared" ref="G261:G262" si="30">L261/K261</f>
         <v>0.95227963685377781</v>
       </c>
       <c r="H261" s="3">
@@ -14115,6 +14118,44 @@
       </c>
       <c r="E262" s="1" t="s">
         <v>425</v>
+      </c>
+      <c r="F262" s="3">
+        <f t="shared" si="29"/>
+        <v>0.66583719426919541</v>
+      </c>
+      <c r="G262" s="3">
+        <f t="shared" si="30"/>
+        <v>0.95172870627870398</v>
+      </c>
+      <c r="H262" s="3">
+        <f>M262/K262</f>
+        <v>4.8271293721296016E-2</v>
+      </c>
+      <c r="I262" s="3">
+        <f>O262/L262</f>
+        <v>0.12883202514521366</v>
+      </c>
+      <c r="J262" s="2">
+        <v>77003.566999999995</v>
+      </c>
+      <c r="K262" s="2">
+        <v>51271.839</v>
+      </c>
+      <c r="L262" s="2">
+        <v>48796.881000000001</v>
+      </c>
+      <c r="M262" s="2">
+        <v>2474.9580000000001</v>
+      </c>
+      <c r="N262" s="2">
+        <f>J262-K262</f>
+        <v>25731.727999999996</v>
+      </c>
+      <c r="O262" s="2">
+        <v>6286.6009999999997</v>
+      </c>
+      <c r="P262" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="263" spans="1:16" x14ac:dyDescent="0.25">
@@ -15122,7 +15163,7 @@
       <selection activeCell="B147" sqref="B147"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C152" sqref="C152"/>
+      <selection pane="bottomRight" activeCell="B153" sqref="B153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16612,6 +16653,9 @@
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>618</v>
+      </c>
+      <c r="B153" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Monthly labor update - April 2023
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="634">
   <si>
     <t xml:space="preserve">LFS Round</t>
   </si>
@@ -1504,6 +1504,9 @@
   </si>
   <si>
     <t xml:space="preserve">2023 Apr</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/unemployment-rate-april-2023-estimated-45-percent</t>
   </si>
   <si>
     <t xml:space="preserve">2023 May</t>
@@ -1995,7 +1998,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="3" xfId="0" applyNumberFormat="1"/>
@@ -2016,7 +2019,6 @@
     <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -12707,7 +12709,7 @@
         <v>32</v>
       </c>
       <c r="F230" s="11">
-        <f t="shared" ref="F230:G262" si="23">K230/J230</f>
+        <f t="shared" ref="F230:G263" si="23">K230/J230</f>
         <v>0.6168840849278201</v>
       </c>
       <c r="G230" s="11">
@@ -12715,11 +12717,11 @@
         <v>0.94678254834076803</v>
       </c>
       <c r="H230" s="11">
-        <f t="shared" ref="H230:H262" si="25">M230/K230</f>
+        <f t="shared" ref="H230:H263" si="25">M230/K230</f>
         <v>0.053217451659231869</v>
       </c>
       <c r="I230" s="11">
-        <f t="shared" ref="I230:I262" si="26">O230/L230</f>
+        <f t="shared" ref="I230:I263" si="26">O230/L230</f>
         <v>0.14805990963342192</v>
       </c>
       <c r="J230" s="12">
@@ -12943,7 +12945,7 @@
         <v>4500.7385000000004</v>
       </c>
       <c r="N234" s="2">
-        <f t="shared" ref="N230:N262" si="27">J234-K234</f>
+        <f t="shared" ref="N230:N263" si="27">J234-K234</f>
         <v>29852.987999999998</v>
       </c>
       <c r="O234" s="2">
@@ -13696,7 +13698,7 @@
       <c r="D249" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E249" s="20"/>
+      <c r="E249" s="1"/>
       <c r="F249" s="3">
         <f t="shared" si="23"/>
         <v>0.63826219480167501</v>
@@ -13749,7 +13751,7 @@
       <c r="D250" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E250" s="20"/>
+      <c r="E250" s="1"/>
       <c r="F250" s="3">
         <f t="shared" si="23"/>
         <v>0.6537498781738148</v>
@@ -13802,43 +13804,41 @@
       <c r="D251" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E251" s="1" t="s">
-        <v>425</v>
-      </c>
+      <c r="E251" s="1"/>
       <c r="F251" s="3">
         <f t="shared" si="23"/>
-        <v>0.63363855623736731</v>
+        <v>0.63366250397700341</v>
       </c>
       <c r="G251" s="3">
         <f t="shared" si="24"/>
-        <v>0.94292277756557008</v>
+        <v>0.9429205862523472</v>
       </c>
       <c r="H251" s="3">
         <f t="shared" si="25"/>
-        <v>0.057077222434429822</v>
+        <v>0.057079393084359387</v>
       </c>
       <c r="I251" s="3">
         <f t="shared" si="26"/>
-        <v>0.14022888931866281</v>
+        <v>0.14031470194644458</v>
       </c>
       <c r="J251" s="2">
-        <v>76373.801000000007</v>
+        <v>76373.456999999995</v>
       </c>
       <c r="K251" s="2">
-        <v>48393.385000000002</v>
+        <v>48394.995999999999</v>
       </c>
       <c r="L251" s="2">
-        <v>45631.224999999999</v>
+        <v>45632.637999999999</v>
       </c>
       <c r="M251" s="2">
-        <v>2762.1599999999999</v>
+        <v>2762.357</v>
       </c>
       <c r="N251" s="2">
         <f t="shared" si="27"/>
-        <v>27980.416000000005</v>
+        <v>27978.460999999996</v>
       </c>
       <c r="O251" s="2">
-        <v>6398.8159999999998</v>
+        <v>6402.9300000000003</v>
       </c>
       <c r="P251" t="s">
         <v>470</v>
@@ -14322,7 +14322,7 @@
         <v>0.6448960129797745</v>
       </c>
       <c r="G261" s="3">
-        <f t="shared" ref="G261:G262" si="28">L261/K261</f>
+        <f t="shared" ref="G261:G263" si="28">L261/K261</f>
         <v>0.95227963685377781</v>
       </c>
       <c r="H261" s="3">
@@ -14428,19 +14428,19 @@
         <v>425</v>
       </c>
       <c r="F263" s="3">
-        <f>K263/J263</f>
+        <f t="shared" si="23"/>
         <v>0.66011891735401695</v>
       </c>
       <c r="G263" s="3">
-        <f>L263/K263</f>
+        <f t="shared" si="28"/>
         <v>0.95261458141964861</v>
       </c>
       <c r="H263" s="3">
-        <f>M263/K263</f>
+        <f t="shared" si="25"/>
         <v>0.047385418580351439</v>
       </c>
       <c r="I263" s="3">
-        <f>O263/L263</f>
+        <f t="shared" si="26"/>
         <v>0.11201161369487571</v>
       </c>
       <c r="J263" s="2">
@@ -14456,7 +14456,7 @@
         <v>2416.5529999999999</v>
       </c>
       <c r="N263" s="2">
-        <f>J263-K263</f>
+        <f t="shared" si="27"/>
         <v>26257.683999999994</v>
       </c>
       <c r="O263" s="2">
@@ -14482,10 +14482,48 @@
       <c r="E264" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="F264" s="3">
+        <f>K264/J264</f>
+        <v>0.65123306419898641</v>
+      </c>
+      <c r="G264" s="3">
+        <f>L264/K264</f>
+        <v>0.95515903764699206</v>
+      </c>
+      <c r="H264" s="3">
+        <f>M264/K264</f>
+        <v>0.044840962353008003</v>
+      </c>
+      <c r="I264" s="3">
+        <f>O264/L264</f>
+        <v>0.12909300311013253</v>
+      </c>
+      <c r="J264" s="2">
+        <v>77259.926999999996</v>
+      </c>
+      <c r="K264" s="2">
+        <v>50314.218999999997</v>
+      </c>
+      <c r="L264" s="2">
+        <v>48058.080999999998</v>
+      </c>
+      <c r="M264" s="2">
+        <v>2256.1379999999999</v>
+      </c>
+      <c r="N264" s="2">
+        <f>J264-K264</f>
+        <v>26945.707999999999</v>
+      </c>
+      <c r="O264" s="2">
+        <v>6203.9620000000004</v>
+      </c>
+      <c r="P264" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B265" s="1" t="s">
         <v>489</v>
@@ -14499,10 +14537,11 @@
       <c r="E265" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="O265" s="2"/>
     </row>
     <row r="266">
       <c r="A266" s="1" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B266" s="1" t="s">
         <v>489</v>
@@ -14516,10 +14555,11 @@
       <c r="E266" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="O266" s="2"/>
     </row>
     <row r="267">
       <c r="A267" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B267" s="1" t="s">
         <v>489</v>
@@ -14533,10 +14573,11 @@
       <c r="E267" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="O267" s="2"/>
     </row>
     <row r="268">
       <c r="A268" s="1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B268" s="1" t="s">
         <v>489</v>
@@ -14550,10 +14591,11 @@
       <c r="E268" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="O268" s="2"/>
     </row>
     <row r="269">
       <c r="A269" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B269" s="1" t="s">
         <v>489</v>
@@ -14567,10 +14609,11 @@
       <c r="E269" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="O269" s="2"/>
     </row>
     <row r="270">
       <c r="A270" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>489</v>
@@ -14584,10 +14627,11 @@
       <c r="E270" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="O270" s="2"/>
     </row>
     <row r="271">
       <c r="A271" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>489</v>
@@ -14601,10 +14645,11 @@
       <c r="E271" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="O271" s="2"/>
     </row>
     <row r="272">
       <c r="A272" s="1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>489</v>
@@ -14618,10 +14663,11 @@
       <c r="E272" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="O272" s="2"/>
     </row>
     <row r="273">
       <c r="A273" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>489</v>
@@ -14635,6 +14681,7 @@
       <c r="E273" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="O273" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -14657,61 +14704,61 @@
     <col customWidth="1" min="2" max="9" width="16.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" s="21" customFormat="1" ht="57">
-      <c r="A1" s="21" t="s">
+    <row r="1" s="20" customFormat="1" ht="57">
+      <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>505</v>
-      </c>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>506</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>507</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>508</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="E1" s="20" t="s">
         <v>509</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="F1" s="20" t="s">
         <v>510</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>511</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="H1" s="20" t="s">
         <v>512</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="2">
       <c r="A2">
         <v>1995</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="21">
         <v>43156</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="21">
         <v>65.799999999999997</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2" s="21">
         <v>28380</v>
       </c>
-      <c r="E2" s="22">
+      <c r="E2" s="21">
         <v>90.5</v>
       </c>
-      <c r="F2" s="22">
+      <c r="F2" s="21">
         <v>25677</v>
       </c>
-      <c r="G2" s="22">
+      <c r="G2" s="21">
         <v>9.5</v>
       </c>
-      <c r="H2" s="22">
+      <c r="H2" s="21">
         <v>2704</v>
       </c>
-      <c r="I2" s="22">
+      <c r="I2" s="21">
         <v>20</v>
       </c>
     </row>
@@ -14719,28 +14766,28 @@
       <c r="A3">
         <v>1996</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="21">
         <v>44599</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="21">
         <v>66.700000000000003</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="21">
         <v>29733</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="21">
         <v>91.400000000000006</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="21">
         <v>27186</v>
       </c>
-      <c r="G3" s="22">
+      <c r="G3" s="21">
         <v>8.5999999999999996</v>
       </c>
-      <c r="H3" s="22">
+      <c r="H3" s="21">
         <v>2546</v>
       </c>
-      <c r="I3" s="22">
+      <c r="I3" s="21">
         <v>21</v>
       </c>
     </row>
@@ -14748,28 +14795,28 @@
       <c r="A4">
         <v>1997</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="21">
         <v>44658</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="21">
         <v>64.700000000000003</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="21">
         <v>28901</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="21">
         <v>91.200000000000003</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="21">
         <v>26365</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="21">
         <v>8.8000000000000007</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="21">
         <v>2537</v>
       </c>
-      <c r="I4" s="22">
+      <c r="I4" s="21">
         <v>21.899999999999999</v>
       </c>
     </row>
@@ -14777,28 +14824,28 @@
       <c r="A5">
         <v>1998</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="21">
         <v>45964</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="21">
         <v>64.599999999999994</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="21">
         <v>29674</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="21">
         <v>89.700000000000003</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="21">
         <v>26631</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="21">
         <v>10.300000000000001</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="21">
         <v>3043</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="21">
         <v>21.600000000000001</v>
       </c>
     </row>
@@ -14806,28 +14853,28 @@
       <c r="A6">
         <v>1999</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="21">
         <v>47270</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="21">
         <v>65.099999999999994</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="21">
         <v>30759</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="21">
         <v>90.200000000000003</v>
       </c>
-      <c r="F6" s="22">
+      <c r="F6" s="21">
         <v>27742</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="21">
         <v>9.8000000000000007</v>
       </c>
-      <c r="H6" s="22">
+      <c r="H6" s="21">
         <v>3017</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="21">
         <v>22.100000000000001</v>
       </c>
     </row>
@@ -14835,28 +14882,28 @@
       <c r="A7">
         <v>2000</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="21">
         <v>48587</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="21">
         <v>63.600000000000001</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="21">
         <v>30911</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="21">
         <v>88.809808805926693</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="21">
         <v>27452</v>
       </c>
-      <c r="G7" s="22">
+      <c r="G7" s="21">
         <v>11.190191194073307</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="21">
         <v>3459</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="21">
         <v>21.699999999999999</v>
       </c>
     </row>
@@ -14864,28 +14911,28 @@
       <c r="A8">
         <v>2001</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="21">
         <v>48929</v>
       </c>
-      <c r="C8" s="22">
+      <c r="C8" s="21">
         <v>67.099999999999994</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="21">
         <v>32809</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="21">
         <v>88.865859977445211</v>
       </c>
-      <c r="F8" s="22">
+      <c r="F8" s="21">
         <v>29156</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="21">
         <v>11.134140022554787</v>
       </c>
-      <c r="H8" s="22">
+      <c r="H8" s="21">
         <v>3653</v>
       </c>
-      <c r="I8" s="22">
+      <c r="I8" s="21">
         <v>17.199999999999999</v>
       </c>
     </row>
@@ -14893,28 +14940,28 @@
       <c r="A9">
         <v>2002</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="21">
         <v>50344</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="21">
         <v>67.400000000000006</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="21">
         <v>33936</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="21">
         <v>88.584394153701083</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="21">
         <v>30062</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="21">
         <v>11.415605846298915</v>
       </c>
-      <c r="H9" s="22">
+      <c r="H9" s="21">
         <v>3874</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I9" s="21">
         <v>17</v>
       </c>
     </row>
@@ -14922,28 +14969,28 @@
       <c r="A10">
         <v>2003</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="21">
         <v>51793</v>
       </c>
-      <c r="C10" s="22">
+      <c r="C10" s="21">
         <v>66.700000000000003</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="21">
         <v>34571</v>
       </c>
-      <c r="E10" s="22">
+      <c r="E10" s="21">
         <v>88.614734893407771</v>
       </c>
-      <c r="F10" s="22">
+      <c r="F10" s="21">
         <v>30635</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="21">
         <v>11.385265106592231</v>
       </c>
-      <c r="H10" s="22">
+      <c r="H10" s="21">
         <v>3936</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10" s="21">
         <v>17</v>
       </c>
     </row>
@@ -14951,28 +14998,28 @@
       <c r="A11">
         <v>2004</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="21">
         <v>53144</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="21">
         <v>67.5</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="21">
         <v>35862</v>
       </c>
-      <c r="E11" s="22">
+      <c r="E11" s="21">
         <v>88.151804138084884</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="21">
         <v>31613</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="21">
         <v>11.848195861915119</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="21">
         <v>4249</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I11" s="21">
         <v>17.600000000000001</v>
       </c>
     </row>
@@ -14980,28 +15027,28 @@
       <c r="A12">
         <v>2005</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="21">
         <v>54388</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="21">
         <v>64.716310972814028</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="21">
         <v>35286</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="21">
         <v>92.21337414156298</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="21">
         <v>32539</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="21">
         <v>7.7866258584370058</v>
       </c>
-      <c r="H12" s="22">
+      <c r="H12" s="21">
         <v>2747.6666666666665</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="21">
         <v>21</v>
       </c>
     </row>
@@ -15009,28 +15056,28 @@
       <c r="A13">
         <v>2006</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="21">
         <v>55230</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="21">
         <v>64.200000000000003</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="21">
         <v>35464</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="21">
         <v>92.02312138728324</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="21">
         <v>32636</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="21">
         <v>7.9768786127167628</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="21">
         <v>2829</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="21">
         <v>22.600000000000001</v>
       </c>
     </row>
@@ -15038,28 +15085,28 @@
       <c r="A14">
         <v>2007</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="21">
         <v>56565</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="21">
         <v>64</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="21">
         <v>36213</v>
       </c>
-      <c r="E14" s="22">
+      <c r="E14" s="21">
         <v>92.67390163753349</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="21">
         <v>33560</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="21">
         <v>7.3260983624665172</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="21">
         <v>2653</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I14" s="21">
         <v>20.100000000000001</v>
       </c>
     </row>
@@ -15067,28 +15114,28 @@
       <c r="A15">
         <v>2008</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B15" s="21">
         <v>57848</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="21">
         <v>63.600000000000001</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="21">
         <v>36805</v>
       </c>
-      <c r="E15" s="22">
+      <c r="E15" s="21">
         <v>92.620567857628046</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="21">
         <v>34089</v>
       </c>
-      <c r="G15" s="22">
+      <c r="G15" s="21">
         <v>7.4000000000000004</v>
       </c>
-      <c r="H15" s="22">
+      <c r="H15" s="21">
         <v>2716</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I15" s="21">
         <v>19.300000000000001</v>
       </c>
     </row>
@@ -15096,28 +15143,28 @@
       <c r="A16">
         <v>2009</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="21">
         <v>59237</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="21">
         <v>63.966355487279912</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="21">
         <v>37891.75</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="21">
         <v>92.530036221604973</v>
       </c>
-      <c r="F16" s="22">
+      <c r="F16" s="21">
         <v>35061.25</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="21">
         <v>7.4699637783950337</v>
       </c>
-      <c r="H16" s="22">
+      <c r="H16" s="21">
         <v>2830.5</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I16" s="21">
         <v>19.087311490605728</v>
       </c>
     </row>
@@ -15125,28 +15172,28 @@
       <c r="A17">
         <v>2010</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17" s="21">
         <v>60717</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="21">
         <v>64.099999999999994</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="21">
         <v>38893</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="21">
         <v>92.700000000000003</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="21">
         <v>36035</v>
       </c>
-      <c r="G17" s="22">
+      <c r="G17" s="21">
         <v>7.2999999999999998</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="21">
         <v>2859</v>
       </c>
-      <c r="I17" s="22">
+      <c r="I17" s="21">
         <v>18.699999999999999</v>
       </c>
     </row>
@@ -15154,28 +15201,28 @@
       <c r="A18">
         <v>2011</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="21">
         <v>61882.531999999999</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="21">
         <v>64.647477174980494</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="21">
         <v>40006.042999999998</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="21">
         <v>92.967334369303501</v>
       </c>
-      <c r="F18" s="22">
+      <c r="F18" s="21">
         <v>37192.042999999998</v>
       </c>
-      <c r="G18" s="22">
+      <c r="G18" s="21">
         <v>7.0326656306965027</v>
       </c>
-      <c r="H18" s="22">
+      <c r="H18" s="21">
         <v>2814</v>
       </c>
-      <c r="I18" s="22">
+      <c r="I18" s="21">
         <v>19.260093482899016</v>
       </c>
     </row>
@@ -15183,28 +15230,28 @@
       <c r="A19">
         <v>2012</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="21">
         <v>62985.349249999999</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="21">
         <v>64.183842721170592</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="21">
         <v>40426.417499999996</v>
       </c>
-      <c r="E19" s="22">
+      <c r="E19" s="21">
         <v>93.008986636028297</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="21">
         <v>37600.201249999998</v>
       </c>
-      <c r="G19" s="22">
+      <c r="G19" s="21">
         <v>6.9910133639717156</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H19" s="21">
         <v>2826.2162499999999</v>
       </c>
-      <c r="I19" s="22">
+      <c r="I19" s="21">
         <v>19.984181600623746</v>
       </c>
     </row>
@@ -15212,28 +15259,28 @@
       <c r="A20">
         <v>2013</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="21">
         <v>64173.311000000002</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="21">
         <v>63.92431465784896</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="21">
         <v>41022.349249999999</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="21">
         <v>92.919384059897538</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="21">
         <v>38117.714249999997</v>
       </c>
-      <c r="G20" s="22">
+      <c r="G20" s="21">
         <v>7.0806159401024553</v>
       </c>
-      <c r="H20" s="22">
+      <c r="H20" s="21">
         <v>2904.6350000000002</v>
       </c>
-      <c r="I20" s="22">
+      <c r="I20" s="21">
         <v>19.338649090166786</v>
       </c>
     </row>
@@ -15241,28 +15288,28 @@
       <c r="A21">
         <v>2014</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="21">
         <v>64033.078333333338</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="21">
         <v>64.621820071277213</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D21" s="21">
         <v>41379.340666666671</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="21">
         <v>93.407133553328265</v>
       </c>
-      <c r="F21" s="22">
+      <c r="F21" s="21">
         <v>38651.256000000001</v>
       </c>
-      <c r="G21" s="22">
+      <c r="G21" s="21">
         <v>6.5928664466717537</v>
       </c>
-      <c r="H21" s="22">
+      <c r="H21" s="21">
         <v>2728.0846666666666</v>
       </c>
-      <c r="I21" s="22">
+      <c r="I21" s="21">
         <v>18.41672363764841</v>
       </c>
     </row>
@@ -15270,28 +15317,28 @@
       <c r="A22">
         <v>2015</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="21">
         <v>64936</v>
       </c>
-      <c r="C22" s="22">
+      <c r="C22" s="21">
         <v>63.700000000000003</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22" s="21">
         <v>41342</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="21">
         <v>93.700000000000003</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="21">
         <v>38741</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="21">
         <v>6.2999999999999998</v>
       </c>
-      <c r="H22" s="22">
+      <c r="H22" s="21">
         <v>2958</v>
       </c>
-      <c r="I22" s="22">
+      <c r="I22" s="21">
         <v>18.5</v>
       </c>
     </row>
@@ -15299,28 +15346,28 @@
       <c r="A23">
         <v>2016</v>
       </c>
-      <c r="B23" s="22">
+      <c r="B23" s="21">
         <v>68311</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23" s="21">
         <v>63.5</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="21">
         <v>43361</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="21">
         <v>94.599999999999994</v>
       </c>
-      <c r="F23" s="22">
+      <c r="F23" s="21">
         <v>40998</v>
       </c>
-      <c r="G23" s="22">
+      <c r="G23" s="21">
         <v>5.4000000000000004</v>
       </c>
-      <c r="H23" s="22">
+      <c r="H23" s="21">
         <v>2363</v>
       </c>
-      <c r="I23" s="22">
+      <c r="I23" s="21">
         <v>18.300000000000001</v>
       </c>
     </row>
@@ -15328,28 +15375,28 @@
       <c r="A24">
         <v>2017</v>
       </c>
-      <c r="B24" s="22">
+      <c r="B24" s="21">
         <v>69890.685750000004</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="21">
         <v>61.200000000000003</v>
       </c>
-      <c r="D24" s="22">
+      <c r="D24" s="21">
         <v>42775</v>
       </c>
-      <c r="E24" s="22">
+      <c r="E24" s="21">
         <v>94.281162928439798</v>
       </c>
-      <c r="F24" s="22">
+      <c r="F24" s="21">
         <v>40334</v>
       </c>
-      <c r="G24" s="22">
+      <c r="G24" s="21">
         <v>5.7188370715601895</v>
       </c>
-      <c r="H24" s="22">
+      <c r="H24" s="21">
         <v>2441</v>
       </c>
-      <c r="I24" s="22">
+      <c r="I24" s="21">
         <v>16.100000000000001</v>
       </c>
     </row>
@@ -15357,28 +15404,28 @@
       <c r="A25">
         <v>2018</v>
       </c>
-      <c r="B25" s="22">
+      <c r="B25" s="21">
         <v>71339</v>
       </c>
-      <c r="C25" s="22">
+      <c r="C25" s="21">
         <v>60.899999999999999</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="21">
         <v>43462</v>
       </c>
-      <c r="E25" s="22">
+      <c r="E25" s="21">
         <v>94.700000000000003</v>
       </c>
-      <c r="F25" s="22">
+      <c r="F25" s="21">
         <v>41160</v>
       </c>
-      <c r="G25" s="22">
+      <c r="G25" s="21">
         <v>5.2999999999999998</v>
       </c>
-      <c r="H25" s="22">
+      <c r="H25" s="21">
         <v>2302</v>
       </c>
-      <c r="I25" s="22">
+      <c r="I25" s="21">
         <v>16.399999999999999</v>
       </c>
     </row>
@@ -15386,28 +15433,28 @@
       <c r="A26">
         <v>2019</v>
       </c>
-      <c r="B26" s="22">
+      <c r="B26" s="21">
         <v>72932</v>
       </c>
-      <c r="C26" s="22">
+      <c r="C26" s="21">
         <v>61.299999999999997</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="21">
         <v>44692</v>
       </c>
-      <c r="E26" s="22">
+      <c r="E26" s="21">
         <v>94.900000000000006</v>
       </c>
-      <c r="F26" s="22">
+      <c r="F26" s="21">
         <v>42428</v>
       </c>
-      <c r="G26" s="22">
+      <c r="G26" s="21">
         <v>5.0999999999999996</v>
       </c>
-      <c r="H26" s="22">
+      <c r="H26" s="21">
         <v>2264</v>
       </c>
-      <c r="I26" s="22">
+      <c r="I26" s="21">
         <v>13.986046950127273</v>
       </c>
     </row>
@@ -15415,27 +15462,27 @@
       <c r="A27">
         <v>2020</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
     </row>
     <row r="28">
       <c r="A28">
         <v>2021</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -15461,37 +15508,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B1" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B3" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>518</v>
-      </c>
-      <c r="C5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>519</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="C5" s="23" t="s">
         <v>520</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="6">
@@ -15906,7 +15953,7 @@
         <v>295</v>
       </c>
       <c r="B61" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="D61" t="s">
         <v>296</v>
@@ -15917,7 +15964,7 @@
         <v>297</v>
       </c>
       <c r="B62" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="D62" t="s">
         <v>298</v>
@@ -15928,7 +15975,7 @@
         <v>299</v>
       </c>
       <c r="B63" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="D63" t="s">
         <v>300</v>
@@ -15939,7 +15986,7 @@
         <v>301</v>
       </c>
       <c r="B64" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="D64" t="s">
         <v>302</v>
@@ -15955,7 +16002,7 @@
         <v>304</v>
       </c>
       <c r="B66" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="D66" t="s">
         <v>305</v>
@@ -15966,7 +16013,7 @@
         <v>306</v>
       </c>
       <c r="B67" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D67" t="s">
         <v>307</v>
@@ -15977,7 +16024,7 @@
         <v>308</v>
       </c>
       <c r="B68" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D68" t="s">
         <v>309</v>
@@ -15988,7 +16035,7 @@
         <v>310</v>
       </c>
       <c r="B69" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D69" t="s">
         <v>311</v>
@@ -16007,7 +16054,7 @@
         <v>314</v>
       </c>
       <c r="B71" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D71" t="s">
         <v>315</v>
@@ -16018,7 +16065,7 @@
         <v>316</v>
       </c>
       <c r="B72" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D72" t="s">
         <v>317</v>
@@ -16029,7 +16076,7 @@
         <v>318</v>
       </c>
       <c r="B73" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D73" t="s">
         <v>319</v>
@@ -16040,7 +16087,7 @@
         <v>320</v>
       </c>
       <c r="B74" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D74" t="s">
         <v>321</v>
@@ -16051,7 +16098,7 @@
         <v>322</v>
       </c>
       <c r="B75" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C75" t="s">
         <v>323</v>
@@ -16062,7 +16109,7 @@
         <v>324</v>
       </c>
       <c r="B76" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D76" t="s">
         <v>325</v>
@@ -16073,13 +16120,13 @@
         <v>326</v>
       </c>
       <c r="B77" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C77" t="s">
         <v>327</v>
       </c>
       <c r="D77" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="78">
@@ -16087,13 +16134,13 @@
         <v>328</v>
       </c>
       <c r="B78" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C78" t="s">
         <v>329</v>
       </c>
       <c r="D78" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="79">
@@ -16101,13 +16148,13 @@
         <v>330</v>
       </c>
       <c r="B79" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C79" t="s">
         <v>331</v>
       </c>
       <c r="D79" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="80">
@@ -16115,7 +16162,7 @@
         <v>332</v>
       </c>
       <c r="B80" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C80" t="s">
         <v>333</v>
@@ -16126,13 +16173,13 @@
         <v>334</v>
       </c>
       <c r="B81" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C81" t="s">
         <v>335</v>
       </c>
       <c r="D81" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="82">
@@ -16140,13 +16187,13 @@
         <v>336</v>
       </c>
       <c r="B82" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="C82" t="s">
         <v>337</v>
       </c>
       <c r="D82" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="83">
@@ -16154,13 +16201,13 @@
         <v>338</v>
       </c>
       <c r="B83" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C83" t="s">
         <v>339</v>
       </c>
       <c r="D83" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="84">
@@ -16168,13 +16215,13 @@
         <v>340</v>
       </c>
       <c r="B84" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C84" t="s">
         <v>341</v>
       </c>
       <c r="D84" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="85">
@@ -16182,7 +16229,7 @@
         <v>342</v>
       </c>
       <c r="B85" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C85" t="s">
         <v>343</v>
@@ -16193,13 +16240,13 @@
         <v>344</v>
       </c>
       <c r="B86" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C86" t="s">
         <v>345</v>
       </c>
       <c r="D86" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="87">
@@ -16207,13 +16254,13 @@
         <v>346</v>
       </c>
       <c r="B87" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C87" t="s">
         <v>347</v>
       </c>
       <c r="D87" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="88">
@@ -16221,13 +16268,13 @@
         <v>348</v>
       </c>
       <c r="B88" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C88" t="s">
         <v>349</v>
       </c>
       <c r="D88" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="89">
@@ -16235,13 +16282,13 @@
         <v>350</v>
       </c>
       <c r="B89" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C89" t="s">
         <v>351</v>
       </c>
       <c r="D89" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="90">
@@ -16249,7 +16296,7 @@
         <v>352</v>
       </c>
       <c r="B90" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C90" t="s">
         <v>353</v>
@@ -16260,13 +16307,13 @@
         <v>354</v>
       </c>
       <c r="B91" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="C91" t="s">
         <v>355</v>
       </c>
       <c r="D91" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="92">
@@ -16274,13 +16321,13 @@
         <v>356</v>
       </c>
       <c r="B92" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C92" t="s">
         <v>357</v>
       </c>
       <c r="D92" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="93">
@@ -16288,13 +16335,13 @@
         <v>358</v>
       </c>
       <c r="B93" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C93" t="s">
         <v>359</v>
       </c>
       <c r="D93" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="94">
@@ -16302,13 +16349,13 @@
         <v>360</v>
       </c>
       <c r="B94" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C94" t="s">
         <v>361</v>
       </c>
       <c r="D94" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="95">
@@ -16316,7 +16363,7 @@
         <v>362</v>
       </c>
       <c r="B95" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C95" t="s">
         <v>363</v>
@@ -16327,13 +16374,13 @@
         <v>364</v>
       </c>
       <c r="B96" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C96" t="s">
         <v>365</v>
       </c>
       <c r="D96" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="97">
@@ -16341,13 +16388,13 @@
         <v>366</v>
       </c>
       <c r="B97" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C97" t="s">
         <v>367</v>
       </c>
       <c r="D97" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="98">
@@ -16355,13 +16402,13 @@
         <v>368</v>
       </c>
       <c r="B98" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C98" t="s">
         <v>369</v>
       </c>
       <c r="D98" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="99">
@@ -16369,13 +16416,13 @@
         <v>370</v>
       </c>
       <c r="B99" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C99" t="s">
         <v>371</v>
       </c>
       <c r="D99" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="100">
@@ -16383,7 +16430,7 @@
         <v>372</v>
       </c>
       <c r="B100" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C100" t="s">
         <v>373</v>
@@ -16394,13 +16441,13 @@
         <v>374</v>
       </c>
       <c r="B101" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C101" t="s">
         <v>375</v>
       </c>
       <c r="D101" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="102">
@@ -16408,13 +16455,13 @@
         <v>376</v>
       </c>
       <c r="B102" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C102" t="s">
         <v>377</v>
       </c>
       <c r="D102" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="103">
@@ -16422,13 +16469,13 @@
         <v>379</v>
       </c>
       <c r="B103" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="C103" t="s">
         <v>380</v>
       </c>
       <c r="D103" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="104">
@@ -16436,13 +16483,13 @@
         <v>381</v>
       </c>
       <c r="B104" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="C104" t="s">
         <v>382</v>
       </c>
       <c r="D104" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="105">
@@ -16450,7 +16497,7 @@
         <v>383</v>
       </c>
       <c r="B105" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C105" t="s">
         <v>384</v>
@@ -16461,13 +16508,13 @@
         <v>385</v>
       </c>
       <c r="B106" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C106" t="s">
         <v>386</v>
       </c>
       <c r="D106" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="107">
@@ -16475,13 +16522,13 @@
         <v>387</v>
       </c>
       <c r="B107" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="C107" t="s">
         <v>388</v>
       </c>
       <c r="D107" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="108">
@@ -16489,13 +16536,13 @@
         <v>389</v>
       </c>
       <c r="B108" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="C108" t="s">
         <v>390</v>
       </c>
       <c r="D108" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="109">
@@ -16503,13 +16550,13 @@
         <v>391</v>
       </c>
       <c r="B109" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C109" t="s">
         <v>392</v>
       </c>
       <c r="D109" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="110">
@@ -16517,7 +16564,7 @@
         <v>393</v>
       </c>
       <c r="B110" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C110" t="s">
         <v>394</v>
@@ -16528,13 +16575,13 @@
         <v>395</v>
       </c>
       <c r="B111" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C111" t="s">
         <v>396</v>
       </c>
       <c r="D111" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="112">
@@ -16542,13 +16589,13 @@
         <v>397</v>
       </c>
       <c r="B112" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C112" t="s">
         <v>398</v>
       </c>
       <c r="D112" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="113">
@@ -16556,13 +16603,13 @@
         <v>399</v>
       </c>
       <c r="B113" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="C113" t="s">
         <v>400</v>
       </c>
       <c r="D113" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="114">
@@ -16570,13 +16617,13 @@
         <v>401</v>
       </c>
       <c r="B114" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="C114" t="s">
         <v>402</v>
       </c>
       <c r="D114" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="115">
@@ -16584,7 +16631,7 @@
         <v>403</v>
       </c>
       <c r="B115" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="C115" t="s">
         <v>404</v>
@@ -16595,13 +16642,13 @@
         <v>405</v>
       </c>
       <c r="B116" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C116" t="s">
         <v>406</v>
       </c>
       <c r="D116" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="117">
@@ -16609,13 +16656,13 @@
         <v>407</v>
       </c>
       <c r="B117" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C117" t="s">
         <v>408</v>
       </c>
       <c r="D117" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="118">
@@ -16623,13 +16670,13 @@
         <v>409</v>
       </c>
       <c r="B118" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="C118" t="s">
         <v>410</v>
       </c>
       <c r="D118" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="119">
@@ -16637,13 +16684,13 @@
         <v>411</v>
       </c>
       <c r="B119" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="C119" t="s">
         <v>412</v>
       </c>
       <c r="D119" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="120">
@@ -16651,7 +16698,7 @@
         <v>413</v>
       </c>
       <c r="B120" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="C120" t="s">
         <v>414</v>
@@ -16662,13 +16709,13 @@
         <v>415</v>
       </c>
       <c r="B121" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C121" t="s">
         <v>416</v>
       </c>
       <c r="D121" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="122">
@@ -16676,13 +16723,13 @@
         <v>418</v>
       </c>
       <c r="B122" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="C122" t="s">
         <v>419</v>
       </c>
       <c r="D122" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="123">
@@ -16690,13 +16737,13 @@
         <v>420</v>
       </c>
       <c r="B123" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="C123" t="s">
         <v>421</v>
       </c>
       <c r="D123" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="124">
@@ -16704,13 +16751,13 @@
         <v>422</v>
       </c>
       <c r="B124" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C124" t="s">
         <v>423</v>
       </c>
       <c r="D124" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="125">
@@ -16777,7 +16824,7 @@
         <v>445</v>
       </c>
       <c r="D132" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="133">
@@ -16949,7 +16996,7 @@
       <c r="A154" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="B154" s="25" t="s">
+      <c r="B154" s="24" t="s">
         <v>494</v>
       </c>
     </row>
@@ -16957,50 +17004,53 @@
       <c r="A155" s="1" t="s">
         <v>495</v>
       </c>
+      <c r="B155" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
   </sheetData>
@@ -17025,59 +17075,59 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B1" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B2" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B3" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B4" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B5" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="C8" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="D8" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="E8" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="F8" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
Monthly labor update - May 2023
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="635">
   <si>
     <t xml:space="preserve">LFS Round</t>
   </si>
@@ -1510,6 +1510,9 @@
   </si>
   <si>
     <t xml:space="preserve">2023 May</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/unemployment-rate-may-2023-was-estimated-43-percent</t>
   </si>
   <si>
     <t xml:space="preserve">2023 Jun</t>
@@ -1978,20 +1981,20 @@
   </fills>
   <borders count="2">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="2">
@@ -12709,7 +12712,7 @@
         <v>32</v>
       </c>
       <c r="F230" s="11">
-        <f t="shared" ref="F230:G263" si="23">K230/J230</f>
+        <f t="shared" ref="F230:G264" si="23">K230/J230</f>
         <v>0.6168840849278201</v>
       </c>
       <c r="G230" s="11">
@@ -12717,11 +12720,11 @@
         <v>0.94678254834076803</v>
       </c>
       <c r="H230" s="11">
-        <f t="shared" ref="H230:H263" si="25">M230/K230</f>
+        <f t="shared" ref="H230:H264" si="25">M230/K230</f>
         <v>0.053217451659231869</v>
       </c>
       <c r="I230" s="11">
-        <f t="shared" ref="I230:I263" si="26">O230/L230</f>
+        <f t="shared" ref="I230:I264" si="26">O230/L230</f>
         <v>0.14805990963342192</v>
       </c>
       <c r="J230" s="12">
@@ -12945,7 +12948,7 @@
         <v>4500.7385000000004</v>
       </c>
       <c r="N234" s="2">
-        <f t="shared" ref="N230:N263" si="27">J234-K234</f>
+        <f t="shared" ref="N230:N264" si="27">J234-K234</f>
         <v>29852.987999999998</v>
       </c>
       <c r="O234" s="2">
@@ -13857,9 +13860,7 @@
       <c r="D252" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E252" s="1" t="s">
-        <v>425</v>
-      </c>
+      <c r="E252" s="1"/>
       <c r="F252" s="3">
         <f t="shared" si="23"/>
         <v>0.64040035214677771</v>
@@ -14322,7 +14323,7 @@
         <v>0.6448960129797745</v>
       </c>
       <c r="G261" s="3">
-        <f t="shared" ref="G261:G263" si="28">L261/K261</f>
+        <f t="shared" ref="G261:G264" si="28">L261/K261</f>
         <v>0.95227963685377781</v>
       </c>
       <c r="H261" s="3">
@@ -14483,19 +14484,19 @@
         <v>425</v>
       </c>
       <c r="F264" s="3">
-        <f>K264/J264</f>
+        <f t="shared" si="23"/>
         <v>0.65123306419898641</v>
       </c>
       <c r="G264" s="3">
-        <f>L264/K264</f>
+        <f t="shared" si="28"/>
         <v>0.95515903764699206</v>
       </c>
       <c r="H264" s="3">
-        <f>M264/K264</f>
+        <f t="shared" si="25"/>
         <v>0.044840962353008003</v>
       </c>
       <c r="I264" s="3">
-        <f>O264/L264</f>
+        <f t="shared" si="26"/>
         <v>0.12909300311013253</v>
       </c>
       <c r="J264" s="2">
@@ -14511,7 +14512,7 @@
         <v>2256.1379999999999</v>
       </c>
       <c r="N264" s="2">
-        <f>J264-K264</f>
+        <f t="shared" si="27"/>
         <v>26945.707999999999</v>
       </c>
       <c r="O264" s="2">
@@ -14537,11 +14538,48 @@
       <c r="E265" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="O265" s="2"/>
+      <c r="F265" s="3">
+        <f>K265/J265</f>
+        <v>0.65346941408460835</v>
+      </c>
+      <c r="G265" s="3">
+        <f>L265/K265</f>
+        <v>0.95701872106453656</v>
+      </c>
+      <c r="H265" s="3">
+        <f>M265/K265</f>
+        <v>0.042981278935463475</v>
+      </c>
+      <c r="I265" s="3">
+        <f>O265/L265</f>
+        <v>0.11729164330819054</v>
+      </c>
+      <c r="J265" s="2">
+        <v>77169.572</v>
+      </c>
+      <c r="K265" s="2">
+        <v>50427.955000000002</v>
+      </c>
+      <c r="L265" s="2">
+        <v>48260.497000000003</v>
+      </c>
+      <c r="M265" s="2">
+        <v>2167.4580000000001</v>
+      </c>
+      <c r="N265" s="2">
+        <f>J265-K265</f>
+        <v>26741.616999999998</v>
+      </c>
+      <c r="O265" s="2">
+        <v>5660.5529999999999</v>
+      </c>
+      <c r="P265" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B266" s="1" t="s">
         <v>489</v>
@@ -14559,7 +14597,7 @@
     </row>
     <row r="267">
       <c r="A267" s="1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B267" s="1" t="s">
         <v>489</v>
@@ -14577,7 +14615,7 @@
     </row>
     <row r="268">
       <c r="A268" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B268" s="1" t="s">
         <v>489</v>
@@ -14595,7 +14633,7 @@
     </row>
     <row r="269">
       <c r="A269" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B269" s="1" t="s">
         <v>489</v>
@@ -14613,7 +14651,7 @@
     </row>
     <row r="270">
       <c r="A270" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>489</v>
@@ -14631,7 +14669,7 @@
     </row>
     <row r="271">
       <c r="A271" s="1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>489</v>
@@ -14649,7 +14687,7 @@
     </row>
     <row r="272">
       <c r="A272" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>489</v>
@@ -14667,7 +14705,7 @@
     </row>
     <row r="273">
       <c r="A273" s="1" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>489</v>
@@ -14709,28 +14747,28 @@
         <v>1</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="2">
@@ -15508,23 +15546,23 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B1" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B3" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="5">
@@ -15532,13 +15570,13 @@
         <v>0</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="6">
@@ -15953,7 +15991,7 @@
         <v>295</v>
       </c>
       <c r="B61" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="D61" t="s">
         <v>296</v>
@@ -15964,7 +16002,7 @@
         <v>297</v>
       </c>
       <c r="B62" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="D62" t="s">
         <v>298</v>
@@ -15975,7 +16013,7 @@
         <v>299</v>
       </c>
       <c r="B63" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="D63" t="s">
         <v>300</v>
@@ -15986,7 +16024,7 @@
         <v>301</v>
       </c>
       <c r="B64" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="D64" t="s">
         <v>302</v>
@@ -16002,7 +16040,7 @@
         <v>304</v>
       </c>
       <c r="B66" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D66" t="s">
         <v>305</v>
@@ -16013,7 +16051,7 @@
         <v>306</v>
       </c>
       <c r="B67" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D67" t="s">
         <v>307</v>
@@ -16024,7 +16062,7 @@
         <v>308</v>
       </c>
       <c r="B68" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D68" t="s">
         <v>309</v>
@@ -16035,7 +16073,7 @@
         <v>310</v>
       </c>
       <c r="B69" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D69" t="s">
         <v>311</v>
@@ -16054,7 +16092,7 @@
         <v>314</v>
       </c>
       <c r="B71" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D71" t="s">
         <v>315</v>
@@ -16065,7 +16103,7 @@
         <v>316</v>
       </c>
       <c r="B72" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D72" t="s">
         <v>317</v>
@@ -16076,7 +16114,7 @@
         <v>318</v>
       </c>
       <c r="B73" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D73" t="s">
         <v>319</v>
@@ -16087,7 +16125,7 @@
         <v>320</v>
       </c>
       <c r="B74" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="D74" t="s">
         <v>321</v>
@@ -16098,7 +16136,7 @@
         <v>322</v>
       </c>
       <c r="B75" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C75" t="s">
         <v>323</v>
@@ -16109,7 +16147,7 @@
         <v>324</v>
       </c>
       <c r="B76" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D76" t="s">
         <v>325</v>
@@ -16120,13 +16158,13 @@
         <v>326</v>
       </c>
       <c r="B77" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="C77" t="s">
         <v>327</v>
       </c>
       <c r="D77" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="78">
@@ -16134,13 +16172,13 @@
         <v>328</v>
       </c>
       <c r="B78" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C78" t="s">
         <v>329</v>
       </c>
       <c r="D78" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="79">
@@ -16148,13 +16186,13 @@
         <v>330</v>
       </c>
       <c r="B79" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C79" t="s">
         <v>331</v>
       </c>
       <c r="D79" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="80">
@@ -16162,7 +16200,7 @@
         <v>332</v>
       </c>
       <c r="B80" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C80" t="s">
         <v>333</v>
@@ -16173,13 +16211,13 @@
         <v>334</v>
       </c>
       <c r="B81" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C81" t="s">
         <v>335</v>
       </c>
       <c r="D81" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="82">
@@ -16187,13 +16225,13 @@
         <v>336</v>
       </c>
       <c r="B82" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="C82" t="s">
         <v>337</v>
       </c>
       <c r="D82" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="83">
@@ -16201,13 +16239,13 @@
         <v>338</v>
       </c>
       <c r="B83" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="C83" t="s">
         <v>339</v>
       </c>
       <c r="D83" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="84">
@@ -16215,13 +16253,13 @@
         <v>340</v>
       </c>
       <c r="B84" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C84" t="s">
         <v>341</v>
       </c>
       <c r="D84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="85">
@@ -16229,7 +16267,7 @@
         <v>342</v>
       </c>
       <c r="B85" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C85" t="s">
         <v>343</v>
@@ -16240,13 +16278,13 @@
         <v>344</v>
       </c>
       <c r="B86" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C86" t="s">
         <v>345</v>
       </c>
       <c r="D86" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="87">
@@ -16254,13 +16292,13 @@
         <v>346</v>
       </c>
       <c r="B87" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C87" t="s">
         <v>347</v>
       </c>
       <c r="D87" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="88">
@@ -16268,13 +16306,13 @@
         <v>348</v>
       </c>
       <c r="B88" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C88" t="s">
         <v>349</v>
       </c>
       <c r="D88" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="89">
@@ -16282,13 +16320,13 @@
         <v>350</v>
       </c>
       <c r="B89" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C89" t="s">
         <v>351</v>
       </c>
       <c r="D89" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="90">
@@ -16296,7 +16334,7 @@
         <v>352</v>
       </c>
       <c r="B90" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="C90" t="s">
         <v>353</v>
@@ -16307,13 +16345,13 @@
         <v>354</v>
       </c>
       <c r="B91" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C91" t="s">
         <v>355</v>
       </c>
       <c r="D91" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="92">
@@ -16321,13 +16359,13 @@
         <v>356</v>
       </c>
       <c r="B92" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C92" t="s">
         <v>357</v>
       </c>
       <c r="D92" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="93">
@@ -16335,13 +16373,13 @@
         <v>358</v>
       </c>
       <c r="B93" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="C93" t="s">
         <v>359</v>
       </c>
       <c r="D93" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="94">
@@ -16349,13 +16387,13 @@
         <v>360</v>
       </c>
       <c r="B94" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C94" t="s">
         <v>361</v>
       </c>
       <c r="D94" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="95">
@@ -16363,7 +16401,7 @@
         <v>362</v>
       </c>
       <c r="B95" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C95" t="s">
         <v>363</v>
@@ -16374,13 +16412,13 @@
         <v>364</v>
       </c>
       <c r="B96" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C96" t="s">
         <v>365</v>
       </c>
       <c r="D96" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="97">
@@ -16388,13 +16426,13 @@
         <v>366</v>
       </c>
       <c r="B97" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C97" t="s">
         <v>367</v>
       </c>
       <c r="D97" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="98">
@@ -16402,13 +16440,13 @@
         <v>368</v>
       </c>
       <c r="B98" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C98" t="s">
         <v>369</v>
       </c>
       <c r="D98" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="99">
@@ -16416,13 +16454,13 @@
         <v>370</v>
       </c>
       <c r="B99" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C99" t="s">
         <v>371</v>
       </c>
       <c r="D99" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="100">
@@ -16430,7 +16468,7 @@
         <v>372</v>
       </c>
       <c r="B100" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="C100" t="s">
         <v>373</v>
@@ -16441,13 +16479,13 @@
         <v>374</v>
       </c>
       <c r="B101" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C101" t="s">
         <v>375</v>
       </c>
       <c r="D101" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="102">
@@ -16455,13 +16493,13 @@
         <v>376</v>
       </c>
       <c r="B102" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C102" t="s">
         <v>377</v>
       </c>
       <c r="D102" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="103">
@@ -16469,13 +16507,13 @@
         <v>379</v>
       </c>
       <c r="B103" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="C103" t="s">
         <v>380</v>
       </c>
       <c r="D103" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="104">
@@ -16483,13 +16521,13 @@
         <v>381</v>
       </c>
       <c r="B104" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="C104" t="s">
         <v>382</v>
       </c>
       <c r="D104" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="105">
@@ -16497,7 +16535,7 @@
         <v>383</v>
       </c>
       <c r="B105" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C105" t="s">
         <v>384</v>
@@ -16508,13 +16546,13 @@
         <v>385</v>
       </c>
       <c r="B106" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C106" t="s">
         <v>386</v>
       </c>
       <c r="D106" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="107">
@@ -16522,13 +16560,13 @@
         <v>387</v>
       </c>
       <c r="B107" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C107" t="s">
         <v>388</v>
       </c>
       <c r="D107" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="108">
@@ -16536,13 +16574,13 @@
         <v>389</v>
       </c>
       <c r="B108" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C108" t="s">
         <v>390</v>
       </c>
       <c r="D108" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="109">
@@ -16550,13 +16588,13 @@
         <v>391</v>
       </c>
       <c r="B109" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="C109" t="s">
         <v>392</v>
       </c>
       <c r="D109" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="110">
@@ -16564,7 +16602,7 @@
         <v>393</v>
       </c>
       <c r="B110" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C110" t="s">
         <v>394</v>
@@ -16575,13 +16613,13 @@
         <v>395</v>
       </c>
       <c r="B111" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C111" t="s">
         <v>396</v>
       </c>
       <c r="D111" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="112">
@@ -16589,13 +16627,13 @@
         <v>397</v>
       </c>
       <c r="B112" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="C112" t="s">
         <v>398</v>
       </c>
       <c r="D112" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="113">
@@ -16603,13 +16641,13 @@
         <v>399</v>
       </c>
       <c r="B113" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="C113" t="s">
         <v>400</v>
       </c>
       <c r="D113" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="114">
@@ -16617,13 +16655,13 @@
         <v>401</v>
       </c>
       <c r="B114" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="C114" t="s">
         <v>402</v>
       </c>
       <c r="D114" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="115">
@@ -16631,7 +16669,7 @@
         <v>403</v>
       </c>
       <c r="B115" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="C115" t="s">
         <v>404</v>
@@ -16642,13 +16680,13 @@
         <v>405</v>
       </c>
       <c r="B116" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="C116" t="s">
         <v>406</v>
       </c>
       <c r="D116" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="117">
@@ -16656,13 +16694,13 @@
         <v>407</v>
       </c>
       <c r="B117" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="C117" t="s">
         <v>408</v>
       </c>
       <c r="D117" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="118">
@@ -16670,13 +16708,13 @@
         <v>409</v>
       </c>
       <c r="B118" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="C118" t="s">
         <v>410</v>
       </c>
       <c r="D118" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="119">
@@ -16684,13 +16722,13 @@
         <v>411</v>
       </c>
       <c r="B119" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="C119" t="s">
         <v>412</v>
       </c>
       <c r="D119" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="120">
@@ -16698,7 +16736,7 @@
         <v>413</v>
       </c>
       <c r="B120" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C120" t="s">
         <v>414</v>
@@ -16709,13 +16747,13 @@
         <v>415</v>
       </c>
       <c r="B121" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C121" t="s">
         <v>416</v>
       </c>
       <c r="D121" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="122">
@@ -16723,13 +16761,13 @@
         <v>418</v>
       </c>
       <c r="B122" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C122" t="s">
         <v>419</v>
       </c>
       <c r="D122" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="123">
@@ -16737,13 +16775,13 @@
         <v>420</v>
       </c>
       <c r="B123" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="C123" t="s">
         <v>421</v>
       </c>
       <c r="D123" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="124">
@@ -16751,13 +16789,13 @@
         <v>422</v>
       </c>
       <c r="B124" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C124" t="s">
         <v>423</v>
       </c>
       <c r="D124" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="125">
@@ -16824,7 +16862,7 @@
         <v>445</v>
       </c>
       <c r="D132" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="133">
@@ -17012,45 +17050,48 @@
       <c r="A156" s="1" t="s">
         <v>497</v>
       </c>
+      <c r="B156" s="24" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
   </sheetData>
@@ -17075,59 +17116,59 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="B1" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B2" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B3" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B4" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B5" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="C8" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="D8" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="E8" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="F8" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
Monthly labor update - June 2023
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="637">
   <si>
     <t xml:space="preserve">LFS Round</t>
   </si>
@@ -1518,6 +1518,9 @@
     <t xml:space="preserve">2023 Jun</t>
   </si>
   <si>
+    <t>https://psa.gov.ph/content/employment-rate-june-2023-was-estimated-955-percent</t>
+  </si>
+  <si>
     <t xml:space="preserve">2023 Jul</t>
   </si>
   <si>
@@ -1570,6 +1573,9 @@
   </si>
   <si>
     <t>https://psa.gov.ph/statistics/survey/labor-and-employment/labor-force-survey/table</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/statistics/labor-force-survey/press-release/stat-tables</t>
   </si>
   <si>
     <t xml:space="preserve">ISH Bulletin</t>
@@ -12712,7 +12718,7 @@
         <v>32</v>
       </c>
       <c r="F230" s="11">
-        <f t="shared" ref="F230:G264" si="23">K230/J230</f>
+        <f t="shared" ref="F230:G265" si="23">K230/J230</f>
         <v>0.6168840849278201</v>
       </c>
       <c r="G230" s="11">
@@ -12720,11 +12726,11 @@
         <v>0.94678254834076803</v>
       </c>
       <c r="H230" s="11">
-        <f t="shared" ref="H230:H264" si="25">M230/K230</f>
+        <f t="shared" ref="H230:H265" si="25">M230/K230</f>
         <v>0.053217451659231869</v>
       </c>
       <c r="I230" s="11">
-        <f t="shared" ref="I230:I264" si="26">O230/L230</f>
+        <f t="shared" ref="I230:I265" si="26">O230/L230</f>
         <v>0.14805990963342192</v>
       </c>
       <c r="J230" s="12">
@@ -12948,7 +12954,7 @@
         <v>4500.7385000000004</v>
       </c>
       <c r="N234" s="2">
-        <f t="shared" ref="N230:N264" si="27">J234-K234</f>
+        <f t="shared" ref="N230:N265" si="27">J234-K234</f>
         <v>29852.987999999998</v>
       </c>
       <c r="O234" s="2">
@@ -13913,9 +13919,7 @@
       <c r="D253" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E253" s="1" t="s">
-        <v>425</v>
-      </c>
+      <c r="E253" s="1"/>
       <c r="F253" s="3">
         <f t="shared" si="23"/>
         <v>0.64778131062774802</v>
@@ -14323,7 +14327,7 @@
         <v>0.6448960129797745</v>
       </c>
       <c r="G261" s="3">
-        <f t="shared" ref="G261:G264" si="28">L261/K261</f>
+        <f t="shared" ref="G261:G265" si="28">L261/K261</f>
         <v>0.95227963685377781</v>
       </c>
       <c r="H261" s="3">
@@ -14539,19 +14543,19 @@
         <v>425</v>
       </c>
       <c r="F265" s="3">
-        <f>K265/J265</f>
+        <f t="shared" si="23"/>
         <v>0.65346941408460835</v>
       </c>
       <c r="G265" s="3">
-        <f>L265/K265</f>
+        <f t="shared" si="28"/>
         <v>0.95701872106453656</v>
       </c>
       <c r="H265" s="3">
-        <f>M265/K265</f>
+        <f t="shared" si="25"/>
         <v>0.042981278935463475</v>
       </c>
       <c r="I265" s="3">
-        <f>O265/L265</f>
+        <f t="shared" si="26"/>
         <v>0.11729164330819054</v>
       </c>
       <c r="J265" s="2">
@@ -14567,7 +14571,7 @@
         <v>2167.4580000000001</v>
       </c>
       <c r="N265" s="2">
-        <f>J265-K265</f>
+        <f t="shared" si="27"/>
         <v>26741.616999999998</v>
       </c>
       <c r="O265" s="2">
@@ -14593,11 +14597,48 @@
       <c r="E266" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="O266" s="2"/>
+      <c r="F266" s="3">
+        <f>K266/J266</f>
+        <v>0.66074689027081135</v>
+      </c>
+      <c r="G266" s="3">
+        <f>L266/K266</f>
+        <v>0.95452702169224368</v>
+      </c>
+      <c r="H266" s="3">
+        <f>M266/K266</f>
+        <v>0.045472978307756408</v>
+      </c>
+      <c r="I266" s="3">
+        <f>O266/L266</f>
+        <v>0.1202847318998803</v>
+      </c>
+      <c r="J266" s="2">
+        <v>77440.425000000003</v>
+      </c>
+      <c r="K266" s="2">
+        <v>51168.519999999997</v>
+      </c>
+      <c r="L266" s="2">
+        <v>48841.735000000001</v>
+      </c>
+      <c r="M266" s="2">
+        <v>2326.7849999999999</v>
+      </c>
+      <c r="N266" s="2">
+        <f>J266-K266</f>
+        <v>26271.905000000006</v>
+      </c>
+      <c r="O266" s="2">
+        <v>5874.915</v>
+      </c>
+      <c r="P266" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B267" s="1" t="s">
         <v>489</v>
@@ -14615,7 +14656,7 @@
     </row>
     <row r="268">
       <c r="A268" s="1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B268" s="1" t="s">
         <v>489</v>
@@ -14633,7 +14674,7 @@
     </row>
     <row r="269">
       <c r="A269" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B269" s="1" t="s">
         <v>489</v>
@@ -14651,7 +14692,7 @@
     </row>
     <row r="270">
       <c r="A270" s="1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>489</v>
@@ -14669,7 +14710,7 @@
     </row>
     <row r="271">
       <c r="A271" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>489</v>
@@ -14687,7 +14728,7 @@
     </row>
     <row r="272">
       <c r="A272" s="1" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>489</v>
@@ -14705,7 +14746,7 @@
     </row>
     <row r="273">
       <c r="A273" s="1" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>489</v>
@@ -14747,28 +14788,28 @@
         <v>1</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="2">
@@ -15534,7 +15575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView zoomScale="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B153" activeCellId="0" sqref="B153"/>
     </sheetView>
   </sheetViews>
@@ -15546,636 +15587,627 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B1" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>518</v>
-      </c>
       <c r="B3" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="22" t="s">
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B4" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="23" t="s">
-        <v>520</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>521</v>
-      </c>
-      <c r="D5" s="23" t="s">
+      <c r="B6" s="23" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B6" t="s">
-        <v>194</v>
+      <c r="C6" s="23" t="s">
+        <v>523</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
+      </c>
+      <c r="B10" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B14" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
+      </c>
+      <c r="B15" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B16" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B17" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B18" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B19" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
+      </c>
+      <c r="B20" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B21" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B22" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B23" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B24" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
+      </c>
+      <c r="B25" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B26" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B27" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B28" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B29" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
+      </c>
+      <c r="B30" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B31" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B32" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B33" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B34" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
+      </c>
+      <c r="B35" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B36" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B37" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B38" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B39" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
+      </c>
+      <c r="B40" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="B41" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B42" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B43" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B44" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
+      </c>
+      <c r="B45" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B46" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B47" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B48" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B49" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
+      </c>
+      <c r="B50" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B51" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B52" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B53" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B54" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
+      </c>
+      <c r="B55" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="B56" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B57" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B58" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B59" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
+      </c>
+      <c r="B60" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="B61" t="s">
-        <v>523</v>
-      </c>
-      <c r="D61" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B62" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="D62" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B63" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="D63" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B64" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D64" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
+      </c>
+      <c r="B65" t="s">
+        <v>528</v>
+      </c>
+      <c r="D65" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="B66" t="s">
-        <v>527</v>
-      </c>
-      <c r="D66" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B67" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D67" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B68" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D68" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B69" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D69" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B70" t="s">
-        <v>313</v>
+        <v>532</v>
+      </c>
+      <c r="D70" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B71" t="s">
-        <v>531</v>
-      </c>
-      <c r="D71" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B72" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D72" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B73" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="D73" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B74" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D74" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B75" t="s">
-        <v>535</v>
-      </c>
-      <c r="C75" t="s">
-        <v>323</v>
+        <v>536</v>
+      </c>
+      <c r="D75" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B76" t="s">
-        <v>536</v>
-      </c>
-      <c r="D76" t="s">
-        <v>325</v>
+        <v>537</v>
+      </c>
+      <c r="C76" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B77" t="s">
-        <v>537</v>
-      </c>
-      <c r="C77" t="s">
-        <v>327</v>
+        <v>538</v>
       </c>
       <c r="D77" t="s">
-        <v>538</v>
+        <v>325</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B78" t="s">
         <v>539</v>
       </c>
       <c r="C78" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D78" t="s">
         <v>540</v>
@@ -16183,13 +16215,13 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B79" t="s">
         <v>541</v>
       </c>
       <c r="C79" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D79" t="s">
         <v>542</v>
@@ -16197,38 +16229,38 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B80" t="s">
         <v>543</v>
       </c>
       <c r="C80" t="s">
-        <v>333</v>
+        <v>331</v>
+      </c>
+      <c r="D80" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B81" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="C81" t="s">
-        <v>335</v>
-      </c>
-      <c r="D81" t="s">
-        <v>545</v>
+        <v>333</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B82" t="s">
         <v>546</v>
       </c>
       <c r="C82" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D82" t="s">
         <v>547</v>
@@ -16236,13 +16268,13 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B83" t="s">
         <v>548</v>
       </c>
       <c r="C83" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D83" t="s">
         <v>549</v>
@@ -16250,13 +16282,13 @@
     </row>
     <row r="84">
       <c r="A84" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B84" t="s">
         <v>550</v>
       </c>
       <c r="C84" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D84" t="s">
         <v>551</v>
@@ -16264,38 +16296,38 @@
     </row>
     <row r="85">
       <c r="A85" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B85" t="s">
         <v>552</v>
       </c>
       <c r="C85" t="s">
-        <v>343</v>
+        <v>341</v>
+      </c>
+      <c r="D85" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B86" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C86" t="s">
-        <v>345</v>
-      </c>
-      <c r="D86" t="s">
-        <v>554</v>
+        <v>343</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B87" t="s">
         <v>555</v>
       </c>
       <c r="C87" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D87" t="s">
         <v>556</v>
@@ -16303,13 +16335,13 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B88" t="s">
         <v>557</v>
       </c>
       <c r="C88" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D88" t="s">
         <v>558</v>
@@ -16317,13 +16349,13 @@
     </row>
     <row r="89">
       <c r="A89" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B89" t="s">
         <v>559</v>
       </c>
       <c r="C89" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D89" t="s">
         <v>560</v>
@@ -16331,38 +16363,38 @@
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B90" t="s">
         <v>561</v>
       </c>
       <c r="C90" t="s">
-        <v>353</v>
+        <v>351</v>
+      </c>
+      <c r="D90" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B91" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="C91" t="s">
-        <v>355</v>
-      </c>
-      <c r="D91" t="s">
-        <v>563</v>
+        <v>353</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B92" t="s">
         <v>564</v>
       </c>
       <c r="C92" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D92" t="s">
         <v>565</v>
@@ -16370,13 +16402,13 @@
     </row>
     <row r="93">
       <c r="A93" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B93" t="s">
         <v>566</v>
       </c>
       <c r="C93" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D93" t="s">
         <v>567</v>
@@ -16384,13 +16416,13 @@
     </row>
     <row r="94">
       <c r="A94" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B94" t="s">
         <v>568</v>
       </c>
       <c r="C94" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D94" t="s">
         <v>569</v>
@@ -16398,38 +16430,38 @@
     </row>
     <row r="95">
       <c r="A95" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B95" t="s">
         <v>570</v>
       </c>
       <c r="C95" t="s">
-        <v>363</v>
+        <v>361</v>
+      </c>
+      <c r="D95" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B96" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C96" t="s">
-        <v>365</v>
-      </c>
-      <c r="D96" t="s">
-        <v>572</v>
+        <v>363</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B97" t="s">
         <v>573</v>
       </c>
       <c r="C97" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D97" t="s">
         <v>574</v>
@@ -16437,13 +16469,13 @@
     </row>
     <row r="98">
       <c r="A98" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B98" t="s">
         <v>575</v>
       </c>
       <c r="C98" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D98" t="s">
         <v>576</v>
@@ -16451,13 +16483,13 @@
     </row>
     <row r="99">
       <c r="A99" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B99" t="s">
         <v>577</v>
       </c>
       <c r="C99" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D99" t="s">
         <v>578</v>
@@ -16465,38 +16497,38 @@
     </row>
     <row r="100">
       <c r="A100" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B100" t="s">
         <v>579</v>
       </c>
       <c r="C100" t="s">
-        <v>373</v>
+        <v>371</v>
+      </c>
+      <c r="D100" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B101" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C101" t="s">
-        <v>375</v>
-      </c>
-      <c r="D101" t="s">
-        <v>581</v>
+        <v>373</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B102" t="s">
         <v>582</v>
       </c>
       <c r="C102" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D102" t="s">
         <v>583</v>
@@ -16504,13 +16536,13 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B103" t="s">
         <v>584</v>
       </c>
       <c r="C103" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D103" t="s">
         <v>585</v>
@@ -16518,13 +16550,13 @@
     </row>
     <row r="104">
       <c r="A104" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B104" t="s">
         <v>586</v>
       </c>
       <c r="C104" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D104" t="s">
         <v>587</v>
@@ -16532,38 +16564,38 @@
     </row>
     <row r="105">
       <c r="A105" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B105" t="s">
         <v>588</v>
       </c>
       <c r="C105" t="s">
-        <v>384</v>
+        <v>382</v>
+      </c>
+      <c r="D105" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B106" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="C106" t="s">
-        <v>386</v>
-      </c>
-      <c r="D106" t="s">
-        <v>590</v>
+        <v>384</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B107" t="s">
         <v>591</v>
       </c>
       <c r="C107" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D107" t="s">
         <v>592</v>
@@ -16571,13 +16603,13 @@
     </row>
     <row r="108">
       <c r="A108" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B108" t="s">
         <v>593</v>
       </c>
       <c r="C108" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D108" t="s">
         <v>594</v>
@@ -16585,13 +16617,13 @@
     </row>
     <row r="109">
       <c r="A109" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B109" t="s">
         <v>595</v>
       </c>
       <c r="C109" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D109" t="s">
         <v>596</v>
@@ -16599,38 +16631,38 @@
     </row>
     <row r="110">
       <c r="A110" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B110" t="s">
         <v>597</v>
       </c>
       <c r="C110" t="s">
-        <v>394</v>
+        <v>392</v>
+      </c>
+      <c r="D110" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B111" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C111" t="s">
-        <v>396</v>
-      </c>
-      <c r="D111" t="s">
-        <v>599</v>
+        <v>394</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B112" t="s">
         <v>600</v>
       </c>
       <c r="C112" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D112" t="s">
         <v>601</v>
@@ -16638,13 +16670,13 @@
     </row>
     <row r="113">
       <c r="A113" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B113" t="s">
         <v>602</v>
       </c>
       <c r="C113" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D113" t="s">
         <v>603</v>
@@ -16652,13 +16684,13 @@
     </row>
     <row r="114">
       <c r="A114" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B114" t="s">
         <v>604</v>
       </c>
       <c r="C114" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D114" t="s">
         <v>605</v>
@@ -16666,38 +16698,38 @@
     </row>
     <row r="115">
       <c r="A115" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B115" t="s">
         <v>606</v>
       </c>
       <c r="C115" t="s">
-        <v>404</v>
+        <v>402</v>
+      </c>
+      <c r="D115" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B116" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C116" t="s">
-        <v>406</v>
-      </c>
-      <c r="D116" t="s">
-        <v>608</v>
+        <v>404</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B117" t="s">
         <v>609</v>
       </c>
       <c r="C117" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D117" t="s">
         <v>610</v>
@@ -16705,13 +16737,13 @@
     </row>
     <row r="118">
       <c r="A118" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B118" t="s">
         <v>611</v>
       </c>
       <c r="C118" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D118" t="s">
         <v>612</v>
@@ -16719,13 +16751,13 @@
     </row>
     <row r="119">
       <c r="A119" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B119" t="s">
         <v>613</v>
       </c>
       <c r="C119" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D119" t="s">
         <v>614</v>
@@ -16733,38 +16765,38 @@
     </row>
     <row r="120">
       <c r="A120" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B120" t="s">
         <v>615</v>
       </c>
       <c r="C120" t="s">
-        <v>414</v>
+        <v>412</v>
+      </c>
+      <c r="D120" t="s">
+        <v>616</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B121" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="C121" t="s">
-        <v>416</v>
-      </c>
-      <c r="D121" t="s">
-        <v>617</v>
+        <v>414</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B122" t="s">
         <v>618</v>
       </c>
       <c r="C122" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D122" t="s">
         <v>619</v>
@@ -16772,13 +16804,13 @@
     </row>
     <row r="123">
       <c r="A123" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B123" t="s">
         <v>620</v>
       </c>
       <c r="C123" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D123" t="s">
         <v>621</v>
@@ -16786,13 +16818,13 @@
     </row>
     <row r="124">
       <c r="A124" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B124" t="s">
         <v>622</v>
       </c>
       <c r="C124" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D124" t="s">
         <v>623</v>
@@ -16800,267 +16832,279 @@
     </row>
     <row r="125">
       <c r="A125" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B125" t="s">
-        <v>426</v>
+        <v>624</v>
+      </c>
+      <c r="C125" t="s">
+        <v>423</v>
+      </c>
+      <c r="D125" t="s">
+        <v>625</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B126" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B127" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B128" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B129" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B130" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B131" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B132" t="s">
-        <v>445</v>
-      </c>
-      <c r="D132" t="s">
-        <v>624</v>
+        <v>443</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B133" t="s">
-        <v>448</v>
+        <v>445</v>
+      </c>
+      <c r="D133" t="s">
+        <v>626</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B134" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B135" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B136" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B137" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="B138" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B139" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B140" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B141" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B142" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B143" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B144" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B145" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B146" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B147" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B148" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="B149" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B150" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
+      </c>
+      <c r="B151" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="B152" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B153" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="s">
-        <v>493</v>
-      </c>
-      <c r="B154" s="24" t="s">
-        <v>494</v>
+        <v>491</v>
+      </c>
+      <c r="B154" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="s">
-        <v>495</v>
-      </c>
-      <c r="B155" t="s">
-        <v>496</v>
+        <v>493</v>
+      </c>
+      <c r="B155" s="24" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="s">
-        <v>497</v>
-      </c>
-      <c r="B156" s="24" t="s">
-        <v>498</v>
+        <v>495</v>
+      </c>
+      <c r="B156" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
+      </c>
+      <c r="B157" s="24" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="B158" s="24" t="s">
         <v>500</v>
       </c>
     </row>
@@ -17092,6 +17136,11 @@
     <row r="164">
       <c r="A164" s="1" t="s">
         <v>506</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="s">
+        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -17116,59 +17165,59 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="B1" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="B2" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="B3" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="B4" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="B5" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="C8" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="D8" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
       <c r="E8" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
       <c r="F8" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
Monthly labor update - July 2023
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="638">
   <si>
     <t xml:space="preserve">LFS Round</t>
   </si>
@@ -1522,6 +1522,9 @@
   </si>
   <si>
     <t xml:space="preserve">2023 Jul</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/employment-rate-july-2023-was-estimated-952-percent</t>
   </si>
   <si>
     <t xml:space="preserve">2023 Aug</t>
@@ -12718,7 +12721,7 @@
         <v>32</v>
       </c>
       <c r="F230" s="11">
-        <f t="shared" ref="F230:G265" si="23">K230/J230</f>
+        <f t="shared" ref="F230:G266" si="23">K230/J230</f>
         <v>0.6168840849278201</v>
       </c>
       <c r="G230" s="11">
@@ -12726,11 +12729,11 @@
         <v>0.94678254834076803</v>
       </c>
       <c r="H230" s="11">
-        <f t="shared" ref="H230:H265" si="25">M230/K230</f>
+        <f t="shared" ref="H230:H266" si="25">M230/K230</f>
         <v>0.053217451659231869</v>
       </c>
       <c r="I230" s="11">
-        <f t="shared" ref="I230:I265" si="26">O230/L230</f>
+        <f t="shared" ref="I230:I266" si="26">O230/L230</f>
         <v>0.14805990963342192</v>
       </c>
       <c r="J230" s="12">
@@ -12954,7 +12957,7 @@
         <v>4500.7385000000004</v>
       </c>
       <c r="N234" s="2">
-        <f t="shared" ref="N230:N265" si="27">J234-K234</f>
+        <f t="shared" ref="N230:N266" si="27">J234-K234</f>
         <v>29852.987999999998</v>
       </c>
       <c r="O234" s="2">
@@ -13972,43 +13975,41 @@
       <c r="D254" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E254" s="1" t="s">
-        <v>425</v>
-      </c>
+      <c r="E254" s="1"/>
       <c r="F254" s="3">
         <f t="shared" si="23"/>
-        <v>0.65232467715785714</v>
+        <v>0.65229908532939429</v>
       </c>
       <c r="G254" s="3">
         <f t="shared" si="24"/>
-        <v>0.94795101230329137</v>
+        <v>0.94793870537269542</v>
       </c>
       <c r="H254" s="3">
         <f t="shared" si="25"/>
-        <v>0.052048987696708626</v>
+        <v>0.052061274623940772</v>
       </c>
       <c r="I254" s="3">
         <f t="shared" si="26"/>
-        <v>0.13805717088869338</v>
+        <v>0.13803909834283151</v>
       </c>
       <c r="J254" s="2">
-        <v>76639.157999999996</v>
+        <v>76639.065000000002</v>
       </c>
       <c r="K254" s="2">
-        <v>49993.614000000001</v>
+        <v>49991.591999999997</v>
       </c>
       <c r="L254" s="2">
-        <v>47391.497000000003</v>
+        <v>47388.964999999997</v>
       </c>
       <c r="M254" s="2">
-        <v>2602.1170000000002</v>
+        <v>2602.6260000000002</v>
       </c>
       <c r="N254" s="2">
         <f t="shared" si="27"/>
-        <v>26645.543999999994</v>
+        <v>26647.473000000005</v>
       </c>
       <c r="O254" s="2">
-        <v>6542.7359999999999</v>
+        <v>6541.5299999999997</v>
       </c>
       <c r="P254" t="s">
         <v>476</v>
@@ -14327,7 +14328,7 @@
         <v>0.6448960129797745</v>
       </c>
       <c r="G261" s="3">
-        <f t="shared" ref="G261:G265" si="28">L261/K261</f>
+        <f t="shared" ref="G261:G266" si="28">L261/K261</f>
         <v>0.95227963685377781</v>
       </c>
       <c r="H261" s="3">
@@ -14598,19 +14599,19 @@
         <v>425</v>
       </c>
       <c r="F266" s="3">
-        <f>K266/J266</f>
+        <f t="shared" si="23"/>
         <v>0.66074689027081135</v>
       </c>
       <c r="G266" s="3">
-        <f>L266/K266</f>
+        <f t="shared" si="28"/>
         <v>0.95452702169224368</v>
       </c>
       <c r="H266" s="3">
-        <f>M266/K266</f>
+        <f t="shared" si="25"/>
         <v>0.045472978307756408</v>
       </c>
       <c r="I266" s="3">
-        <f>O266/L266</f>
+        <f t="shared" si="26"/>
         <v>0.1202847318998803</v>
       </c>
       <c r="J266" s="2">
@@ -14626,7 +14627,7 @@
         <v>2326.7849999999999</v>
       </c>
       <c r="N266" s="2">
-        <f>J266-K266</f>
+        <f t="shared" si="27"/>
         <v>26271.905000000006</v>
       </c>
       <c r="O266" s="2">
@@ -14652,11 +14653,47 @@
       <c r="E267" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="O267" s="2"/>
+      <c r="F267" s="3">
+        <f>K267/J267</f>
+        <v>0.60093428895027345</v>
+      </c>
+      <c r="G267" s="3">
+        <f>L267/K267</f>
+        <v>0.95153046680920927</v>
+      </c>
+      <c r="H267" s="3">
+        <f>M267/K267</f>
+        <v>0.048469511870375633</v>
+      </c>
+      <c r="I267" s="3">
+        <f>O267/L267</f>
+        <v>0.1591729879729373</v>
+      </c>
+      <c r="J267" s="2">
+        <v>78050.800000000003</v>
+      </c>
+      <c r="K267" s="2">
+        <v>46903.402000000002</v>
+      </c>
+      <c r="L267" s="2">
+        <v>44630.016000000003</v>
+      </c>
+      <c r="M267" s="2">
+        <v>2273.3850000000002</v>
+      </c>
+      <c r="N267" s="2">
+        <v>31147.399000000001</v>
+      </c>
+      <c r="O267" s="2">
+        <v>7103.893</v>
+      </c>
+      <c r="P267" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B268" s="1" t="s">
         <v>489</v>
@@ -14674,7 +14711,7 @@
     </row>
     <row r="269">
       <c r="A269" s="1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B269" s="1" t="s">
         <v>489</v>
@@ -14692,7 +14729,7 @@
     </row>
     <row r="270">
       <c r="A270" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>489</v>
@@ -14710,7 +14747,7 @@
     </row>
     <row r="271">
       <c r="A271" s="1" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>489</v>
@@ -14728,7 +14765,7 @@
     </row>
     <row r="272">
       <c r="A272" s="1" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>489</v>
@@ -14746,7 +14783,7 @@
     </row>
     <row r="273">
       <c r="A273" s="1" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>489</v>
@@ -14788,28 +14825,28 @@
         <v>1</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="2">
@@ -15587,28 +15624,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B1" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B4" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="6">
@@ -15616,13 +15653,13 @@
         <v>0</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="7">
@@ -16037,7 +16074,7 @@
         <v>295</v>
       </c>
       <c r="B62" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="D62" t="s">
         <v>296</v>
@@ -16048,7 +16085,7 @@
         <v>297</v>
       </c>
       <c r="B63" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="D63" t="s">
         <v>298</v>
@@ -16059,7 +16096,7 @@
         <v>299</v>
       </c>
       <c r="B64" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="D64" t="s">
         <v>300</v>
@@ -16070,7 +16107,7 @@
         <v>301</v>
       </c>
       <c r="B65" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D65" t="s">
         <v>302</v>
@@ -16086,7 +16123,7 @@
         <v>304</v>
       </c>
       <c r="B67" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D67" t="s">
         <v>305</v>
@@ -16097,7 +16134,7 @@
         <v>306</v>
       </c>
       <c r="B68" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D68" t="s">
         <v>307</v>
@@ -16108,7 +16145,7 @@
         <v>308</v>
       </c>
       <c r="B69" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="D69" t="s">
         <v>309</v>
@@ -16119,7 +16156,7 @@
         <v>310</v>
       </c>
       <c r="B70" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D70" t="s">
         <v>311</v>
@@ -16138,7 +16175,7 @@
         <v>314</v>
       </c>
       <c r="B72" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="D72" t="s">
         <v>315</v>
@@ -16149,7 +16186,7 @@
         <v>316</v>
       </c>
       <c r="B73" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D73" t="s">
         <v>317</v>
@@ -16160,7 +16197,7 @@
         <v>318</v>
       </c>
       <c r="B74" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D74" t="s">
         <v>319</v>
@@ -16171,7 +16208,7 @@
         <v>320</v>
       </c>
       <c r="B75" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="D75" t="s">
         <v>321</v>
@@ -16182,7 +16219,7 @@
         <v>322</v>
       </c>
       <c r="B76" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C76" t="s">
         <v>323</v>
@@ -16193,7 +16230,7 @@
         <v>324</v>
       </c>
       <c r="B77" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D77" t="s">
         <v>325</v>
@@ -16204,13 +16241,13 @@
         <v>326</v>
       </c>
       <c r="B78" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C78" t="s">
         <v>327</v>
       </c>
       <c r="D78" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="79">
@@ -16218,13 +16255,13 @@
         <v>328</v>
       </c>
       <c r="B79" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="C79" t="s">
         <v>329</v>
       </c>
       <c r="D79" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="80">
@@ -16232,13 +16269,13 @@
         <v>330</v>
       </c>
       <c r="B80" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C80" t="s">
         <v>331</v>
       </c>
       <c r="D80" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="81">
@@ -16246,7 +16283,7 @@
         <v>332</v>
       </c>
       <c r="B81" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="C81" t="s">
         <v>333</v>
@@ -16257,13 +16294,13 @@
         <v>334</v>
       </c>
       <c r="B82" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C82" t="s">
         <v>335</v>
       </c>
       <c r="D82" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="83">
@@ -16271,13 +16308,13 @@
         <v>336</v>
       </c>
       <c r="B83" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C83" t="s">
         <v>337</v>
       </c>
       <c r="D83" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="84">
@@ -16285,13 +16322,13 @@
         <v>338</v>
       </c>
       <c r="B84" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C84" t="s">
         <v>339</v>
       </c>
       <c r="D84" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="85">
@@ -16299,13 +16336,13 @@
         <v>340</v>
       </c>
       <c r="B85" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="C85" t="s">
         <v>341</v>
       </c>
       <c r="D85" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="86">
@@ -16313,7 +16350,7 @@
         <v>342</v>
       </c>
       <c r="B86" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C86" t="s">
         <v>343</v>
@@ -16324,13 +16361,13 @@
         <v>344</v>
       </c>
       <c r="B87" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C87" t="s">
         <v>345</v>
       </c>
       <c r="D87" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="88">
@@ -16338,13 +16375,13 @@
         <v>346</v>
       </c>
       <c r="B88" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C88" t="s">
         <v>347</v>
       </c>
       <c r="D88" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="89">
@@ -16352,13 +16389,13 @@
         <v>348</v>
       </c>
       <c r="B89" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C89" t="s">
         <v>349</v>
       </c>
       <c r="D89" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="90">
@@ -16366,13 +16403,13 @@
         <v>350</v>
       </c>
       <c r="B90" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C90" t="s">
         <v>351</v>
       </c>
       <c r="D90" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="91">
@@ -16380,7 +16417,7 @@
         <v>352</v>
       </c>
       <c r="B91" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="C91" t="s">
         <v>353</v>
@@ -16391,13 +16428,13 @@
         <v>354</v>
       </c>
       <c r="B92" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C92" t="s">
         <v>355</v>
       </c>
       <c r="D92" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="93">
@@ -16405,13 +16442,13 @@
         <v>356</v>
       </c>
       <c r="B93" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="C93" t="s">
         <v>357</v>
       </c>
       <c r="D93" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="94">
@@ -16419,13 +16456,13 @@
         <v>358</v>
       </c>
       <c r="B94" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="C94" t="s">
         <v>359</v>
       </c>
       <c r="D94" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="95">
@@ -16433,13 +16470,13 @@
         <v>360</v>
       </c>
       <c r="B95" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C95" t="s">
         <v>361</v>
       </c>
       <c r="D95" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="96">
@@ -16447,7 +16484,7 @@
         <v>362</v>
       </c>
       <c r="B96" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C96" t="s">
         <v>363</v>
@@ -16458,13 +16495,13 @@
         <v>364</v>
       </c>
       <c r="B97" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C97" t="s">
         <v>365</v>
       </c>
       <c r="D97" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="98">
@@ -16472,13 +16509,13 @@
         <v>366</v>
       </c>
       <c r="B98" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C98" t="s">
         <v>367</v>
       </c>
       <c r="D98" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="99">
@@ -16486,13 +16523,13 @@
         <v>368</v>
       </c>
       <c r="B99" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C99" t="s">
         <v>369</v>
       </c>
       <c r="D99" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="100">
@@ -16500,13 +16537,13 @@
         <v>370</v>
       </c>
       <c r="B100" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C100" t="s">
         <v>371</v>
       </c>
       <c r="D100" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="101">
@@ -16514,7 +16551,7 @@
         <v>372</v>
       </c>
       <c r="B101" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C101" t="s">
         <v>373</v>
@@ -16525,13 +16562,13 @@
         <v>374</v>
       </c>
       <c r="B102" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="C102" t="s">
         <v>375</v>
       </c>
       <c r="D102" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="103">
@@ -16539,13 +16576,13 @@
         <v>376</v>
       </c>
       <c r="B103" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="C103" t="s">
         <v>377</v>
       </c>
       <c r="D103" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="104">
@@ -16553,13 +16590,13 @@
         <v>379</v>
       </c>
       <c r="B104" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C104" t="s">
         <v>380</v>
       </c>
       <c r="D104" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="105">
@@ -16567,13 +16604,13 @@
         <v>381</v>
       </c>
       <c r="B105" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="C105" t="s">
         <v>382</v>
       </c>
       <c r="D105" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="106">
@@ -16581,7 +16618,7 @@
         <v>383</v>
       </c>
       <c r="B106" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="C106" t="s">
         <v>384</v>
@@ -16592,13 +16629,13 @@
         <v>385</v>
       </c>
       <c r="B107" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="C107" t="s">
         <v>386</v>
       </c>
       <c r="D107" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="108">
@@ -16606,13 +16643,13 @@
         <v>387</v>
       </c>
       <c r="B108" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C108" t="s">
         <v>388</v>
       </c>
       <c r="D108" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="109">
@@ -16620,13 +16657,13 @@
         <v>389</v>
       </c>
       <c r="B109" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C109" t="s">
         <v>390</v>
       </c>
       <c r="D109" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="110">
@@ -16634,13 +16671,13 @@
         <v>391</v>
       </c>
       <c r="B110" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="C110" t="s">
         <v>392</v>
       </c>
       <c r="D110" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="111">
@@ -16648,7 +16685,7 @@
         <v>393</v>
       </c>
       <c r="B111" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="C111" t="s">
         <v>394</v>
@@ -16659,13 +16696,13 @@
         <v>395</v>
       </c>
       <c r="B112" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="C112" t="s">
         <v>396</v>
       </c>
       <c r="D112" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="113">
@@ -16673,13 +16710,13 @@
         <v>397</v>
       </c>
       <c r="B113" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="C113" t="s">
         <v>398</v>
       </c>
       <c r="D113" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="114">
@@ -16687,13 +16724,13 @@
         <v>399</v>
       </c>
       <c r="B114" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="C114" t="s">
         <v>400</v>
       </c>
       <c r="D114" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="115">
@@ -16701,13 +16738,13 @@
         <v>401</v>
       </c>
       <c r="B115" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="C115" t="s">
         <v>402</v>
       </c>
       <c r="D115" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="116">
@@ -16715,7 +16752,7 @@
         <v>403</v>
       </c>
       <c r="B116" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="C116" t="s">
         <v>404</v>
@@ -16726,13 +16763,13 @@
         <v>405</v>
       </c>
       <c r="B117" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="C117" t="s">
         <v>406</v>
       </c>
       <c r="D117" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="118">
@@ -16740,13 +16777,13 @@
         <v>407</v>
       </c>
       <c r="B118" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="C118" t="s">
         <v>408</v>
       </c>
       <c r="D118" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="119">
@@ -16754,13 +16791,13 @@
         <v>409</v>
       </c>
       <c r="B119" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="C119" t="s">
         <v>410</v>
       </c>
       <c r="D119" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="120">
@@ -16768,13 +16805,13 @@
         <v>411</v>
       </c>
       <c r="B120" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C120" t="s">
         <v>412</v>
       </c>
       <c r="D120" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="121">
@@ -16782,7 +16819,7 @@
         <v>413</v>
       </c>
       <c r="B121" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C121" t="s">
         <v>414</v>
@@ -16793,13 +16830,13 @@
         <v>415</v>
       </c>
       <c r="B122" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="C122" t="s">
         <v>416</v>
       </c>
       <c r="D122" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="123">
@@ -16807,13 +16844,13 @@
         <v>418</v>
       </c>
       <c r="B123" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C123" t="s">
         <v>419</v>
       </c>
       <c r="D123" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="124">
@@ -16821,13 +16858,13 @@
         <v>420</v>
       </c>
       <c r="B124" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="C124" t="s">
         <v>421</v>
       </c>
       <c r="D124" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="125">
@@ -16835,13 +16872,13 @@
         <v>422</v>
       </c>
       <c r="B125" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="C125" t="s">
         <v>423</v>
       </c>
       <c r="D125" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="126">
@@ -16908,7 +16945,7 @@
         <v>445</v>
       </c>
       <c r="D133" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="134">
@@ -17112,35 +17149,38 @@
       <c r="A159" s="1" t="s">
         <v>501</v>
       </c>
+      <c r="B159" s="24" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
   </sheetData>
@@ -17165,59 +17205,59 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B1" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B2" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B3" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B4" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="B5" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C8" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="D8" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="E8" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F8" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
Aug to Sep 2023
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="638">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="640">
   <si>
     <t xml:space="preserve">LFS Round</t>
   </si>
@@ -1530,7 +1530,13 @@
     <t xml:space="preserve">2023 Aug</t>
   </si>
   <si>
+    <t>https://psa.gov.ph/content/employment-rate-august-2023-was-estimated-956-percent</t>
+  </si>
+  <si>
     <t xml:space="preserve">2023 Sep</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/unemployment-rate-september-2023-was-estimated-45-percent</t>
   </si>
   <si>
     <t xml:space="preserve">2023 Oct</t>
@@ -2031,15 +2037,15 @@
     <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="4" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="162" xfId="0" applyNumberFormat="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma 3" xfId="1"/>
@@ -12721,7 +12727,7 @@
         <v>32</v>
       </c>
       <c r="F230" s="11">
-        <f t="shared" ref="F230:G266" si="23">K230/J230</f>
+        <f t="shared" ref="F230:G267" si="23">K230/J230</f>
         <v>0.6168840849278201</v>
       </c>
       <c r="G230" s="11">
@@ -12729,11 +12735,11 @@
         <v>0.94678254834076803</v>
       </c>
       <c r="H230" s="11">
-        <f t="shared" ref="H230:H266" si="25">M230/K230</f>
+        <f t="shared" ref="H230:H267" si="25">M230/K230</f>
         <v>0.053217451659231869</v>
       </c>
       <c r="I230" s="11">
-        <f t="shared" ref="I230:I266" si="26">O230/L230</f>
+        <f t="shared" ref="I230:I267" si="26">O230/L230</f>
         <v>0.14805990963342192</v>
       </c>
       <c r="J230" s="12">
@@ -14028,43 +14034,41 @@
       <c r="D255" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E255" s="1" t="s">
-        <v>425</v>
-      </c>
+      <c r="E255" s="1"/>
       <c r="F255" s="3">
         <f t="shared" si="23"/>
-        <v>0.66062996242102423</v>
+        <v>0.66064860773722345</v>
       </c>
       <c r="G255" s="3">
         <f t="shared" si="24"/>
-        <v>0.94696892591578208</v>
+        <v>0.94695747626336979</v>
       </c>
       <c r="H255" s="3">
         <f t="shared" si="25"/>
-        <v>0.053031093866359173</v>
+        <v>0.053042523736630362</v>
       </c>
       <c r="I255" s="3">
         <f t="shared" si="26"/>
-        <v>0.14686722697712487</v>
+        <v>0.14691838897372533</v>
       </c>
       <c r="J255" s="2">
-        <v>76518.850000000006</v>
+        <v>76518.637000000002</v>
       </c>
       <c r="K255" s="2">
-        <v>50550.644999999997</v>
+        <v>50551.930999999997</v>
       </c>
       <c r="L255" s="2">
-        <v>47869.889999999999</v>
+        <v>47870.529000000002</v>
       </c>
       <c r="M255" s="2">
-        <v>2680.7559999999999</v>
+        <v>2681.402</v>
       </c>
       <c r="N255" s="2">
         <f t="shared" si="27"/>
-        <v>25968.205000000009</v>
+        <v>25966.706000000006</v>
       </c>
       <c r="O255" s="2">
-        <v>7030.518</v>
+        <v>7033.0609999999997</v>
       </c>
       <c r="P255" t="s">
         <v>478</v>
@@ -14083,9 +14087,7 @@
       <c r="D256" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E256" s="1" t="s">
-        <v>425</v>
-      </c>
+      <c r="E256" s="1"/>
       <c r="F256" s="3">
         <f t="shared" si="23"/>
         <v>0.65181823366707692</v>
@@ -14328,7 +14330,7 @@
         <v>0.6448960129797745</v>
       </c>
       <c r="G261" s="3">
-        <f t="shared" ref="G261:G266" si="28">L261/K261</f>
+        <f t="shared" ref="G261:G267" si="28">L261/K261</f>
         <v>0.95227963685377781</v>
       </c>
       <c r="H261" s="3">
@@ -14654,19 +14656,19 @@
         <v>425</v>
       </c>
       <c r="F267" s="3">
-        <f>K267/J267</f>
+        <f t="shared" si="23"/>
         <v>0.60093428895027345</v>
       </c>
       <c r="G267" s="3">
-        <f>L267/K267</f>
+        <f t="shared" si="28"/>
         <v>0.95153046680920927</v>
       </c>
       <c r="H267" s="3">
-        <f>M267/K267</f>
+        <f t="shared" si="25"/>
         <v>0.048469511870375633</v>
       </c>
       <c r="I267" s="3">
-        <f>O267/L267</f>
+        <f t="shared" si="26"/>
         <v>0.1591729879729373</v>
       </c>
       <c r="J267" s="2">
@@ -14682,7 +14684,8 @@
         <v>2273.3850000000002</v>
       </c>
       <c r="N267" s="2">
-        <v>31147.399000000001</v>
+        <f>J267-K267</f>
+        <v>31147.398000000001</v>
       </c>
       <c r="O267" s="2">
         <v>7103.893</v>
@@ -14707,11 +14710,48 @@
       <c r="E268" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="O268" s="2"/>
+      <c r="F268" s="3">
+        <f>K268/J268</f>
+        <v>0.64650853861229718</v>
+      </c>
+      <c r="G268" s="3">
+        <f>L268/K268</f>
+        <v>0.95597557716757331</v>
+      </c>
+      <c r="H268" s="3">
+        <f>M268/K268</f>
+        <v>0.044024422832426691</v>
+      </c>
+      <c r="I268" s="3">
+        <f>O268/L268</f>
+        <v>0.11711656128289734</v>
+      </c>
+      <c r="J268" s="2">
+        <v>77782.486999999994</v>
+      </c>
+      <c r="K268" s="2">
+        <v>50287.042000000001</v>
+      </c>
+      <c r="L268" s="2">
+        <v>48073.184000000001</v>
+      </c>
+      <c r="M268" s="2">
+        <v>2213.8580000000002</v>
+      </c>
+      <c r="N268" s="2">
+        <f>J268-K268</f>
+        <v>27495.444999999992</v>
+      </c>
+      <c r="O268" s="2">
+        <v>5630.1660000000002</v>
+      </c>
+      <c r="P268" s="20" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B269" s="1" t="s">
         <v>489</v>
@@ -14725,11 +14765,48 @@
       <c r="E269" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="O269" s="2"/>
+      <c r="F269" s="3">
+        <f>K269/J269</f>
+        <v>0.64049609363750415</v>
+      </c>
+      <c r="G269" s="3">
+        <f>L269/K269</f>
+        <v>0.9546663534776707</v>
+      </c>
+      <c r="H269" s="3">
+        <f>M269/K269</f>
+        <v>0.045333646522329352</v>
+      </c>
+      <c r="I269" s="3">
+        <f>O269/L269</f>
+        <v>0.10725448980279445</v>
+      </c>
+      <c r="J269" s="2">
+        <v>77954.235000000001</v>
+      </c>
+      <c r="K269" s="2">
+        <v>49929.383000000002</v>
+      </c>
+      <c r="L269" s="2">
+        <v>47665.902000000002</v>
+      </c>
+      <c r="M269" s="2">
+        <v>2263.4810000000002</v>
+      </c>
+      <c r="N269" s="2">
+        <f>J269-K269</f>
+        <v>28024.851999999999</v>
+      </c>
+      <c r="O269" s="2">
+        <v>5112.3819999999996</v>
+      </c>
+      <c r="P269" s="20" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>489</v>
@@ -14747,7 +14824,7 @@
     </row>
     <row r="271">
       <c r="A271" s="1" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>489</v>
@@ -14765,7 +14842,7 @@
     </row>
     <row r="272">
       <c r="A272" s="1" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>489</v>
@@ -14783,7 +14860,7 @@
     </row>
     <row r="273">
       <c r="A273" s="1" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>489</v>
@@ -14820,61 +14897,61 @@
     <col customWidth="1" min="2" max="9" width="16.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" s="20" customFormat="1" ht="57">
-      <c r="A1" s="20" t="s">
+    <row r="1" s="21" customFormat="1" ht="57">
+      <c r="A1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>509</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>510</v>
-      </c>
-      <c r="D1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>511</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>512</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="D1" s="21" t="s">
         <v>513</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="E1" s="21" t="s">
         <v>514</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="F1" s="21" t="s">
         <v>515</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="G1" s="21" t="s">
         <v>516</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>517</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="2">
       <c r="A2">
         <v>1995</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="22">
         <v>43156</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="22">
         <v>65.799999999999997</v>
       </c>
-      <c r="D2" s="21">
+      <c r="D2" s="22">
         <v>28380</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="22">
         <v>90.5</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="22">
         <v>25677</v>
       </c>
-      <c r="G2" s="21">
+      <c r="G2" s="22">
         <v>9.5</v>
       </c>
-      <c r="H2" s="21">
+      <c r="H2" s="22">
         <v>2704</v>
       </c>
-      <c r="I2" s="21">
+      <c r="I2" s="22">
         <v>20</v>
       </c>
     </row>
@@ -14882,28 +14959,28 @@
       <c r="A3">
         <v>1996</v>
       </c>
-      <c r="B3" s="21">
+      <c r="B3" s="22">
         <v>44599</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="22">
         <v>66.700000000000003</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="22">
         <v>29733</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="22">
         <v>91.400000000000006</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="22">
         <v>27186</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="22">
         <v>8.5999999999999996</v>
       </c>
-      <c r="H3" s="21">
+      <c r="H3" s="22">
         <v>2546</v>
       </c>
-      <c r="I3" s="21">
+      <c r="I3" s="22">
         <v>21</v>
       </c>
     </row>
@@ -14911,28 +14988,28 @@
       <c r="A4">
         <v>1997</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="22">
         <v>44658</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="22">
         <v>64.700000000000003</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="22">
         <v>28901</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="22">
         <v>91.200000000000003</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="22">
         <v>26365</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="22">
         <v>8.8000000000000007</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="22">
         <v>2537</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I4" s="22">
         <v>21.899999999999999</v>
       </c>
     </row>
@@ -14940,28 +15017,28 @@
       <c r="A5">
         <v>1998</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="22">
         <v>45964</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="22">
         <v>64.599999999999994</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="22">
         <v>29674</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="22">
         <v>89.700000000000003</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="22">
         <v>26631</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="22">
         <v>10.300000000000001</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="22">
         <v>3043</v>
       </c>
-      <c r="I5" s="21">
+      <c r="I5" s="22">
         <v>21.600000000000001</v>
       </c>
     </row>
@@ -14969,28 +15046,28 @@
       <c r="A6">
         <v>1999</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="22">
         <v>47270</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="22">
         <v>65.099999999999994</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="22">
         <v>30759</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="22">
         <v>90.200000000000003</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="22">
         <v>27742</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="22">
         <v>9.8000000000000007</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="22">
         <v>3017</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6" s="22">
         <v>22.100000000000001</v>
       </c>
     </row>
@@ -14998,28 +15075,28 @@
       <c r="A7">
         <v>2000</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="22">
         <v>48587</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="22">
         <v>63.600000000000001</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="22">
         <v>30911</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="22">
         <v>88.809808805926693</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="22">
         <v>27452</v>
       </c>
-      <c r="G7" s="21">
+      <c r="G7" s="22">
         <v>11.190191194073307</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="22">
         <v>3459</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="22">
         <v>21.699999999999999</v>
       </c>
     </row>
@@ -15027,28 +15104,28 @@
       <c r="A8">
         <v>2001</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="22">
         <v>48929</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="22">
         <v>67.099999999999994</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="22">
         <v>32809</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="22">
         <v>88.865859977445211</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="22">
         <v>29156</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="22">
         <v>11.134140022554787</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="22">
         <v>3653</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="22">
         <v>17.199999999999999</v>
       </c>
     </row>
@@ -15056,28 +15133,28 @@
       <c r="A9">
         <v>2002</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="22">
         <v>50344</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="22">
         <v>67.400000000000006</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="22">
         <v>33936</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="22">
         <v>88.584394153701083</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="22">
         <v>30062</v>
       </c>
-      <c r="G9" s="21">
+      <c r="G9" s="22">
         <v>11.415605846298915</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="22">
         <v>3874</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="22">
         <v>17</v>
       </c>
     </row>
@@ -15085,28 +15162,28 @@
       <c r="A10">
         <v>2003</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="22">
         <v>51793</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="22">
         <v>66.700000000000003</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="22">
         <v>34571</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="22">
         <v>88.614734893407771</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="22">
         <v>30635</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="22">
         <v>11.385265106592231</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="22">
         <v>3936</v>
       </c>
-      <c r="I10" s="21">
+      <c r="I10" s="22">
         <v>17</v>
       </c>
     </row>
@@ -15114,28 +15191,28 @@
       <c r="A11">
         <v>2004</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="22">
         <v>53144</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="22">
         <v>67.5</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="22">
         <v>35862</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="22">
         <v>88.151804138084884</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="22">
         <v>31613</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="22">
         <v>11.848195861915119</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="22">
         <v>4249</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="22">
         <v>17.600000000000001</v>
       </c>
     </row>
@@ -15143,28 +15220,28 @@
       <c r="A12">
         <v>2005</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="22">
         <v>54388</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="22">
         <v>64.716310972814028</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="22">
         <v>35286</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="22">
         <v>92.21337414156298</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="22">
         <v>32539</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="22">
         <v>7.7866258584370058</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="22">
         <v>2747.6666666666665</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="22">
         <v>21</v>
       </c>
     </row>
@@ -15172,28 +15249,28 @@
       <c r="A13">
         <v>2006</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="22">
         <v>55230</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="22">
         <v>64.200000000000003</v>
       </c>
-      <c r="D13" s="21">
+      <c r="D13" s="22">
         <v>35464</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="22">
         <v>92.02312138728324</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="22">
         <v>32636</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="22">
         <v>7.9768786127167628</v>
       </c>
-      <c r="H13" s="21">
+      <c r="H13" s="22">
         <v>2829</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I13" s="22">
         <v>22.600000000000001</v>
       </c>
     </row>
@@ -15201,28 +15278,28 @@
       <c r="A14">
         <v>2007</v>
       </c>
-      <c r="B14" s="21">
+      <c r="B14" s="22">
         <v>56565</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="22">
         <v>64</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="22">
         <v>36213</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="22">
         <v>92.67390163753349</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="22">
         <v>33560</v>
       </c>
-      <c r="G14" s="21">
+      <c r="G14" s="22">
         <v>7.3260983624665172</v>
       </c>
-      <c r="H14" s="21">
+      <c r="H14" s="22">
         <v>2653</v>
       </c>
-      <c r="I14" s="21">
+      <c r="I14" s="22">
         <v>20.100000000000001</v>
       </c>
     </row>
@@ -15230,28 +15307,28 @@
       <c r="A15">
         <v>2008</v>
       </c>
-      <c r="B15" s="21">
+      <c r="B15" s="22">
         <v>57848</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="22">
         <v>63.600000000000001</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="22">
         <v>36805</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="22">
         <v>92.620567857628046</v>
       </c>
-      <c r="F15" s="21">
+      <c r="F15" s="22">
         <v>34089</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="22">
         <v>7.4000000000000004</v>
       </c>
-      <c r="H15" s="21">
+      <c r="H15" s="22">
         <v>2716</v>
       </c>
-      <c r="I15" s="21">
+      <c r="I15" s="22">
         <v>19.300000000000001</v>
       </c>
     </row>
@@ -15259,28 +15336,28 @@
       <c r="A16">
         <v>2009</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="22">
         <v>59237</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="22">
         <v>63.966355487279912</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="22">
         <v>37891.75</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="22">
         <v>92.530036221604973</v>
       </c>
-      <c r="F16" s="21">
+      <c r="F16" s="22">
         <v>35061.25</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="22">
         <v>7.4699637783950337</v>
       </c>
-      <c r="H16" s="21">
+      <c r="H16" s="22">
         <v>2830.5</v>
       </c>
-      <c r="I16" s="21">
+      <c r="I16" s="22">
         <v>19.087311490605728</v>
       </c>
     </row>
@@ -15288,28 +15365,28 @@
       <c r="A17">
         <v>2010</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="22">
         <v>60717</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="22">
         <v>64.099999999999994</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="22">
         <v>38893</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="22">
         <v>92.700000000000003</v>
       </c>
-      <c r="F17" s="21">
+      <c r="F17" s="22">
         <v>36035</v>
       </c>
-      <c r="G17" s="21">
+      <c r="G17" s="22">
         <v>7.2999999999999998</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="22">
         <v>2859</v>
       </c>
-      <c r="I17" s="21">
+      <c r="I17" s="22">
         <v>18.699999999999999</v>
       </c>
     </row>
@@ -15317,28 +15394,28 @@
       <c r="A18">
         <v>2011</v>
       </c>
-      <c r="B18" s="21">
+      <c r="B18" s="22">
         <v>61882.531999999999</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C18" s="22">
         <v>64.647477174980494</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="22">
         <v>40006.042999999998</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="22">
         <v>92.967334369303501</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="22">
         <v>37192.042999999998</v>
       </c>
-      <c r="G18" s="21">
+      <c r="G18" s="22">
         <v>7.0326656306965027</v>
       </c>
-      <c r="H18" s="21">
+      <c r="H18" s="22">
         <v>2814</v>
       </c>
-      <c r="I18" s="21">
+      <c r="I18" s="22">
         <v>19.260093482899016</v>
       </c>
     </row>
@@ -15346,28 +15423,28 @@
       <c r="A19">
         <v>2012</v>
       </c>
-      <c r="B19" s="21">
+      <c r="B19" s="22">
         <v>62985.349249999999</v>
       </c>
-      <c r="C19" s="21">
+      <c r="C19" s="22">
         <v>64.183842721170592</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D19" s="22">
         <v>40426.417499999996</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E19" s="22">
         <v>93.008986636028297</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="22">
         <v>37600.201249999998</v>
       </c>
-      <c r="G19" s="21">
+      <c r="G19" s="22">
         <v>6.9910133639717156</v>
       </c>
-      <c r="H19" s="21">
+      <c r="H19" s="22">
         <v>2826.2162499999999</v>
       </c>
-      <c r="I19" s="21">
+      <c r="I19" s="22">
         <v>19.984181600623746</v>
       </c>
     </row>
@@ -15375,28 +15452,28 @@
       <c r="A20">
         <v>2013</v>
       </c>
-      <c r="B20" s="21">
+      <c r="B20" s="22">
         <v>64173.311000000002</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C20" s="22">
         <v>63.92431465784896</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D20" s="22">
         <v>41022.349249999999</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="22">
         <v>92.919384059897538</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F20" s="22">
         <v>38117.714249999997</v>
       </c>
-      <c r="G20" s="21">
+      <c r="G20" s="22">
         <v>7.0806159401024553</v>
       </c>
-      <c r="H20" s="21">
+      <c r="H20" s="22">
         <v>2904.6350000000002</v>
       </c>
-      <c r="I20" s="21">
+      <c r="I20" s="22">
         <v>19.338649090166786</v>
       </c>
     </row>
@@ -15404,28 +15481,28 @@
       <c r="A21">
         <v>2014</v>
       </c>
-      <c r="B21" s="21">
+      <c r="B21" s="22">
         <v>64033.078333333338</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="22">
         <v>64.621820071277213</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="22">
         <v>41379.340666666671</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="22">
         <v>93.407133553328265</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="22">
         <v>38651.256000000001</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="22">
         <v>6.5928664466717537</v>
       </c>
-      <c r="H21" s="21">
+      <c r="H21" s="22">
         <v>2728.0846666666666</v>
       </c>
-      <c r="I21" s="21">
+      <c r="I21" s="22">
         <v>18.41672363764841</v>
       </c>
     </row>
@@ -15433,28 +15510,28 @@
       <c r="A22">
         <v>2015</v>
       </c>
-      <c r="B22" s="21">
+      <c r="B22" s="22">
         <v>64936</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="22">
         <v>63.700000000000003</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="22">
         <v>41342</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="22">
         <v>93.700000000000003</v>
       </c>
-      <c r="F22" s="21">
+      <c r="F22" s="22">
         <v>38741</v>
       </c>
-      <c r="G22" s="21">
+      <c r="G22" s="22">
         <v>6.2999999999999998</v>
       </c>
-      <c r="H22" s="21">
+      <c r="H22" s="22">
         <v>2958</v>
       </c>
-      <c r="I22" s="21">
+      <c r="I22" s="22">
         <v>18.5</v>
       </c>
     </row>
@@ -15462,28 +15539,28 @@
       <c r="A23">
         <v>2016</v>
       </c>
-      <c r="B23" s="21">
+      <c r="B23" s="22">
         <v>68311</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C23" s="22">
         <v>63.5</v>
       </c>
-      <c r="D23" s="21">
+      <c r="D23" s="22">
         <v>43361</v>
       </c>
-      <c r="E23" s="21">
+      <c r="E23" s="22">
         <v>94.599999999999994</v>
       </c>
-      <c r="F23" s="21">
+      <c r="F23" s="22">
         <v>40998</v>
       </c>
-      <c r="G23" s="21">
+      <c r="G23" s="22">
         <v>5.4000000000000004</v>
       </c>
-      <c r="H23" s="21">
+      <c r="H23" s="22">
         <v>2363</v>
       </c>
-      <c r="I23" s="21">
+      <c r="I23" s="22">
         <v>18.300000000000001</v>
       </c>
     </row>
@@ -15491,28 +15568,28 @@
       <c r="A24">
         <v>2017</v>
       </c>
-      <c r="B24" s="21">
+      <c r="B24" s="22">
         <v>69890.685750000004</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="22">
         <v>61.200000000000003</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="22">
         <v>42775</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="22">
         <v>94.281162928439798</v>
       </c>
-      <c r="F24" s="21">
+      <c r="F24" s="22">
         <v>40334</v>
       </c>
-      <c r="G24" s="21">
+      <c r="G24" s="22">
         <v>5.7188370715601895</v>
       </c>
-      <c r="H24" s="21">
+      <c r="H24" s="22">
         <v>2441</v>
       </c>
-      <c r="I24" s="21">
+      <c r="I24" s="22">
         <v>16.100000000000001</v>
       </c>
     </row>
@@ -15520,28 +15597,28 @@
       <c r="A25">
         <v>2018</v>
       </c>
-      <c r="B25" s="21">
+      <c r="B25" s="22">
         <v>71339</v>
       </c>
-      <c r="C25" s="21">
+      <c r="C25" s="22">
         <v>60.899999999999999</v>
       </c>
-      <c r="D25" s="21">
+      <c r="D25" s="22">
         <v>43462</v>
       </c>
-      <c r="E25" s="21">
+      <c r="E25" s="22">
         <v>94.700000000000003</v>
       </c>
-      <c r="F25" s="21">
+      <c r="F25" s="22">
         <v>41160</v>
       </c>
-      <c r="G25" s="21">
+      <c r="G25" s="22">
         <v>5.2999999999999998</v>
       </c>
-      <c r="H25" s="21">
+      <c r="H25" s="22">
         <v>2302</v>
       </c>
-      <c r="I25" s="21">
+      <c r="I25" s="22">
         <v>16.399999999999999</v>
       </c>
     </row>
@@ -15549,28 +15626,28 @@
       <c r="A26">
         <v>2019</v>
       </c>
-      <c r="B26" s="21">
+      <c r="B26" s="22">
         <v>72932</v>
       </c>
-      <c r="C26" s="21">
+      <c r="C26" s="22">
         <v>61.299999999999997</v>
       </c>
-      <c r="D26" s="21">
+      <c r="D26" s="22">
         <v>44692</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E26" s="22">
         <v>94.900000000000006</v>
       </c>
-      <c r="F26" s="21">
+      <c r="F26" s="22">
         <v>42428</v>
       </c>
-      <c r="G26" s="21">
+      <c r="G26" s="22">
         <v>5.0999999999999996</v>
       </c>
-      <c r="H26" s="21">
+      <c r="H26" s="22">
         <v>2264</v>
       </c>
-      <c r="I26" s="21">
+      <c r="I26" s="22">
         <v>13.986046950127273</v>
       </c>
     </row>
@@ -15578,27 +15655,27 @@
       <c r="A27">
         <v>2020</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
     </row>
     <row r="28">
       <c r="A28">
         <v>2021</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
@@ -15624,42 +15701,42 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="B1" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="B4" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="23" t="s">
-        <v>523</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>524</v>
-      </c>
-      <c r="D6" s="23" t="s">
+      <c r="B6" s="24" t="s">
         <v>525</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>526</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="7">
@@ -16074,7 +16151,7 @@
         <v>295</v>
       </c>
       <c r="B62" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="D62" t="s">
         <v>296</v>
@@ -16085,7 +16162,7 @@
         <v>297</v>
       </c>
       <c r="B63" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="D63" t="s">
         <v>298</v>
@@ -16096,7 +16173,7 @@
         <v>299</v>
       </c>
       <c r="B64" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="D64" t="s">
         <v>300</v>
@@ -16107,7 +16184,7 @@
         <v>301</v>
       </c>
       <c r="B65" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="D65" t="s">
         <v>302</v>
@@ -16123,7 +16200,7 @@
         <v>304</v>
       </c>
       <c r="B67" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D67" t="s">
         <v>305</v>
@@ -16134,7 +16211,7 @@
         <v>306</v>
       </c>
       <c r="B68" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="D68" t="s">
         <v>307</v>
@@ -16145,7 +16222,7 @@
         <v>308</v>
       </c>
       <c r="B69" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="D69" t="s">
         <v>309</v>
@@ -16156,7 +16233,7 @@
         <v>310</v>
       </c>
       <c r="B70" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="D70" t="s">
         <v>311</v>
@@ -16175,7 +16252,7 @@
         <v>314</v>
       </c>
       <c r="B72" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="D72" t="s">
         <v>315</v>
@@ -16186,7 +16263,7 @@
         <v>316</v>
       </c>
       <c r="B73" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="D73" t="s">
         <v>317</v>
@@ -16197,7 +16274,7 @@
         <v>318</v>
       </c>
       <c r="B74" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="D74" t="s">
         <v>319</v>
@@ -16208,7 +16285,7 @@
         <v>320</v>
       </c>
       <c r="B75" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="D75" t="s">
         <v>321</v>
@@ -16219,7 +16296,7 @@
         <v>322</v>
       </c>
       <c r="B76" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="C76" t="s">
         <v>323</v>
@@ -16230,7 +16307,7 @@
         <v>324</v>
       </c>
       <c r="B77" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="D77" t="s">
         <v>325</v>
@@ -16241,13 +16318,13 @@
         <v>326</v>
       </c>
       <c r="B78" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="C78" t="s">
         <v>327</v>
       </c>
       <c r="D78" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="79">
@@ -16255,13 +16332,13 @@
         <v>328</v>
       </c>
       <c r="B79" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="C79" t="s">
         <v>329</v>
       </c>
       <c r="D79" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="80">
@@ -16269,13 +16346,13 @@
         <v>330</v>
       </c>
       <c r="B80" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C80" t="s">
         <v>331</v>
       </c>
       <c r="D80" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="81">
@@ -16283,7 +16360,7 @@
         <v>332</v>
       </c>
       <c r="B81" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="C81" t="s">
         <v>333</v>
@@ -16294,13 +16371,13 @@
         <v>334</v>
       </c>
       <c r="B82" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="C82" t="s">
         <v>335</v>
       </c>
       <c r="D82" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
     </row>
     <row r="83">
@@ -16308,13 +16385,13 @@
         <v>336</v>
       </c>
       <c r="B83" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C83" t="s">
         <v>337</v>
       </c>
       <c r="D83" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
     </row>
     <row r="84">
@@ -16322,13 +16399,13 @@
         <v>338</v>
       </c>
       <c r="B84" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="C84" t="s">
         <v>339</v>
       </c>
       <c r="D84" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
     </row>
     <row r="85">
@@ -16336,13 +16413,13 @@
         <v>340</v>
       </c>
       <c r="B85" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="C85" t="s">
         <v>341</v>
       </c>
       <c r="D85" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="86">
@@ -16350,7 +16427,7 @@
         <v>342</v>
       </c>
       <c r="B86" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="C86" t="s">
         <v>343</v>
@@ -16361,13 +16438,13 @@
         <v>344</v>
       </c>
       <c r="B87" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="C87" t="s">
         <v>345</v>
       </c>
       <c r="D87" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
     </row>
     <row r="88">
@@ -16375,13 +16452,13 @@
         <v>346</v>
       </c>
       <c r="B88" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="C88" t="s">
         <v>347</v>
       </c>
       <c r="D88" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="89">
@@ -16389,13 +16466,13 @@
         <v>348</v>
       </c>
       <c r="B89" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="C89" t="s">
         <v>349</v>
       </c>
       <c r="D89" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
     </row>
     <row r="90">
@@ -16403,13 +16480,13 @@
         <v>350</v>
       </c>
       <c r="B90" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="C90" t="s">
         <v>351</v>
       </c>
       <c r="D90" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="91">
@@ -16417,7 +16494,7 @@
         <v>352</v>
       </c>
       <c r="B91" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="C91" t="s">
         <v>353</v>
@@ -16428,13 +16505,13 @@
         <v>354</v>
       </c>
       <c r="B92" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="C92" t="s">
         <v>355</v>
       </c>
       <c r="D92" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
     </row>
     <row r="93">
@@ -16442,13 +16519,13 @@
         <v>356</v>
       </c>
       <c r="B93" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="C93" t="s">
         <v>357</v>
       </c>
       <c r="D93" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="94">
@@ -16456,13 +16533,13 @@
         <v>358</v>
       </c>
       <c r="B94" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="C94" t="s">
         <v>359</v>
       </c>
       <c r="D94" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="95">
@@ -16470,13 +16547,13 @@
         <v>360</v>
       </c>
       <c r="B95" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="C95" t="s">
         <v>361</v>
       </c>
       <c r="D95" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="96">
@@ -16484,7 +16561,7 @@
         <v>362</v>
       </c>
       <c r="B96" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="C96" t="s">
         <v>363</v>
@@ -16495,13 +16572,13 @@
         <v>364</v>
       </c>
       <c r="B97" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="C97" t="s">
         <v>365</v>
       </c>
       <c r="D97" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="98">
@@ -16509,13 +16586,13 @@
         <v>366</v>
       </c>
       <c r="B98" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="C98" t="s">
         <v>367</v>
       </c>
       <c r="D98" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="99">
@@ -16523,13 +16600,13 @@
         <v>368</v>
       </c>
       <c r="B99" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="C99" t="s">
         <v>369</v>
       </c>
       <c r="D99" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="100">
@@ -16537,13 +16614,13 @@
         <v>370</v>
       </c>
       <c r="B100" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="C100" t="s">
         <v>371</v>
       </c>
       <c r="D100" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="101">
@@ -16551,7 +16628,7 @@
         <v>372</v>
       </c>
       <c r="B101" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="C101" t="s">
         <v>373</v>
@@ -16562,13 +16639,13 @@
         <v>374</v>
       </c>
       <c r="B102" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="C102" t="s">
         <v>375</v>
       </c>
       <c r="D102" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
     </row>
     <row r="103">
@@ -16576,13 +16653,13 @@
         <v>376</v>
       </c>
       <c r="B103" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="C103" t="s">
         <v>377</v>
       </c>
       <c r="D103" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
     </row>
     <row r="104">
@@ -16590,13 +16667,13 @@
         <v>379</v>
       </c>
       <c r="B104" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="C104" t="s">
         <v>380</v>
       </c>
       <c r="D104" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
     </row>
     <row r="105">
@@ -16604,13 +16681,13 @@
         <v>381</v>
       </c>
       <c r="B105" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="C105" t="s">
         <v>382</v>
       </c>
       <c r="D105" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="106">
@@ -16618,7 +16695,7 @@
         <v>383</v>
       </c>
       <c r="B106" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="C106" t="s">
         <v>384</v>
@@ -16629,13 +16706,13 @@
         <v>385</v>
       </c>
       <c r="B107" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C107" t="s">
         <v>386</v>
       </c>
       <c r="D107" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
     </row>
     <row r="108">
@@ -16643,13 +16720,13 @@
         <v>387</v>
       </c>
       <c r="B108" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="C108" t="s">
         <v>388</v>
       </c>
       <c r="D108" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
     </row>
     <row r="109">
@@ -16657,13 +16734,13 @@
         <v>389</v>
       </c>
       <c r="B109" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="C109" t="s">
         <v>390</v>
       </c>
       <c r="D109" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
     </row>
     <row r="110">
@@ -16671,13 +16748,13 @@
         <v>391</v>
       </c>
       <c r="B110" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="C110" t="s">
         <v>392</v>
       </c>
       <c r="D110" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
     </row>
     <row r="111">
@@ -16685,7 +16762,7 @@
         <v>393</v>
       </c>
       <c r="B111" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="C111" t="s">
         <v>394</v>
@@ -16696,13 +16773,13 @@
         <v>395</v>
       </c>
       <c r="B112" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="C112" t="s">
         <v>396</v>
       </c>
       <c r="D112" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
     </row>
     <row r="113">
@@ -16710,13 +16787,13 @@
         <v>397</v>
       </c>
       <c r="B113" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="C113" t="s">
         <v>398</v>
       </c>
       <c r="D113" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
     </row>
     <row r="114">
@@ -16724,13 +16801,13 @@
         <v>399</v>
       </c>
       <c r="B114" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="C114" t="s">
         <v>400</v>
       </c>
       <c r="D114" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
     </row>
     <row r="115">
@@ -16738,13 +16815,13 @@
         <v>401</v>
       </c>
       <c r="B115" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="C115" t="s">
         <v>402</v>
       </c>
       <c r="D115" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
     </row>
     <row r="116">
@@ -16752,7 +16829,7 @@
         <v>403</v>
       </c>
       <c r="B116" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="C116" t="s">
         <v>404</v>
@@ -16763,13 +16840,13 @@
         <v>405</v>
       </c>
       <c r="B117" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="C117" t="s">
         <v>406</v>
       </c>
       <c r="D117" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
     </row>
     <row r="118">
@@ -16777,13 +16854,13 @@
         <v>407</v>
       </c>
       <c r="B118" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="C118" t="s">
         <v>408</v>
       </c>
       <c r="D118" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
     </row>
     <row r="119">
@@ -16791,13 +16868,13 @@
         <v>409</v>
       </c>
       <c r="B119" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="C119" t="s">
         <v>410</v>
       </c>
       <c r="D119" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="120">
@@ -16805,13 +16882,13 @@
         <v>411</v>
       </c>
       <c r="B120" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="C120" t="s">
         <v>412</v>
       </c>
       <c r="D120" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
     </row>
     <row r="121">
@@ -16819,7 +16896,7 @@
         <v>413</v>
       </c>
       <c r="B121" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="C121" t="s">
         <v>414</v>
@@ -16830,13 +16907,13 @@
         <v>415</v>
       </c>
       <c r="B122" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="C122" t="s">
         <v>416</v>
       </c>
       <c r="D122" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
     </row>
     <row r="123">
@@ -16844,13 +16921,13 @@
         <v>418</v>
       </c>
       <c r="B123" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="C123" t="s">
         <v>419</v>
       </c>
       <c r="D123" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
     </row>
     <row r="124">
@@ -16858,13 +16935,13 @@
         <v>420</v>
       </c>
       <c r="B124" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="C124" t="s">
         <v>421</v>
       </c>
       <c r="D124" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
     </row>
     <row r="125">
@@ -16872,13 +16949,13 @@
         <v>422</v>
       </c>
       <c r="B125" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="C125" t="s">
         <v>423</v>
       </c>
       <c r="D125" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
     </row>
     <row r="126">
@@ -16945,7 +17022,7 @@
         <v>445</v>
       </c>
       <c r="D133" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
     </row>
     <row r="134">
@@ -17117,7 +17194,7 @@
       <c r="A155" s="1" t="s">
         <v>493</v>
       </c>
-      <c r="B155" s="24" t="s">
+      <c r="B155" s="20" t="s">
         <v>494</v>
       </c>
     </row>
@@ -17133,7 +17210,7 @@
       <c r="A157" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="B157" s="24" t="s">
+      <c r="B157" s="20" t="s">
         <v>498</v>
       </c>
     </row>
@@ -17141,7 +17218,7 @@
       <c r="A158" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="B158" s="24" t="s">
+      <c r="B158" s="20" t="s">
         <v>500</v>
       </c>
     </row>
@@ -17149,7 +17226,7 @@
       <c r="A159" s="1" t="s">
         <v>501</v>
       </c>
-      <c r="B159" s="24" t="s">
+      <c r="B159" s="20" t="s">
         <v>502</v>
       </c>
     </row>
@@ -17157,30 +17234,36 @@
       <c r="A160" s="1" t="s">
         <v>503</v>
       </c>
+      <c r="B160" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="s">
-        <v>504</v>
+        <v>505</v>
+      </c>
+      <c r="B161" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
   </sheetData>
@@ -17205,59 +17288,59 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="B1" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="B2" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="B3" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="B4" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="B5" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="C8" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="D8" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="E8" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="F8" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
Monthly labor update - Oct to Nov 2023
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="642">
   <si>
     <t xml:space="preserve">LFS Round</t>
   </si>
@@ -1542,7 +1542,13 @@
     <t xml:space="preserve">2023 Oct</t>
   </si>
   <si>
+    <t>https://psa.gov.ph/content/employment-rate-october-2023-was-estimated-958-percent</t>
+  </si>
+  <si>
     <t xml:space="preserve">2023 Nov</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/unemployment-rate-november-2023-was-estimated-36-percent</t>
   </si>
   <si>
     <t xml:space="preserve">2023 Dec</t>
@@ -12727,7 +12733,7 @@
         <v>32</v>
       </c>
       <c r="F230" s="11">
-        <f t="shared" ref="F230:G267" si="23">K230/J230</f>
+        <f t="shared" ref="F230:G269" si="23">K230/J230</f>
         <v>0.6168840849278201</v>
       </c>
       <c r="G230" s="11">
@@ -12735,11 +12741,11 @@
         <v>0.94678254834076803</v>
       </c>
       <c r="H230" s="11">
-        <f t="shared" ref="H230:H267" si="25">M230/K230</f>
+        <f t="shared" ref="H230:H269" si="25">M230/K230</f>
         <v>0.053217451659231869</v>
       </c>
       <c r="I230" s="11">
-        <f t="shared" ref="I230:I267" si="26">O230/L230</f>
+        <f t="shared" ref="I230:I269" si="26">O230/L230</f>
         <v>0.14805990963342192</v>
       </c>
       <c r="J230" s="12">
@@ -12963,7 +12969,7 @@
         <v>4500.7385000000004</v>
       </c>
       <c r="N234" s="2">
-        <f t="shared" ref="N230:N266" si="27">J234-K234</f>
+        <f t="shared" ref="N230:N269" si="27">J234-K234</f>
         <v>29852.987999999998</v>
       </c>
       <c r="O234" s="2">
@@ -14140,43 +14146,41 @@
       <c r="D257" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E257" s="1" t="s">
-        <v>425</v>
-      </c>
+      <c r="E257" s="1"/>
       <c r="F257" s="3">
         <f t="shared" si="23"/>
-        <v>0.64150515020588861</v>
+        <v>0.64137679304591599</v>
       </c>
       <c r="G257" s="3">
         <f t="shared" si="23"/>
-        <v>0.95457810864448256</v>
+        <v>0.95457282741668548</v>
       </c>
       <c r="H257" s="3">
         <f t="shared" si="25"/>
-        <v>0.045421891355517427</v>
+        <v>0.045427192866344689</v>
       </c>
       <c r="I257" s="3">
         <f t="shared" si="26"/>
-        <v>0.14165943993595939</v>
+        <v>0.14168495116529178</v>
       </c>
       <c r="J257" s="2">
-        <v>76925.080000000002</v>
+        <v>76869.475999999995</v>
       </c>
       <c r="K257" s="2">
-        <v>49347.834999999999</v>
+        <v>49302.298000000003</v>
       </c>
       <c r="L257" s="2">
-        <v>47106.362999999998</v>
+        <v>47062.633999999998</v>
       </c>
       <c r="M257" s="2">
-        <v>2241.4720000000002</v>
+        <v>2239.665</v>
       </c>
       <c r="N257" s="2">
         <f t="shared" si="27"/>
-        <v>27577.245000000003</v>
+        <v>27567.177999999993</v>
       </c>
       <c r="O257" s="2">
-        <v>6673.0609999999997</v>
+        <v>6668.067</v>
       </c>
       <c r="P257" t="s">
         <v>482</v>
@@ -14195,43 +14199,41 @@
       <c r="D258" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E258" s="1" t="s">
-        <v>425</v>
-      </c>
+      <c r="E258" s="1"/>
       <c r="F258" s="3">
         <f t="shared" si="23"/>
-        <v>0.67455240427974039</v>
+        <v>0.6745385967197346</v>
       </c>
       <c r="G258" s="3">
         <f t="shared" si="23"/>
-        <v>0.95804382818007605</v>
+        <v>0.95804296935248212</v>
       </c>
       <c r="H258" s="3">
         <f t="shared" si="25"/>
-        <v>0.041956171819923928</v>
+        <v>0.041957030647517823</v>
       </c>
       <c r="I258" s="3">
         <f t="shared" si="26"/>
-        <v>0.14407099218100131</v>
+        <v>0.14404123664299703</v>
       </c>
       <c r="J258" s="2">
         <v>76914.385999999999</v>
       </c>
       <c r="K258" s="2">
-        <v>51882.784</v>
+        <v>51881.722000000002</v>
       </c>
       <c r="L258" s="2">
-        <v>49705.981</v>
+        <v>49704.919000000002</v>
       </c>
       <c r="M258" s="2">
         <v>2176.8029999999999</v>
       </c>
       <c r="N258" s="2">
         <f t="shared" si="27"/>
-        <v>25031.601999999999</v>
+        <v>25032.663999999997</v>
       </c>
       <c r="O258" s="2">
-        <v>7161.1899999999996</v>
+        <v>7159.558</v>
       </c>
       <c r="P258" t="s">
         <v>484</v>
@@ -14330,7 +14332,7 @@
         <v>0.6448960129797745</v>
       </c>
       <c r="G261" s="3">
-        <f t="shared" ref="G261:G267" si="28">L261/K261</f>
+        <f t="shared" ref="G261:G269" si="28">L261/K261</f>
         <v>0.95227963685377781</v>
       </c>
       <c r="H261" s="3">
@@ -14684,7 +14686,7 @@
         <v>2273.3850000000002</v>
       </c>
       <c r="N267" s="2">
-        <f>J267-K267</f>
+        <f t="shared" si="27"/>
         <v>31147.398000000001</v>
       </c>
       <c r="O267" s="2">
@@ -14711,19 +14713,19 @@
         <v>425</v>
       </c>
       <c r="F268" s="3">
-        <f>K268/J268</f>
+        <f t="shared" si="23"/>
         <v>0.64650853861229718</v>
       </c>
       <c r="G268" s="3">
-        <f>L268/K268</f>
+        <f t="shared" si="28"/>
         <v>0.95597557716757331</v>
       </c>
       <c r="H268" s="3">
-        <f>M268/K268</f>
+        <f t="shared" si="25"/>
         <v>0.044024422832426691</v>
       </c>
       <c r="I268" s="3">
-        <f>O268/L268</f>
+        <f t="shared" si="26"/>
         <v>0.11711656128289734</v>
       </c>
       <c r="J268" s="2">
@@ -14739,7 +14741,7 @@
         <v>2213.8580000000002</v>
       </c>
       <c r="N268" s="2">
-        <f>J268-K268</f>
+        <f t="shared" si="27"/>
         <v>27495.444999999992</v>
       </c>
       <c r="O268" s="2">
@@ -14766,19 +14768,19 @@
         <v>425</v>
       </c>
       <c r="F269" s="3">
-        <f>K269/J269</f>
+        <f t="shared" si="23"/>
         <v>0.64049609363750415</v>
       </c>
       <c r="G269" s="3">
-        <f>L269/K269</f>
+        <f t="shared" si="28"/>
         <v>0.9546663534776707</v>
       </c>
       <c r="H269" s="3">
-        <f>M269/K269</f>
+        <f t="shared" si="25"/>
         <v>0.045333646522329352</v>
       </c>
       <c r="I269" s="3">
-        <f>O269/L269</f>
+        <f t="shared" si="26"/>
         <v>0.10725448980279445</v>
       </c>
       <c r="J269" s="2">
@@ -14794,7 +14796,7 @@
         <v>2263.4810000000002</v>
       </c>
       <c r="N269" s="2">
-        <f>J269-K269</f>
+        <f t="shared" si="27"/>
         <v>28024.851999999999</v>
       </c>
       <c r="O269" s="2">
@@ -14820,11 +14822,48 @@
       <c r="E270" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="O270" s="2"/>
+      <c r="F270" s="3">
+        <f>K270/J270</f>
+        <v>0.63948145527591993</v>
+      </c>
+      <c r="G270" s="3">
+        <f>L270/K270</f>
+        <v>0.95811114232113281</v>
+      </c>
+      <c r="H270" s="3">
+        <f>M270/K270</f>
+        <v>0.041888877722409047</v>
+      </c>
+      <c r="I270" s="3">
+        <f>O270/L270</f>
+        <v>0.11711953156940362</v>
+      </c>
+      <c r="J270" s="2">
+        <v>78018.497000000003</v>
+      </c>
+      <c r="K270" s="2">
+        <v>49891.381999999998</v>
+      </c>
+      <c r="L270" s="2">
+        <v>47801.489000000001</v>
+      </c>
+      <c r="M270" s="2">
+        <v>2089.8939999999998</v>
+      </c>
+      <c r="N270" s="2">
+        <f>J270-K270</f>
+        <v>28127.115000000005</v>
+      </c>
+      <c r="O270" s="2">
+        <v>5598.4880000000003</v>
+      </c>
+      <c r="P270" t="s">
+        <v>508</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>489</v>
@@ -14838,11 +14877,48 @@
       <c r="E271" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="O271" s="2"/>
+      <c r="F271" s="3">
+        <f>K271/J271</f>
+        <v>0.65894503512117253</v>
+      </c>
+      <c r="G271" s="3">
+        <f>L271/K271</f>
+        <v>0.96437912074012655</v>
+      </c>
+      <c r="H271" s="3">
+        <f>M271/K271</f>
+        <v>0.035620879259873485</v>
+      </c>
+      <c r="I271" s="3">
+        <f>O271/L271</f>
+        <v>0.11658680306005918</v>
+      </c>
+      <c r="J271" s="2">
+        <v>78107.585999999996</v>
+      </c>
+      <c r="K271" s="2">
+        <v>51468.606</v>
+      </c>
+      <c r="L271" s="2">
+        <v>49635.249000000003</v>
+      </c>
+      <c r="M271" s="2">
+        <v>1833.357</v>
+      </c>
+      <c r="N271" s="2">
+        <f>J271-K271</f>
+        <v>26638.979999999996</v>
+      </c>
+      <c r="O271" s="2">
+        <v>5786.8149999999996</v>
+      </c>
+      <c r="P271" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>489</v>
@@ -14860,7 +14936,7 @@
     </row>
     <row r="273">
       <c r="A273" s="1" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>489</v>
@@ -14902,28 +14978,28 @@
         <v>1</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
     </row>
     <row r="2">
@@ -15701,28 +15777,28 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="B1" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="B4" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
     </row>
     <row r="6">
@@ -15730,13 +15806,13 @@
         <v>0</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
     </row>
     <row r="7">
@@ -16151,7 +16227,7 @@
         <v>295</v>
       </c>
       <c r="B62" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="D62" t="s">
         <v>296</v>
@@ -16162,7 +16238,7 @@
         <v>297</v>
       </c>
       <c r="B63" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="D63" t="s">
         <v>298</v>
@@ -16173,7 +16249,7 @@
         <v>299</v>
       </c>
       <c r="B64" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D64" t="s">
         <v>300</v>
@@ -16184,7 +16260,7 @@
         <v>301</v>
       </c>
       <c r="B65" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="D65" t="s">
         <v>302</v>
@@ -16200,7 +16276,7 @@
         <v>304</v>
       </c>
       <c r="B67" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="D67" t="s">
         <v>305</v>
@@ -16211,7 +16287,7 @@
         <v>306</v>
       </c>
       <c r="B68" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="D68" t="s">
         <v>307</v>
@@ -16222,7 +16298,7 @@
         <v>308</v>
       </c>
       <c r="B69" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="D69" t="s">
         <v>309</v>
@@ -16233,7 +16309,7 @@
         <v>310</v>
       </c>
       <c r="B70" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="D70" t="s">
         <v>311</v>
@@ -16252,7 +16328,7 @@
         <v>314</v>
       </c>
       <c r="B72" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="D72" t="s">
         <v>315</v>
@@ -16263,7 +16339,7 @@
         <v>316</v>
       </c>
       <c r="B73" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="D73" t="s">
         <v>317</v>
@@ -16274,7 +16350,7 @@
         <v>318</v>
       </c>
       <c r="B74" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="D74" t="s">
         <v>319</v>
@@ -16285,7 +16361,7 @@
         <v>320</v>
       </c>
       <c r="B75" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="D75" t="s">
         <v>321</v>
@@ -16296,7 +16372,7 @@
         <v>322</v>
       </c>
       <c r="B76" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="C76" t="s">
         <v>323</v>
@@ -16307,7 +16383,7 @@
         <v>324</v>
       </c>
       <c r="B77" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="D77" t="s">
         <v>325</v>
@@ -16318,13 +16394,13 @@
         <v>326</v>
       </c>
       <c r="B78" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="C78" t="s">
         <v>327</v>
       </c>
       <c r="D78" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
     </row>
     <row r="79">
@@ -16332,13 +16408,13 @@
         <v>328</v>
       </c>
       <c r="B79" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C79" t="s">
         <v>329</v>
       </c>
       <c r="D79" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
     </row>
     <row r="80">
@@ -16346,13 +16422,13 @@
         <v>330</v>
       </c>
       <c r="B80" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="C80" t="s">
         <v>331</v>
       </c>
       <c r="D80" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
     </row>
     <row r="81">
@@ -16360,7 +16436,7 @@
         <v>332</v>
       </c>
       <c r="B81" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="C81" t="s">
         <v>333</v>
@@ -16371,13 +16447,13 @@
         <v>334</v>
       </c>
       <c r="B82" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="C82" t="s">
         <v>335</v>
       </c>
       <c r="D82" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
     </row>
     <row r="83">
@@ -16385,13 +16461,13 @@
         <v>336</v>
       </c>
       <c r="B83" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="C83" t="s">
         <v>337</v>
       </c>
       <c r="D83" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
     </row>
     <row r="84">
@@ -16399,13 +16475,13 @@
         <v>338</v>
       </c>
       <c r="B84" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="C84" t="s">
         <v>339</v>
       </c>
       <c r="D84" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
     </row>
     <row r="85">
@@ -16413,13 +16489,13 @@
         <v>340</v>
       </c>
       <c r="B85" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="C85" t="s">
         <v>341</v>
       </c>
       <c r="D85" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
     </row>
     <row r="86">
@@ -16427,7 +16503,7 @@
         <v>342</v>
       </c>
       <c r="B86" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="C86" t="s">
         <v>343</v>
@@ -16438,13 +16514,13 @@
         <v>344</v>
       </c>
       <c r="B87" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="C87" t="s">
         <v>345</v>
       </c>
       <c r="D87" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
     </row>
     <row r="88">
@@ -16452,13 +16528,13 @@
         <v>346</v>
       </c>
       <c r="B88" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="C88" t="s">
         <v>347</v>
       </c>
       <c r="D88" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
     </row>
     <row r="89">
@@ -16466,13 +16542,13 @@
         <v>348</v>
       </c>
       <c r="B89" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="C89" t="s">
         <v>349</v>
       </c>
       <c r="D89" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
     </row>
     <row r="90">
@@ -16480,13 +16556,13 @@
         <v>350</v>
       </c>
       <c r="B90" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="C90" t="s">
         <v>351</v>
       </c>
       <c r="D90" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
     </row>
     <row r="91">
@@ -16494,7 +16570,7 @@
         <v>352</v>
       </c>
       <c r="B91" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="C91" t="s">
         <v>353</v>
@@ -16505,13 +16581,13 @@
         <v>354</v>
       </c>
       <c r="B92" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="C92" t="s">
         <v>355</v>
       </c>
       <c r="D92" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
     </row>
     <row r="93">
@@ -16519,13 +16595,13 @@
         <v>356</v>
       </c>
       <c r="B93" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="C93" t="s">
         <v>357</v>
       </c>
       <c r="D93" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
     </row>
     <row r="94">
@@ -16533,13 +16609,13 @@
         <v>358</v>
       </c>
       <c r="B94" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="C94" t="s">
         <v>359</v>
       </c>
       <c r="D94" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="95">
@@ -16547,13 +16623,13 @@
         <v>360</v>
       </c>
       <c r="B95" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
       <c r="C95" t="s">
         <v>361</v>
       </c>
       <c r="D95" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="96">
@@ -16561,7 +16637,7 @@
         <v>362</v>
       </c>
       <c r="B96" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="C96" t="s">
         <v>363</v>
@@ -16572,13 +16648,13 @@
         <v>364</v>
       </c>
       <c r="B97" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="C97" t="s">
         <v>365</v>
       </c>
       <c r="D97" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="98">
@@ -16586,13 +16662,13 @@
         <v>366</v>
       </c>
       <c r="B98" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="C98" t="s">
         <v>367</v>
       </c>
       <c r="D98" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
     </row>
     <row r="99">
@@ -16600,13 +16676,13 @@
         <v>368</v>
       </c>
       <c r="B99" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="C99" t="s">
         <v>369</v>
       </c>
       <c r="D99" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
     </row>
     <row r="100">
@@ -16614,13 +16690,13 @@
         <v>370</v>
       </c>
       <c r="B100" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="C100" t="s">
         <v>371</v>
       </c>
       <c r="D100" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
     </row>
     <row r="101">
@@ -16628,7 +16704,7 @@
         <v>372</v>
       </c>
       <c r="B101" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="C101" t="s">
         <v>373</v>
@@ -16639,13 +16715,13 @@
         <v>374</v>
       </c>
       <c r="B102" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="C102" t="s">
         <v>375</v>
       </c>
       <c r="D102" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
     </row>
     <row r="103">
@@ -16653,13 +16729,13 @@
         <v>376</v>
       </c>
       <c r="B103" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="C103" t="s">
         <v>377</v>
       </c>
       <c r="D103" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
     </row>
     <row r="104">
@@ -16667,13 +16743,13 @@
         <v>379</v>
       </c>
       <c r="B104" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="C104" t="s">
         <v>380</v>
       </c>
       <c r="D104" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="105">
@@ -16681,13 +16757,13 @@
         <v>381</v>
       </c>
       <c r="B105" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="C105" t="s">
         <v>382</v>
       </c>
       <c r="D105" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
     </row>
     <row r="106">
@@ -16695,7 +16771,7 @@
         <v>383</v>
       </c>
       <c r="B106" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="C106" t="s">
         <v>384</v>
@@ -16706,13 +16782,13 @@
         <v>385</v>
       </c>
       <c r="B107" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="C107" t="s">
         <v>386</v>
       </c>
       <c r="D107" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
     </row>
     <row r="108">
@@ -16720,13 +16796,13 @@
         <v>387</v>
       </c>
       <c r="B108" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="C108" t="s">
         <v>388</v>
       </c>
       <c r="D108" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
     </row>
     <row r="109">
@@ -16734,13 +16810,13 @@
         <v>389</v>
       </c>
       <c r="B109" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="C109" t="s">
         <v>390</v>
       </c>
       <c r="D109" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
     </row>
     <row r="110">
@@ -16748,13 +16824,13 @@
         <v>391</v>
       </c>
       <c r="B110" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="C110" t="s">
         <v>392</v>
       </c>
       <c r="D110" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
     </row>
     <row r="111">
@@ -16762,7 +16838,7 @@
         <v>393</v>
       </c>
       <c r="B111" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="C111" t="s">
         <v>394</v>
@@ -16773,13 +16849,13 @@
         <v>395</v>
       </c>
       <c r="B112" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="C112" t="s">
         <v>396</v>
       </c>
       <c r="D112" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
     </row>
     <row r="113">
@@ -16787,13 +16863,13 @@
         <v>397</v>
       </c>
       <c r="B113" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="C113" t="s">
         <v>398</v>
       </c>
       <c r="D113" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
     </row>
     <row r="114">
@@ -16801,13 +16877,13 @@
         <v>399</v>
       </c>
       <c r="B114" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="C114" t="s">
         <v>400</v>
       </c>
       <c r="D114" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
     </row>
     <row r="115">
@@ -16815,13 +16891,13 @@
         <v>401</v>
       </c>
       <c r="B115" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="C115" t="s">
         <v>402</v>
       </c>
       <c r="D115" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
     </row>
     <row r="116">
@@ -16829,7 +16905,7 @@
         <v>403</v>
       </c>
       <c r="B116" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="C116" t="s">
         <v>404</v>
@@ -16840,13 +16916,13 @@
         <v>405</v>
       </c>
       <c r="B117" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="C117" t="s">
         <v>406</v>
       </c>
       <c r="D117" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
     </row>
     <row r="118">
@@ -16854,13 +16930,13 @@
         <v>407</v>
       </c>
       <c r="B118" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
       <c r="C118" t="s">
         <v>408</v>
       </c>
       <c r="D118" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
     </row>
     <row r="119">
@@ -16868,13 +16944,13 @@
         <v>409</v>
       </c>
       <c r="B119" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="C119" t="s">
         <v>410</v>
       </c>
       <c r="D119" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
     </row>
     <row r="120">
@@ -16882,13 +16958,13 @@
         <v>411</v>
       </c>
       <c r="B120" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="C120" t="s">
         <v>412</v>
       </c>
       <c r="D120" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
     </row>
     <row r="121">
@@ -16896,7 +16972,7 @@
         <v>413</v>
       </c>
       <c r="B121" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="C121" t="s">
         <v>414</v>
@@ -16907,13 +16983,13 @@
         <v>415</v>
       </c>
       <c r="B122" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="C122" t="s">
         <v>416</v>
       </c>
       <c r="D122" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
     </row>
     <row r="123">
@@ -16921,13 +16997,13 @@
         <v>418</v>
       </c>
       <c r="B123" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="C123" t="s">
         <v>419</v>
       </c>
       <c r="D123" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
     </row>
     <row r="124">
@@ -16935,13 +17011,13 @@
         <v>420</v>
       </c>
       <c r="B124" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="C124" t="s">
         <v>421</v>
       </c>
       <c r="D124" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
     </row>
     <row r="125">
@@ -16949,13 +17025,13 @@
         <v>422</v>
       </c>
       <c r="B125" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="C125" t="s">
         <v>423</v>
       </c>
       <c r="D125" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
     </row>
     <row r="126">
@@ -17022,7 +17098,7 @@
         <v>445</v>
       </c>
       <c r="D133" t="s">
-        <v>629</v>
+        <v>631</v>
       </c>
     </row>
     <row r="134">
@@ -17250,20 +17326,26 @@
       <c r="A162" s="1" t="s">
         <v>507</v>
       </c>
+      <c r="B162" s="20" t="s">
+        <v>508</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="s">
-        <v>508</v>
+        <v>509</v>
+      </c>
+      <c r="B163" s="20" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
     </row>
   </sheetData>
@@ -17288,59 +17370,59 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="B1" t="s">
-        <v>631</v>
+        <v>633</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="B2" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="B3" t="s">
-        <v>635</v>
+        <v>637</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="B4" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="B5" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="C8" t="s">
-        <v>632</v>
+        <v>634</v>
       </c>
       <c r="D8" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="E8" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="F8" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
Monthly labor update - Jan 2024
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD00CD78-7112-4D03-9355-ACB84DC438D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F21BBE0-A023-48FB-BE0B-472B14694240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="2100" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1649" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="658">
   <si>
     <t>LFS Round</t>
   </si>
@@ -1965,6 +1965,51 @@
   </si>
   <si>
     <t>https://psa.gov.ph/content/unemployment-rate-december-2023-was-estimated-31-percent</t>
+  </si>
+  <si>
+    <t>2024 Jan</t>
+  </si>
+  <si>
+    <t>2024 Feb</t>
+  </si>
+  <si>
+    <t>2024 Mar</t>
+  </si>
+  <si>
+    <t>2024 Apr</t>
+  </si>
+  <si>
+    <t>2024 May</t>
+  </si>
+  <si>
+    <t>2024 Jun</t>
+  </si>
+  <si>
+    <t>2024 Jul</t>
+  </si>
+  <si>
+    <t>2024 Aug</t>
+  </si>
+  <si>
+    <t>2024 Sep</t>
+  </si>
+  <si>
+    <t>2024 Oct</t>
+  </si>
+  <si>
+    <t>2024 Nov</t>
+  </si>
+  <si>
+    <t>2024 Dec</t>
+  </si>
+  <si>
+    <t>2024 Annual</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/employment-rate-january-2024-was-estimated-955-percent</t>
+  </si>
+  <si>
+    <t>2024</t>
   </si>
 </sst>
 </file>
@@ -2306,14 +2351,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P273"/>
+  <dimension ref="A1:P286"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="I260" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D257" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F263" sqref="F263"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O273" sqref="O273"/>
+      <selection pane="bottomRight" activeCell="F275" sqref="F275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14062,43 +14107,40 @@
       <c r="D261" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E261" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F261" s="3">
         <f t="shared" si="23"/>
-        <v>0.6448960129797745</v>
+        <v>0.64496706057503939</v>
       </c>
       <c r="G261" s="3">
         <f t="shared" ref="G261:G269" si="28">L261/K261</f>
-        <v>0.95227963685377781</v>
+        <v>0.95217877356047176</v>
       </c>
       <c r="H261" s="3">
         <f t="shared" si="25"/>
-        <v>4.7720383257059969E-2</v>
+        <v>4.7821206330903025E-2</v>
       </c>
       <c r="I261" s="3">
         <f t="shared" si="26"/>
-        <v>0.14053252516574691</v>
+        <v>0.14053308980559728</v>
       </c>
       <c r="J261" s="2">
-        <v>77104.574999999997</v>
+        <v>77104.563999999998</v>
       </c>
       <c r="K261" s="2">
-        <v>49724.432999999997</v>
+        <v>49729.904000000002</v>
       </c>
       <c r="L261" s="2">
-        <v>47351.565000000002</v>
+        <v>47351.758999999998</v>
       </c>
       <c r="M261" s="2">
-        <v>2372.8690000000001</v>
+        <v>2378.1439999999998</v>
       </c>
       <c r="N261" s="2">
         <f t="shared" si="27"/>
-        <v>27380.142</v>
+        <v>27374.659999999996</v>
       </c>
       <c r="O261" s="2">
-        <v>6654.4350000000004</v>
+        <v>6654.4889999999996</v>
       </c>
       <c r="P261" t="s">
         <v>490</v>
@@ -14561,11 +14603,11 @@
         <v>425</v>
       </c>
       <c r="F270" s="3">
-        <f>K270/J270</f>
+        <f t="shared" ref="F270:G272" si="29">K270/J270</f>
         <v>0.63948145527591993</v>
       </c>
       <c r="G270" s="3">
-        <f>L270/K270</f>
+        <f t="shared" si="29"/>
         <v>0.95811114232113281</v>
       </c>
       <c r="H270" s="3">
@@ -14616,11 +14658,11 @@
         <v>425</v>
       </c>
       <c r="F271" s="3">
-        <f>K271/J271</f>
+        <f t="shared" si="29"/>
         <v>0.65894503512117253</v>
       </c>
       <c r="G271" s="3">
-        <f>L271/K271</f>
+        <f t="shared" si="29"/>
         <v>0.96437912074012655</v>
       </c>
       <c r="H271" s="3">
@@ -14671,11 +14713,11 @@
         <v>425</v>
       </c>
       <c r="F272" s="3">
-        <f>K272/J272</f>
+        <f t="shared" si="29"/>
         <v>0.66648310129709132</v>
       </c>
       <c r="G272" s="3">
-        <f>L272/K272</f>
+        <f t="shared" si="29"/>
         <v>0.96926281261604486</v>
       </c>
       <c r="H272" s="3">
@@ -14709,7 +14751,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="273" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>512</v>
       </c>
@@ -14726,6 +14768,265 @@
         <v>425</v>
       </c>
       <c r="O273" s="2"/>
+    </row>
+    <row r="274" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A274" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="B274" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D274" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E274" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F274" s="3">
+        <f t="shared" ref="F274" si="30">K274/J274</f>
+        <v>0.6114444374307062</v>
+      </c>
+      <c r="G274" s="3">
+        <f t="shared" ref="G274" si="31">L274/K274</f>
+        <v>0.95528747408394488</v>
+      </c>
+      <c r="H274" s="3">
+        <f>M274/K274</f>
+        <v>4.4712525916055137E-2</v>
+      </c>
+      <c r="I274" s="3">
+        <f>O274/L274</f>
+        <v>0.13917804379986054</v>
+      </c>
+      <c r="J274" s="2">
+        <v>78655.154999999999</v>
+      </c>
+      <c r="K274" s="2">
+        <v>48093.256999999998</v>
+      </c>
+      <c r="L274" s="2">
+        <v>45942.885999999999</v>
+      </c>
+      <c r="M274" s="2">
+        <v>2150.3710000000001</v>
+      </c>
+      <c r="N274" s="2">
+        <f>J274-K274</f>
+        <v>30561.898000000001</v>
+      </c>
+      <c r="O274" s="2">
+        <v>6394.241</v>
+      </c>
+      <c r="P274" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="275" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A275" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="D275" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E275" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="276" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A276" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D276" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E276" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="277" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A277" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D277" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E277" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="278" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A278" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D278" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E278" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="279" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A279" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="D279" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E279" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="280" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A280" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D280" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E280" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="281" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A281" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D281" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E281" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="282" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A282" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D282" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E282" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="283" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A283" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E283" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="284" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A284" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D284" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E284" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="285" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A285" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="D285" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E285" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="286" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A286" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D286" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E286" s="1" t="s">
+        <v>425</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14737,12 +15038,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15583,14 +15884,14 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D165"/>
+  <dimension ref="A1:D178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B154" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B161" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B153" sqref="B153"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B164" sqref="B164"/>
+      <selection pane="bottomRight" activeCell="B166" sqref="B166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17173,6 +17474,74 @@
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>512</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="B166" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>655</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Monthly labor update - Feb 2024
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F21BBE0-A023-48FB-BE0B-472B14694240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADE6CDD-C142-4B6A-B547-22E79C5858F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4935" yWindow="2280" windowWidth="11130" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="659">
   <si>
     <t>LFS Round</t>
   </si>
@@ -2010,6 +2010,9 @@
   </si>
   <si>
     <t>2024</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/unemployment-rate-february-2024-was-estimated-35-percent</t>
   </si>
 </sst>
 </file>
@@ -2354,11 +2357,11 @@
   <dimension ref="A1:P286"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D257" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F248" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F263" sqref="F263"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F275" sqref="F275"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14164,15 +14167,15 @@
       </c>
       <c r="F262" s="3">
         <f t="shared" si="23"/>
-        <v>0.66583719426919541</v>
+        <v>0.66583720725560669</v>
       </c>
       <c r="G262" s="3">
         <f t="shared" si="28"/>
-        <v>0.95172870627870398</v>
+        <v>0.95172868771629815</v>
       </c>
       <c r="H262" s="3">
         <f t="shared" si="25"/>
-        <v>4.8271293721296016E-2</v>
+        <v>4.8271292779818321E-2</v>
       </c>
       <c r="I262" s="3">
         <f t="shared" si="26"/>
@@ -14182,7 +14185,7 @@
         <v>77003.566999999995</v>
       </c>
       <c r="K262" s="2">
-        <v>51271.839</v>
+        <v>51271.839999999997</v>
       </c>
       <c r="L262" s="2">
         <v>48796.881000000001</v>
@@ -14192,7 +14195,7 @@
       </c>
       <c r="N262" s="2">
         <f t="shared" si="27"/>
-        <v>25731.727999999996</v>
+        <v>25731.726999999999</v>
       </c>
       <c r="O262" s="2">
         <v>6286.6009999999997</v>
@@ -14786,11 +14789,11 @@
         <v>425</v>
       </c>
       <c r="F274" s="3">
-        <f t="shared" ref="F274" si="30">K274/J274</f>
+        <f t="shared" ref="F274:F275" si="30">K274/J274</f>
         <v>0.6114444374307062</v>
       </c>
       <c r="G274" s="3">
-        <f t="shared" ref="G274" si="31">L274/K274</f>
+        <f t="shared" ref="G274:G275" si="31">L274/K274</f>
         <v>0.95528747408394488</v>
       </c>
       <c r="H274" s="3">
@@ -14839,6 +14842,44 @@
       </c>
       <c r="E275" s="1" t="s">
         <v>425</v>
+      </c>
+      <c r="F275" s="3">
+        <f t="shared" si="30"/>
+        <v>0.64804378119674044</v>
+      </c>
+      <c r="G275" s="3">
+        <f t="shared" si="31"/>
+        <v>0.96461365744041938</v>
+      </c>
+      <c r="H275" s="3">
+        <f>M275/K275</f>
+        <v>3.5386342559580682E-2</v>
+      </c>
+      <c r="I275" s="3">
+        <f>O275/L275</f>
+        <v>0.12413474921669926</v>
+      </c>
+      <c r="J275" s="2">
+        <v>78306.858999999997</v>
+      </c>
+      <c r="K275" s="2">
+        <v>50746.273000000001</v>
+      </c>
+      <c r="L275" s="2">
+        <v>48950.548000000003</v>
+      </c>
+      <c r="M275" s="2">
+        <v>1795.7249999999999</v>
+      </c>
+      <c r="N275" s="2">
+        <f>J275-K275</f>
+        <v>27560.585999999996</v>
+      </c>
+      <c r="O275" s="2">
+        <v>6076.4639999999999</v>
+      </c>
+      <c r="P275" t="s">
+        <v>658</v>
       </c>
     </row>
     <row r="276" spans="1:16" x14ac:dyDescent="0.25">
@@ -15039,7 +15080,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -15891,7 +15932,7 @@
       <selection activeCell="B153" sqref="B153"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B166" sqref="B166"/>
+      <selection pane="bottomRight" activeCell="B168" sqref="B168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17487,6 +17528,9 @@
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>644</v>
+      </c>
+      <c r="B167" t="s">
+        <v>658</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Monthly labor update - Mar 2024
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADE6CDD-C142-4B6A-B547-22E79C5858F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C96FF05-768F-4477-94E3-175831A80031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4935" yWindow="2280" windowWidth="11130" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="660">
   <si>
     <t>LFS Round</t>
   </si>
@@ -2013,6 +2013,9 @@
   </si>
   <si>
     <t>https://psa.gov.ph/content/unemployment-rate-february-2024-was-estimated-35-percent</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/unemployment-rate-march-2024-was-estimated-39-percent</t>
   </si>
 </sst>
 </file>
@@ -2357,11 +2360,11 @@
   <dimension ref="A1:P286"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F248" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E269" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F263" sqref="F263"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F281" sqref="F281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14162,9 +14165,6 @@
       <c r="D262" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E262" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F262" s="3">
         <f t="shared" si="23"/>
         <v>0.66583720725560669</v>
@@ -14217,9 +14217,6 @@
       <c r="D263" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E263" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F263" s="3">
         <f t="shared" si="23"/>
         <v>0.66011891735401695</v>
@@ -14789,11 +14786,11 @@
         <v>425</v>
       </c>
       <c r="F274" s="3">
-        <f t="shared" ref="F274:F275" si="30">K274/J274</f>
+        <f t="shared" ref="F274:F276" si="30">K274/J274</f>
         <v>0.6114444374307062</v>
       </c>
       <c r="G274" s="3">
-        <f t="shared" ref="G274:G275" si="31">L274/K274</f>
+        <f t="shared" ref="G274:G276" si="31">L274/K274</f>
         <v>0.95528747408394488</v>
       </c>
       <c r="H274" s="3">
@@ -14897,6 +14894,44 @@
       </c>
       <c r="E276" s="1" t="s">
         <v>425</v>
+      </c>
+      <c r="F276" s="3">
+        <f t="shared" si="30"/>
+        <v>0.65317873180475028</v>
+      </c>
+      <c r="G276" s="3">
+        <f t="shared" si="31"/>
+        <v>0.96089400764617972</v>
+      </c>
+      <c r="H276" s="3">
+        <f>M276/K276</f>
+        <v>3.9105992353820243E-2</v>
+      </c>
+      <c r="I276" s="3">
+        <f>O276/L276</f>
+        <v>0.10967110358956031</v>
+      </c>
+      <c r="J276" s="2">
+        <v>78314.534</v>
+      </c>
+      <c r="K276" s="2">
+        <v>51153.387999999999</v>
+      </c>
+      <c r="L276" s="2">
+        <v>49152.983999999997</v>
+      </c>
+      <c r="M276" s="2">
+        <v>2000.404</v>
+      </c>
+      <c r="N276" s="2">
+        <f>J276-K276</f>
+        <v>27161.146000000001</v>
+      </c>
+      <c r="O276" s="2">
+        <v>5390.6620000000003</v>
+      </c>
+      <c r="P276" t="s">
+        <v>659</v>
       </c>
     </row>
     <row r="277" spans="1:16" x14ac:dyDescent="0.25">
@@ -17537,6 +17572,9 @@
       <c r="A168" s="1" t="s">
         <v>645</v>
       </c>
+      <c r="B168" t="s">
+        <v>659</v>
+      </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">

</xml_diff>

<commit_message>
Monthly labor update - Apr to May 2024
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C96FF05-768F-4477-94E3-175831A80031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A843922-C3F2-415C-A327-163D5362B0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1730" uniqueCount="660">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="662">
   <si>
     <t>LFS Round</t>
   </si>
@@ -2016,6 +2016,12 @@
   </si>
   <si>
     <t>https://psa.gov.ph/content/unemployment-rate-march-2024-was-estimated-39-percent</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/unemployment-rate-april-2024-was-estimated-40-percent</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/employment-rate-may-2024-was-estimated-959-percent</t>
   </si>
 </sst>
 </file>
@@ -2359,12 +2365,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P286"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E269" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D256" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F263" sqref="F263"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F281" sqref="F281"/>
+      <selection pane="bottomRight" activeCell="D280" sqref="D280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14269,9 +14275,6 @@
       <c r="D264" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E264" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F264" s="3">
         <f t="shared" si="23"/>
         <v>0.65123306419898641</v>
@@ -14324,9 +14327,6 @@
       <c r="D265" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E265" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F265" s="3">
         <f t="shared" si="23"/>
         <v>0.65346941408460835</v>
@@ -14786,11 +14786,11 @@
         <v>425</v>
       </c>
       <c r="F274" s="3">
-        <f t="shared" ref="F274:F276" si="30">K274/J274</f>
+        <f t="shared" ref="F274:F278" si="30">K274/J274</f>
         <v>0.6114444374307062</v>
       </c>
       <c r="G274" s="3">
-        <f t="shared" ref="G274:G276" si="31">L274/K274</f>
+        <f t="shared" ref="G274:G278" si="31">L274/K274</f>
         <v>0.95528747408394488</v>
       </c>
       <c r="H274" s="3">
@@ -14950,6 +14950,44 @@
       <c r="E277" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="F277" s="3">
+        <f t="shared" si="30"/>
+        <v>0.64103029582549154</v>
+      </c>
+      <c r="G277" s="3">
+        <f t="shared" si="31"/>
+        <v>0.9595020441819837</v>
+      </c>
+      <c r="H277" s="3">
+        <f>M277/K277</f>
+        <v>4.0497955818016275E-2</v>
+      </c>
+      <c r="I277" s="3">
+        <f>O277/L277</f>
+        <v>0.14553115271545977</v>
+      </c>
+      <c r="J277" s="2">
+        <v>78617.498000000007</v>
+      </c>
+      <c r="K277" s="2">
+        <v>50396.197999999997</v>
+      </c>
+      <c r="L277" s="2">
+        <v>48355.254999999997</v>
+      </c>
+      <c r="M277" s="2">
+        <v>2040.943</v>
+      </c>
+      <c r="N277" s="2">
+        <f>J277-K277</f>
+        <v>28221.30000000001</v>
+      </c>
+      <c r="O277" s="2">
+        <v>7037.1959999999999</v>
+      </c>
+      <c r="P277" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="278" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
@@ -14966,6 +15004,44 @@
       </c>
       <c r="E278" s="1" t="s">
         <v>425</v>
+      </c>
+      <c r="F278" s="3">
+        <f t="shared" si="30"/>
+        <v>0.64820526458333438</v>
+      </c>
+      <c r="G278" s="3">
+        <f t="shared" si="31"/>
+        <v>0.95867987903546048</v>
+      </c>
+      <c r="H278" s="3">
+        <f>M278/K278</f>
+        <v>4.1320120964539651E-2</v>
+      </c>
+      <c r="I278" s="3">
+        <f>O278/L278</f>
+        <v>9.85360462451631E-2</v>
+      </c>
+      <c r="J278" s="2">
+        <v>78635.017000000007</v>
+      </c>
+      <c r="K278" s="2">
+        <v>50971.631999999998</v>
+      </c>
+      <c r="L278" s="2">
+        <v>48865.478000000003</v>
+      </c>
+      <c r="M278" s="2">
+        <v>2106.154</v>
+      </c>
+      <c r="N278" s="2">
+        <f>J278-K278</f>
+        <v>27663.385000000009</v>
+      </c>
+      <c r="O278" s="2">
+        <v>4815.0110000000004</v>
+      </c>
+      <c r="P278" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="279" spans="1:16" x14ac:dyDescent="0.25">
@@ -15112,14 +15188,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15943,14 +16019,43 @@
       <c r="A29">
         <v>2022</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
+      <c r="B29" s="21">
+        <v>76598.736999999994</v>
+      </c>
+      <c r="C29" s="21">
+        <v>64.7</v>
+      </c>
+      <c r="D29" s="21">
+        <v>49561.608999999997</v>
+      </c>
+      <c r="E29" s="21">
+        <v>94.61</v>
+      </c>
+      <c r="F29" s="21">
+        <v>46890.39</v>
+      </c>
+      <c r="G29" s="21">
+        <v>5.39</v>
+      </c>
+      <c r="H29" s="21">
+        <v>2671.2190000000001</v>
+      </c>
+      <c r="I29" s="21">
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2023</v>
+      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15963,11 +16068,11 @@
   <dimension ref="A1:D178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B161" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B158" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B153" sqref="B153"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B168" sqref="B168"/>
+      <selection pane="bottomRight" activeCell="A171" sqref="A171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17580,10 +17685,16 @@
       <c r="A169" s="1" t="s">
         <v>646</v>
       </c>
+      <c r="B169" t="s">
+        <v>660</v>
+      </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>647</v>
+      </c>
+      <c r="B170" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
@@ -17634,10 +17745,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17924,6 +18035,14 @@
       <c r="A31">
         <v>2022</v>
       </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2023</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Monthly labor update - Jun 2024
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A843922-C3F2-415C-A327-163D5362B0EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A089D4C-19BA-4D65-8A93-053BB9952F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1732" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1733" uniqueCount="663">
   <si>
     <t>LFS Round</t>
   </si>
@@ -2022,6 +2022,9 @@
   </si>
   <si>
     <t>https://psa.gov.ph/content/employment-rate-may-2024-was-estimated-959-percent</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/employment-rate-june-2024-was-estimated-969-percent</t>
   </si>
 </sst>
 </file>
@@ -2365,12 +2368,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P286"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D256" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="E253" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F263" sqref="F263"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D280" sqref="D280"/>
+      <selection pane="bottomRight" activeCell="F280" sqref="F280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14379,43 +14382,40 @@
       <c r="D266" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E266" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F266" s="3">
         <f t="shared" si="23"/>
-        <v>0.66074689027081135</v>
+        <v>0.66074217697023219</v>
       </c>
       <c r="G266" s="3">
         <f t="shared" si="28"/>
-        <v>0.95452702169224368</v>
+        <v>0.95452728362005634</v>
       </c>
       <c r="H266" s="3">
         <f t="shared" si="25"/>
-        <v>4.5472978307756408E-2</v>
+        <v>4.5472716379943739E-2</v>
       </c>
       <c r="I266" s="3">
         <f t="shared" si="26"/>
-        <v>0.1202847318998803</v>
+        <v>0.12028369375161235</v>
       </c>
       <c r="J266" s="2">
         <v>77440.425000000003</v>
       </c>
       <c r="K266" s="2">
-        <v>51168.52</v>
+        <v>51168.154999999999</v>
       </c>
       <c r="L266" s="2">
-        <v>48841.735000000001</v>
+        <v>48841.4</v>
       </c>
       <c r="M266" s="2">
-        <v>2326.7849999999999</v>
+        <v>2326.7550000000001</v>
       </c>
       <c r="N266" s="2">
         <f t="shared" si="27"/>
-        <v>26271.905000000006</v>
+        <v>26272.270000000004</v>
       </c>
       <c r="O266" s="2">
-        <v>5874.915</v>
+        <v>5874.8239999999996</v>
       </c>
       <c r="P266" t="s">
         <v>500</v>
@@ -15060,6 +15060,44 @@
       <c r="E279" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="F279" s="3">
+        <f t="shared" ref="F279" si="32">K279/J279</f>
+        <v>0.65995564923197714</v>
+      </c>
+      <c r="G279" s="3">
+        <f t="shared" ref="G279" si="33">L279/K279</f>
+        <v>0.96878736298544643</v>
+      </c>
+      <c r="H279" s="3">
+        <f>M279/K279</f>
+        <v>3.1212637014553603E-2</v>
+      </c>
+      <c r="I279" s="3">
+        <f>O279/L279</f>
+        <v>0.12098454750123523</v>
+      </c>
+      <c r="J279" s="2">
+        <v>78638.547999999995</v>
+      </c>
+      <c r="K279" s="2">
+        <v>51897.953999999998</v>
+      </c>
+      <c r="L279" s="2">
+        <v>50278.082000000002</v>
+      </c>
+      <c r="M279" s="2">
+        <v>1619.8720000000001</v>
+      </c>
+      <c r="N279" s="2">
+        <f>J279-K279</f>
+        <v>26740.593999999997</v>
+      </c>
+      <c r="O279" s="2">
+        <v>6082.8710000000001</v>
+      </c>
+      <c r="P279" t="s">
+        <v>662</v>
+      </c>
     </row>
     <row r="280" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
@@ -15182,7 +15220,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -15190,7 +15228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight"/>
@@ -16072,7 +16110,7 @@
       <selection activeCell="B153" sqref="B153"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A171" sqref="A171"/>
+      <selection pane="bottomRight" activeCell="B171" sqref="B171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17700,6 +17738,9 @@
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>648</v>
+      </c>
+      <c r="B171" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Monthly labor update - Jul 2024
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A089D4C-19BA-4D65-8A93-053BB9952F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9AC6AF-1DE0-4E4B-B2C0-0BFD5C315F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="2865" windowWidth="12810" windowHeight="10545" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1733" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1734" uniqueCount="664">
   <si>
     <t>LFS Round</t>
   </si>
@@ -2025,6 +2025,9 @@
   </si>
   <si>
     <t>https://psa.gov.ph/content/employment-rate-june-2024-was-estimated-969-percent</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/unemployment-rate-july-2024-was-estimated-47-percent</t>
   </si>
 </sst>
 </file>
@@ -2368,12 +2371,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P286"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E253" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="G271" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F263" sqref="F263"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F280" sqref="F280"/>
+      <selection pane="bottomRight" activeCell="H281" sqref="H281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14434,43 +14437,40 @@
       <c r="D267" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E267" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F267" s="3">
         <f t="shared" si="23"/>
-        <v>0.60093428895027345</v>
+        <v>0.60034823121217606</v>
       </c>
       <c r="G267" s="3">
         <f t="shared" si="28"/>
-        <v>0.95153046680920927</v>
+        <v>0.95113554410636325</v>
       </c>
       <c r="H267" s="3">
         <f t="shared" si="25"/>
-        <v>4.8469511870375633E-2</v>
+        <v>4.88644558936367E-2</v>
       </c>
       <c r="I267" s="3">
         <f t="shared" si="26"/>
-        <v>0.1591729879729373</v>
+        <v>0.15865117978004073</v>
       </c>
       <c r="J267" s="2">
-        <v>78050.8</v>
+        <v>78029.766000000003</v>
       </c>
       <c r="K267" s="2">
-        <v>46903.402000000002</v>
+        <v>46845.031999999999</v>
       </c>
       <c r="L267" s="2">
-        <v>44630.016000000003</v>
+        <v>44555.974999999999</v>
       </c>
       <c r="M267" s="2">
-        <v>2273.3850000000002</v>
+        <v>2289.0569999999998</v>
       </c>
       <c r="N267" s="2">
         <f t="shared" si="27"/>
-        <v>31147.398000000001</v>
+        <v>31184.734000000004</v>
       </c>
       <c r="O267" s="2">
-        <v>7103.893</v>
+        <v>7068.8580000000002</v>
       </c>
       <c r="P267" t="s">
         <v>502</v>
@@ -14794,11 +14794,11 @@
         <v>0.95528747408394488</v>
       </c>
       <c r="H274" s="3">
-        <f>M274/K274</f>
+        <f t="shared" ref="H274:H279" si="32">M274/K274</f>
         <v>4.4712525916055137E-2</v>
       </c>
       <c r="I274" s="3">
-        <f>O274/L274</f>
+        <f t="shared" ref="I274:I279" si="33">O274/L274</f>
         <v>0.13917804379986054</v>
       </c>
       <c r="J274" s="2">
@@ -14814,7 +14814,7 @@
         <v>2150.3710000000001</v>
       </c>
       <c r="N274" s="2">
-        <f>J274-K274</f>
+        <f t="shared" ref="N274:N280" si="34">J274-K274</f>
         <v>30561.898000000001</v>
       </c>
       <c r="O274" s="2">
@@ -14849,11 +14849,11 @@
         <v>0.96461365744041938</v>
       </c>
       <c r="H275" s="3">
-        <f>M275/K275</f>
+        <f t="shared" si="32"/>
         <v>3.5386342559580682E-2</v>
       </c>
       <c r="I275" s="3">
-        <f>O275/L275</f>
+        <f t="shared" si="33"/>
         <v>0.12413474921669926</v>
       </c>
       <c r="J275" s="2">
@@ -14869,7 +14869,7 @@
         <v>1795.7249999999999</v>
       </c>
       <c r="N275" s="2">
-        <f>J275-K275</f>
+        <f t="shared" si="34"/>
         <v>27560.585999999996</v>
       </c>
       <c r="O275" s="2">
@@ -14904,11 +14904,11 @@
         <v>0.96089400764617972</v>
       </c>
       <c r="H276" s="3">
-        <f>M276/K276</f>
+        <f t="shared" si="32"/>
         <v>3.9105992353820243E-2</v>
       </c>
       <c r="I276" s="3">
-        <f>O276/L276</f>
+        <f t="shared" si="33"/>
         <v>0.10967110358956031</v>
       </c>
       <c r="J276" s="2">
@@ -14924,7 +14924,7 @@
         <v>2000.404</v>
       </c>
       <c r="N276" s="2">
-        <f>J276-K276</f>
+        <f t="shared" si="34"/>
         <v>27161.146000000001</v>
       </c>
       <c r="O276" s="2">
@@ -14959,11 +14959,11 @@
         <v>0.9595020441819837</v>
       </c>
       <c r="H277" s="3">
-        <f>M277/K277</f>
+        <f t="shared" si="32"/>
         <v>4.0497955818016275E-2</v>
       </c>
       <c r="I277" s="3">
-        <f>O277/L277</f>
+        <f t="shared" si="33"/>
         <v>0.14553115271545977</v>
       </c>
       <c r="J277" s="2">
@@ -14979,7 +14979,7 @@
         <v>2040.943</v>
       </c>
       <c r="N277" s="2">
-        <f>J277-K277</f>
+        <f t="shared" si="34"/>
         <v>28221.30000000001</v>
       </c>
       <c r="O277" s="2">
@@ -15014,11 +15014,11 @@
         <v>0.95867987903546048</v>
       </c>
       <c r="H278" s="3">
-        <f>M278/K278</f>
+        <f t="shared" si="32"/>
         <v>4.1320120964539651E-2</v>
       </c>
       <c r="I278" s="3">
-        <f>O278/L278</f>
+        <f t="shared" si="33"/>
         <v>9.85360462451631E-2</v>
       </c>
       <c r="J278" s="2">
@@ -15034,7 +15034,7 @@
         <v>2106.154</v>
       </c>
       <c r="N278" s="2">
-        <f>J278-K278</f>
+        <f t="shared" si="34"/>
         <v>27663.385000000009</v>
       </c>
       <c r="O278" s="2">
@@ -15061,19 +15061,19 @@
         <v>425</v>
       </c>
       <c r="F279" s="3">
-        <f t="shared" ref="F279" si="32">K279/J279</f>
+        <f t="shared" ref="F279" si="35">K279/J279</f>
         <v>0.65995564923197714</v>
       </c>
       <c r="G279" s="3">
-        <f t="shared" ref="G279" si="33">L279/K279</f>
+        <f t="shared" ref="G279" si="36">L279/K279</f>
         <v>0.96878736298544643</v>
       </c>
       <c r="H279" s="3">
-        <f>M279/K279</f>
+        <f t="shared" si="32"/>
         <v>3.1212637014553603E-2</v>
       </c>
       <c r="I279" s="3">
-        <f>O279/L279</f>
+        <f t="shared" si="33"/>
         <v>0.12098454750123523</v>
       </c>
       <c r="J279" s="2">
@@ -15089,7 +15089,7 @@
         <v>1619.8720000000001</v>
       </c>
       <c r="N279" s="2">
-        <f>J279-K279</f>
+        <f t="shared" si="34"/>
         <v>26740.593999999997</v>
       </c>
       <c r="O279" s="2">
@@ -15114,6 +15114,44 @@
       </c>
       <c r="E280" s="1" t="s">
         <v>425</v>
+      </c>
+      <c r="F280" s="3">
+        <f t="shared" ref="F280" si="37">K280/J280</f>
+        <v>0.63469480625870289</v>
+      </c>
+      <c r="G280" s="3">
+        <f t="shared" ref="G280" si="38">L280/K280</f>
+        <v>0.95256802192614232</v>
+      </c>
+      <c r="H280" s="3">
+        <f t="shared" ref="H280" si="39">M280/K280</f>
+        <v>4.7431978073857746E-2</v>
+      </c>
+      <c r="I280" s="3">
+        <f t="shared" ref="I280" si="40">O280/L280</f>
+        <v>0.12110610167973515</v>
+      </c>
+      <c r="J280" s="2">
+        <v>78893.918000000005</v>
+      </c>
+      <c r="K280" s="2">
+        <v>50073.56</v>
+      </c>
+      <c r="L280" s="2">
+        <v>47698.472000000002</v>
+      </c>
+      <c r="M280" s="2">
+        <v>2375.0880000000002</v>
+      </c>
+      <c r="N280" s="2">
+        <f t="shared" si="34"/>
+        <v>28820.358000000007</v>
+      </c>
+      <c r="O280" s="2">
+        <v>5776.576</v>
+      </c>
+      <c r="P280" t="s">
+        <v>663</v>
       </c>
     </row>
     <row r="281" spans="1:16" x14ac:dyDescent="0.25">
@@ -15229,7 +15267,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -16106,11 +16144,11 @@
   <dimension ref="A1:D178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B158" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B164" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B153" sqref="B153"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B171" sqref="B171"/>
+      <selection pane="bottomRight" activeCell="B173" sqref="B173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17747,6 +17785,9 @@
       <c r="A172" s="1" t="s">
         <v>649</v>
       </c>
+      <c r="B172" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
@@ -17788,8 +17829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Monthly labor update - Aug 2024
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9AC6AF-1DE0-4E4B-B2C0-0BFD5C315F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD7BF97-7123-43AD-9954-6B211B8B2E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="2865" windowWidth="12810" windowHeight="10545" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1734" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1735" uniqueCount="665">
   <si>
     <t>LFS Round</t>
   </si>
@@ -2028,6 +2028,9 @@
   </si>
   <si>
     <t>https://psa.gov.ph/content/unemployment-rate-july-2024-was-estimated-47-percent</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/employment-rate-august-2024-was-estimated-960-percent</t>
   </si>
 </sst>
 </file>
@@ -2371,12 +2374,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P286"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G271" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="E274" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F263" sqref="F263"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H281" sqref="H281"/>
+      <selection pane="bottomRight" activeCell="F282" sqref="F282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14489,20 +14492,17 @@
       <c r="D268" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E268" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F268" s="3">
         <f t="shared" si="23"/>
-        <v>0.64650853861229718</v>
+        <v>0.64657361752909759</v>
       </c>
       <c r="G268" s="3">
         <f t="shared" si="28"/>
-        <v>0.95597557716757331</v>
+        <v>0.95587935632997179</v>
       </c>
       <c r="H268" s="3">
         <f t="shared" si="25"/>
-        <v>4.4024422832426691E-2</v>
+        <v>4.4120623786191165E-2</v>
       </c>
       <c r="I268" s="3">
         <f t="shared" si="26"/>
@@ -14512,17 +14512,17 @@
         <v>77782.486999999994</v>
       </c>
       <c r="K268" s="2">
-        <v>50287.042000000001</v>
+        <v>50292.103999999999</v>
       </c>
       <c r="L268" s="2">
         <v>48073.184000000001</v>
       </c>
       <c r="M268" s="2">
-        <v>2213.8580000000002</v>
+        <v>2218.9189999999999</v>
       </c>
       <c r="N268" s="2">
         <f t="shared" si="27"/>
-        <v>27495.444999999992</v>
+        <v>27490.382999999994</v>
       </c>
       <c r="O268" s="2">
         <v>5630.1660000000002</v>
@@ -14814,7 +14814,7 @@
         <v>2150.3710000000001</v>
       </c>
       <c r="N274" s="2">
-        <f t="shared" ref="N274:N280" si="34">J274-K274</f>
+        <f t="shared" ref="N274:N281" si="34">J274-K274</f>
         <v>30561.898000000001</v>
       </c>
       <c r="O274" s="2">
@@ -15170,6 +15170,44 @@
       <c r="E281" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="F281" s="3">
+        <f t="shared" ref="F281" si="41">K281/J281</f>
+        <v>0.64807383986548939</v>
+      </c>
+      <c r="G281" s="3">
+        <f t="shared" ref="G281" si="42">L281/K281</f>
+        <v>0.95958742054697199</v>
+      </c>
+      <c r="H281" s="3">
+        <f t="shared" ref="H281" si="43">M281/K281</f>
+        <v>4.0412579453028008E-2</v>
+      </c>
+      <c r="I281" s="3">
+        <f t="shared" ref="I281" si="44">O281/L281</f>
+        <v>0.11156186785894412</v>
+      </c>
+      <c r="J281" s="2">
+        <v>79040.339000000007</v>
+      </c>
+      <c r="K281" s="2">
+        <v>51223.976000000002</v>
+      </c>
+      <c r="L281" s="2">
+        <v>49153.883000000002</v>
+      </c>
+      <c r="M281" s="2">
+        <v>2070.0929999999998</v>
+      </c>
+      <c r="N281" s="2">
+        <f t="shared" si="34"/>
+        <v>27816.363000000005</v>
+      </c>
+      <c r="O281" s="2">
+        <v>5483.6989999999996</v>
+      </c>
+      <c r="P281" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="282" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
@@ -15187,6 +15225,7 @@
       <c r="E282" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="O282" s="2"/>
     </row>
     <row r="283" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
@@ -15204,6 +15243,7 @@
       <c r="E283" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="O283" s="2"/>
     </row>
     <row r="284" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
@@ -15221,6 +15261,7 @@
       <c r="E284" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="O284" s="2"/>
     </row>
     <row r="285" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
@@ -15238,6 +15279,7 @@
       <c r="E285" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="O285" s="2"/>
     </row>
     <row r="286" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
@@ -15255,6 +15297,7 @@
       <c r="E286" s="1" t="s">
         <v>425</v>
       </c>
+      <c r="O286" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16148,7 +16191,7 @@
       <selection activeCell="B153" sqref="B153"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B173" sqref="B173"/>
+      <selection pane="bottomRight" activeCell="B174" sqref="B174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17793,6 +17836,9 @@
       <c r="A173" s="1" t="s">
         <v>650</v>
       </c>
+      <c r="B173" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
@@ -17829,7 +17875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Monthly labor update - Sep 2024
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD7BF97-7123-43AD-9954-6B211B8B2E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83769EEC-3D1F-4865-A452-BEB592314463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1735" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="668">
   <si>
     <t>LFS Round</t>
   </si>
@@ -2031,6 +2031,15 @@
   </si>
   <si>
     <t>https://psa.gov.ph/content/employment-rate-august-2024-was-estimated-960-percent</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/unemployment-rate-september-2024-was-estimated-37-percent</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/2022-annual-provincial-labor-market-statistics-preliminary-results</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/2023-annual-provincial-labor-market-statistics-preliminary-results</t>
   </si>
 </sst>
 </file>
@@ -2375,11 +2384,11 @@
   <dimension ref="A1:P286"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E274" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D261" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F263" sqref="F263"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F282" sqref="F282"/>
+      <selection pane="bottomRight" activeCell="E271" sqref="E271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13432,43 +13441,40 @@
       <c r="D247" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E247" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F247" s="3">
         <f t="shared" si="23"/>
-        <v>0.63346515961840855</v>
+        <v>0.63349976614538095</v>
       </c>
       <c r="G247" s="3">
         <f t="shared" si="24"/>
-        <v>0.92218769100179576</v>
+        <v>0.92212451482816615</v>
       </c>
       <c r="H247" s="3">
         <f t="shared" si="25"/>
-        <v>7.781231423920712E-2</v>
+        <v>7.7875485171833958E-2</v>
       </c>
       <c r="I247" s="3">
         <f t="shared" si="26"/>
-        <v>0.15919453293482841</v>
+        <v>0.15919765650368964</v>
       </c>
       <c r="J247" s="2">
-        <v>75301.370999999999</v>
+        <v>75301.057000000001</v>
       </c>
       <c r="K247" s="2">
-        <v>47700.794999999998</v>
+        <v>47703.201999999997</v>
       </c>
       <c r="L247" s="2">
-        <v>43989.086000000003</v>
+        <v>43988.292000000001</v>
       </c>
       <c r="M247" s="2">
-        <v>3711.7092499999999</v>
+        <v>3714.91</v>
       </c>
       <c r="N247" s="2">
         <f t="shared" si="27"/>
-        <v>27600.576000000001</v>
+        <v>27597.855000000003</v>
       </c>
       <c r="O247" s="2">
-        <v>7002.8220000000001</v>
+        <v>7002.8329999999996</v>
       </c>
       <c r="P247" t="s">
         <v>461</v>
@@ -14111,8 +14117,43 @@
       <c r="D260" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E260" s="1" t="s">
-        <v>425</v>
+      <c r="F260" s="3">
+        <f t="shared" si="23"/>
+        <v>0.64701787195983929</v>
+      </c>
+      <c r="G260" s="3">
+        <f t="shared" si="23"/>
+        <v>0.94610142228678085</v>
+      </c>
+      <c r="H260" s="3">
+        <f t="shared" si="25"/>
+        <v>5.3898577713219167E-2</v>
+      </c>
+      <c r="I260" s="3">
+        <f t="shared" si="26"/>
+        <v>0.14238773709421168</v>
+      </c>
+      <c r="J260" s="2">
+        <v>76594.062000000005</v>
+      </c>
+      <c r="K260" s="2">
+        <v>49557.726999999999</v>
+      </c>
+      <c r="L260" s="2">
+        <v>46886.635999999999</v>
+      </c>
+      <c r="M260" s="2">
+        <v>2671.0909999999999</v>
+      </c>
+      <c r="N260" s="2">
+        <f t="shared" si="27"/>
+        <v>27036.335000000006</v>
+      </c>
+      <c r="O260" s="2">
+        <v>6676.0820000000003</v>
+      </c>
+      <c r="P260" t="s">
+        <v>666</v>
       </c>
     </row>
     <row r="261" spans="1:16" x14ac:dyDescent="0.25">
@@ -14544,43 +14585,40 @@
       <c r="D269" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E269" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F269" s="3">
         <f t="shared" si="23"/>
-        <v>0.64049609363750415</v>
+        <v>0.64049602949730688</v>
       </c>
       <c r="G269" s="3">
         <f t="shared" si="28"/>
-        <v>0.9546663534776707</v>
+        <v>0.95466676953195773</v>
       </c>
       <c r="H269" s="3">
         <f t="shared" si="25"/>
-        <v>4.5333646522329352E-2</v>
+        <v>4.5333210439753524E-2</v>
       </c>
       <c r="I269" s="3">
         <f t="shared" si="26"/>
-        <v>0.10725448980279445</v>
+        <v>0.1072527544733325</v>
       </c>
       <c r="J269" s="2">
         <v>77954.235000000001</v>
       </c>
       <c r="K269" s="2">
-        <v>49929.383000000002</v>
+        <v>49929.377999999997</v>
       </c>
       <c r="L269" s="2">
-        <v>47665.902000000002</v>
+        <v>47665.917999999998</v>
       </c>
       <c r="M269" s="2">
-        <v>2263.4810000000002</v>
+        <v>2263.4589999999998</v>
       </c>
       <c r="N269" s="2">
         <f t="shared" si="27"/>
-        <v>28024.851999999999</v>
+        <v>28024.857000000004</v>
       </c>
       <c r="O269" s="2">
-        <v>5112.3819999999996</v>
+        <v>5112.3010000000004</v>
       </c>
       <c r="P269" t="s">
         <v>506</v>
@@ -14603,7 +14641,7 @@
         <v>425</v>
       </c>
       <c r="F270" s="3">
-        <f t="shared" ref="F270:G272" si="29">K270/J270</f>
+        <f t="shared" ref="F270:G273" si="29">K270/J270</f>
         <v>0.63948145527591993</v>
       </c>
       <c r="G270" s="3">
@@ -14767,7 +14805,44 @@
       <c r="E273" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="O273" s="2"/>
+      <c r="F273" s="3">
+        <f t="shared" si="29"/>
+        <v>0.64906934649063885</v>
+      </c>
+      <c r="G273" s="3">
+        <f t="shared" si="29"/>
+        <v>0.95650041271321051</v>
+      </c>
+      <c r="H273" s="3">
+        <f>M273/K273</f>
+        <v>4.3499567436219029E-2</v>
+      </c>
+      <c r="I273" s="3">
+        <f>O273/L273</f>
+        <v>0.1234203342058449</v>
+      </c>
+      <c r="J273" s="2">
+        <v>77613.256999999998</v>
+      </c>
+      <c r="K273" s="2">
+        <v>50376.385999999999</v>
+      </c>
+      <c r="L273" s="2">
+        <v>48185.034</v>
+      </c>
+      <c r="M273" s="2">
+        <v>2191.3510000000001</v>
+      </c>
+      <c r="N273" s="2">
+        <f>J273-K273</f>
+        <v>27236.870999999999</v>
+      </c>
+      <c r="O273" s="2">
+        <v>5947.0129999999999</v>
+      </c>
+      <c r="P273" t="s">
+        <v>667</v>
+      </c>
     </row>
     <row r="274" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
@@ -14814,7 +14889,7 @@
         <v>2150.3710000000001</v>
       </c>
       <c r="N274" s="2">
-        <f t="shared" ref="N274:N281" si="34">J274-K274</f>
+        <f t="shared" ref="N274:N282" si="34">J274-K274</f>
         <v>30561.898000000001</v>
       </c>
       <c r="O274" s="2">
@@ -15171,19 +15246,19 @@
         <v>425</v>
       </c>
       <c r="F281" s="3">
-        <f t="shared" ref="F281" si="41">K281/J281</f>
+        <f t="shared" ref="F281:F282" si="41">K281/J281</f>
         <v>0.64807383986548939</v>
       </c>
       <c r="G281" s="3">
-        <f t="shared" ref="G281" si="42">L281/K281</f>
+        <f t="shared" ref="G281:G282" si="42">L281/K281</f>
         <v>0.95958742054697199</v>
       </c>
       <c r="H281" s="3">
-        <f t="shared" ref="H281" si="43">M281/K281</f>
+        <f t="shared" ref="H281:H282" si="43">M281/K281</f>
         <v>4.0412579453028008E-2</v>
       </c>
       <c r="I281" s="3">
-        <f t="shared" ref="I281" si="44">O281/L281</f>
+        <f t="shared" ref="I281:I282" si="44">O281/L281</f>
         <v>0.11156186785894412</v>
       </c>
       <c r="J281" s="2">
@@ -15225,7 +15300,44 @@
       <c r="E282" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="O282" s="2"/>
+      <c r="F282" s="3">
+        <f t="shared" si="41"/>
+        <v>0.65692169377521137</v>
+      </c>
+      <c r="G282" s="3">
+        <f t="shared" si="42"/>
+        <v>0.963426043702307</v>
+      </c>
+      <c r="H282" s="3">
+        <f t="shared" si="43"/>
+        <v>3.6573956297693035E-2</v>
+      </c>
+      <c r="I282" s="3">
+        <f t="shared" si="44"/>
+        <v>0.11917612348984245</v>
+      </c>
+      <c r="J282" s="2">
+        <v>78800.184999999998</v>
+      </c>
+      <c r="K282" s="2">
+        <v>51765.550999999999</v>
+      </c>
+      <c r="L282" s="2">
+        <v>49872.28</v>
+      </c>
+      <c r="M282" s="2">
+        <v>1893.271</v>
+      </c>
+      <c r="N282" s="2">
+        <f t="shared" si="34"/>
+        <v>27034.633999999998</v>
+      </c>
+      <c r="O282" s="2">
+        <v>5943.585</v>
+      </c>
+      <c r="P282" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="283" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
@@ -15310,11 +15422,11 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16187,7 +16299,7 @@
   <dimension ref="A1:D178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B164" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B166" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B153" sqref="B153"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -17843,6 +17955,9 @@
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>651</v>
+      </c>
+      <c r="B174" t="s">
+        <v>665</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Monthly labor update - Nov 2024
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BDD5C0-85C0-4DBF-B75E-2DD72550D78D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AE9F2E-3E28-489F-A4E0-CFD566FAFCB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1977" uniqueCount="763">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1979" uniqueCount="765">
   <si>
     <t>LFS Round</t>
   </si>
@@ -2326,6 +2326,12 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/employment-rate-november-2024-was-estimated-968-percent</t>
+  </si>
+  <si>
+    <t>2024Nov</t>
   </si>
 </sst>
 </file>
@@ -2338,11 +2344,18 @@
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2442,8 +2455,8 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2470,27 +2483,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2722,12 +2735,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P286"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E267" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D267" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F263" sqref="F263"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F284" sqref="F284"/>
+      <selection pane="bottomRight" activeCell="G284" sqref="G284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15028,9 +15041,6 @@
       <c r="D271" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E271" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F271" s="3">
         <f t="shared" si="29"/>
         <v>0.65894503512117253</v>
@@ -15225,7 +15235,7 @@
         <v>2150.3710000000001</v>
       </c>
       <c r="N274" s="2">
-        <f t="shared" ref="N274:N283" si="34">J274-K274</f>
+        <f t="shared" ref="N274:N284" si="34">J274-K274</f>
         <v>30561.898000000001</v>
       </c>
       <c r="O274" s="2">
@@ -15582,19 +15592,19 @@
         <v>425</v>
       </c>
       <c r="F281" s="3">
-        <f t="shared" ref="F281:F283" si="41">K281/J281</f>
+        <f t="shared" ref="F281:F284" si="41">K281/J281</f>
         <v>0.64807383986548939</v>
       </c>
       <c r="G281" s="3">
-        <f t="shared" ref="G281:G283" si="42">L281/K281</f>
+        <f t="shared" ref="G281:G284" si="42">L281/K281</f>
         <v>0.95958742054697199</v>
       </c>
       <c r="H281" s="3">
-        <f t="shared" ref="H281:H283" si="43">M281/K281</f>
+        <f t="shared" ref="H281:H284" si="43">M281/K281</f>
         <v>4.0412579453028008E-2</v>
       </c>
       <c r="I281" s="3">
-        <f t="shared" ref="I281:I283" si="44">O281/L281</f>
+        <f t="shared" ref="I281:I284" si="44">O281/L281</f>
         <v>0.11156186785894412</v>
       </c>
       <c r="J281" s="2">
@@ -15746,7 +15756,44 @@
       <c r="E284" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="O284" s="2"/>
+      <c r="F284" s="3">
+        <f t="shared" si="41"/>
+        <v>0.64579733417179253</v>
+      </c>
+      <c r="G284" s="3">
+        <f t="shared" si="42"/>
+        <v>0.9675279024117095</v>
+      </c>
+      <c r="H284" s="3">
+        <f t="shared" si="43"/>
+        <v>3.2472097588290456E-2</v>
+      </c>
+      <c r="I284" s="3">
+        <f t="shared" si="44"/>
+        <v>0.10808609651845406</v>
+      </c>
+      <c r="J284" s="2">
+        <v>79288.304999999993</v>
+      </c>
+      <c r="K284" s="2">
+        <v>51204.175999999999</v>
+      </c>
+      <c r="L284" s="2">
+        <v>49541.468999999997</v>
+      </c>
+      <c r="M284" s="2">
+        <v>1662.7070000000001</v>
+      </c>
+      <c r="N284" s="2">
+        <f t="shared" si="34"/>
+        <v>28084.128999999994</v>
+      </c>
+      <c r="O284" s="2">
+        <v>5354.7439999999997</v>
+      </c>
+      <c r="P284" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="285" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
@@ -15792,23 +15839,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B3FDD3-8CAB-4986-8439-B73CD0CD9872}">
-  <dimension ref="A1:BQ54"/>
+  <dimension ref="A1:BR54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="BO2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="BS24" sqref="BS24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" style="24" customWidth="1"/>
-    <col min="2" max="69" width="10.7109375" style="24" customWidth="1"/>
-    <col min="70" max="16384" width="9.140625" style="24"/>
+    <col min="2" max="70" width="10.7109375" style="24" customWidth="1"/>
+    <col min="71" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>685</v>
       </c>
@@ -15980,10 +16027,10 @@
       <c r="BE1" s="24" t="s">
         <v>707</v>
       </c>
-      <c r="BF1" s="31" t="s">
+      <c r="BF1" s="36" t="s">
         <v>706</v>
       </c>
-      <c r="BG1" s="24" t="s">
+      <c r="BG1" s="31" t="s">
         <v>705</v>
       </c>
       <c r="BH1" s="24" t="s">
@@ -16016,8 +16063,11 @@
       <c r="BQ1" s="24" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="2" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR1" s="35" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="2" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>694</v>
       </c>
@@ -16193,8 +16243,11 @@
       <c r="BQ2" s="26">
         <v>48156.966</v>
       </c>
-    </row>
-    <row r="3" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR2" s="26">
+        <v>49541.468999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>691</v>
       </c>
@@ -16262,8 +16315,9 @@
       <c r="BO3" s="26"/>
       <c r="BP3" s="26"/>
       <c r="BQ3" s="26"/>
-    </row>
-    <row r="4" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR3" s="26"/>
+    </row>
+    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>693</v>
       </c>
@@ -16439,8 +16493,11 @@
       <c r="BQ4" s="26">
         <v>9049.2219999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR4" s="26">
+        <v>8714.152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>692</v>
       </c>
@@ -16616,8 +16673,11 @@
       <c r="BQ5" s="26">
         <v>1137.5129999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR5" s="26">
+        <v>1203.7929999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>685</v>
       </c>
@@ -16683,8 +16743,9 @@
       <c r="BO6" s="26"/>
       <c r="BP6" s="26"/>
       <c r="BQ6" s="26"/>
-    </row>
-    <row r="7" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR6" s="26"/>
+    </row>
+    <row r="7" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>690</v>
       </c>
@@ -16860,8 +16921,11 @@
       <c r="BQ7" s="26">
         <v>262.99700000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR7" s="26">
+        <v>267.584</v>
+      </c>
+    </row>
+    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>689</v>
       </c>
@@ -17037,8 +17101,11 @@
       <c r="BQ8" s="26">
         <v>3479.509</v>
       </c>
-    </row>
-    <row r="9" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR8" s="26">
+        <v>3710.7510000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>688</v>
       </c>
@@ -17214,8 +17281,11 @@
       <c r="BQ9" s="26">
         <v>93.953999999999994</v>
       </c>
-    </row>
-    <row r="10" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR9" s="26">
+        <v>70.995000000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>687</v>
       </c>
@@ -17391,8 +17461,11 @@
       <c r="BQ10" s="26">
         <v>81.600999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR10" s="26">
+        <v>53.923000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>686</v>
       </c>
@@ -17568,8 +17641,11 @@
       <c r="BQ11" s="26">
         <v>4688.4880000000003</v>
       </c>
-    </row>
-    <row r="12" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR11" s="26">
+        <v>4763.9870000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
         <v>669</v>
       </c>
@@ -17635,8 +17711,9 @@
       <c r="BO12" s="26"/>
       <c r="BP12" s="26"/>
       <c r="BQ12" s="26"/>
-    </row>
-    <row r="13" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR12" s="26"/>
+    </row>
+    <row r="13" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>683</v>
       </c>
@@ -17812,8 +17889,11 @@
       <c r="BQ13" s="26">
         <v>9825.6129999999994</v>
       </c>
-    </row>
-    <row r="14" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR13" s="26">
+        <v>10571.767</v>
+      </c>
+    </row>
+    <row r="14" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>682</v>
       </c>
@@ -17989,8 +18069,11 @@
       <c r="BQ14" s="26">
         <v>3734.8620000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR14" s="26">
+        <v>3848.0129999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>681</v>
       </c>
@@ -18166,8 +18249,11 @@
       <c r="BQ15" s="26">
         <v>2507.5239999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR15" s="26">
+        <v>2896.1390000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>680</v>
       </c>
@@ -18343,8 +18429,11 @@
       <c r="BQ16" s="26">
         <v>541.06700000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR16" s="26">
+        <v>488.35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>679</v>
       </c>
@@ -18520,8 +18609,11 @@
       <c r="BQ17" s="26">
         <v>714.04899999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR17" s="26">
+        <v>661.50599999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>678</v>
       </c>
@@ -18697,8 +18789,11 @@
       <c r="BQ18" s="26">
         <v>236.655</v>
       </c>
-    </row>
-    <row r="19" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR18" s="26">
+        <v>242.67099999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>677</v>
       </c>
@@ -18874,8 +18969,11 @@
       <c r="BQ19" s="26">
         <v>419.29399999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR19" s="26">
+        <v>370.48599999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>676</v>
       </c>
@@ -19051,8 +19149,11 @@
       <c r="BQ20" s="26">
         <v>2790.6610000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR20" s="26">
+        <v>2644.9749999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>675</v>
       </c>
@@ -19228,8 +19329,11 @@
       <c r="BQ21" s="26">
         <v>2878.7660000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR21" s="26">
+        <v>2836.6239999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>674</v>
       </c>
@@ -19405,8 +19509,11 @@
       <c r="BQ22" s="26">
         <v>1623.857</v>
       </c>
-    </row>
-    <row r="23" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR22" s="26">
+        <v>1635.202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>673</v>
       </c>
@@ -19582,8 +19689,11 @@
       <c r="BQ23" s="26">
         <v>792.34400000000005</v>
       </c>
-    </row>
-    <row r="24" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR23" s="26">
+        <v>881.52300000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>672</v>
       </c>
@@ -19759,8 +19869,11 @@
       <c r="BQ24" s="26">
         <v>401.62</v>
       </c>
-    </row>
-    <row r="25" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR24" s="26">
+        <v>450.57799999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>671</v>
       </c>
@@ -19936,8 +20049,11 @@
       <c r="BQ25" s="26">
         <v>2896.8890000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR25" s="26">
+        <v>3225.143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>670</v>
       </c>
@@ -20113,8 +20229,11 @@
       <c r="BQ26" s="26">
         <v>0.48299999999999998</v>
       </c>
-    </row>
-    <row r="27" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR26" s="26">
+        <v>3.3079999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
         <v>694</v>
       </c>
@@ -20218,8 +20337,9 @@
       <c r="BO27" s="26"/>
       <c r="BP27" s="26"/>
       <c r="BQ27" s="26"/>
-    </row>
-    <row r="28" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR27" s="26"/>
+    </row>
+    <row r="28" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
         <v>691</v>
       </c>
@@ -20295,8 +20415,9 @@
       <c r="BO28" s="26"/>
       <c r="BP28" s="26"/>
       <c r="BQ28" s="26"/>
-    </row>
-    <row r="29" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR28" s="26"/>
+    </row>
+    <row r="29" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>693</v>
       </c>
@@ -20400,8 +20521,9 @@
       <c r="BO29" s="26"/>
       <c r="BP29" s="26"/>
       <c r="BQ29" s="26"/>
-    </row>
-    <row r="30" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR29" s="26"/>
+    </row>
+    <row r="30" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>692</v>
       </c>
@@ -20505,8 +20627,9 @@
       <c r="BO30" s="26"/>
       <c r="BP30" s="26"/>
       <c r="BQ30" s="26"/>
-    </row>
-    <row r="31" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR30" s="26"/>
+    </row>
+    <row r="31" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
         <v>685</v>
       </c>
@@ -20581,8 +20704,9 @@
       <c r="BO31" s="26"/>
       <c r="BP31" s="26"/>
       <c r="BQ31" s="26"/>
-    </row>
-    <row r="32" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR31" s="26"/>
+    </row>
+    <row r="32" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>690</v>
       </c>
@@ -20686,8 +20810,9 @@
       <c r="BO32" s="26"/>
       <c r="BP32" s="26"/>
       <c r="BQ32" s="26"/>
-    </row>
-    <row r="33" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR32" s="26"/>
+    </row>
+    <row r="33" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>689</v>
       </c>
@@ -20791,8 +20916,9 @@
       <c r="BO33" s="26"/>
       <c r="BP33" s="26"/>
       <c r="BQ33" s="26"/>
-    </row>
-    <row r="34" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR33" s="26"/>
+    </row>
+    <row r="34" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>688</v>
       </c>
@@ -20896,8 +21022,9 @@
       <c r="BO34" s="26"/>
       <c r="BP34" s="26"/>
       <c r="BQ34" s="26"/>
-    </row>
-    <row r="35" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR34" s="26"/>
+    </row>
+    <row r="35" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>687</v>
       </c>
@@ -21001,8 +21128,9 @@
       <c r="BO35" s="26"/>
       <c r="BP35" s="26"/>
       <c r="BQ35" s="26"/>
-    </row>
-    <row r="36" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR35" s="26"/>
+    </row>
+    <row r="36" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>686</v>
       </c>
@@ -21106,8 +21234,9 @@
       <c r="BO36" s="26"/>
       <c r="BP36" s="26"/>
       <c r="BQ36" s="26"/>
-    </row>
-    <row r="37" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR36" s="26"/>
+    </row>
+    <row r="37" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
         <v>669</v>
       </c>
@@ -21183,8 +21312,9 @@
       <c r="BO37" s="26"/>
       <c r="BP37" s="26"/>
       <c r="BQ37" s="26"/>
-    </row>
-    <row r="38" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR37" s="26"/>
+    </row>
+    <row r="38" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>683</v>
       </c>
@@ -21288,8 +21418,9 @@
       <c r="BO38" s="26"/>
       <c r="BP38" s="26"/>
       <c r="BQ38" s="26"/>
-    </row>
-    <row r="39" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR38" s="26"/>
+    </row>
+    <row r="39" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
         <v>682</v>
       </c>
@@ -21393,8 +21524,9 @@
       <c r="BO39" s="26"/>
       <c r="BP39" s="26"/>
       <c r="BQ39" s="26"/>
-    </row>
-    <row r="40" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR39" s="26"/>
+    </row>
+    <row r="40" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>681</v>
       </c>
@@ -21498,8 +21630,9 @@
       <c r="BO40" s="26"/>
       <c r="BP40" s="26"/>
       <c r="BQ40" s="26"/>
-    </row>
-    <row r="41" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR40" s="26"/>
+    </row>
+    <row r="41" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
         <v>680</v>
       </c>
@@ -21603,8 +21736,9 @@
       <c r="BO41" s="26"/>
       <c r="BP41" s="26"/>
       <c r="BQ41" s="26"/>
-    </row>
-    <row r="42" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR41" s="26"/>
+    </row>
+    <row r="42" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
         <v>679</v>
       </c>
@@ -21708,8 +21842,9 @@
       <c r="BO42" s="26"/>
       <c r="BP42" s="26"/>
       <c r="BQ42" s="26"/>
-    </row>
-    <row r="43" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR42" s="26"/>
+    </row>
+    <row r="43" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
         <v>678</v>
       </c>
@@ -21813,8 +21948,9 @@
       <c r="BO43" s="26"/>
       <c r="BP43" s="26"/>
       <c r="BQ43" s="26"/>
-    </row>
-    <row r="44" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR43" s="26"/>
+    </row>
+    <row r="44" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
         <v>677</v>
       </c>
@@ -21918,8 +22054,9 @@
       <c r="BO44" s="26"/>
       <c r="BP44" s="26"/>
       <c r="BQ44" s="26"/>
-    </row>
-    <row r="45" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR44" s="26"/>
+    </row>
+    <row r="45" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>676</v>
       </c>
@@ -22023,8 +22160,9 @@
       <c r="BO45" s="26"/>
       <c r="BP45" s="26"/>
       <c r="BQ45" s="26"/>
-    </row>
-    <row r="46" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR45" s="26"/>
+    </row>
+    <row r="46" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
         <v>675</v>
       </c>
@@ -22128,8 +22266,9 @@
       <c r="BO46" s="26"/>
       <c r="BP46" s="26"/>
       <c r="BQ46" s="26"/>
-    </row>
-    <row r="47" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR46" s="26"/>
+    </row>
+    <row r="47" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A47" s="25" t="s">
         <v>674</v>
       </c>
@@ -22233,8 +22372,9 @@
       <c r="BO47" s="26"/>
       <c r="BP47" s="26"/>
       <c r="BQ47" s="26"/>
-    </row>
-    <row r="48" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR47" s="26"/>
+    </row>
+    <row r="48" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A48" s="25" t="s">
         <v>673</v>
       </c>
@@ -22338,8 +22478,9 @@
       <c r="BO48" s="26"/>
       <c r="BP48" s="26"/>
       <c r="BQ48" s="26"/>
-    </row>
-    <row r="49" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR48" s="26"/>
+    </row>
+    <row r="49" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
         <v>672</v>
       </c>
@@ -22443,8 +22584,9 @@
       <c r="BO49" s="26"/>
       <c r="BP49" s="26"/>
       <c r="BQ49" s="26"/>
-    </row>
-    <row r="50" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR49" s="26"/>
+    </row>
+    <row r="50" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A50" s="25" t="s">
         <v>671</v>
       </c>
@@ -22548,8 +22690,9 @@
       <c r="BO50" s="26"/>
       <c r="BP50" s="26"/>
       <c r="BQ50" s="26"/>
-    </row>
-    <row r="51" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR50" s="26"/>
+    </row>
+    <row r="51" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A51" s="25" t="s">
         <v>670</v>
       </c>
@@ -22653,10 +22796,9 @@
       <c r="BO51" s="26"/>
       <c r="BP51" s="26"/>
       <c r="BQ51" s="26"/>
-    </row>
-    <row r="52" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:69" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR51" s="26"/>
+    </row>
+    <row r="54" spans="1:70" x14ac:dyDescent="0.25">
       <c r="A54" s="25"/>
     </row>
   </sheetData>
@@ -22667,7 +22809,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AF30"/>
+  <dimension ref="A1:AE30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -22680,7 +22822,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="9" width="16.42578125" customWidth="1"/>
-    <col min="11" max="31" width="20.7109375" style="33" customWidth="1"/>
+    <col min="11" max="31" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -22711,67 +22853,67 @@
       <c r="I1" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="33" t="s">
         <v>693</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="33" t="s">
         <v>692</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="M1" s="33" t="s">
         <v>690</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="N1" s="33" t="s">
         <v>689</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="O1" s="33" t="s">
         <v>688</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="33" t="s">
         <v>687</v>
       </c>
-      <c r="Q1" s="34" t="s">
+      <c r="Q1" s="33" t="s">
         <v>686</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="R1" s="33" t="s">
         <v>683</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="S1" s="33" t="s">
         <v>682</v>
       </c>
-      <c r="T1" s="34" t="s">
+      <c r="T1" s="33" t="s">
         <v>681</v>
       </c>
-      <c r="U1" s="34" t="s">
+      <c r="U1" s="33" t="s">
         <v>680</v>
       </c>
-      <c r="V1" s="34" t="s">
+      <c r="V1" s="33" t="s">
         <v>679</v>
       </c>
-      <c r="W1" s="34" t="s">
+      <c r="W1" s="33" t="s">
         <v>678</v>
       </c>
-      <c r="X1" s="34" t="s">
+      <c r="X1" s="33" t="s">
         <v>677</v>
       </c>
-      <c r="Y1" s="34" t="s">
+      <c r="Y1" s="33" t="s">
         <v>676</v>
       </c>
-      <c r="Z1" s="34" t="s">
+      <c r="Z1" s="33" t="s">
         <v>675</v>
       </c>
-      <c r="AA1" s="34" t="s">
+      <c r="AA1" s="33" t="s">
         <v>674</v>
       </c>
-      <c r="AB1" s="34" t="s">
+      <c r="AB1" s="33" t="s">
         <v>673</v>
       </c>
-      <c r="AC1" s="34" t="s">
+      <c r="AC1" s="33" t="s">
         <v>672</v>
       </c>
-      <c r="AD1" s="34" t="s">
+      <c r="AD1" s="33" t="s">
         <v>671</v>
       </c>
-      <c r="AE1" s="34" t="s">
+      <c r="AE1" s="33" t="s">
         <v>670</v>
       </c>
     </row>
@@ -22803,27 +22945,27 @@
       <c r="I2" s="21">
         <v>20</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35"/>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35"/>
-      <c r="X2" s="35"/>
-      <c r="Y2" s="35"/>
-      <c r="Z2" s="35"/>
-      <c r="AA2" s="35"/>
-      <c r="AB2" s="35"/>
-      <c r="AC2" s="35"/>
-      <c r="AD2" s="35"/>
-      <c r="AE2" s="35"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="34"/>
+      <c r="V2" s="34"/>
+      <c r="W2" s="34"/>
+      <c r="X2" s="34"/>
+      <c r="Y2" s="34"/>
+      <c r="Z2" s="34"/>
+      <c r="AA2" s="34"/>
+      <c r="AB2" s="34"/>
+      <c r="AC2" s="34"/>
+      <c r="AD2" s="34"/>
+      <c r="AE2" s="34"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -22853,27 +22995,27 @@
       <c r="I3" s="21">
         <v>21</v>
       </c>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
-      <c r="R3" s="35"/>
-      <c r="S3" s="35"/>
-      <c r="T3" s="35"/>
-      <c r="U3" s="35"/>
-      <c r="V3" s="35"/>
-      <c r="W3" s="35"/>
-      <c r="X3" s="35"/>
-      <c r="Y3" s="35"/>
-      <c r="Z3" s="35"/>
-      <c r="AA3" s="35"/>
-      <c r="AB3" s="35"/>
-      <c r="AC3" s="35"/>
-      <c r="AD3" s="35"/>
-      <c r="AE3" s="35"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="34"/>
+      <c r="V3" s="34"/>
+      <c r="W3" s="34"/>
+      <c r="X3" s="34"/>
+      <c r="Y3" s="34"/>
+      <c r="Z3" s="34"/>
+      <c r="AA3" s="34"/>
+      <c r="AB3" s="34"/>
+      <c r="AC3" s="34"/>
+      <c r="AD3" s="34"/>
+      <c r="AE3" s="34"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -22903,27 +23045,27 @@
       <c r="I4" s="21">
         <v>21.9</v>
       </c>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="35"/>
-      <c r="S4" s="35"/>
-      <c r="T4" s="35"/>
-      <c r="U4" s="35"/>
-      <c r="V4" s="35"/>
-      <c r="W4" s="35"/>
-      <c r="X4" s="35"/>
-      <c r="Y4" s="35"/>
-      <c r="Z4" s="35"/>
-      <c r="AA4" s="35"/>
-      <c r="AB4" s="35"/>
-      <c r="AC4" s="35"/>
-      <c r="AD4" s="35"/>
-      <c r="AE4" s="35"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="34"/>
+      <c r="U4" s="34"/>
+      <c r="V4" s="34"/>
+      <c r="W4" s="34"/>
+      <c r="X4" s="34"/>
+      <c r="Y4" s="34"/>
+      <c r="Z4" s="34"/>
+      <c r="AA4" s="34"/>
+      <c r="AB4" s="34"/>
+      <c r="AC4" s="34"/>
+      <c r="AD4" s="34"/>
+      <c r="AE4" s="34"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -22953,27 +23095,27 @@
       <c r="I5" s="21">
         <v>21.6</v>
       </c>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
-      <c r="R5" s="35"/>
-      <c r="S5" s="35"/>
-      <c r="T5" s="35"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="35"/>
-      <c r="W5" s="35"/>
-      <c r="X5" s="35"/>
-      <c r="Y5" s="35"/>
-      <c r="Z5" s="35"/>
-      <c r="AA5" s="35"/>
-      <c r="AB5" s="35"/>
-      <c r="AC5" s="35"/>
-      <c r="AD5" s="35"/>
-      <c r="AE5" s="35"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="34"/>
+      <c r="V5" s="34"/>
+      <c r="W5" s="34"/>
+      <c r="X5" s="34"/>
+      <c r="Y5" s="34"/>
+      <c r="Z5" s="34"/>
+      <c r="AA5" s="34"/>
+      <c r="AB5" s="34"/>
+      <c r="AC5" s="34"/>
+      <c r="AD5" s="34"/>
+      <c r="AE5" s="34"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -23003,27 +23145,27 @@
       <c r="I6" s="21">
         <v>22.1</v>
       </c>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="35"/>
-      <c r="S6" s="35"/>
-      <c r="T6" s="35"/>
-      <c r="U6" s="35"/>
-      <c r="V6" s="35"/>
-      <c r="W6" s="35"/>
-      <c r="X6" s="35"/>
-      <c r="Y6" s="35"/>
-      <c r="Z6" s="35"/>
-      <c r="AA6" s="35"/>
-      <c r="AB6" s="35"/>
-      <c r="AC6" s="35"/>
-      <c r="AD6" s="35"/>
-      <c r="AE6" s="35"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="34"/>
+      <c r="S6" s="34"/>
+      <c r="T6" s="34"/>
+      <c r="U6" s="34"/>
+      <c r="V6" s="34"/>
+      <c r="W6" s="34"/>
+      <c r="X6" s="34"/>
+      <c r="Y6" s="34"/>
+      <c r="Z6" s="34"/>
+      <c r="AA6" s="34"/>
+      <c r="AB6" s="34"/>
+      <c r="AC6" s="34"/>
+      <c r="AD6" s="34"/>
+      <c r="AE6" s="34"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -23053,27 +23195,27 @@
       <c r="I7" s="21">
         <v>21.7</v>
       </c>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="35"/>
-      <c r="R7" s="35"/>
-      <c r="S7" s="35"/>
-      <c r="T7" s="35"/>
-      <c r="U7" s="35"/>
-      <c r="V7" s="35"/>
-      <c r="W7" s="35"/>
-      <c r="X7" s="35"/>
-      <c r="Y7" s="35"/>
-      <c r="Z7" s="35"/>
-      <c r="AA7" s="35"/>
-      <c r="AB7" s="35"/>
-      <c r="AC7" s="35"/>
-      <c r="AD7" s="35"/>
-      <c r="AE7" s="35"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="34"/>
+      <c r="S7" s="34"/>
+      <c r="T7" s="34"/>
+      <c r="U7" s="34"/>
+      <c r="V7" s="34"/>
+      <c r="W7" s="34"/>
+      <c r="X7" s="34"/>
+      <c r="Y7" s="34"/>
+      <c r="Z7" s="34"/>
+      <c r="AA7" s="34"/>
+      <c r="AB7" s="34"/>
+      <c r="AC7" s="34"/>
+      <c r="AD7" s="34"/>
+      <c r="AE7" s="34"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -23103,27 +23245,27 @@
       <c r="I8" s="21">
         <v>17.2</v>
       </c>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="35"/>
-      <c r="P8" s="35"/>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="35"/>
-      <c r="S8" s="35"/>
-      <c r="T8" s="35"/>
-      <c r="U8" s="35"/>
-      <c r="V8" s="35"/>
-      <c r="W8" s="35"/>
-      <c r="X8" s="35"/>
-      <c r="Y8" s="35"/>
-      <c r="Z8" s="35"/>
-      <c r="AA8" s="35"/>
-      <c r="AB8" s="35"/>
-      <c r="AC8" s="35"/>
-      <c r="AD8" s="35"/>
-      <c r="AE8" s="35"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="34"/>
+      <c r="S8" s="34"/>
+      <c r="T8" s="34"/>
+      <c r="U8" s="34"/>
+      <c r="V8" s="34"/>
+      <c r="W8" s="34"/>
+      <c r="X8" s="34"/>
+      <c r="Y8" s="34"/>
+      <c r="Z8" s="34"/>
+      <c r="AA8" s="34"/>
+      <c r="AB8" s="34"/>
+      <c r="AC8" s="34"/>
+      <c r="AD8" s="34"/>
+      <c r="AE8" s="34"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -23153,27 +23295,27 @@
       <c r="I9" s="21">
         <v>17</v>
       </c>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="35"/>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="35"/>
-      <c r="S9" s="35"/>
-      <c r="T9" s="35"/>
-      <c r="U9" s="35"/>
-      <c r="V9" s="35"/>
-      <c r="W9" s="35"/>
-      <c r="X9" s="35"/>
-      <c r="Y9" s="35"/>
-      <c r="Z9" s="35"/>
-      <c r="AA9" s="35"/>
-      <c r="AB9" s="35"/>
-      <c r="AC9" s="35"/>
-      <c r="AD9" s="35"/>
-      <c r="AE9" s="35"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="34"/>
+      <c r="T9" s="34"/>
+      <c r="U9" s="34"/>
+      <c r="V9" s="34"/>
+      <c r="W9" s="34"/>
+      <c r="X9" s="34"/>
+      <c r="Y9" s="34"/>
+      <c r="Z9" s="34"/>
+      <c r="AA9" s="34"/>
+      <c r="AB9" s="34"/>
+      <c r="AC9" s="34"/>
+      <c r="AD9" s="34"/>
+      <c r="AE9" s="34"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -23203,27 +23345,27 @@
       <c r="I10" s="21">
         <v>17</v>
       </c>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="35"/>
-      <c r="R10" s="35"/>
-      <c r="S10" s="35"/>
-      <c r="T10" s="35"/>
-      <c r="U10" s="35"/>
-      <c r="V10" s="35"/>
-      <c r="W10" s="35"/>
-      <c r="X10" s="35"/>
-      <c r="Y10" s="35"/>
-      <c r="Z10" s="35"/>
-      <c r="AA10" s="35"/>
-      <c r="AB10" s="35"/>
-      <c r="AC10" s="35"/>
-      <c r="AD10" s="35"/>
-      <c r="AE10" s="35"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+      <c r="Q10" s="34"/>
+      <c r="R10" s="34"/>
+      <c r="S10" s="34"/>
+      <c r="T10" s="34"/>
+      <c r="U10" s="34"/>
+      <c r="V10" s="34"/>
+      <c r="W10" s="34"/>
+      <c r="X10" s="34"/>
+      <c r="Y10" s="34"/>
+      <c r="Z10" s="34"/>
+      <c r="AA10" s="34"/>
+      <c r="AB10" s="34"/>
+      <c r="AC10" s="34"/>
+      <c r="AD10" s="34"/>
+      <c r="AE10" s="34"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -23253,27 +23395,27 @@
       <c r="I11" s="21">
         <v>17.600000000000001</v>
       </c>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="35"/>
-      <c r="S11" s="35"/>
-      <c r="T11" s="35"/>
-      <c r="U11" s="35"/>
-      <c r="V11" s="35"/>
-      <c r="W11" s="35"/>
-      <c r="X11" s="35"/>
-      <c r="Y11" s="35"/>
-      <c r="Z11" s="35"/>
-      <c r="AA11" s="35"/>
-      <c r="AB11" s="35"/>
-      <c r="AC11" s="35"/>
-      <c r="AD11" s="35"/>
-      <c r="AE11" s="35"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="34"/>
+      <c r="T11" s="34"/>
+      <c r="U11" s="34"/>
+      <c r="V11" s="34"/>
+      <c r="W11" s="34"/>
+      <c r="X11" s="34"/>
+      <c r="Y11" s="34"/>
+      <c r="Z11" s="34"/>
+      <c r="AA11" s="34"/>
+      <c r="AB11" s="34"/>
+      <c r="AC11" s="34"/>
+      <c r="AD11" s="34"/>
+      <c r="AE11" s="34"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -23303,27 +23445,27 @@
       <c r="I12" s="21">
         <v>21</v>
       </c>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="35"/>
-      <c r="R12" s="35"/>
-      <c r="S12" s="35"/>
-      <c r="T12" s="35"/>
-      <c r="U12" s="35"/>
-      <c r="V12" s="35"/>
-      <c r="W12" s="35"/>
-      <c r="X12" s="35"/>
-      <c r="Y12" s="35"/>
-      <c r="Z12" s="35"/>
-      <c r="AA12" s="35"/>
-      <c r="AB12" s="35"/>
-      <c r="AC12" s="35"/>
-      <c r="AD12" s="35"/>
-      <c r="AE12" s="35"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="34"/>
+      <c r="T12" s="34"/>
+      <c r="U12" s="34"/>
+      <c r="V12" s="34"/>
+      <c r="W12" s="34"/>
+      <c r="X12" s="34"/>
+      <c r="Y12" s="34"/>
+      <c r="Z12" s="34"/>
+      <c r="AA12" s="34"/>
+      <c r="AB12" s="34"/>
+      <c r="AC12" s="34"/>
+      <c r="AD12" s="34"/>
+      <c r="AE12" s="34"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -23353,27 +23495,27 @@
       <c r="I13" s="21">
         <v>22.6</v>
       </c>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="35"/>
-      <c r="S13" s="35"/>
-      <c r="T13" s="35"/>
-      <c r="U13" s="35"/>
-      <c r="V13" s="35"/>
-      <c r="W13" s="35"/>
-      <c r="X13" s="35"/>
-      <c r="Y13" s="35"/>
-      <c r="Z13" s="35"/>
-      <c r="AA13" s="35"/>
-      <c r="AB13" s="35"/>
-      <c r="AC13" s="35"/>
-      <c r="AD13" s="35"/>
-      <c r="AE13" s="35"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="34"/>
+      <c r="S13" s="34"/>
+      <c r="T13" s="34"/>
+      <c r="U13" s="34"/>
+      <c r="V13" s="34"/>
+      <c r="W13" s="34"/>
+      <c r="X13" s="34"/>
+      <c r="Y13" s="34"/>
+      <c r="Z13" s="34"/>
+      <c r="AA13" s="34"/>
+      <c r="AB13" s="34"/>
+      <c r="AC13" s="34"/>
+      <c r="AD13" s="34"/>
+      <c r="AE13" s="34"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -23403,27 +23545,27 @@
       <c r="I14" s="21">
         <v>20.100000000000001</v>
       </c>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
-      <c r="T14" s="35"/>
-      <c r="U14" s="35"/>
-      <c r="V14" s="35"/>
-      <c r="W14" s="35"/>
-      <c r="X14" s="35"/>
-      <c r="Y14" s="35"/>
-      <c r="Z14" s="35"/>
-      <c r="AA14" s="35"/>
-      <c r="AB14" s="35"/>
-      <c r="AC14" s="35"/>
-      <c r="AD14" s="35"/>
-      <c r="AE14" s="35"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="34"/>
+      <c r="T14" s="34"/>
+      <c r="U14" s="34"/>
+      <c r="V14" s="34"/>
+      <c r="W14" s="34"/>
+      <c r="X14" s="34"/>
+      <c r="Y14" s="34"/>
+      <c r="Z14" s="34"/>
+      <c r="AA14" s="34"/>
+      <c r="AB14" s="34"/>
+      <c r="AC14" s="34"/>
+      <c r="AD14" s="34"/>
+      <c r="AE14" s="34"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -23453,27 +23595,27 @@
       <c r="I15" s="21">
         <v>19.3</v>
       </c>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="35"/>
-      <c r="S15" s="35"/>
-      <c r="T15" s="35"/>
-      <c r="U15" s="35"/>
-      <c r="V15" s="35"/>
-      <c r="W15" s="35"/>
-      <c r="X15" s="35"/>
-      <c r="Y15" s="35"/>
-      <c r="Z15" s="35"/>
-      <c r="AA15" s="35"/>
-      <c r="AB15" s="35"/>
-      <c r="AC15" s="35"/>
-      <c r="AD15" s="35"/>
-      <c r="AE15" s="35"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="34"/>
+      <c r="S15" s="34"/>
+      <c r="T15" s="34"/>
+      <c r="U15" s="34"/>
+      <c r="V15" s="34"/>
+      <c r="W15" s="34"/>
+      <c r="X15" s="34"/>
+      <c r="Y15" s="34"/>
+      <c r="Z15" s="34"/>
+      <c r="AA15" s="34"/>
+      <c r="AB15" s="34"/>
+      <c r="AC15" s="34"/>
+      <c r="AD15" s="34"/>
+      <c r="AE15" s="34"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -23503,29 +23645,29 @@
       <c r="I16" s="21">
         <v>19.087311490605728</v>
       </c>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="35"/>
-      <c r="S16" s="35"/>
-      <c r="T16" s="35"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="35"/>
-      <c r="X16" s="35"/>
-      <c r="Y16" s="35"/>
-      <c r="Z16" s="35"/>
-      <c r="AA16" s="35"/>
-      <c r="AB16" s="35"/>
-      <c r="AC16" s="35"/>
-      <c r="AD16" s="35"/>
-      <c r="AE16" s="35"/>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="34"/>
+      <c r="T16" s="34"/>
+      <c r="U16" s="34"/>
+      <c r="V16" s="34"/>
+      <c r="W16" s="34"/>
+      <c r="X16" s="34"/>
+      <c r="Y16" s="34"/>
+      <c r="Z16" s="34"/>
+      <c r="AA16" s="34"/>
+      <c r="AB16" s="34"/>
+      <c r="AC16" s="34"/>
+      <c r="AD16" s="34"/>
+      <c r="AE16" s="34"/>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2010</v>
       </c>
@@ -23553,29 +23695,29 @@
       <c r="I17" s="21">
         <v>18.7</v>
       </c>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="35"/>
-      <c r="S17" s="35"/>
-      <c r="T17" s="35"/>
-      <c r="U17" s="35"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="35"/>
-      <c r="X17" s="35"/>
-      <c r="Y17" s="35"/>
-      <c r="Z17" s="35"/>
-      <c r="AA17" s="35"/>
-      <c r="AB17" s="35"/>
-      <c r="AC17" s="35"/>
-      <c r="AD17" s="35"/>
-      <c r="AE17" s="35"/>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="34"/>
+      <c r="T17" s="34"/>
+      <c r="U17" s="34"/>
+      <c r="V17" s="34"/>
+      <c r="W17" s="34"/>
+      <c r="X17" s="34"/>
+      <c r="Y17" s="34"/>
+      <c r="Z17" s="34"/>
+      <c r="AA17" s="34"/>
+      <c r="AB17" s="34"/>
+      <c r="AC17" s="34"/>
+      <c r="AD17" s="34"/>
+      <c r="AE17" s="34"/>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2011</v>
       </c>
@@ -23603,29 +23745,29 @@
       <c r="I18" s="21">
         <v>19.260093482899016</v>
       </c>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="35"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="35"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="35"/>
-      <c r="X18" s="35"/>
-      <c r="Y18" s="35"/>
-      <c r="Z18" s="35"/>
-      <c r="AA18" s="35"/>
-      <c r="AB18" s="35"/>
-      <c r="AC18" s="35"/>
-      <c r="AD18" s="35"/>
-      <c r="AE18" s="35"/>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="34"/>
+      <c r="S18" s="34"/>
+      <c r="T18" s="34"/>
+      <c r="U18" s="34"/>
+      <c r="V18" s="34"/>
+      <c r="W18" s="34"/>
+      <c r="X18" s="34"/>
+      <c r="Y18" s="34"/>
+      <c r="Z18" s="34"/>
+      <c r="AA18" s="34"/>
+      <c r="AB18" s="34"/>
+      <c r="AC18" s="34"/>
+      <c r="AD18" s="34"/>
+      <c r="AE18" s="34"/>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2012</v>
       </c>
@@ -23653,71 +23795,71 @@
       <c r="I19" s="21">
         <v>19.984181600623746</v>
       </c>
-      <c r="K19" s="35">
+      <c r="K19" s="34">
         <v>10660.443499999999</v>
       </c>
-      <c r="L19" s="35">
+      <c r="L19" s="34">
         <v>1432.2945</v>
       </c>
-      <c r="M19" s="35">
+      <c r="M19" s="34">
         <v>249.89350000000002</v>
       </c>
-      <c r="N19" s="35">
+      <c r="N19" s="34">
         <v>3112.3870000000002</v>
       </c>
-      <c r="O19" s="35">
+      <c r="O19" s="34">
         <v>89.460250000000002</v>
       </c>
-      <c r="P19" s="35">
+      <c r="P19" s="34">
         <v>59.448500000000003</v>
       </c>
-      <c r="Q19" s="35">
+      <c r="Q19" s="34">
         <v>2231.9047500000001</v>
       </c>
-      <c r="R19" s="35">
+      <c r="R19" s="34">
         <v>6863.9697500000002</v>
       </c>
-      <c r="S19" s="35">
+      <c r="S19" s="34">
         <v>2616.8715000000002</v>
       </c>
-      <c r="T19" s="35">
+      <c r="T19" s="34">
         <v>1571.3187500000001</v>
       </c>
-      <c r="U19" s="35">
+      <c r="U19" s="34">
         <v>338.03375</v>
       </c>
-      <c r="V19" s="35">
+      <c r="V19" s="34">
         <v>437.43799999999999</v>
       </c>
-      <c r="W19" s="35">
+      <c r="W19" s="34">
         <v>170.4265</v>
       </c>
-      <c r="X19" s="35">
+      <c r="X19" s="34">
         <v>188.90125</v>
       </c>
-      <c r="Y19" s="35">
+      <c r="Y19" s="34">
         <v>936.55849999999998</v>
       </c>
-      <c r="Z19" s="35">
+      <c r="Z19" s="34">
         <v>1957.98875</v>
       </c>
-      <c r="AA19" s="35">
+      <c r="AA19" s="34">
         <v>1200.0219999999999</v>
       </c>
-      <c r="AB19" s="35">
+      <c r="AB19" s="34">
         <v>437.64800000000002</v>
       </c>
-      <c r="AC19" s="35">
+      <c r="AC19" s="34">
         <v>327.77875</v>
       </c>
-      <c r="AD19" s="35">
+      <c r="AD19" s="34">
         <v>2715.1417500000002</v>
       </c>
-      <c r="AE19" s="35">
+      <c r="AE19" s="34">
         <v>2.2725</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2013</v>
       </c>
@@ -23745,71 +23887,71 @@
       <c r="I20" s="21">
         <v>19.338649090166786</v>
       </c>
-      <c r="K20" s="35">
+      <c r="K20" s="34">
         <v>10428.695750000001</v>
       </c>
-      <c r="L20" s="35">
+      <c r="L20" s="34">
         <v>1406.6915000000001</v>
       </c>
-      <c r="M20" s="35">
+      <c r="M20" s="34">
         <v>250.28675000000001</v>
       </c>
-      <c r="N20" s="35">
+      <c r="N20" s="34">
         <v>3159.3564999999999</v>
       </c>
-      <c r="O20" s="35">
+      <c r="O20" s="34">
         <v>94.4375</v>
       </c>
-      <c r="P20" s="35">
+      <c r="P20" s="34">
         <v>60.097000000000001</v>
       </c>
-      <c r="Q20" s="35">
+      <c r="Q20" s="34">
         <v>2372.7269999999999</v>
       </c>
-      <c r="R20" s="35">
+      <c r="R20" s="34">
         <v>7105.4902499999998</v>
       </c>
-      <c r="S20" s="35">
+      <c r="S20" s="34">
         <v>2734.2240000000002</v>
       </c>
-      <c r="T20" s="35">
+      <c r="T20" s="34">
         <v>1606.8902499999999</v>
       </c>
-      <c r="U20" s="35">
+      <c r="U20" s="34">
         <v>344.45125000000002</v>
       </c>
-      <c r="V20" s="35">
+      <c r="V20" s="34">
         <v>448.21800000000002</v>
       </c>
-      <c r="W20" s="35">
+      <c r="W20" s="34">
         <v>172.61799999999999</v>
       </c>
-      <c r="X20" s="35">
+      <c r="X20" s="34">
         <v>193.99700000000001</v>
       </c>
-      <c r="Y20" s="35">
+      <c r="Y20" s="34">
         <v>1015.7535</v>
       </c>
-      <c r="Z20" s="35">
+      <c r="Z20" s="34">
         <v>1965.4057500000001</v>
       </c>
-      <c r="AA20" s="35">
+      <c r="AA20" s="34">
         <v>1225.6490000000001</v>
       </c>
-      <c r="AB20" s="35">
+      <c r="AB20" s="34">
         <v>468.85025000000002</v>
       </c>
-      <c r="AC20" s="35">
+      <c r="AC20" s="34">
         <v>347.25475</v>
       </c>
-      <c r="AD20" s="35">
+      <c r="AD20" s="34">
         <v>2712.7429999999999</v>
       </c>
-      <c r="AE20" s="35">
+      <c r="AE20" s="34">
         <v>3.8767499999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2014</v>
       </c>
@@ -23837,71 +23979,71 @@
       <c r="I21" s="21">
         <v>18.41672363764841</v>
       </c>
-      <c r="K21" s="35">
+      <c r="K21" s="34">
         <v>10404.944333333335</v>
       </c>
-      <c r="L21" s="35">
+      <c r="L21" s="34">
         <v>1396.4763333333333</v>
       </c>
-      <c r="M21" s="35">
+      <c r="M21" s="34">
         <v>239.42033333333336</v>
       </c>
-      <c r="N21" s="35">
+      <c r="N21" s="34">
         <v>3212.1773333333335</v>
       </c>
-      <c r="O21" s="35">
+      <c r="O21" s="34">
         <v>85.983666666666679</v>
       </c>
-      <c r="P21" s="35">
+      <c r="P21" s="34">
         <v>51.211333333333336</v>
       </c>
-      <c r="Q21" s="35">
+      <c r="Q21" s="34">
         <v>2578.3216666666667</v>
       </c>
-      <c r="R21" s="35">
+      <c r="R21" s="34">
         <v>7248.3973333333333</v>
       </c>
-      <c r="S21" s="35">
+      <c r="S21" s="34">
         <v>2686.2336666666665</v>
       </c>
-      <c r="T21" s="35">
+      <c r="T21" s="34">
         <v>1694.479</v>
       </c>
-      <c r="U21" s="35">
+      <c r="U21" s="34">
         <v>352.0556666666667</v>
       </c>
-      <c r="V21" s="35">
+      <c r="V21" s="34">
         <v>491.29066666666671</v>
       </c>
-      <c r="W21" s="35">
+      <c r="W21" s="34">
         <v>167.55500000000001</v>
       </c>
-      <c r="X21" s="35">
+      <c r="X21" s="34">
         <v>208.89333333333335</v>
       </c>
-      <c r="Y21" s="35">
+      <c r="Y21" s="34">
         <v>1085.127</v>
       </c>
-      <c r="Z21" s="35">
+      <c r="Z21" s="34">
         <v>1963.9393333333333</v>
       </c>
-      <c r="AA21" s="35">
+      <c r="AA21" s="34">
         <v>1254.2953333333332</v>
       </c>
-      <c r="AB21" s="35">
+      <c r="AB21" s="34">
         <v>480.31666666666672</v>
       </c>
-      <c r="AC21" s="35">
+      <c r="AC21" s="34">
         <v>348.86966666666672</v>
       </c>
-      <c r="AD21" s="35">
+      <c r="AD21" s="34">
         <v>2694.3966666666665</v>
       </c>
-      <c r="AE21" s="35">
+      <c r="AE21" s="34">
         <v>6.8713333333333333</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2015</v>
       </c>
@@ -23929,71 +24071,71 @@
       <c r="I22" s="21">
         <v>18.5</v>
       </c>
-      <c r="K22" s="35">
+      <c r="K22" s="34">
         <v>9972.65625</v>
       </c>
-      <c r="L22" s="35">
+      <c r="L22" s="34">
         <v>1320.9870000000001</v>
       </c>
-      <c r="M22" s="35">
+      <c r="M22" s="34">
         <v>234.51499999999999</v>
       </c>
-      <c r="N22" s="35">
+      <c r="N22" s="34">
         <v>3208.6109999999999</v>
       </c>
-      <c r="O22" s="35">
+      <c r="O22" s="34">
         <v>83.243750000000006</v>
       </c>
-      <c r="P22" s="35">
+      <c r="P22" s="34">
         <v>51.694249999999997</v>
       </c>
-      <c r="Q22" s="35">
+      <c r="Q22" s="34">
         <v>2696.8139999999999</v>
       </c>
-      <c r="R22" s="35">
+      <c r="R22" s="34">
         <v>7312.9444999999996</v>
       </c>
-      <c r="S22" s="35">
+      <c r="S22" s="34">
         <v>2781.3657499999999</v>
       </c>
-      <c r="T22" s="35">
+      <c r="T22" s="34">
         <v>1716.2962500000001</v>
       </c>
-      <c r="U22" s="35">
+      <c r="U22" s="34">
         <v>381.00024999999999</v>
       </c>
-      <c r="V22" s="35">
+      <c r="V22" s="34">
         <v>497.56099999999998</v>
       </c>
-      <c r="W22" s="35">
+      <c r="W22" s="34">
         <v>184.10300000000001</v>
       </c>
-      <c r="X22" s="35">
+      <c r="X22" s="34">
         <v>208.47225</v>
       </c>
-      <c r="Y22" s="35">
+      <c r="Y22" s="34">
         <v>1138.778</v>
       </c>
-      <c r="Z22" s="35">
+      <c r="Z22" s="34">
         <v>2096.2435</v>
       </c>
-      <c r="AA22" s="35">
+      <c r="AA22" s="34">
         <v>1282.1982499999999</v>
       </c>
-      <c r="AB22" s="35">
+      <c r="AB22" s="34">
         <v>493.75175000000002</v>
       </c>
-      <c r="AC22" s="35">
+      <c r="AC22" s="34">
         <v>343.154</v>
       </c>
-      <c r="AD22" s="35">
+      <c r="AD22" s="34">
         <v>2733.1202499999999</v>
       </c>
-      <c r="AE22" s="35">
+      <c r="AE22" s="34">
         <v>3.3242500000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2016</v>
       </c>
@@ -24021,71 +24163,71 @@
       <c r="I23" s="21">
         <v>18.3</v>
       </c>
-      <c r="K23" s="35">
+      <c r="K23" s="34">
         <v>9801.11175</v>
       </c>
-      <c r="L23" s="35">
+      <c r="L23" s="34">
         <v>1262.58475</v>
       </c>
-      <c r="M23" s="35">
+      <c r="M23" s="34">
         <v>218.7765</v>
       </c>
-      <c r="N23" s="35">
+      <c r="N23" s="34">
         <v>3403.9629999999997</v>
       </c>
-      <c r="O23" s="35">
+      <c r="O23" s="34">
         <v>91.436499999999995</v>
       </c>
-      <c r="P23" s="35">
+      <c r="P23" s="34">
         <v>67.64425</v>
       </c>
-      <c r="Q23" s="35">
+      <c r="Q23" s="34">
         <v>3377.6685000000002</v>
       </c>
-      <c r="R23" s="35">
+      <c r="R23" s="34">
         <v>8039.2467499999993</v>
       </c>
-      <c r="S23" s="35">
+      <c r="S23" s="34">
         <v>3037.8177500000002</v>
       </c>
-      <c r="T23" s="35">
+      <c r="T23" s="34">
         <v>1777.24</v>
       </c>
-      <c r="U23" s="35">
+      <c r="U23" s="34">
         <v>366.48975000000007</v>
       </c>
-      <c r="V23" s="35">
+      <c r="V23" s="34">
         <v>513.846</v>
       </c>
-      <c r="W23" s="35">
+      <c r="W23" s="34">
         <v>193.03750000000002</v>
       </c>
-      <c r="X23" s="35">
+      <c r="X23" s="34">
         <v>212.64449999999999</v>
       </c>
-      <c r="Y23" s="35">
+      <c r="Y23" s="34">
         <v>1370.7760000000001</v>
       </c>
-      <c r="Z23" s="35">
+      <c r="Z23" s="34">
         <v>2195.6932500000003</v>
       </c>
-      <c r="AA23" s="35">
+      <c r="AA23" s="34">
         <v>1303.9195</v>
       </c>
-      <c r="AB23" s="35">
+      <c r="AB23" s="34">
         <v>501.709</v>
       </c>
-      <c r="AC23" s="35">
+      <c r="AC23" s="34">
         <v>361.28475000000003</v>
       </c>
-      <c r="AD23" s="35">
+      <c r="AD23" s="34">
         <v>2897.7039999999997</v>
       </c>
-      <c r="AE23" s="35">
+      <c r="AE23" s="34">
         <v>3.2734999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2017</v>
       </c>
@@ -24113,71 +24255,71 @@
       <c r="I24" s="21">
         <v>16.100000000000001</v>
       </c>
-      <c r="K24" s="35">
+      <c r="K24" s="34">
         <v>9066.4807500000006</v>
       </c>
-      <c r="L24" s="35">
+      <c r="L24" s="34">
         <v>1194.38825</v>
       </c>
-      <c r="M24" s="35">
+      <c r="M24" s="34">
         <v>203.33250000000001</v>
       </c>
-      <c r="N24" s="35">
+      <c r="N24" s="34">
         <v>3481.2064999999998</v>
       </c>
-      <c r="O24" s="35">
+      <c r="O24" s="34">
         <v>79.866500000000002</v>
       </c>
-      <c r="P24" s="35">
+      <c r="P24" s="34">
         <v>68.668499999999995</v>
       </c>
-      <c r="Q24" s="35">
+      <c r="Q24" s="34">
         <v>3536.8052499999999</v>
       </c>
-      <c r="R24" s="35">
+      <c r="R24" s="34">
         <v>7899.74125</v>
       </c>
-      <c r="S24" s="35">
+      <c r="S24" s="34">
         <v>3127.3642500000001</v>
       </c>
-      <c r="T24" s="35">
+      <c r="T24" s="34">
         <v>1739.6975</v>
       </c>
-      <c r="U24" s="35">
+      <c r="U24" s="34">
         <v>396.66750000000002</v>
       </c>
-      <c r="V24" s="35">
+      <c r="V24" s="34">
         <v>506.298</v>
       </c>
-      <c r="W24" s="35">
+      <c r="W24" s="34">
         <v>185.9965</v>
       </c>
-      <c r="X24" s="35">
+      <c r="X24" s="34">
         <v>247.29400000000001</v>
       </c>
-      <c r="Y24" s="35">
+      <c r="Y24" s="34">
         <v>1474.9827499999999</v>
       </c>
-      <c r="Z24" s="35">
+      <c r="Z24" s="34">
         <v>2408.2069999999999</v>
       </c>
-      <c r="AA24" s="35">
+      <c r="AA24" s="34">
         <v>1204.4100000000001</v>
       </c>
-      <c r="AB24" s="35">
+      <c r="AB24" s="34">
         <v>484.36750000000001</v>
       </c>
-      <c r="AC24" s="35">
+      <c r="AC24" s="34">
         <v>325.40724999999998</v>
       </c>
-      <c r="AD24" s="35">
+      <c r="AD24" s="34">
         <v>2701.0129999999999</v>
       </c>
-      <c r="AE24" s="35">
+      <c r="AE24" s="34">
         <v>1.6074999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2018</v>
       </c>
@@ -24205,72 +24347,71 @@
       <c r="I25" s="21">
         <v>16.399999999999999</v>
       </c>
-      <c r="K25" s="35">
+      <c r="K25" s="34">
         <v>8872.2567500000005</v>
       </c>
-      <c r="L25" s="35">
+      <c r="L25" s="34">
         <v>1125.9902500000001</v>
       </c>
-      <c r="M25" s="35">
+      <c r="M25" s="34">
         <v>206.50450000000001</v>
       </c>
-      <c r="N25" s="35">
+      <c r="N25" s="34">
         <v>3625.2837500000001</v>
       </c>
-      <c r="O25" s="35">
+      <c r="O25" s="34">
         <v>87.583999999999989</v>
       </c>
-      <c r="P25" s="35">
+      <c r="P25" s="34">
         <v>61.377000000000002</v>
       </c>
-      <c r="Q25" s="35">
+      <c r="Q25" s="34">
         <v>3865.4722499999998</v>
       </c>
-      <c r="R25" s="35">
+      <c r="R25" s="34">
         <v>7993.9129999999996</v>
       </c>
-      <c r="S25" s="35">
+      <c r="S25" s="34">
         <v>3220.1837500000001</v>
       </c>
-      <c r="T25" s="35">
+      <c r="T25" s="34">
         <v>1727.4402500000001</v>
       </c>
-      <c r="U25" s="35">
+      <c r="U25" s="34">
         <v>403.49475000000001</v>
       </c>
-      <c r="V25" s="35">
+      <c r="V25" s="34">
         <v>540.44375000000002</v>
       </c>
-      <c r="W25" s="35">
+      <c r="W25" s="34">
         <v>203.7055</v>
       </c>
-      <c r="X25" s="35">
+      <c r="X25" s="34">
         <v>274.62925000000001</v>
       </c>
-      <c r="Y25" s="35">
+      <c r="Y25" s="34">
         <v>1583.8875</v>
       </c>
-      <c r="Z25" s="35">
+      <c r="Z25" s="34">
         <v>2559.4537500000001</v>
       </c>
-      <c r="AA25" s="35">
+      <c r="AA25" s="34">
         <v>1196.6400000000001</v>
       </c>
-      <c r="AB25" s="35">
+      <c r="AB25" s="34">
         <v>517.58325000000002</v>
       </c>
-      <c r="AC25" s="35">
+      <c r="AC25" s="34">
         <v>363.09724999999997</v>
       </c>
-      <c r="AD25" s="35">
+      <c r="AD25" s="34">
         <v>2724.06475</v>
       </c>
-      <c r="AE25" s="36">
+      <c r="AE25" s="34">
         <v>3.530250000000001</v>
       </c>
-      <c r="AF25" s="33"/>
-    </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2019</v>
       </c>
@@ -24298,72 +24439,71 @@
       <c r="I26" s="21">
         <v>13.77815166027389</v>
       </c>
-      <c r="K26" s="35">
+      <c r="K26" s="34">
         <v>8070.0662499999999</v>
       </c>
-      <c r="L26" s="35">
+      <c r="L26" s="34">
         <v>1255.126</v>
       </c>
-      <c r="M26" s="35">
+      <c r="M26" s="34">
         <v>176.56825000000001</v>
       </c>
-      <c r="N26" s="35">
+      <c r="N26" s="34">
         <v>3650.78775</v>
       </c>
-      <c r="O26" s="35">
+      <c r="O26" s="34">
         <v>90.5595</v>
       </c>
-      <c r="P26" s="35">
+      <c r="P26" s="34">
         <v>64.483249999999998</v>
       </c>
-      <c r="Q26" s="35">
+      <c r="Q26" s="34">
         <v>4123.3215</v>
       </c>
-      <c r="R26" s="35">
+      <c r="R26" s="34">
         <v>8368.490749999999</v>
       </c>
-      <c r="S26" s="35">
+      <c r="S26" s="34">
         <v>3424.13825</v>
       </c>
-      <c r="T26" s="35">
+      <c r="T26" s="34">
         <v>1932.9702500000001</v>
       </c>
-      <c r="U26" s="35">
+      <c r="U26" s="34">
         <v>433.09775000000002</v>
       </c>
-      <c r="V26" s="35">
+      <c r="V26" s="34">
         <v>585.54950000000008</v>
       </c>
-      <c r="W26" s="35">
+      <c r="W26" s="34">
         <v>236.70500000000001</v>
       </c>
-      <c r="X26" s="35">
+      <c r="X26" s="34">
         <v>309.97000000000003</v>
       </c>
-      <c r="Y26" s="35">
+      <c r="Y26" s="34">
         <v>1692.36</v>
       </c>
-      <c r="Z26" s="35">
+      <c r="Z26" s="34">
         <v>2723.6089999999999</v>
       </c>
-      <c r="AA26" s="35">
+      <c r="AA26" s="34">
         <v>1266.97</v>
       </c>
-      <c r="AB26" s="35">
+      <c r="AB26" s="34">
         <v>542.81275000000005</v>
       </c>
-      <c r="AC26" s="35">
+      <c r="AC26" s="34">
         <v>401.74</v>
       </c>
-      <c r="AD26" s="35">
+      <c r="AD26" s="34">
         <v>2588.1622499999999</v>
       </c>
-      <c r="AE26" s="36">
+      <c r="AE26" s="34">
         <v>0.52550000000000008</v>
       </c>
-      <c r="AF26" s="33"/>
-    </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2020</v>
       </c>
@@ -24391,72 +24531,71 @@
       <c r="I27" s="21">
         <v>16.2</v>
       </c>
-      <c r="K27" s="35">
+      <c r="K27" s="34">
         <v>8574.1839999999993</v>
       </c>
-      <c r="L27" s="35">
+      <c r="L27" s="34">
         <v>1179.499</v>
       </c>
-      <c r="M27" s="35">
+      <c r="M27" s="34">
         <v>184.001</v>
       </c>
-      <c r="N27" s="35">
+      <c r="N27" s="34">
         <v>3183.6959999999999</v>
       </c>
-      <c r="O27" s="35">
+      <c r="O27" s="34">
         <v>80.938999999999993</v>
       </c>
-      <c r="P27" s="35">
+      <c r="P27" s="34">
         <v>58.109000000000002</v>
       </c>
-      <c r="Q27" s="35">
+      <c r="Q27" s="34">
         <v>3699.5619999999999</v>
       </c>
-      <c r="R27" s="35">
+      <c r="R27" s="34">
         <v>8081.0479999999998</v>
       </c>
-      <c r="S27" s="35">
+      <c r="S27" s="34">
         <v>2932.288</v>
       </c>
-      <c r="T27" s="35">
+      <c r="T27" s="34">
         <v>1468.16</v>
       </c>
-      <c r="U27" s="35">
+      <c r="U27" s="34">
         <v>349.64699999999999</v>
       </c>
-      <c r="V27" s="35">
+      <c r="V27" s="34">
         <v>555.76199999999994</v>
       </c>
-      <c r="W27" s="35">
+      <c r="W27" s="34">
         <v>191.977</v>
       </c>
-      <c r="X27" s="35">
+      <c r="X27" s="34">
         <v>260.32100000000003</v>
       </c>
-      <c r="Y27" s="35">
+      <c r="Y27" s="34">
         <v>1608.915</v>
       </c>
-      <c r="Z27" s="35">
+      <c r="Z27" s="34">
         <v>2563.3180000000002</v>
       </c>
-      <c r="AA27" s="35">
+      <c r="AA27" s="34">
         <v>1286.059</v>
       </c>
-      <c r="AB27" s="35">
+      <c r="AB27" s="34">
         <v>542.36599999999999</v>
       </c>
-      <c r="AC27" s="35">
+      <c r="AC27" s="34">
         <v>230.41499999999999</v>
       </c>
-      <c r="AD27" s="35">
+      <c r="AD27" s="34">
         <v>2345.681</v>
       </c>
-      <c r="AE27" s="36">
+      <c r="AE27" s="34">
         <v>1.8979999999999999</v>
       </c>
-      <c r="AF27" s="33"/>
-    </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2021</v>
       </c>
@@ -24484,72 +24623,71 @@
       <c r="I28" s="21">
         <v>15.919764703947065</v>
       </c>
-      <c r="K28" s="35">
+      <c r="K28" s="34">
         <v>9352.7279999999992</v>
       </c>
-      <c r="L28" s="35">
+      <c r="L28" s="34">
         <v>1303.664</v>
       </c>
-      <c r="M28" s="35">
+      <c r="M28" s="34">
         <v>169.72300000000001</v>
       </c>
-      <c r="N28" s="35">
+      <c r="N28" s="34">
         <v>3453.009</v>
       </c>
-      <c r="O28" s="35">
+      <c r="O28" s="34">
         <v>75.843999999999994</v>
       </c>
-      <c r="P28" s="35">
+      <c r="P28" s="34">
         <v>74.724999999999994</v>
       </c>
-      <c r="Q28" s="35">
+      <c r="Q28" s="34">
         <v>4319.1589999999997</v>
       </c>
-      <c r="R28" s="35">
+      <c r="R28" s="34">
         <v>9725.2090000000007</v>
       </c>
-      <c r="S28" s="35">
+      <c r="S28" s="34">
         <v>2938.85</v>
       </c>
-      <c r="T28" s="35">
+      <c r="T28" s="34">
         <v>1416.059</v>
       </c>
-      <c r="U28" s="35">
+      <c r="U28" s="34">
         <v>444.64499999999998</v>
       </c>
-      <c r="V28" s="35">
+      <c r="V28" s="34">
         <v>619.71799999999996</v>
       </c>
-      <c r="W28" s="35">
+      <c r="W28" s="34">
         <v>203.982</v>
       </c>
-      <c r="X28" s="35">
+      <c r="X28" s="34">
         <v>296.346</v>
       </c>
-      <c r="Y28" s="35">
+      <c r="Y28" s="34">
         <v>1831.027</v>
       </c>
-      <c r="Z28" s="35">
+      <c r="Z28" s="34">
         <v>2729.3069999999998</v>
       </c>
-      <c r="AA28" s="35">
+      <c r="AA28" s="34">
         <v>1425.691</v>
       </c>
-      <c r="AB28" s="35">
+      <c r="AB28" s="34">
         <v>658.19399999999996</v>
       </c>
-      <c r="AC28" s="35">
+      <c r="AC28" s="34">
         <v>336.548</v>
       </c>
-      <c r="AD28" s="35">
+      <c r="AD28" s="34">
         <v>2612.96</v>
       </c>
-      <c r="AE28" s="36">
+      <c r="AE28" s="34">
         <v>0.90700000000000003</v>
       </c>
-      <c r="AF28" s="33"/>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2022</v>
       </c>
@@ -24577,72 +24715,71 @@
       <c r="I29" s="21">
         <v>14.24</v>
       </c>
-      <c r="K29" s="35">
+      <c r="K29" s="34">
         <v>9546.11</v>
       </c>
-      <c r="L29" s="35">
+      <c r="L29" s="34">
         <v>1289.6559999999999</v>
       </c>
-      <c r="M29" s="35">
+      <c r="M29" s="34">
         <v>221.846</v>
       </c>
-      <c r="N29" s="35">
+      <c r="N29" s="34">
         <v>3754.212</v>
       </c>
-      <c r="O29" s="35">
+      <c r="O29" s="34">
         <v>95.271000000000001</v>
       </c>
-      <c r="P29" s="35">
+      <c r="P29" s="34">
         <v>72.926000000000002</v>
       </c>
-      <c r="Q29" s="35">
+      <c r="Q29" s="34">
         <v>4381.6570000000002</v>
       </c>
-      <c r="R29" s="35">
+      <c r="R29" s="34">
         <v>10392.92</v>
       </c>
-      <c r="S29" s="35">
+      <c r="S29" s="34">
         <v>3243.9560000000001</v>
       </c>
-      <c r="T29" s="35">
+      <c r="T29" s="34">
         <v>1812.557</v>
       </c>
-      <c r="U29" s="35">
+      <c r="U29" s="34">
         <v>483.87299999999999</v>
       </c>
-      <c r="V29" s="35">
+      <c r="V29" s="34">
         <v>645.24300000000005</v>
       </c>
-      <c r="W29" s="35">
+      <c r="W29" s="34">
         <v>238.16499999999999</v>
       </c>
-      <c r="X29" s="35">
+      <c r="X29" s="34">
         <v>344.74200000000002</v>
       </c>
-      <c r="Y29" s="35">
+      <c r="Y29" s="34">
         <v>2185.5349999999999</v>
       </c>
-      <c r="Z29" s="35">
+      <c r="Z29" s="34">
         <v>2842.9169999999999</v>
       </c>
-      <c r="AA29" s="35">
+      <c r="AA29" s="34">
         <v>1463.85</v>
       </c>
-      <c r="AB29" s="35">
+      <c r="AB29" s="34">
         <v>672.6</v>
       </c>
-      <c r="AC29" s="35">
+      <c r="AC29" s="34">
         <v>410.27800000000002</v>
       </c>
-      <c r="AD29" s="35">
+      <c r="AD29" s="34">
         <v>2790.3829999999998</v>
       </c>
-      <c r="AE29" s="36">
+      <c r="AE29" s="34">
         <v>1.6950000000000001</v>
       </c>
-      <c r="AF29" s="33"/>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2023</v>
       </c>
@@ -24654,27 +24791,27 @@
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
       <c r="I30" s="21"/>
-      <c r="K30" s="35"/>
-      <c r="L30" s="35"/>
-      <c r="M30" s="35"/>
-      <c r="N30" s="35"/>
-      <c r="O30" s="35"/>
-      <c r="P30" s="35"/>
-      <c r="Q30" s="35"/>
-      <c r="R30" s="35"/>
-      <c r="S30" s="35"/>
-      <c r="T30" s="35"/>
-      <c r="U30" s="35"/>
-      <c r="V30" s="35"/>
-      <c r="W30" s="35"/>
-      <c r="X30" s="35"/>
-      <c r="Y30" s="35"/>
-      <c r="Z30" s="35"/>
-      <c r="AA30" s="35"/>
-      <c r="AB30" s="35"/>
-      <c r="AC30" s="35"/>
-      <c r="AD30" s="35"/>
-      <c r="AE30" s="35"/>
+      <c r="K30" s="34"/>
+      <c r="L30" s="34"/>
+      <c r="M30" s="34"/>
+      <c r="N30" s="34"/>
+      <c r="O30" s="34"/>
+      <c r="P30" s="34"/>
+      <c r="Q30" s="34"/>
+      <c r="R30" s="34"/>
+      <c r="S30" s="34"/>
+      <c r="T30" s="34"/>
+      <c r="U30" s="34"/>
+      <c r="V30" s="34"/>
+      <c r="W30" s="34"/>
+      <c r="X30" s="34"/>
+      <c r="Y30" s="34"/>
+      <c r="Z30" s="34"/>
+      <c r="AA30" s="34"/>
+      <c r="AB30" s="34"/>
+      <c r="AC30" s="34"/>
+      <c r="AD30" s="34"/>
+      <c r="AE30" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24691,7 +24828,7 @@
       <selection activeCell="B153" sqref="B153"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B175" sqref="B175"/>
+      <selection pane="bottomRight" activeCell="B177" sqref="B177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26359,6 +26496,9 @@
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>653</v>
+      </c>
+      <c r="B176" t="s">
+        <v>763</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Monthly labor update - Dec 2024
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AE9F2E-3E28-489F-A4E0-CFD566FAFCB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E13997B-8C8B-4A10-A3D2-B2097659ACE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1979" uniqueCount="765">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1981" uniqueCount="767">
   <si>
     <t>LFS Round</t>
   </si>
@@ -2332,6 +2332,12 @@
   </si>
   <si>
     <t>2024Nov</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/unemployment-rate-december-2024-was-estimated-31-percent</t>
+  </si>
+  <si>
+    <t>2024Dec</t>
   </si>
 </sst>
 </file>
@@ -2344,11 +2350,18 @@
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2455,8 +2468,8 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2483,27 +2496,27 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2735,12 +2748,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P286"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D267" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D255" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F263" sqref="F263"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G284" sqref="G284"/>
+      <selection pane="bottomRight" activeCell="F286" sqref="F286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15093,9 +15106,6 @@
       <c r="D272" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E272" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F272" s="3">
         <f t="shared" si="29"/>
         <v>0.66648310129709132</v>
@@ -15235,7 +15245,7 @@
         <v>2150.3710000000001</v>
       </c>
       <c r="N274" s="2">
-        <f t="shared" ref="N274:N284" si="34">J274-K274</f>
+        <f t="shared" ref="N274:N285" si="34">J274-K274</f>
         <v>30561.898000000001</v>
       </c>
       <c r="O274" s="2">
@@ -15592,19 +15602,19 @@
         <v>425</v>
       </c>
       <c r="F281" s="3">
-        <f t="shared" ref="F281:F284" si="41">K281/J281</f>
+        <f t="shared" ref="F281:F285" si="41">K281/J281</f>
         <v>0.64807383986548939</v>
       </c>
       <c r="G281" s="3">
-        <f t="shared" ref="G281:G284" si="42">L281/K281</f>
+        <f t="shared" ref="G281:G285" si="42">L281/K281</f>
         <v>0.95958742054697199</v>
       </c>
       <c r="H281" s="3">
-        <f t="shared" ref="H281:H284" si="43">M281/K281</f>
+        <f t="shared" ref="H281:H285" si="43">M281/K281</f>
         <v>4.0412579453028008E-2</v>
       </c>
       <c r="I281" s="3">
-        <f t="shared" ref="I281:I284" si="44">O281/L281</f>
+        <f t="shared" ref="I281:I285" si="44">O281/L281</f>
         <v>0.11156186785894412</v>
       </c>
       <c r="J281" s="2">
@@ -15811,7 +15821,44 @@
       <c r="E285" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="O285" s="2"/>
+      <c r="F285" s="3">
+        <f t="shared" si="41"/>
+        <v>0.65146777423127411</v>
+      </c>
+      <c r="G285" s="3">
+        <f t="shared" si="42"/>
+        <v>0.96856075692664978</v>
+      </c>
+      <c r="H285" s="3">
+        <f t="shared" si="43"/>
+        <v>3.1439243073350213E-2</v>
+      </c>
+      <c r="I285" s="3">
+        <f t="shared" si="44"/>
+        <v>0.10920608875026799</v>
+      </c>
+      <c r="J285" s="2">
+        <v>79534.983999999997</v>
+      </c>
+      <c r="K285" s="2">
+        <v>51814.478999999999</v>
+      </c>
+      <c r="L285" s="2">
+        <v>50185.470999999998</v>
+      </c>
+      <c r="M285" s="2">
+        <v>1629.008</v>
+      </c>
+      <c r="N285" s="2">
+        <f t="shared" si="34"/>
+        <v>27720.504999999997</v>
+      </c>
+      <c r="O285" s="2">
+        <v>5480.5590000000002</v>
+      </c>
+      <c r="P285" t="s">
+        <v>765</v>
+      </c>
     </row>
     <row r="286" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
@@ -15839,23 +15886,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B3FDD3-8CAB-4986-8439-B73CD0CD9872}">
-  <dimension ref="A1:BR54"/>
+  <dimension ref="A1:BS54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="BO2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="BP2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BS24" sqref="BS24"/>
+      <selection pane="bottomRight" activeCell="BS13" sqref="BS13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" style="24" customWidth="1"/>
-    <col min="2" max="70" width="10.7109375" style="24" customWidth="1"/>
-    <col min="71" max="16384" width="9.140625" style="24"/>
+    <col min="2" max="71" width="10.7109375" style="24" customWidth="1"/>
+    <col min="72" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:70" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>685</v>
       </c>
@@ -16027,7 +16074,7 @@
       <c r="BE1" s="24" t="s">
         <v>707</v>
       </c>
-      <c r="BF1" s="36" t="s">
+      <c r="BF1" s="24" t="s">
         <v>706</v>
       </c>
       <c r="BG1" s="31" t="s">
@@ -16066,8 +16113,11 @@
       <c r="BR1" s="35" t="s">
         <v>764</v>
       </c>
-    </row>
-    <row r="2" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS1" s="36" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>694</v>
       </c>
@@ -16246,8 +16296,11 @@
       <c r="BR2" s="26">
         <v>49541.468999999997</v>
       </c>
-    </row>
-    <row r="3" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS2" s="26">
+        <v>50185.470999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>691</v>
       </c>
@@ -16316,8 +16369,9 @@
       <c r="BP3" s="26"/>
       <c r="BQ3" s="26"/>
       <c r="BR3" s="26"/>
-    </row>
-    <row r="4" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS3" s="26"/>
+    </row>
+    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>693</v>
       </c>
@@ -16461,7 +16515,7 @@
         <v>10708.791999999999</v>
       </c>
       <c r="BG4" s="26">
-        <v>11008.887000000001</v>
+        <v>11007.349</v>
       </c>
       <c r="BH4" s="26">
         <v>8327.1959999999999</v>
@@ -16496,8 +16550,11 @@
       <c r="BR4" s="26">
         <v>8714.152</v>
       </c>
-    </row>
-    <row r="5" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS4" s="26">
+        <v>9448.9699999999993</v>
+      </c>
+    </row>
+    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>692</v>
       </c>
@@ -16676,8 +16733,11 @@
       <c r="BR5" s="26">
         <v>1203.7929999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS5" s="26">
+        <v>1223.2280000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>685</v>
       </c>
@@ -16744,8 +16804,9 @@
       <c r="BP6" s="26"/>
       <c r="BQ6" s="26"/>
       <c r="BR6" s="26"/>
-    </row>
-    <row r="7" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS6" s="26"/>
+    </row>
+    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>690</v>
       </c>
@@ -16924,8 +16985,11 @@
       <c r="BR7" s="26">
         <v>267.584</v>
       </c>
-    </row>
-    <row r="8" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS7" s="26">
+        <v>291.67200000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>689</v>
       </c>
@@ -17069,7 +17133,7 @@
         <v>2946.9659999999999</v>
       </c>
       <c r="BG8" s="26">
-        <v>3793.2669999999998</v>
+        <v>3792.8150000000001</v>
       </c>
       <c r="BH8" s="26">
         <v>3520.1819999999998</v>
@@ -17104,8 +17168,11 @@
       <c r="BR8" s="26">
         <v>3710.7510000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS8" s="26">
+        <v>3405.971</v>
+      </c>
+    </row>
+    <row r="9" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>688</v>
       </c>
@@ -17284,8 +17351,11 @@
       <c r="BR9" s="26">
         <v>70.995000000000005</v>
       </c>
-    </row>
-    <row r="10" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS9" s="26">
+        <v>67.512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>687</v>
       </c>
@@ -17464,8 +17534,11 @@
       <c r="BR10" s="26">
         <v>53.923000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS10" s="26">
+        <v>55.939</v>
+      </c>
+    </row>
+    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>686</v>
       </c>
@@ -17644,8 +17717,11 @@
       <c r="BR11" s="26">
         <v>4763.9870000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS11" s="26">
+        <v>5346.6750000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
         <v>669</v>
       </c>
@@ -17712,8 +17788,9 @@
       <c r="BP12" s="26"/>
       <c r="BQ12" s="26"/>
       <c r="BR12" s="26"/>
-    </row>
-    <row r="13" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS12" s="26"/>
+    </row>
+    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>683</v>
       </c>
@@ -17857,7 +17934,7 @@
         <v>10924.816000000001</v>
       </c>
       <c r="BG13" s="26">
-        <v>10270.275</v>
+        <v>10287.226000000001</v>
       </c>
       <c r="BH13" s="26">
         <v>9054.0400000000009</v>
@@ -17892,8 +17969,11 @@
       <c r="BR13" s="26">
         <v>10571.767</v>
       </c>
-    </row>
-    <row r="14" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS13" s="26">
+        <v>10180.915000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>682</v>
       </c>
@@ -18037,7 +18117,7 @@
         <v>3657.6370000000002</v>
       </c>
       <c r="BG14" s="26">
-        <v>3476.2869999999998</v>
+        <v>3476.6579999999999</v>
       </c>
       <c r="BH14" s="26">
         <v>3648.047</v>
@@ -18072,8 +18152,11 @@
       <c r="BR14" s="26">
         <v>3848.0129999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS14" s="26">
+        <v>4031.569</v>
+      </c>
+    </row>
+    <row r="15" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>681</v>
       </c>
@@ -18217,7 +18300,7 @@
         <v>2343.652</v>
       </c>
       <c r="BG15" s="26">
-        <v>2517.4699999999998</v>
+        <v>2500.431</v>
       </c>
       <c r="BH15" s="26">
         <v>2127.9870000000001</v>
@@ -18252,8 +18335,11 @@
       <c r="BR15" s="26">
         <v>2896.1390000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS15" s="26">
+        <v>2677.1469999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>680</v>
       </c>
@@ -18432,8 +18518,11 @@
       <c r="BR16" s="26">
         <v>488.35</v>
       </c>
-    </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS16" s="26">
+        <v>485.89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>679</v>
       </c>
@@ -18577,7 +18666,7 @@
         <v>656.44299999999998</v>
       </c>
       <c r="BG17" s="26">
-        <v>557.91899999999998</v>
+        <v>561.71299999999997</v>
       </c>
       <c r="BH17" s="26">
         <v>641.48500000000001</v>
@@ -18612,8 +18701,11 @@
       <c r="BR17" s="26">
         <v>661.50599999999997</v>
       </c>
-    </row>
-    <row r="18" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS17" s="26">
+        <v>757.32100000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>678</v>
       </c>
@@ -18757,7 +18849,7 @@
         <v>229.852</v>
       </c>
       <c r="BG18" s="26">
-        <v>241.374</v>
+        <v>243.08099999999999</v>
       </c>
       <c r="BH18" s="26">
         <v>260.29000000000002</v>
@@ -18792,8 +18884,11 @@
       <c r="BR18" s="26">
         <v>242.67099999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS18" s="26">
+        <v>330.81799999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>677</v>
       </c>
@@ -18972,8 +19067,11 @@
       <c r="BR19" s="26">
         <v>370.48599999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS19" s="26">
+        <v>438.92700000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>676</v>
       </c>
@@ -19117,7 +19215,7 @@
         <v>2497.1570000000002</v>
       </c>
       <c r="BG20" s="26">
-        <v>2314.212</v>
+        <v>2308.0479999999998</v>
       </c>
       <c r="BH20" s="26">
         <v>2510.3220000000001</v>
@@ -19152,8 +19250,11 @@
       <c r="BR20" s="26">
         <v>2644.9749999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS20" s="26">
+        <v>2531.3890000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>675</v>
       </c>
@@ -19297,7 +19398,7 @@
         <v>2783.0990000000002</v>
       </c>
       <c r="BG21" s="26">
-        <v>2931.5309999999999</v>
+        <v>2932.6950000000002</v>
       </c>
       <c r="BH21" s="26">
         <v>2737.5479999999998</v>
@@ -19332,8 +19433,11 @@
       <c r="BR21" s="26">
         <v>2836.6239999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS21" s="26">
+        <v>3143.31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>674</v>
       </c>
@@ -19512,8 +19616,11 @@
       <c r="BR22" s="26">
         <v>1635.202</v>
       </c>
-    </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS22" s="26">
+        <v>1585.854</v>
+      </c>
+    </row>
+    <row r="23" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>673</v>
       </c>
@@ -19657,7 +19764,7 @@
         <v>602.27599999999995</v>
       </c>
       <c r="BG23" s="26">
-        <v>642.904</v>
+        <v>641.74</v>
       </c>
       <c r="BH23" s="26">
         <v>688.66700000000003</v>
@@ -19692,8 +19799,11 @@
       <c r="BR23" s="26">
         <v>881.52300000000002</v>
       </c>
-    </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS23" s="26">
+        <v>838.90499999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>672</v>
       </c>
@@ -19872,8 +19982,11 @@
       <c r="BR24" s="26">
         <v>450.57799999999997</v>
       </c>
-    </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS24" s="26">
+        <v>406.45100000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>671</v>
       </c>
@@ -20017,7 +20130,7 @@
         <v>2986.154</v>
       </c>
       <c r="BG25" s="26">
-        <v>3100.518</v>
+        <v>3102.8890000000001</v>
       </c>
       <c r="BH25" s="26">
         <v>2976.7910000000002</v>
@@ -20052,8 +20165,11 @@
       <c r="BR25" s="26">
         <v>3225.143</v>
       </c>
-    </row>
-    <row r="26" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS25" s="26">
+        <v>2937.009</v>
+      </c>
+    </row>
+    <row r="26" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>670</v>
       </c>
@@ -20232,8 +20348,11 @@
       <c r="BR26" s="26">
         <v>3.3079999999999998</v>
       </c>
-    </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS26" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
         <v>694</v>
       </c>
@@ -20338,8 +20457,9 @@
       <c r="BP27" s="26"/>
       <c r="BQ27" s="26"/>
       <c r="BR27" s="26"/>
-    </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS27" s="26"/>
+    </row>
+    <row r="28" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
         <v>691</v>
       </c>
@@ -20416,8 +20536,9 @@
       <c r="BP28" s="26"/>
       <c r="BQ28" s="26"/>
       <c r="BR28" s="26"/>
-    </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS28" s="26"/>
+    </row>
+    <row r="29" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>693</v>
       </c>
@@ -20522,8 +20643,9 @@
       <c r="BP29" s="26"/>
       <c r="BQ29" s="26"/>
       <c r="BR29" s="26"/>
-    </row>
-    <row r="30" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS29" s="26"/>
+    </row>
+    <row r="30" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>692</v>
       </c>
@@ -20628,8 +20750,9 @@
       <c r="BP30" s="26"/>
       <c r="BQ30" s="26"/>
       <c r="BR30" s="26"/>
-    </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS30" s="26"/>
+    </row>
+    <row r="31" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
         <v>685</v>
       </c>
@@ -20705,8 +20828,9 @@
       <c r="BP31" s="26"/>
       <c r="BQ31" s="26"/>
       <c r="BR31" s="26"/>
-    </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS31" s="26"/>
+    </row>
+    <row r="32" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>690</v>
       </c>
@@ -20811,8 +20935,9 @@
       <c r="BP32" s="26"/>
       <c r="BQ32" s="26"/>
       <c r="BR32" s="26"/>
-    </row>
-    <row r="33" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS32" s="26"/>
+    </row>
+    <row r="33" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>689</v>
       </c>
@@ -20917,8 +21042,9 @@
       <c r="BP33" s="26"/>
       <c r="BQ33" s="26"/>
       <c r="BR33" s="26"/>
-    </row>
-    <row r="34" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS33" s="26"/>
+    </row>
+    <row r="34" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>688</v>
       </c>
@@ -21023,8 +21149,9 @@
       <c r="BP34" s="26"/>
       <c r="BQ34" s="26"/>
       <c r="BR34" s="26"/>
-    </row>
-    <row r="35" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS34" s="26"/>
+    </row>
+    <row r="35" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>687</v>
       </c>
@@ -21129,8 +21256,9 @@
       <c r="BP35" s="26"/>
       <c r="BQ35" s="26"/>
       <c r="BR35" s="26"/>
-    </row>
-    <row r="36" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS35" s="26"/>
+    </row>
+    <row r="36" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>686</v>
       </c>
@@ -21235,8 +21363,9 @@
       <c r="BP36" s="26"/>
       <c r="BQ36" s="26"/>
       <c r="BR36" s="26"/>
-    </row>
-    <row r="37" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS36" s="26"/>
+    </row>
+    <row r="37" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
         <v>669</v>
       </c>
@@ -21313,8 +21442,9 @@
       <c r="BP37" s="26"/>
       <c r="BQ37" s="26"/>
       <c r="BR37" s="26"/>
-    </row>
-    <row r="38" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS37" s="26"/>
+    </row>
+    <row r="38" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>683</v>
       </c>
@@ -21419,8 +21549,9 @@
       <c r="BP38" s="26"/>
       <c r="BQ38" s="26"/>
       <c r="BR38" s="26"/>
-    </row>
-    <row r="39" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS38" s="26"/>
+    </row>
+    <row r="39" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
         <v>682</v>
       </c>
@@ -21525,8 +21656,9 @@
       <c r="BP39" s="26"/>
       <c r="BQ39" s="26"/>
       <c r="BR39" s="26"/>
-    </row>
-    <row r="40" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS39" s="26"/>
+    </row>
+    <row r="40" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>681</v>
       </c>
@@ -21631,8 +21763,9 @@
       <c r="BP40" s="26"/>
       <c r="BQ40" s="26"/>
       <c r="BR40" s="26"/>
-    </row>
-    <row r="41" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS40" s="26"/>
+    </row>
+    <row r="41" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
         <v>680</v>
       </c>
@@ -21737,8 +21870,9 @@
       <c r="BP41" s="26"/>
       <c r="BQ41" s="26"/>
       <c r="BR41" s="26"/>
-    </row>
-    <row r="42" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS41" s="26"/>
+    </row>
+    <row r="42" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
         <v>679</v>
       </c>
@@ -21843,8 +21977,9 @@
       <c r="BP42" s="26"/>
       <c r="BQ42" s="26"/>
       <c r="BR42" s="26"/>
-    </row>
-    <row r="43" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS42" s="26"/>
+    </row>
+    <row r="43" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
         <v>678</v>
       </c>
@@ -21949,8 +22084,9 @@
       <c r="BP43" s="26"/>
       <c r="BQ43" s="26"/>
       <c r="BR43" s="26"/>
-    </row>
-    <row r="44" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS43" s="26"/>
+    </row>
+    <row r="44" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
         <v>677</v>
       </c>
@@ -22055,8 +22191,9 @@
       <c r="BP44" s="26"/>
       <c r="BQ44" s="26"/>
       <c r="BR44" s="26"/>
-    </row>
-    <row r="45" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS44" s="26"/>
+    </row>
+    <row r="45" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>676</v>
       </c>
@@ -22161,8 +22298,9 @@
       <c r="BP45" s="26"/>
       <c r="BQ45" s="26"/>
       <c r="BR45" s="26"/>
-    </row>
-    <row r="46" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS45" s="26"/>
+    </row>
+    <row r="46" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
         <v>675</v>
       </c>
@@ -22267,8 +22405,9 @@
       <c r="BP46" s="26"/>
       <c r="BQ46" s="26"/>
       <c r="BR46" s="26"/>
-    </row>
-    <row r="47" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS46" s="26"/>
+    </row>
+    <row r="47" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A47" s="25" t="s">
         <v>674</v>
       </c>
@@ -22373,8 +22512,9 @@
       <c r="BP47" s="26"/>
       <c r="BQ47" s="26"/>
       <c r="BR47" s="26"/>
-    </row>
-    <row r="48" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS47" s="26"/>
+    </row>
+    <row r="48" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A48" s="25" t="s">
         <v>673</v>
       </c>
@@ -22479,8 +22619,9 @@
       <c r="BP48" s="26"/>
       <c r="BQ48" s="26"/>
       <c r="BR48" s="26"/>
-    </row>
-    <row r="49" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS48" s="26"/>
+    </row>
+    <row r="49" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
         <v>672</v>
       </c>
@@ -22585,8 +22726,9 @@
       <c r="BP49" s="26"/>
       <c r="BQ49" s="26"/>
       <c r="BR49" s="26"/>
-    </row>
-    <row r="50" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS49" s="26"/>
+    </row>
+    <row r="50" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A50" s="25" t="s">
         <v>671</v>
       </c>
@@ -22691,8 +22833,9 @@
       <c r="BP50" s="26"/>
       <c r="BQ50" s="26"/>
       <c r="BR50" s="26"/>
-    </row>
-    <row r="51" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS50" s="26"/>
+    </row>
+    <row r="51" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A51" s="25" t="s">
         <v>670</v>
       </c>
@@ -22797,8 +22940,9 @@
       <c r="BP51" s="26"/>
       <c r="BQ51" s="26"/>
       <c r="BR51" s="26"/>
-    </row>
-    <row r="54" spans="1:70" x14ac:dyDescent="0.25">
+      <c r="BS51" s="26"/>
+    </row>
+    <row r="54" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A54" s="25"/>
     </row>
   </sheetData>
@@ -22816,7 +22960,7 @@
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K19" sqref="K19:AE26"/>
+      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24824,7 +24968,7 @@
   <dimension ref="A1:D178"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B160" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B169" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B153" sqref="B153"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -26501,12 +26645,15 @@
         <v>763</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B177" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>655</v>
       </c>

</xml_diff>

<commit_message>
Monthly labor update - Jan 2025
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E13997B-8C8B-4A10-A3D2-B2097659ACE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D702FB-8951-4C9A-AC36-D73E27909534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1981" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2048" uniqueCount="782">
   <si>
     <t>LFS Round</t>
   </si>
@@ -2338,6 +2338,51 @@
   </si>
   <si>
     <t>2024Dec</t>
+  </si>
+  <si>
+    <t>2025 Jan</t>
+  </si>
+  <si>
+    <t>2025 Feb</t>
+  </si>
+  <si>
+    <t>2025 Mar</t>
+  </si>
+  <si>
+    <t>2025 Apr</t>
+  </si>
+  <si>
+    <t>2025 May</t>
+  </si>
+  <si>
+    <t>2025 Jun</t>
+  </si>
+  <si>
+    <t>2025 Jul</t>
+  </si>
+  <si>
+    <t>2025 Aug</t>
+  </si>
+  <si>
+    <t>2025 Sep</t>
+  </si>
+  <si>
+    <t>2025 Oct</t>
+  </si>
+  <si>
+    <t>2025 Nov</t>
+  </si>
+  <si>
+    <t>2025 Dec</t>
+  </si>
+  <si>
+    <t>2025 Annual</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/unemployment-rate-january-2025-was-estimated-43-percent</t>
+  </si>
+  <si>
+    <t>2025</t>
   </si>
 </sst>
 </file>
@@ -2746,14 +2791,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P286"/>
+  <dimension ref="A1:P299"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D255" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D265" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F263" sqref="F263"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F286" sqref="F286"/>
+      <selection pane="bottomRight" activeCell="F288" sqref="F288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15213,43 +15258,40 @@
       <c r="D274" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E274" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F274" s="3">
         <f t="shared" ref="F274:F278" si="30">K274/J274</f>
-        <v>0.6114444374307062</v>
+        <v>0.61119309526396914</v>
       </c>
       <c r="G274" s="3">
         <f t="shared" ref="G274:G278" si="31">L274/K274</f>
-        <v>0.95528747408394488</v>
+        <v>0.95510943155707362</v>
       </c>
       <c r="H274" s="3">
         <f t="shared" ref="H274:H279" si="32">M274/K274</f>
-        <v>4.4712525916055137E-2</v>
+        <v>4.4890568442926361E-2</v>
       </c>
       <c r="I274" s="3">
         <f t="shared" ref="I274:I279" si="33">O274/L274</f>
-        <v>0.13917804379986054</v>
+        <v>0.13717458748837555</v>
       </c>
       <c r="J274" s="2">
-        <v>78655.154999999999</v>
+        <v>78632.404999999999</v>
       </c>
       <c r="K274" s="2">
-        <v>48093.256999999998</v>
+        <v>48059.582999999999</v>
       </c>
       <c r="L274" s="2">
-        <v>45942.885999999999</v>
+        <v>45902.161</v>
       </c>
       <c r="M274" s="2">
-        <v>2150.3710000000001</v>
+        <v>2157.422</v>
       </c>
       <c r="N274" s="2">
-        <f t="shared" ref="N274:N285" si="34">J274-K274</f>
-        <v>30561.898000000001</v>
+        <f t="shared" ref="N274:N287" si="34">J274-K274</f>
+        <v>30572.822</v>
       </c>
       <c r="O274" s="2">
-        <v>6394.241</v>
+        <v>6296.61</v>
       </c>
       <c r="P274" t="s">
         <v>656</v>
@@ -15877,6 +15919,229 @@
         <v>425</v>
       </c>
       <c r="O286" s="2"/>
+    </row>
+    <row r="287" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A287" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D287" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E287" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F287" s="3">
+        <f t="shared" ref="F287" si="45">K287/J287</f>
+        <v>0.63860962824397194</v>
+      </c>
+      <c r="G287" s="3">
+        <f t="shared" ref="G287" si="46">L287/K287</f>
+        <v>0.95726078411505899</v>
+      </c>
+      <c r="H287" s="3">
+        <f t="shared" ref="H287" si="47">M287/K287</f>
+        <v>4.2739215884941006E-2</v>
+      </c>
+      <c r="I287" s="3">
+        <f t="shared" ref="I287" si="48">O287/L287</f>
+        <v>0.13342662775918007</v>
+      </c>
+      <c r="J287" s="2">
+        <v>79315.19</v>
+      </c>
+      <c r="K287" s="2">
+        <v>50651.444000000003</v>
+      </c>
+      <c r="L287" s="2">
+        <v>48486.641000000003</v>
+      </c>
+      <c r="M287" s="2">
+        <v>2164.8029999999999</v>
+      </c>
+      <c r="N287" s="2">
+        <f t="shared" si="34"/>
+        <v>28663.745999999999</v>
+      </c>
+      <c r="O287" s="2">
+        <v>6469.4089999999997</v>
+      </c>
+      <c r="P287" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="288" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A288" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="D288" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A289" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D289" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D290" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D291" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A292" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="D292" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A293" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D293" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A294" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D294" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A295" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B295" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D295" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A296" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D296" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A297" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D297" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A298" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="C298" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="D298" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A299" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="B299" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="C299" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D299" s="1" t="s">
+        <v>417</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15888,7 +16153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B3FDD3-8CAB-4986-8439-B73CD0CD9872}">
   <dimension ref="A1:BS54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="BP2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -24965,14 +25230,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D178"/>
+  <dimension ref="A1:D191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B169" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B175" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B153" sqref="B153"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B177" sqref="B177"/>
+      <selection pane="bottomRight" activeCell="B179" sqref="B179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26656,6 +26921,74 @@
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>655</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="B179" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Monthly labor update - Feb 2025
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D702FB-8951-4C9A-AC36-D73E27909534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861DB5F8-8909-421F-B8F4-AB83C0C39CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2048" uniqueCount="782">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2050" uniqueCount="783">
   <si>
     <t>LFS Round</t>
   </si>
@@ -2383,6 +2383,9 @@
   </si>
   <si>
     <t>2025</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/employment-rate-february-2025-was-estimated-962-percent</t>
   </si>
 </sst>
 </file>
@@ -2793,12 +2796,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P299"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D265" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="K273" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F263" sqref="F263"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F288" sqref="F288"/>
+      <selection pane="bottomRight" activeCell="P289" sqref="P289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15287,7 +15290,7 @@
         <v>2157.422</v>
       </c>
       <c r="N274" s="2">
-        <f t="shared" ref="N274:N287" si="34">J274-K274</f>
+        <f t="shared" ref="N274:N288" si="34">J274-K274</f>
         <v>30572.822</v>
       </c>
       <c r="O274" s="2">
@@ -15310,9 +15313,6 @@
       <c r="D275" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E275" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F275" s="3">
         <f t="shared" si="30"/>
         <v>0.64804378119674044</v>
@@ -15937,19 +15937,19 @@
         <v>425</v>
       </c>
       <c r="F287" s="3">
-        <f t="shared" ref="F287" si="45">K287/J287</f>
+        <f t="shared" ref="F287:F288" si="45">K287/J287</f>
         <v>0.63860962824397194</v>
       </c>
       <c r="G287" s="3">
-        <f t="shared" ref="G287" si="46">L287/K287</f>
+        <f t="shared" ref="G287:G288" si="46">L287/K287</f>
         <v>0.95726078411505899</v>
       </c>
       <c r="H287" s="3">
-        <f t="shared" ref="H287" si="47">M287/K287</f>
+        <f t="shared" ref="H287:H288" si="47">M287/K287</f>
         <v>4.2739215884941006E-2</v>
       </c>
       <c r="I287" s="3">
-        <f t="shared" ref="I287" si="48">O287/L287</f>
+        <f t="shared" ref="I287:I288" si="48">O287/L287</f>
         <v>0.13342662775918007</v>
       </c>
       <c r="J287" s="2">
@@ -15987,6 +15987,47 @@
       </c>
       <c r="D288" s="1" t="s">
         <v>417</v>
+      </c>
+      <c r="E288" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F288" s="3">
+        <f t="shared" si="45"/>
+        <v>0.64473209315915503</v>
+      </c>
+      <c r="G288" s="3">
+        <f t="shared" si="46"/>
+        <v>0.96208863606203909</v>
+      </c>
+      <c r="H288" s="3">
+        <f t="shared" si="47"/>
+        <v>3.7911363937960858E-2</v>
+      </c>
+      <c r="I288" s="3">
+        <f t="shared" si="48"/>
+        <v>0.1008763827044134</v>
+      </c>
+      <c r="J288" s="2">
+        <v>79244.729000000007</v>
+      </c>
+      <c r="K288" s="2">
+        <v>51091.62</v>
+      </c>
+      <c r="L288" s="2">
+        <v>49154.667000000001</v>
+      </c>
+      <c r="M288" s="2">
+        <v>1936.953</v>
+      </c>
+      <c r="N288" s="2">
+        <f t="shared" si="34"/>
+        <v>28153.109000000004</v>
+      </c>
+      <c r="O288" s="2">
+        <v>4958.5450000000001</v>
+      </c>
+      <c r="P288" t="s">
+        <v>782</v>
       </c>
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.25">
@@ -16153,11 +16194,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B3FDD3-8CAB-4986-8439-B73CD0CD9872}">
   <dimension ref="A1:BS54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="BP2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BS13" sqref="BS13"/>
+      <selection pane="bottomRight" activeCell="BT1" sqref="BT1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25237,7 +25278,7 @@
       <selection activeCell="B153" sqref="B153"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B179" sqref="B179"/>
+      <selection pane="bottomRight" activeCell="B180" sqref="B180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26934,6 +26975,9 @@
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>768</v>
+      </c>
+      <c r="B180" t="s">
+        <v>782</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Monthly labor update - Mar 2025
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861DB5F8-8909-421F-B8F4-AB83C0C39CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7219E6A5-E965-4121-BAF8-9A15F8DDF1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2050" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2052" uniqueCount="784">
   <si>
     <t>LFS Round</t>
   </si>
@@ -2386,6 +2386,9 @@
   </si>
   <si>
     <t>https://psa.gov.ph/content/employment-rate-february-2025-was-estimated-962-percent</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/employment-rate-march-2025-was-estimated-961-percent</t>
   </si>
 </sst>
 </file>
@@ -2398,11 +2401,18 @@
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2516,10 +2526,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2544,27 +2554,28 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2797,11 +2808,11 @@
   <dimension ref="A1:P299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K273" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D264" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F263" sqref="F263"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P289" sqref="P289"/>
+      <selection pane="bottomRight" activeCell="F290" sqref="F290"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15290,7 +15301,7 @@
         <v>2157.422</v>
       </c>
       <c r="N274" s="2">
-        <f t="shared" ref="N274:N288" si="34">J274-K274</f>
+        <f t="shared" ref="N274:N289" si="34">J274-K274</f>
         <v>30572.822</v>
       </c>
       <c r="O274" s="2">
@@ -15365,9 +15376,6 @@
       <c r="D276" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E276" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F276" s="3">
         <f t="shared" si="30"/>
         <v>0.65317873180475028</v>
@@ -16030,7 +16038,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>769</v>
       </c>
@@ -16043,8 +16051,49 @@
       <c r="D289" s="1" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E289" s="37" t="s">
+        <v>425</v>
+      </c>
+      <c r="F289" s="3">
+        <f t="shared" ref="F289" si="49">K289/J289</f>
+        <v>0.62855197137035979</v>
+      </c>
+      <c r="G289" s="3">
+        <f t="shared" ref="G289" si="50">L289/K289</f>
+        <v>0.96133642592656232</v>
+      </c>
+      <c r="H289" s="3">
+        <f t="shared" ref="H289" si="51">M289/K289</f>
+        <v>3.8663574073437589E-2</v>
+      </c>
+      <c r="I289" s="3">
+        <f t="shared" ref="I289" si="52">O289/L289</f>
+        <v>0.13404737188395227</v>
+      </c>
+      <c r="J289" s="2">
+        <v>79478.47</v>
+      </c>
+      <c r="K289" s="2">
+        <v>49956.349000000002</v>
+      </c>
+      <c r="L289" s="2">
+        <v>48024.858</v>
+      </c>
+      <c r="M289" s="2">
+        <v>1931.491</v>
+      </c>
+      <c r="N289" s="2">
+        <f t="shared" si="34"/>
+        <v>29522.120999999999</v>
+      </c>
+      <c r="O289" s="2">
+        <v>6437.6059999999998</v>
+      </c>
+      <c r="P289" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="290" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>770</v>
       </c>
@@ -16058,7 +16107,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>771</v>
       </c>
@@ -16072,7 +16121,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>772</v>
       </c>
@@ -16086,7 +16135,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>773</v>
       </c>
@@ -16100,7 +16149,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>774</v>
       </c>
@@ -16114,7 +16163,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>775</v>
       </c>
@@ -16128,7 +16177,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>776</v>
       </c>
@@ -16142,7 +16191,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>777</v>
       </c>
@@ -16156,7 +16205,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>778</v>
       </c>
@@ -16170,7 +16219,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>779</v>
       </c>
@@ -25278,7 +25327,7 @@
       <selection activeCell="B153" sqref="B153"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B180" sqref="B180"/>
+      <selection pane="bottomRight" activeCell="B181" sqref="B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26983,6 +27032,9 @@
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>769</v>
+      </c>
+      <c r="B181" t="s">
+        <v>783</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Monthly labor update - May 2025
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE94612E-EB32-48AF-9007-5FBB99476FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869D0B2E-016E-4065-A5C5-2A31FF340095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1230" yWindow="3975" windowWidth="15270" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2958" uniqueCount="809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2959" uniqueCount="810">
   <si>
     <t>LFS Round</t>
   </si>
@@ -2465,6 +2465,9 @@
   </si>
   <si>
     <t>Not in the Labor Force</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/participation-labor-force-may-2025-increased-5232-million-filipinos-aged-15-years-and-over</t>
   </si>
 </sst>
 </file>
@@ -2901,12 +2904,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P299"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E271" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D288" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F263" sqref="F263"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O274" sqref="O274"/>
+      <selection pane="bottomRight" activeCell="F292" sqref="F292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15395,7 +15398,7 @@
         <v>2157.422</v>
       </c>
       <c r="N274" s="2">
-        <f t="shared" ref="N274:N290" si="34">J274-K274</f>
+        <f t="shared" ref="N274:N291" si="34">J274-K274</f>
         <v>30572.822</v>
       </c>
       <c r="O274" s="2">
@@ -15573,9 +15576,6 @@
       <c r="D278" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E278" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F278" s="3">
         <f t="shared" si="30"/>
         <v>0.64820526458333438</v>
@@ -16251,7 +16251,47 @@
       <c r="D291" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="O291" s="2"/>
+      <c r="E291" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F291" s="3">
+        <f t="shared" ref="F291" si="57">K291/J291</f>
+        <v>0.6584863836337842</v>
+      </c>
+      <c r="G291" s="3">
+        <f t="shared" ref="G291" si="58">L291/K291</f>
+        <v>0.96111235686185403</v>
+      </c>
+      <c r="H291" s="3">
+        <f t="shared" ref="H291" si="59">M291/K291</f>
+        <v>3.8887643138145953E-2</v>
+      </c>
+      <c r="I291" s="3">
+        <f t="shared" ref="I291" si="60">O291/L291</f>
+        <v>0.13129024415128956</v>
+      </c>
+      <c r="J291" s="2">
+        <v>79461.839000000007</v>
+      </c>
+      <c r="K291" s="2">
+        <v>52324.538999999997</v>
+      </c>
+      <c r="L291" s="2">
+        <v>50289.760999999999</v>
+      </c>
+      <c r="M291" s="2">
+        <v>2034.778</v>
+      </c>
+      <c r="N291" s="2">
+        <f t="shared" si="34"/>
+        <v>27137.30000000001</v>
+      </c>
+      <c r="O291" s="2">
+        <v>6602.5550000000003</v>
+      </c>
+      <c r="P291" t="s">
+        <v>809</v>
+      </c>
     </row>
     <row r="292" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
@@ -16384,7 +16424,7 @@
   <dimension ref="A1:AE30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -18396,7 +18436,7 @@
   <dimension ref="A1:BS54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="BL2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="BO2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="BT1" sqref="BT1"/>
@@ -25462,7 +25502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3012B618-0A4E-423F-92B0-9AF730FFC0C6}">
   <dimension ref="A1:AN322"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="T56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -32218,35 +32258,35 @@
       <c r="AE75" s="42"/>
       <c r="AF75" s="42"/>
       <c r="AG75" s="42">
-        <f>AG3-AG21</f>
+        <f t="shared" ref="AG75:AN75" si="0">AG3-AG21</f>
         <v>3848.0793353999989</v>
       </c>
       <c r="AH75" s="42">
-        <f>AH3-AH21</f>
+        <f t="shared" si="0"/>
         <v>3807.6186416599994</v>
       </c>
       <c r="AI75" s="42">
-        <f>AI3-AI21</f>
+        <f t="shared" si="0"/>
         <v>4184.0650000000005</v>
       </c>
       <c r="AJ75" s="42">
-        <f>AJ3-AJ21</f>
+        <f t="shared" si="0"/>
         <v>3963.8060552399993</v>
       </c>
       <c r="AK75" s="42">
-        <f>AK3-AK21</f>
+        <f t="shared" si="0"/>
         <v>4056.4294848</v>
       </c>
       <c r="AL75" s="42">
-        <f>AL3-AL21</f>
+        <f t="shared" si="0"/>
         <v>3921.6707066899999</v>
       </c>
       <c r="AM75" s="42">
-        <f>AM3-AM21</f>
+        <f t="shared" si="0"/>
         <v>3972.902</v>
       </c>
       <c r="AN75" s="42">
-        <f>AN3-AN21</f>
+        <f t="shared" si="0"/>
         <v>3960.0433598200007</v>
       </c>
     </row>
@@ -32300,35 +32340,35 @@
       <c r="AE76" s="42"/>
       <c r="AF76" s="42"/>
       <c r="AG76" s="42">
-        <f t="shared" ref="AG76:AH91" si="0">AG4-AG22</f>
+        <f t="shared" ref="AG76:AH91" si="1">AG4-AG22</f>
         <v>454.08434681999995</v>
       </c>
       <c r="AH76" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>441.00582885999995</v>
       </c>
       <c r="AI76" s="42">
-        <f t="shared" ref="AI76:AJ76" si="1">AI4-AI22</f>
+        <f t="shared" ref="AI76:AJ76" si="2">AI4-AI22</f>
         <v>462.73800000000017</v>
       </c>
       <c r="AJ76" s="42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>432.28631094000002</v>
       </c>
       <c r="AK76" s="42">
-        <f t="shared" ref="AK76:AL91" si="2">AK4-AK22</f>
+        <f t="shared" ref="AK76:AL91" si="3">AK4-AK22</f>
         <v>461.89767676000008</v>
       </c>
       <c r="AL76" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>470.45267699999988</v>
       </c>
       <c r="AM76" s="42">
-        <f t="shared" ref="AM76:AN76" si="3">AM4-AM22</f>
+        <f t="shared" ref="AM76:AN76" si="4">AM4-AM22</f>
         <v>424.35500000000002</v>
       </c>
       <c r="AN76" s="42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>473.24849901999994</v>
       </c>
     </row>
@@ -32382,35 +32422,35 @@
       <c r="AE77" s="42"/>
       <c r="AF77" s="42"/>
       <c r="AG77" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1316.9154189399997</v>
       </c>
       <c r="AH77" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1314.7478057599997</v>
       </c>
       <c r="AI77" s="42">
-        <f t="shared" ref="AI77:AJ77" si="4">AI5-AI23</f>
+        <f t="shared" ref="AI77:AJ77" si="5">AI5-AI23</f>
         <v>1524.3390000000004</v>
       </c>
       <c r="AJ77" s="42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1342.18953225</v>
       </c>
       <c r="AK77" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1460.0015051800001</v>
       </c>
       <c r="AL77" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1339.0845440000003</v>
       </c>
       <c r="AM77" s="42">
-        <f t="shared" ref="AM77:AN77" si="5">AM5-AM23</f>
+        <f t="shared" ref="AM77:AN77" si="6">AM5-AM23</f>
         <v>1474.0529999999999</v>
       </c>
       <c r="AN77" s="42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1415.5487145000002</v>
       </c>
     </row>
@@ -32464,35 +32504,35 @@
       <c r="AE78" s="42"/>
       <c r="AF78" s="42"/>
       <c r="AG78" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>896.21360127999992</v>
       </c>
       <c r="AH78" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>927.45969032000016</v>
       </c>
       <c r="AI78" s="42">
-        <f t="shared" ref="AI78:AJ78" si="6">AI6-AI24</f>
+        <f t="shared" ref="AI78:AJ78" si="7">AI6-AI24</f>
         <v>1000.2569999999998</v>
       </c>
       <c r="AJ78" s="42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>902.56027133999987</v>
       </c>
       <c r="AK78" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>953.65139687999999</v>
       </c>
       <c r="AL78" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>871.43107229999987</v>
       </c>
       <c r="AM78" s="42">
-        <f t="shared" ref="AM78:AN78" si="7">AM6-AM24</f>
+        <f t="shared" ref="AM78:AN78" si="8">AM6-AM24</f>
         <v>959.85300000000007</v>
       </c>
       <c r="AN78" s="42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>909.12926809999976</v>
       </c>
     </row>
@@ -32546,35 +32586,35 @@
       <c r="AE79" s="42"/>
       <c r="AF79" s="42"/>
       <c r="AG79" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3276.1097171400006</v>
       </c>
       <c r="AH79" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3274.2127575000004</v>
       </c>
       <c r="AI79" s="42">
-        <f t="shared" ref="AI79:AJ79" si="8">AI7-AI25</f>
+        <f t="shared" ref="AI79:AJ79" si="9">AI7-AI25</f>
         <v>3773.1760000000004</v>
       </c>
       <c r="AJ79" s="42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3401.7746899000003</v>
       </c>
       <c r="AK79" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3762.7256515600002</v>
       </c>
       <c r="AL79" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3282.9260004800008</v>
       </c>
       <c r="AM79" s="42">
-        <f t="shared" ref="AM79:AN79" si="9">AM7-AM25</f>
+        <f t="shared" ref="AM79:AN79" si="10">AM7-AM25</f>
         <v>3365.9450000000006</v>
       </c>
       <c r="AN79" s="42">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3610.9202801000001</v>
       </c>
     </row>
@@ -32628,35 +32668,35 @@
       <c r="AE80" s="42"/>
       <c r="AF80" s="42"/>
       <c r="AG80" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4255.8744605400016</v>
       </c>
       <c r="AH80" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4208.1987573599999</v>
       </c>
       <c r="AI80" s="42">
-        <f t="shared" ref="AI80:AJ80" si="10">AI8-AI26</f>
+        <f t="shared" ref="AI80:AJ80" si="11">AI8-AI26</f>
         <v>4656.7450000000017</v>
       </c>
       <c r="AJ80" s="42">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4521.3877016000006</v>
       </c>
       <c r="AK80" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4628.6599123200003</v>
       </c>
       <c r="AL80" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4249.5789026899984</v>
       </c>
       <c r="AM80" s="42">
-        <f t="shared" ref="AM80:AN80" si="11">AM8-AM26</f>
+        <f t="shared" ref="AM80:AN80" si="12">AM8-AM26</f>
         <v>4479.6899999999987</v>
       </c>
       <c r="AN80" s="42">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4612.9053185599996</v>
       </c>
     </row>
@@ -32710,35 +32750,35 @@
       <c r="AE81" s="42"/>
       <c r="AF81" s="42"/>
       <c r="AG81" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>760.90976855999997</v>
       </c>
       <c r="AH81" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>740.96325457000012</v>
       </c>
       <c r="AI81" s="42">
-        <f t="shared" ref="AI81:AJ81" si="12">AI9-AI27</f>
+        <f t="shared" ref="AI81:AJ81" si="13">AI9-AI27</f>
         <v>810.27300000000014</v>
       </c>
       <c r="AJ81" s="42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>836.45604666000008</v>
       </c>
       <c r="AK81" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>762.50959792000003</v>
       </c>
       <c r="AL81" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>768.52296204000004</v>
       </c>
       <c r="AM81" s="42">
-        <f t="shared" ref="AM81:AN81" si="13">AM9-AM27</f>
+        <f t="shared" ref="AM81:AN81" si="14">AM9-AM27</f>
         <v>756.91600000000017</v>
       </c>
       <c r="AN81" s="42">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>786.92560320000007</v>
       </c>
     </row>
@@ -32792,35 +32832,35 @@
       <c r="AE82" s="42"/>
       <c r="AF82" s="42"/>
       <c r="AG82" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1681.3322735999996</v>
       </c>
       <c r="AH82" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1599.9274405199999</v>
       </c>
       <c r="AI82" s="42">
-        <f t="shared" ref="AI82:AJ82" si="14">AI10-AI28</f>
+        <f t="shared" ref="AI82:AJ82" si="15">AI10-AI28</f>
         <v>1776.1569999999997</v>
       </c>
       <c r="AJ82" s="42">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1566.2368944</v>
       </c>
       <c r="AK82" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1846.55748988</v>
       </c>
       <c r="AL82" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1638.4353924900001</v>
       </c>
       <c r="AM82" s="42">
-        <f t="shared" ref="AM82:AN82" si="15">AM10-AM28</f>
+        <f t="shared" ref="AM82:AN82" si="16">AM10-AM28</f>
         <v>1646.9969999999998</v>
       </c>
       <c r="AN82" s="42">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1743.5605136399995</v>
       </c>
     </row>
@@ -32874,35 +32914,35 @@
       <c r="AE83" s="42"/>
       <c r="AF83" s="42"/>
       <c r="AG83" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2021.7139125000003</v>
       </c>
       <c r="AH83" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1919.0605448300003</v>
       </c>
       <c r="AI83" s="42">
-        <f t="shared" ref="AI83:AJ83" si="16">AI11-AI29</f>
+        <f t="shared" ref="AI83:AJ83" si="17">AI11-AI29</f>
         <v>2200.4110000000001</v>
       </c>
       <c r="AJ83" s="42">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>2103.56161071</v>
       </c>
       <c r="AK83" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2161.7812875</v>
       </c>
       <c r="AL83" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2137.8690692999999</v>
       </c>
       <c r="AM83" s="42">
-        <f t="shared" ref="AM83:AN83" si="17">AM11-AM29</f>
+        <f t="shared" ref="AM83:AN83" si="18">AM11-AM29</f>
         <v>2234.5159999999996</v>
       </c>
       <c r="AN83" s="42">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2064.1052032500002</v>
       </c>
     </row>
@@ -32956,35 +32996,35 @@
       <c r="AE84" s="42"/>
       <c r="AF84" s="42"/>
       <c r="AG84" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1976.2434568800004</v>
       </c>
       <c r="AH84" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1871.5645617499995</v>
       </c>
       <c r="AI84" s="42">
-        <f t="shared" ref="AI84:AJ84" si="18">AI12-AI30</f>
+        <f t="shared" ref="AI84:AJ84" si="19">AI12-AI30</f>
         <v>2267.4649999999992</v>
       </c>
       <c r="AJ84" s="42">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1944.6649431599999</v>
       </c>
       <c r="AK84" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2263.5368491899999</v>
       </c>
       <c r="AL84" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2102.21497344</v>
       </c>
       <c r="AM84" s="42">
-        <f t="shared" ref="AM84:AN84" si="19">AM12-AM30</f>
+        <f t="shared" ref="AM84:AN84" si="20">AM12-AM30</f>
         <v>2008.5270000000005</v>
       </c>
       <c r="AN84" s="42">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2081.8784489399995</v>
       </c>
     </row>
@@ -33038,35 +33078,35 @@
       <c r="AE85" s="42"/>
       <c r="AF85" s="42"/>
       <c r="AG85" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1182.6516150900002</v>
       </c>
       <c r="AH85" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1127.9380158999998</v>
       </c>
       <c r="AI85" s="42">
-        <f t="shared" ref="AI85:AJ85" si="20">AI13-AI31</f>
+        <f t="shared" ref="AI85:AJ85" si="21">AI13-AI31</f>
         <v>1322.5039999999999</v>
       </c>
       <c r="AJ85" s="42">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1200.05694963</v>
       </c>
       <c r="AK85" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1365.7120175999999</v>
       </c>
       <c r="AL85" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1259.5445331000001</v>
       </c>
       <c r="AM85" s="42">
-        <f t="shared" ref="AM85:AN85" si="21">AM13-AM31</f>
+        <f t="shared" ref="AM85:AN85" si="22">AM13-AM31</f>
         <v>1275.0529999999999</v>
       </c>
       <c r="AN85" s="42">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1222.1156504400001</v>
       </c>
     </row>
@@ -33120,35 +33160,35 @@
       <c r="AE86" s="42"/>
       <c r="AF86" s="42"/>
       <c r="AG86" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>906.48217959000021</v>
       </c>
       <c r="AH86" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>945.03587052000012</v>
       </c>
       <c r="AI86" s="42">
-        <f t="shared" ref="AI86:AJ86" si="22">AI14-AI32</f>
+        <f t="shared" ref="AI86:AJ86" si="23">AI14-AI32</f>
         <v>1079.5370000000003</v>
       </c>
       <c r="AJ86" s="42">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1056.8057752199998</v>
       </c>
       <c r="AK86" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1101.4214624399999</v>
       </c>
       <c r="AL86" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1074.1714222800001</v>
       </c>
       <c r="AM86" s="42">
-        <f t="shared" ref="AM86:AN86" si="23">AM14-AM32</f>
+        <f t="shared" ref="AM86:AN86" si="24">AM14-AM32</f>
         <v>992.34599999999978</v>
       </c>
       <c r="AN86" s="42">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1022.2930389399999</v>
       </c>
     </row>
@@ -33202,35 +33242,35 @@
       <c r="AE87" s="42"/>
       <c r="AF87" s="42"/>
       <c r="AG87" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1111.8914365999999</v>
       </c>
       <c r="AH87" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1221.15101284</v>
       </c>
       <c r="AI87" s="42">
-        <f t="shared" ref="AI87:AJ87" si="24">AI15-AI33</f>
+        <f t="shared" ref="AI87:AJ87" si="25">AI15-AI33</f>
         <v>1423.9380000000001</v>
       </c>
       <c r="AJ87" s="42">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1193.8226369400004</v>
       </c>
       <c r="AK87" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1402.2142187999998</v>
       </c>
       <c r="AL87" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1202.4963702499999</v>
       </c>
       <c r="AM87" s="42">
-        <f t="shared" ref="AM87:AN87" si="25">AM15-AM33</f>
+        <f t="shared" ref="AM87:AN87" si="26">AM15-AM33</f>
         <v>1283.962</v>
       </c>
       <c r="AN87" s="42">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1315.2028605599999</v>
       </c>
     </row>
@@ -33284,35 +33324,35 @@
       <c r="AE88" s="42"/>
       <c r="AF88" s="42"/>
       <c r="AG88" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1379.2933674799997</v>
       </c>
       <c r="AH88" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1384.0313372999999</v>
       </c>
       <c r="AI88" s="42">
-        <f t="shared" ref="AI88:AJ88" si="26">AI16-AI34</f>
+        <f t="shared" ref="AI88:AJ88" si="27">AI16-AI34</f>
         <v>1586.1130000000003</v>
       </c>
       <c r="AJ88" s="42">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>1364.21516084</v>
       </c>
       <c r="AK88" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1501.12462448</v>
       </c>
       <c r="AL88" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1454.5839353999995</v>
       </c>
       <c r="AM88" s="42">
-        <f t="shared" ref="AM88:AN88" si="27">AM16-AM34</f>
+        <f t="shared" ref="AM88:AN88" si="28">AM16-AM34</f>
         <v>1436.125</v>
       </c>
       <c r="AN88" s="42">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>1405.4974949999996</v>
       </c>
     </row>
@@ -33366,35 +33406,35 @@
       <c r="AE89" s="42"/>
       <c r="AF89" s="42"/>
       <c r="AG89" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>934.66129535999971</v>
       </c>
       <c r="AH89" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>893.11676222999995</v>
       </c>
       <c r="AI89" s="42">
-        <f t="shared" ref="AI89:AJ89" si="28">AI17-AI35</f>
+        <f t="shared" ref="AI89:AJ89" si="29">AI17-AI35</f>
         <v>1141.6849999999999</v>
       </c>
       <c r="AJ89" s="42">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>941.77107647999992</v>
       </c>
       <c r="AK89" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1057.5670403199999</v>
       </c>
       <c r="AL89" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>951.13299599999982</v>
       </c>
       <c r="AM89" s="42">
-        <f t="shared" ref="AM89:AN89" si="29">AM17-AM35</f>
+        <f t="shared" ref="AM89:AN89" si="30">AM17-AM35</f>
         <v>1054.5749999999998</v>
       </c>
       <c r="AN89" s="42">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>938.20057664999968</v>
       </c>
     </row>
@@ -33448,35 +33488,35 @@
       <c r="AE90" s="42"/>
       <c r="AF90" s="42"/>
       <c r="AG90" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>561.179934</v>
       </c>
       <c r="AH90" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>451.49214927999992</v>
       </c>
       <c r="AI90" s="42">
-        <f t="shared" ref="AI90:AJ90" si="30">AI18-AI36</f>
+        <f t="shared" ref="AI90:AJ90" si="31">AI18-AI36</f>
         <v>668.15999999999985</v>
       </c>
       <c r="AJ90" s="42">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>545.69862743999988</v>
       </c>
       <c r="AK90" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>668.98839107999993</v>
       </c>
       <c r="AL90" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>603.94059014999993</v>
       </c>
       <c r="AM90" s="42">
-        <f t="shared" ref="AM90:AN90" si="31">AM18-AM36</f>
+        <f t="shared" ref="AM90:AN90" si="32">AM18-AM36</f>
         <v>572.81700000000023</v>
       </c>
       <c r="AN90" s="42">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>586.1642191200001</v>
       </c>
     </row>
@@ -33530,35 +33570,35 @@
       <c r="AE91" s="42"/>
       <c r="AF91" s="42"/>
       <c r="AG91" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>810.99451116</v>
       </c>
       <c r="AH91" s="42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>818.17964220000022</v>
       </c>
       <c r="AI91" s="42">
-        <f t="shared" ref="AI91:AJ91" si="32">AI19-AI37</f>
+        <f t="shared" ref="AI91:AJ91" si="33">AI19-AI37</f>
         <v>1307.171</v>
       </c>
       <c r="AJ91" s="42">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>804.71481874000028</v>
       </c>
       <c r="AK91" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1107.19743576</v>
       </c>
       <c r="AL91" s="42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>893.09570071999997</v>
       </c>
       <c r="AM91" s="42">
-        <f t="shared" ref="AM91:AN91" si="33">AM19-AM37</f>
+        <f t="shared" ref="AM91:AN91" si="34">AM19-AM37</f>
         <v>881.72699999999986</v>
       </c>
       <c r="AN91" s="42">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>950.92591387999983</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Monthly labor update - Jun 2025
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869D0B2E-016E-4065-A5C5-2A31FF340095}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C3B3AE-5E22-4093-A21D-03051EE918ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="3975" windowWidth="15270" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2959" uniqueCount="810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2999" uniqueCount="821">
   <si>
     <t>LFS Round</t>
   </si>
@@ -2468,6 +2468,39 @@
   </si>
   <si>
     <t>https://psa.gov.ph/content/participation-labor-force-may-2025-increased-5232-million-filipinos-aged-15-years-and-over</t>
+  </si>
+  <si>
+    <t>INDUSTRY</t>
+  </si>
+  <si>
+    <t>AGRICULTURE</t>
+  </si>
+  <si>
+    <t>SERVICES</t>
+  </si>
+  <si>
+    <t>PSY 2009 onwards</t>
+  </si>
+  <si>
+    <t>YLS 2006</t>
+  </si>
+  <si>
+    <t>LFS 1992</t>
+  </si>
+  <si>
+    <t>LFS 1991</t>
+  </si>
+  <si>
+    <t>LFS 1988</t>
+  </si>
+  <si>
+    <t>LFS 1989</t>
+  </si>
+  <si>
+    <t>LFS 1990</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/participation-labor-force-june-2025-increased-5242-million-filipinos-aged-15-years-and-over</t>
   </si>
 </sst>
 </file>
@@ -2480,11 +2513,25 @@
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2540,6 +2587,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2612,11 +2665,11 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2641,37 +2694,41 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2904,12 +2961,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P299"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D288" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D266" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F263" sqref="F263"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F292" sqref="F292"/>
+      <selection pane="bottomRight" activeCell="F293" sqref="F293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15398,7 +15455,7 @@
         <v>2157.422</v>
       </c>
       <c r="N274" s="2">
-        <f t="shared" ref="N274:N291" si="34">J274-K274</f>
+        <f t="shared" ref="N274:N292" si="34">J274-K274</f>
         <v>30572.822</v>
       </c>
       <c r="O274" s="2">
@@ -15628,9 +15685,6 @@
       <c r="D279" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E279" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F279" s="3">
         <f t="shared" ref="F279" si="35">K279/J279</f>
         <v>0.65995564923197714</v>
@@ -16306,7 +16360,47 @@
       <c r="D292" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="O292" s="2"/>
+      <c r="E292" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F292" s="3">
+        <f t="shared" ref="F292" si="61">K292/J292</f>
+        <v>0.65710331091544816</v>
+      </c>
+      <c r="G292" s="3">
+        <f t="shared" ref="G292" si="62">L292/K292</f>
+        <v>0.96282180199484058</v>
+      </c>
+      <c r="H292" s="3">
+        <f t="shared" ref="H292" si="63">M292/K292</f>
+        <v>3.7178178929830163E-2</v>
+      </c>
+      <c r="I292" s="3">
+        <f t="shared" ref="I292" si="64">O292/L292</f>
+        <v>0.11416914389709779</v>
+      </c>
+      <c r="J292" s="2">
+        <v>79780.05</v>
+      </c>
+      <c r="K292" s="2">
+        <v>52423.735000000001</v>
+      </c>
+      <c r="L292" s="2">
+        <v>50474.714999999997</v>
+      </c>
+      <c r="M292" s="2">
+        <v>1949.019</v>
+      </c>
+      <c r="N292" s="2">
+        <f t="shared" si="34"/>
+        <v>27356.315000000002</v>
+      </c>
+      <c r="O292" s="2">
+        <v>5762.6549999999997</v>
+      </c>
+      <c r="P292" t="s">
+        <v>820</v>
+      </c>
     </row>
     <row r="293" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
@@ -16421,23 +16515,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AE30"/>
+  <dimension ref="A1:AK45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomRight" activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="9" width="16.42578125" customWidth="1"/>
-    <col min="11" max="31" width="20.7109375" customWidth="1"/>
+    <col min="14" max="37" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>1</v>
       </c>
@@ -16465,104 +16559,107 @@
       <c r="I1" s="20" t="s">
         <v>520</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="N1" s="20" t="s">
+        <v>811</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>810</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>812</v>
+      </c>
+      <c r="Q1" s="33" t="s">
         <v>693</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="R1" s="33" t="s">
         <v>692</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="S1" s="33" t="s">
         <v>690</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="T1" s="33" t="s">
         <v>689</v>
       </c>
-      <c r="O1" s="33" t="s">
+      <c r="U1" s="33" t="s">
         <v>688</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="V1" s="33" t="s">
         <v>687</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="W1" s="33" t="s">
         <v>686</v>
       </c>
-      <c r="R1" s="33" t="s">
+      <c r="X1" s="33" t="s">
         <v>683</v>
       </c>
-      <c r="S1" s="33" t="s">
+      <c r="Y1" s="33" t="s">
         <v>682</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="Z1" s="33" t="s">
         <v>681</v>
       </c>
-      <c r="U1" s="33" t="s">
+      <c r="AA1" s="33" t="s">
         <v>680</v>
       </c>
-      <c r="V1" s="33" t="s">
+      <c r="AB1" s="33" t="s">
         <v>679</v>
       </c>
-      <c r="W1" s="33" t="s">
+      <c r="AC1" s="33" t="s">
         <v>678</v>
       </c>
-      <c r="X1" s="33" t="s">
+      <c r="AD1" s="33" t="s">
         <v>677</v>
       </c>
-      <c r="Y1" s="33" t="s">
+      <c r="AE1" s="33" t="s">
         <v>676</v>
       </c>
-      <c r="Z1" s="33" t="s">
+      <c r="AF1" s="33" t="s">
         <v>675</v>
       </c>
-      <c r="AA1" s="33" t="s">
+      <c r="AG1" s="33" t="s">
         <v>674</v>
       </c>
-      <c r="AB1" s="33" t="s">
+      <c r="AH1" s="33" t="s">
         <v>673</v>
       </c>
-      <c r="AC1" s="33" t="s">
+      <c r="AI1" s="33" t="s">
         <v>672</v>
       </c>
-      <c r="AD1" s="33" t="s">
+      <c r="AJ1" s="33" t="s">
         <v>671</v>
       </c>
-      <c r="AE1" s="33" t="s">
+      <c r="AK1" s="33" t="s">
         <v>670</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1995</v>
+        <v>1980</v>
       </c>
       <c r="B2" s="21">
-        <v>43156</v>
+        <v>28967</v>
       </c>
       <c r="C2" s="21">
-        <v>65.8</v>
+        <v>59.6</v>
       </c>
       <c r="D2" s="21">
-        <v>28380</v>
+        <v>17268</v>
       </c>
       <c r="E2" s="21">
-        <v>90.5</v>
+        <v>92.1</v>
       </c>
       <c r="F2" s="21">
-        <v>25677</v>
+        <v>15900</v>
       </c>
       <c r="G2" s="21">
-        <v>9.5</v>
+        <v>7.9</v>
       </c>
       <c r="H2" s="21">
-        <v>2704</v>
-      </c>
-      <c r="I2" s="21">
-        <v>20</v>
-      </c>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
+        <v>1368</v>
+      </c>
+      <c r="I2" s="21"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
       <c r="Q2" s="34"/>
       <c r="R2" s="34"/>
       <c r="S2" s="34"/>
@@ -16578,41 +16675,41 @@
       <c r="AC2" s="34"/>
       <c r="AD2" s="34"/>
       <c r="AE2" s="34"/>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF2" s="34"/>
+      <c r="AG2" s="34"/>
+      <c r="AH2" s="34"/>
+      <c r="AI2" s="34"/>
+      <c r="AJ2" s="34"/>
+      <c r="AK2" s="34"/>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1996</v>
+        <v>1981</v>
       </c>
       <c r="B3" s="21">
-        <v>44599</v>
+        <v>29501</v>
       </c>
       <c r="C3" s="21">
-        <v>66.7</v>
+        <v>61.7</v>
       </c>
       <c r="D3" s="21">
-        <v>29733</v>
+        <v>18202</v>
       </c>
       <c r="E3" s="21">
-        <v>91.4</v>
+        <v>91.2</v>
       </c>
       <c r="F3" s="21">
-        <v>27186</v>
+        <v>16595</v>
       </c>
       <c r="G3" s="21">
-        <v>8.6</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="H3" s="21">
-        <v>2546</v>
-      </c>
-      <c r="I3" s="21">
-        <v>21</v>
-      </c>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="34"/>
+        <v>1606</v>
+      </c>
+      <c r="I3" s="21"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
       <c r="Q3" s="34"/>
       <c r="R3" s="34"/>
       <c r="S3" s="34"/>
@@ -16628,41 +16725,41 @@
       <c r="AC3" s="34"/>
       <c r="AD3" s="34"/>
       <c r="AE3" s="34"/>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF3" s="34"/>
+      <c r="AG3" s="34"/>
+      <c r="AH3" s="34"/>
+      <c r="AI3" s="34"/>
+      <c r="AJ3" s="34"/>
+      <c r="AK3" s="34"/>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1997</v>
+        <v>1982</v>
       </c>
       <c r="B4" s="21">
-        <v>44658</v>
+        <v>30414</v>
       </c>
       <c r="C4" s="21">
-        <v>64.7</v>
+        <v>61</v>
       </c>
       <c r="D4" s="21">
-        <v>28901</v>
+        <v>18551</v>
       </c>
       <c r="E4" s="21">
-        <v>91.2</v>
+        <v>90.6</v>
       </c>
       <c r="F4" s="21">
-        <v>26365</v>
+        <v>16808</v>
       </c>
       <c r="G4" s="21">
-        <v>8.8000000000000007</v>
+        <v>9.4</v>
       </c>
       <c r="H4" s="21">
-        <v>2537</v>
-      </c>
-      <c r="I4" s="21">
-        <v>21.9</v>
-      </c>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="34"/>
+        <v>1742</v>
+      </c>
+      <c r="I4" s="21"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
       <c r="Q4" s="34"/>
       <c r="R4" s="34"/>
       <c r="S4" s="34"/>
@@ -16678,41 +16775,41 @@
       <c r="AC4" s="34"/>
       <c r="AD4" s="34"/>
       <c r="AE4" s="34"/>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF4" s="34"/>
+      <c r="AG4" s="34"/>
+      <c r="AH4" s="34"/>
+      <c r="AI4" s="34"/>
+      <c r="AJ4" s="34"/>
+      <c r="AK4" s="34"/>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1998</v>
+        <v>1983</v>
       </c>
       <c r="B5" s="21">
-        <v>45964</v>
+        <v>31278</v>
       </c>
       <c r="C5" s="21">
-        <v>64.599999999999994</v>
+        <v>63.5</v>
       </c>
       <c r="D5" s="21">
-        <v>29674</v>
+        <v>19855</v>
       </c>
       <c r="E5" s="21">
-        <v>89.7</v>
+        <v>89.6</v>
       </c>
       <c r="F5" s="21">
-        <v>26631</v>
+        <v>17791</v>
       </c>
       <c r="G5" s="21">
-        <v>10.3</v>
+        <v>10.4</v>
       </c>
       <c r="H5" s="21">
-        <v>3043</v>
-      </c>
-      <c r="I5" s="21">
-        <v>21.6</v>
-      </c>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
+        <v>2064</v>
+      </c>
+      <c r="I5" s="21"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
       <c r="Q5" s="34"/>
       <c r="R5" s="34"/>
       <c r="S5" s="34"/>
@@ -16728,41 +16825,41 @@
       <c r="AC5" s="34"/>
       <c r="AD5" s="34"/>
       <c r="AE5" s="34"/>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF5" s="34"/>
+      <c r="AG5" s="34"/>
+      <c r="AH5" s="34"/>
+      <c r="AI5" s="34"/>
+      <c r="AJ5" s="34"/>
+      <c r="AK5" s="34"/>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1999</v>
+        <v>1984</v>
       </c>
       <c r="B6" s="21">
-        <v>47270</v>
+        <v>32261</v>
       </c>
       <c r="C6" s="21">
-        <v>65.099999999999994</v>
+        <v>63.3</v>
       </c>
       <c r="D6" s="21">
-        <v>30759</v>
+        <v>20416</v>
       </c>
       <c r="E6" s="21">
-        <v>90.2</v>
+        <v>89.6</v>
       </c>
       <c r="F6" s="21">
-        <v>27742</v>
+        <v>18292</v>
       </c>
       <c r="G6" s="21">
-        <v>9.8000000000000007</v>
+        <v>10.4</v>
       </c>
       <c r="H6" s="21">
-        <v>3017</v>
-      </c>
-      <c r="I6" s="21">
-        <v>22.1</v>
-      </c>
-      <c r="K6" s="34"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
+        <v>2124</v>
+      </c>
+      <c r="I6" s="21"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
       <c r="Q6" s="34"/>
       <c r="R6" s="34"/>
       <c r="S6" s="34"/>
@@ -16778,41 +16875,41 @@
       <c r="AC6" s="34"/>
       <c r="AD6" s="34"/>
       <c r="AE6" s="34"/>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF6" s="34"/>
+      <c r="AG6" s="34"/>
+      <c r="AH6" s="34"/>
+      <c r="AI6" s="34"/>
+      <c r="AJ6" s="34"/>
+      <c r="AK6" s="34"/>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2000</v>
+        <v>1985</v>
       </c>
       <c r="B7" s="21">
-        <v>48587</v>
+        <v>32889</v>
       </c>
       <c r="C7" s="21">
-        <v>63.6</v>
+        <v>63.1</v>
       </c>
       <c r="D7" s="21">
-        <v>30911</v>
+        <v>20743</v>
       </c>
       <c r="E7" s="21">
-        <v>88.809808805926693</v>
+        <v>87.4</v>
       </c>
       <c r="F7" s="21">
-        <v>27452</v>
+        <v>18136</v>
       </c>
       <c r="G7" s="21">
-        <v>11.190191194073307</v>
+        <v>12.6</v>
       </c>
       <c r="H7" s="21">
-        <v>3459</v>
-      </c>
-      <c r="I7" s="21">
-        <v>21.7</v>
-      </c>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="34"/>
+        <v>2608</v>
+      </c>
+      <c r="I7" s="21"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
       <c r="Q7" s="34"/>
       <c r="R7" s="34"/>
       <c r="S7" s="34"/>
@@ -16828,42 +16925,45 @@
       <c r="AC7" s="34"/>
       <c r="AD7" s="34"/>
       <c r="AE7" s="34"/>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF7" s="34"/>
+      <c r="AG7" s="34"/>
+      <c r="AH7" s="34"/>
+      <c r="AI7" s="34"/>
+      <c r="AJ7" s="34"/>
+      <c r="AK7" s="34"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2001</v>
+        <v>1986</v>
       </c>
       <c r="B8" s="21">
-        <v>48929</v>
+        <v>33469</v>
       </c>
       <c r="C8" s="21">
-        <v>67.099999999999994</v>
+        <v>63.8</v>
       </c>
       <c r="D8" s="21">
-        <v>32809</v>
+        <v>21362</v>
       </c>
       <c r="E8" s="21">
-        <v>88.865859977445211</v>
+        <v>88.2</v>
       </c>
       <c r="F8" s="21">
-        <v>29156</v>
+        <v>18836</v>
       </c>
       <c r="G8" s="21">
-        <v>11.134140022554787</v>
+        <v>11.8</v>
       </c>
       <c r="H8" s="21">
-        <v>3653</v>
-      </c>
-      <c r="I8" s="21">
-        <v>17.2</v>
-      </c>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
-      <c r="O8" s="34"/>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="34"/>
+        <v>2526</v>
+      </c>
+      <c r="I8" s="21"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
       <c r="R8" s="34"/>
       <c r="S8" s="34"/>
       <c r="T8" s="34"/>
@@ -16878,41 +16978,43 @@
       <c r="AC8" s="34"/>
       <c r="AD8" s="34"/>
       <c r="AE8" s="34"/>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF8" s="34"/>
+      <c r="AG8" s="34"/>
+      <c r="AH8" s="34"/>
+      <c r="AI8" s="34"/>
+      <c r="AJ8" s="34"/>
+      <c r="AK8" s="34"/>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2002</v>
+        <v>1987</v>
       </c>
       <c r="B9" s="21">
-        <v>50344</v>
+        <v>34462</v>
       </c>
       <c r="C9" s="21">
-        <v>67.400000000000006</v>
+        <v>65.5</v>
       </c>
       <c r="D9" s="21">
-        <v>33936</v>
+        <v>22563</v>
       </c>
       <c r="E9" s="21">
-        <v>88.584394153701083</v>
+        <v>88.8</v>
       </c>
       <c r="F9" s="21">
-        <v>30062</v>
+        <v>20040</v>
       </c>
       <c r="G9" s="21">
-        <v>11.415605846298915</v>
+        <v>11.2</v>
       </c>
       <c r="H9" s="21">
-        <v>3874</v>
+        <v>2523</v>
       </c>
       <c r="I9" s="21">
-        <v>17</v>
-      </c>
-      <c r="K9" s="34"/>
-      <c r="L9" s="34"/>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
+        <v>26.5</v>
+      </c>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
       <c r="Q9" s="34"/>
       <c r="R9" s="34"/>
       <c r="S9" s="34"/>
@@ -16928,41 +17030,57 @@
       <c r="AC9" s="34"/>
       <c r="AD9" s="34"/>
       <c r="AE9" s="34"/>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF9" s="34"/>
+      <c r="AG9" s="34"/>
+      <c r="AH9" s="34"/>
+      <c r="AI9" s="34"/>
+      <c r="AJ9" s="34"/>
+      <c r="AK9" s="34"/>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2003</v>
+        <v>1988</v>
       </c>
       <c r="B10" s="21">
-        <v>51793</v>
+        <v>35478</v>
       </c>
       <c r="C10" s="21">
-        <v>66.7</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="D10" s="21">
-        <v>34571</v>
+        <v>23449</v>
       </c>
       <c r="E10" s="21">
-        <v>88.614734893407771</v>
+        <v>90.4</v>
       </c>
       <c r="F10" s="21">
-        <v>30635</v>
+        <v>21205</v>
       </c>
       <c r="G10" s="21">
-        <v>11.385265106592231</v>
+        <v>9.6</v>
       </c>
       <c r="H10" s="21">
-        <v>3936</v>
+        <v>2244</v>
       </c>
       <c r="I10" s="21">
-        <v>17</v>
-      </c>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
+        <v>23.5</v>
+      </c>
+      <c r="L10" s="48" t="s">
+        <v>817</v>
+      </c>
+      <c r="M10" s="48"/>
+      <c r="N10" s="47">
+        <f>AVERAGE(9974, 10089, 9891, 9920)</f>
+        <v>9968.5</v>
+      </c>
+      <c r="O10" s="47">
+        <f>AVERAGE(SUM(145,2085,85,762),SUM(176,2158,80,836),SUM(163,2250,80,865),SUM(157,2238,95,858))</f>
+        <v>3258.25</v>
+      </c>
+      <c r="P10" s="47">
+        <f>AVERAGE(SUM(2795,955,393,3632),SUM(2788,1025,406,3582,1),SUM(2930,1029,381,3765,1),SUM(2972,1049,379,3827,2))</f>
+        <v>7978</v>
+      </c>
       <c r="Q10" s="34"/>
       <c r="R10" s="34"/>
       <c r="S10" s="34"/>
@@ -16978,41 +17096,57 @@
       <c r="AC10" s="34"/>
       <c r="AD10" s="34"/>
       <c r="AE10" s="34"/>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF10" s="34"/>
+      <c r="AG10" s="34"/>
+      <c r="AH10" s="34"/>
+      <c r="AI10" s="34"/>
+      <c r="AJ10" s="34"/>
+      <c r="AK10" s="34"/>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2004</v>
+        <v>1989</v>
       </c>
       <c r="B11" s="21">
-        <v>53144</v>
+        <v>36520</v>
       </c>
       <c r="C11" s="21">
-        <v>67.5</v>
+        <v>66</v>
       </c>
       <c r="D11" s="21">
-        <v>35862</v>
+        <v>24120</v>
       </c>
       <c r="E11" s="21">
-        <v>88.151804138084884</v>
+        <v>90.8</v>
       </c>
       <c r="F11" s="21">
-        <v>31613</v>
+        <v>21908</v>
       </c>
       <c r="G11" s="21">
-        <v>11.848195861915119</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="H11" s="21">
-        <v>4249</v>
+        <v>2212</v>
       </c>
       <c r="I11" s="21">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
-      <c r="P11" s="34"/>
+        <v>23.2</v>
+      </c>
+      <c r="L11" s="48" t="s">
+        <v>818</v>
+      </c>
+      <c r="M11" s="48"/>
+      <c r="N11" s="47">
+        <f>AVERAGE(9650, 10205, 9896, 9852)</f>
+        <v>9900.75</v>
+      </c>
+      <c r="O11" s="47">
+        <f>AVERAGE(SUM(182,2321,89,949),SUM(180,2309,96,959),SUM(156,2336,96,905),SUM(154,2298,83,911))</f>
+        <v>3506</v>
+      </c>
+      <c r="P11" s="47">
+        <f>AVERAGE(SUM(3010,1055,388,3907,1),SUM(3138,1082,399,3965,10),SUM(3098,1055,405,3925,16),SUM(3074,1095,398,3972,13))</f>
+        <v>8501.5</v>
+      </c>
       <c r="Q11" s="34"/>
       <c r="R11" s="34"/>
       <c r="S11" s="34"/>
@@ -17028,41 +17162,57 @@
       <c r="AC11" s="34"/>
       <c r="AD11" s="34"/>
       <c r="AE11" s="34"/>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF11" s="34"/>
+      <c r="AG11" s="34"/>
+      <c r="AH11" s="34"/>
+      <c r="AI11" s="34"/>
+      <c r="AJ11" s="34"/>
+      <c r="AK11" s="34"/>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2005</v>
+        <v>1990</v>
       </c>
       <c r="B12" s="21">
-        <v>54388</v>
+        <v>37636</v>
       </c>
       <c r="C12" s="21">
-        <v>64.716310972814028</v>
+        <v>64.400000000000006</v>
       </c>
       <c r="D12" s="21">
-        <v>35286</v>
+        <v>24244</v>
       </c>
       <c r="E12" s="21">
-        <v>92.21337414156298</v>
+        <v>91.6</v>
       </c>
       <c r="F12" s="21">
-        <v>32539</v>
+        <v>22212</v>
       </c>
       <c r="G12" s="21">
-        <v>7.7866258584370058</v>
+        <v>8.4</v>
       </c>
       <c r="H12" s="21">
-        <v>2747.6666666666665</v>
+        <v>2032</v>
       </c>
       <c r="I12" s="21">
-        <v>21</v>
-      </c>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="34"/>
-      <c r="P12" s="34"/>
+        <v>22.4</v>
+      </c>
+      <c r="L12" s="48" t="s">
+        <v>819</v>
+      </c>
+      <c r="M12" s="48"/>
+      <c r="N12" s="47">
+        <f>AVERAGE(9750, 10008, 10185)</f>
+        <v>9981</v>
+      </c>
+      <c r="O12" s="47">
+        <f>AVERAGE(SUM(139, 2309, 84, 959),SUM(116, 2210, 91, 970),SUM(133, 2188, 91, 974))</f>
+        <v>3421.3333333333335</v>
+      </c>
+      <c r="P12" s="47">
+        <f>AVERAGE(SUM(3188, 1062, 410, 3983, 16),SUM(3134, 1089, 451, 4119, 14),SUM(3145, 1137, 444, 4220, 15))</f>
+        <v>8809</v>
+      </c>
       <c r="Q12" s="34"/>
       <c r="R12" s="34"/>
       <c r="S12" s="34"/>
@@ -17078,41 +17228,57 @@
       <c r="AC12" s="34"/>
       <c r="AD12" s="34"/>
       <c r="AE12" s="34"/>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF12" s="34"/>
+      <c r="AG12" s="34"/>
+      <c r="AH12" s="34"/>
+      <c r="AI12" s="34"/>
+      <c r="AJ12" s="34"/>
+      <c r="AK12" s="34"/>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2006</v>
+        <v>1991</v>
       </c>
       <c r="B13" s="21">
-        <v>55230</v>
+        <v>38599</v>
       </c>
       <c r="C13" s="21">
-        <v>64.2</v>
+        <v>66.400000000000006</v>
       </c>
       <c r="D13" s="21">
-        <v>35464</v>
+        <v>25631</v>
       </c>
       <c r="E13" s="21">
-        <v>92.02312138728324</v>
+        <v>89.4</v>
       </c>
       <c r="F13" s="21">
-        <v>32636</v>
+        <v>22914</v>
       </c>
       <c r="G13" s="21">
-        <v>7.9768786127167628</v>
+        <v>10.6</v>
       </c>
       <c r="H13" s="21">
-        <v>2829</v>
+        <v>2716</v>
       </c>
       <c r="I13" s="21">
-        <v>22.6</v>
-      </c>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="34"/>
+        <v>22.5</v>
+      </c>
+      <c r="L13" s="48" t="s">
+        <v>816</v>
+      </c>
+      <c r="M13" s="48"/>
+      <c r="N13" s="47">
+        <f>AVERAGE(9999,10538,10219,10403)</f>
+        <v>10289.75</v>
+      </c>
+      <c r="O13" s="47">
+        <f>AVERAGE(SUM(130,2292,97,974),SUM(150, 2434, 102, 1033),SUM(132, 2378, 99, 1019),SUM(150,2391,99,1046))</f>
+        <v>3631.5</v>
+      </c>
+      <c r="P13" s="47">
+        <f>AVERAGE(SUM(3228,1170,476,4159,8),SUM(3409,1148,467,4263,15),SUM(3065,1106,464,4093,10),SUM(3172,1143,451,4116,9))</f>
+        <v>8993</v>
+      </c>
       <c r="Q13" s="34"/>
       <c r="R13" s="34"/>
       <c r="S13" s="34"/>
@@ -17128,41 +17294,57 @@
       <c r="AC13" s="34"/>
       <c r="AD13" s="34"/>
       <c r="AE13" s="34"/>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF13" s="34"/>
+      <c r="AG13" s="34"/>
+      <c r="AH13" s="34"/>
+      <c r="AI13" s="34"/>
+      <c r="AJ13" s="34"/>
+      <c r="AK13" s="34"/>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2007</v>
+        <v>1992</v>
       </c>
       <c r="B14" s="21">
-        <v>56565</v>
+        <v>39831</v>
       </c>
       <c r="C14" s="21">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D14" s="21">
-        <v>36213</v>
+        <v>26290</v>
       </c>
       <c r="E14" s="21">
-        <v>92.67390163753349</v>
+        <v>90.1</v>
       </c>
       <c r="F14" s="21">
-        <v>33560</v>
+        <v>23696</v>
       </c>
       <c r="G14" s="21">
-        <v>7.3260983624665172</v>
+        <v>9.9</v>
       </c>
       <c r="H14" s="21">
-        <v>2653</v>
+        <v>2594</v>
       </c>
       <c r="I14" s="21">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="34"/>
-      <c r="P14" s="34"/>
+        <v>20</v>
+      </c>
+      <c r="L14" s="48" t="s">
+        <v>815</v>
+      </c>
+      <c r="M14" s="48"/>
+      <c r="N14" s="47">
+        <f>AVERAGE(10297, 10873, 10867, 10869)</f>
+        <v>10726.5</v>
+      </c>
+      <c r="O14" s="47">
+        <f>AVERAGE(SUM(146, 2452, 96, 1084),SUM(153, 2559, 93, 1074),SUM(146, 2535, 84, 1055),SUM(143, 2546, 92, 1035))</f>
+        <v>3823.25</v>
+      </c>
+      <c r="P14" s="47">
+        <f>AVERAGE(SUM(3177, 1150, 454, 4163, 15),SUM(3320, 1229, 427, 4193, 16),SUM(3325, 1217, 445, 4202, 23),SUM(3283, 1221, 452, 4254, 21))</f>
+        <v>9146.75</v>
+      </c>
       <c r="Q14" s="34"/>
       <c r="R14" s="34"/>
       <c r="S14" s="34"/>
@@ -17178,41 +17360,53 @@
       <c r="AC14" s="34"/>
       <c r="AD14" s="34"/>
       <c r="AE14" s="34"/>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF14" s="34"/>
+      <c r="AG14" s="34"/>
+      <c r="AH14" s="34"/>
+      <c r="AI14" s="34"/>
+      <c r="AJ14" s="34"/>
+      <c r="AK14" s="34"/>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2008</v>
+        <v>1993</v>
       </c>
       <c r="B15" s="21">
-        <v>57848</v>
+        <v>41004</v>
       </c>
       <c r="C15" s="21">
-        <v>63.6</v>
+        <v>65.599999999999994</v>
       </c>
       <c r="D15" s="21">
-        <v>36805</v>
+        <v>26879</v>
       </c>
       <c r="E15" s="21">
-        <v>92.620567857628046</v>
+        <v>90.7</v>
       </c>
       <c r="F15" s="21">
-        <v>34089</v>
+        <v>24382</v>
       </c>
       <c r="G15" s="21">
-        <v>7.4</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="H15" s="21">
-        <v>2716</v>
+        <v>2497</v>
       </c>
       <c r="I15" s="21">
-        <v>19.3</v>
-      </c>
-      <c r="K15" s="34"/>
-      <c r="L15" s="34"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
-      <c r="O15" s="34"/>
-      <c r="P15" s="34"/>
+        <v>21.7</v>
+      </c>
+      <c r="L15" t="s">
+        <v>814</v>
+      </c>
+      <c r="N15" s="2">
+        <v>11139</v>
+      </c>
+      <c r="O15" s="2">
+        <v>3804</v>
+      </c>
+      <c r="P15" s="2">
+        <v>9440</v>
+      </c>
       <c r="Q15" s="34"/>
       <c r="R15" s="34"/>
       <c r="S15" s="34"/>
@@ -17228,41 +17422,53 @@
       <c r="AC15" s="34"/>
       <c r="AD15" s="34"/>
       <c r="AE15" s="34"/>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF15" s="34"/>
+      <c r="AG15" s="34"/>
+      <c r="AH15" s="34"/>
+      <c r="AI15" s="34"/>
+      <c r="AJ15" s="34"/>
+      <c r="AK15" s="34"/>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2009</v>
+        <v>1994</v>
       </c>
       <c r="B16" s="21">
-        <v>59237</v>
+        <v>42213</v>
       </c>
       <c r="C16" s="21">
-        <v>63.966355487279912</v>
+        <v>65.5</v>
       </c>
       <c r="D16" s="21">
-        <v>37891.75</v>
+        <v>27654</v>
       </c>
       <c r="E16" s="21">
-        <v>92.530036221604973</v>
+        <v>90.5</v>
       </c>
       <c r="F16" s="21">
-        <v>35061.25</v>
+        <v>25032</v>
       </c>
       <c r="G16" s="21">
-        <v>7.4699637783950337</v>
+        <v>9.5</v>
       </c>
       <c r="H16" s="21">
-        <v>2830.5</v>
+        <v>2622</v>
       </c>
       <c r="I16" s="21">
-        <v>19.087311490605728</v>
-      </c>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
-      <c r="O16" s="34"/>
-      <c r="P16" s="34"/>
+        <v>21.4</v>
+      </c>
+      <c r="L16" t="s">
+        <v>814</v>
+      </c>
+      <c r="N16" s="2">
+        <v>11286</v>
+      </c>
+      <c r="O16" s="2">
+        <v>3948</v>
+      </c>
+      <c r="P16" s="2">
+        <v>9798</v>
+      </c>
       <c r="Q16" s="34"/>
       <c r="R16" s="34"/>
       <c r="S16" s="34"/>
@@ -17278,41 +17484,53 @@
       <c r="AC16" s="34"/>
       <c r="AD16" s="34"/>
       <c r="AE16" s="34"/>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF16" s="34"/>
+      <c r="AG16" s="34"/>
+      <c r="AH16" s="34"/>
+      <c r="AI16" s="34"/>
+      <c r="AJ16" s="34"/>
+      <c r="AK16" s="34"/>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2010</v>
+        <v>1995</v>
       </c>
       <c r="B17" s="21">
-        <v>60717</v>
+        <v>43156</v>
       </c>
       <c r="C17" s="21">
-        <v>64.099999999999994</v>
+        <v>65.8</v>
       </c>
       <c r="D17" s="21">
-        <v>38893</v>
+        <v>28380</v>
       </c>
       <c r="E17" s="21">
-        <v>92.7</v>
+        <v>90.5</v>
       </c>
       <c r="F17" s="21">
-        <v>36035</v>
+        <v>25676</v>
       </c>
       <c r="G17" s="21">
-        <v>7.3</v>
+        <v>9.5</v>
       </c>
       <c r="H17" s="21">
-        <v>2859</v>
+        <v>2704</v>
       </c>
       <c r="I17" s="21">
-        <v>18.7</v>
-      </c>
-      <c r="K17" s="34"/>
-      <c r="L17" s="34"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
-      <c r="O17" s="34"/>
-      <c r="P17" s="34"/>
+        <v>20</v>
+      </c>
+      <c r="L17" t="s">
+        <v>814</v>
+      </c>
+      <c r="N17" s="2">
+        <v>11147</v>
+      </c>
+      <c r="O17" s="2">
+        <v>4139</v>
+      </c>
+      <c r="P17" s="2">
+        <v>10391</v>
+      </c>
       <c r="Q17" s="34"/>
       <c r="R17" s="34"/>
       <c r="S17" s="34"/>
@@ -17328,41 +17546,53 @@
       <c r="AC17" s="34"/>
       <c r="AD17" s="34"/>
       <c r="AE17" s="34"/>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF17" s="34"/>
+      <c r="AG17" s="34"/>
+      <c r="AH17" s="34"/>
+      <c r="AI17" s="34"/>
+      <c r="AJ17" s="34"/>
+      <c r="AK17" s="34"/>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2011</v>
+        <v>1996</v>
       </c>
       <c r="B18" s="21">
-        <v>61882.531999999999</v>
+        <v>44599</v>
       </c>
       <c r="C18" s="21">
-        <v>64.647477174980494</v>
+        <v>66.7</v>
       </c>
       <c r="D18" s="21">
-        <v>40006.042999999998</v>
+        <v>29733</v>
       </c>
       <c r="E18" s="21">
-        <v>92.967334369303501</v>
+        <v>91.4</v>
       </c>
       <c r="F18" s="21">
-        <v>37192.042999999998</v>
+        <v>27186</v>
       </c>
       <c r="G18" s="21">
-        <v>7.0326656306965027</v>
+        <v>8.6</v>
       </c>
       <c r="H18" s="21">
-        <v>2814</v>
+        <v>2546</v>
       </c>
       <c r="I18" s="21">
-        <v>19.260093482899016</v>
-      </c>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="34"/>
-      <c r="P18" s="34"/>
+        <v>21</v>
+      </c>
+      <c r="L18" t="s">
+        <v>814</v>
+      </c>
+      <c r="N18" s="2">
+        <v>11523</v>
+      </c>
+      <c r="O18" s="2">
+        <v>4430</v>
+      </c>
+      <c r="P18" s="2">
+        <v>11112</v>
+      </c>
       <c r="Q18" s="34"/>
       <c r="R18" s="34"/>
       <c r="S18" s="34"/>
@@ -17378,1037 +17608,744 @@
       <c r="AC18" s="34"/>
       <c r="AD18" s="34"/>
       <c r="AE18" s="34"/>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF18" s="34"/>
+      <c r="AG18" s="34"/>
+      <c r="AH18" s="34"/>
+      <c r="AI18" s="34"/>
+      <c r="AJ18" s="34"/>
+      <c r="AK18" s="34"/>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2012</v>
+        <v>1997</v>
       </c>
       <c r="B19" s="21">
-        <v>62985.349249999999</v>
+        <v>43704</v>
       </c>
       <c r="C19" s="21">
-        <v>64.183842721170592</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="D19" s="21">
-        <v>40426.417499999996</v>
+        <v>28902</v>
       </c>
       <c r="E19" s="21">
-        <v>93.008986636028297</v>
+        <v>91.2</v>
       </c>
       <c r="F19" s="21">
-        <v>37600.201249999998</v>
+        <v>26365</v>
       </c>
       <c r="G19" s="21">
-        <v>6.9910133639717156</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="H19" s="21">
-        <v>2826.2162499999999</v>
+        <v>2537</v>
       </c>
       <c r="I19" s="21">
-        <v>19.984181600623746</v>
-      </c>
-      <c r="K19" s="34">
-        <v>10660.443499999999</v>
-      </c>
-      <c r="L19" s="34">
-        <v>1432.2945</v>
-      </c>
-      <c r="M19" s="34">
-        <v>249.89350000000002</v>
-      </c>
-      <c r="N19" s="34">
-        <v>3112.3870000000002</v>
-      </c>
-      <c r="O19" s="34">
-        <v>89.460250000000002</v>
-      </c>
-      <c r="P19" s="34">
-        <v>59.448500000000003</v>
-      </c>
-      <c r="Q19" s="34">
-        <v>2231.9047500000001</v>
-      </c>
-      <c r="R19" s="34">
-        <v>6863.9697500000002</v>
-      </c>
-      <c r="S19" s="34">
-        <v>2616.8715000000002</v>
-      </c>
-      <c r="T19" s="34">
-        <v>1571.3187500000001</v>
-      </c>
-      <c r="U19" s="34">
-        <v>338.03375</v>
-      </c>
-      <c r="V19" s="34">
-        <v>437.43799999999999</v>
-      </c>
-      <c r="W19" s="34">
-        <v>170.4265</v>
-      </c>
-      <c r="X19" s="34">
-        <v>188.90125</v>
-      </c>
-      <c r="Y19" s="34">
-        <v>936.55849999999998</v>
-      </c>
-      <c r="Z19" s="34">
-        <v>1957.98875</v>
-      </c>
-      <c r="AA19" s="34">
-        <v>1200.0219999999999</v>
-      </c>
-      <c r="AB19" s="34">
-        <v>437.64800000000002</v>
-      </c>
-      <c r="AC19" s="34">
-        <v>327.77875</v>
-      </c>
-      <c r="AD19" s="34">
-        <v>2715.1417500000002</v>
-      </c>
-      <c r="AE19" s="34">
-        <v>2.2725</v>
-      </c>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+        <v>21.9</v>
+      </c>
+      <c r="L19" t="s">
+        <v>814</v>
+      </c>
+      <c r="N19" s="47">
+        <v>10762.656278188706</v>
+      </c>
+      <c r="O19" s="47">
+        <v>4404.9479523723612</v>
+      </c>
+      <c r="P19" s="47">
+        <v>11197.157946960129</v>
+      </c>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="34"/>
+      <c r="S19" s="34"/>
+      <c r="T19" s="34"/>
+      <c r="U19" s="34"/>
+      <c r="V19" s="34"/>
+      <c r="W19" s="34"/>
+      <c r="X19" s="34"/>
+      <c r="Y19" s="34"/>
+      <c r="Z19" s="34"/>
+      <c r="AA19" s="34"/>
+      <c r="AB19" s="34"/>
+      <c r="AC19" s="34"/>
+      <c r="AD19" s="34"/>
+      <c r="AE19" s="34"/>
+      <c r="AF19" s="34"/>
+      <c r="AG19" s="34"/>
+      <c r="AH19" s="34"/>
+      <c r="AI19" s="34"/>
+      <c r="AJ19" s="34"/>
+      <c r="AK19" s="34"/>
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2013</v>
+        <v>1998</v>
       </c>
       <c r="B20" s="21">
-        <v>64173.311000000002</v>
+        <v>44995</v>
       </c>
       <c r="C20" s="21">
-        <v>63.92431465784896</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="D20" s="21">
-        <v>41022.349249999999</v>
+        <v>29674</v>
       </c>
       <c r="E20" s="21">
-        <v>92.919384059897538</v>
+        <v>89.7</v>
       </c>
       <c r="F20" s="21">
-        <v>38117.714249999997</v>
+        <v>26631</v>
       </c>
       <c r="G20" s="21">
-        <v>7.0806159401024553</v>
+        <v>10.3</v>
       </c>
       <c r="H20" s="21">
-        <v>2904.6350000000002</v>
+        <v>3043</v>
       </c>
       <c r="I20" s="21">
-        <v>19.338649090166786</v>
-      </c>
-      <c r="K20" s="34">
-        <v>10428.695750000001</v>
-      </c>
-      <c r="L20" s="34">
-        <v>1406.6915000000001</v>
-      </c>
-      <c r="M20" s="34">
-        <v>250.28675000000001</v>
-      </c>
-      <c r="N20" s="34">
-        <v>3159.3564999999999</v>
-      </c>
-      <c r="O20" s="34">
-        <v>94.4375</v>
-      </c>
-      <c r="P20" s="34">
-        <v>60.097000000000001</v>
-      </c>
-      <c r="Q20" s="34">
-        <v>2372.7269999999999</v>
-      </c>
-      <c r="R20" s="34">
-        <v>7105.4902499999998</v>
-      </c>
-      <c r="S20" s="34">
-        <v>2734.2240000000002</v>
-      </c>
-      <c r="T20" s="34">
-        <v>1606.8902499999999</v>
-      </c>
-      <c r="U20" s="34">
-        <v>344.45125000000002</v>
-      </c>
-      <c r="V20" s="34">
-        <v>448.21800000000002</v>
-      </c>
-      <c r="W20" s="34">
-        <v>172.61799999999999</v>
-      </c>
-      <c r="X20" s="34">
-        <v>193.99700000000001</v>
-      </c>
-      <c r="Y20" s="34">
-        <v>1015.7535</v>
-      </c>
-      <c r="Z20" s="34">
-        <v>1965.4057500000001</v>
-      </c>
-      <c r="AA20" s="34">
-        <v>1225.6490000000001</v>
-      </c>
-      <c r="AB20" s="34">
-        <v>468.85025000000002</v>
-      </c>
-      <c r="AC20" s="34">
-        <v>347.25475</v>
-      </c>
-      <c r="AD20" s="34">
-        <v>2712.7429999999999</v>
-      </c>
-      <c r="AE20" s="34">
-        <v>3.8767499999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2014</v>
-      </c>
-      <c r="B21" s="21">
-        <v>64033.078333333338</v>
-      </c>
-      <c r="C21" s="21">
-        <v>64.621820071277213</v>
-      </c>
-      <c r="D21" s="21">
-        <v>41379.340666666671</v>
-      </c>
-      <c r="E21" s="21">
-        <v>93.407133553328265</v>
-      </c>
-      <c r="F21" s="21">
-        <v>38651.256000000001</v>
-      </c>
-      <c r="G21" s="21">
-        <v>6.5928664466717537</v>
-      </c>
-      <c r="H21" s="21">
-        <v>2728.0846666666666</v>
-      </c>
-      <c r="I21" s="21">
-        <v>18.41672363764841</v>
-      </c>
-      <c r="K21" s="34">
-        <v>10404.944333333335</v>
-      </c>
-      <c r="L21" s="34">
-        <v>1396.4763333333333</v>
-      </c>
-      <c r="M21" s="34">
-        <v>239.42033333333336</v>
-      </c>
-      <c r="N21" s="34">
-        <v>3212.1773333333335</v>
-      </c>
-      <c r="O21" s="34">
-        <v>85.983666666666679</v>
-      </c>
-      <c r="P21" s="34">
-        <v>51.211333333333336</v>
-      </c>
-      <c r="Q21" s="34">
-        <v>2578.3216666666667</v>
-      </c>
-      <c r="R21" s="34">
-        <v>7248.3973333333333</v>
-      </c>
-      <c r="S21" s="34">
-        <v>2686.2336666666665</v>
-      </c>
-      <c r="T21" s="34">
-        <v>1694.479</v>
-      </c>
-      <c r="U21" s="34">
-        <v>352.0556666666667</v>
-      </c>
-      <c r="V21" s="34">
-        <v>491.29066666666671</v>
-      </c>
-      <c r="W21" s="34">
-        <v>167.55500000000001</v>
-      </c>
-      <c r="X21" s="34">
-        <v>208.89333333333335</v>
-      </c>
-      <c r="Y21" s="34">
-        <v>1085.127</v>
-      </c>
-      <c r="Z21" s="34">
-        <v>1963.9393333333333</v>
-      </c>
-      <c r="AA21" s="34">
-        <v>1254.2953333333332</v>
-      </c>
-      <c r="AB21" s="34">
-        <v>480.31666666666672</v>
-      </c>
-      <c r="AC21" s="34">
-        <v>348.86966666666672</v>
-      </c>
-      <c r="AD21" s="34">
-        <v>2694.3966666666665</v>
-      </c>
-      <c r="AE21" s="34">
-        <v>6.8713333333333333</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+        <v>21.6</v>
+      </c>
+      <c r="L20" t="s">
+        <v>814</v>
+      </c>
+      <c r="N20" s="2">
+        <v>10091</v>
+      </c>
+      <c r="O20">
+        <v>4542</v>
+      </c>
+      <c r="P20">
+        <v>11999</v>
+      </c>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="34"/>
+      <c r="S20" s="34"/>
+      <c r="T20" s="34"/>
+      <c r="U20" s="34"/>
+      <c r="V20" s="34"/>
+      <c r="W20" s="34"/>
+      <c r="X20" s="34"/>
+      <c r="Y20" s="34"/>
+      <c r="Z20" s="34"/>
+      <c r="AA20" s="34"/>
+      <c r="AB20" s="34"/>
+      <c r="AC20" s="34"/>
+      <c r="AD20" s="34"/>
+      <c r="AE20" s="34"/>
+      <c r="AF20" s="34"/>
+      <c r="AG20" s="34"/>
+      <c r="AH20" s="34"/>
+      <c r="AI20" s="34"/>
+      <c r="AJ20" s="34"/>
+      <c r="AK20" s="34"/>
+    </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>1999</v>
+      </c>
+      <c r="B21" s="45">
+        <v>46321</v>
+      </c>
+      <c r="C21" s="45">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="D21" s="45">
+        <v>30759</v>
+      </c>
+      <c r="E21" s="45">
+        <v>90.2</v>
+      </c>
+      <c r="F21" s="45">
+        <v>27742</v>
+      </c>
+      <c r="G21" s="45">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="H21" s="45">
+        <v>3017</v>
+      </c>
+      <c r="I21" s="45">
+        <v>22.1</v>
+      </c>
+      <c r="L21" t="s">
+        <v>814</v>
+      </c>
+      <c r="N21" s="2">
+        <v>10774</v>
+      </c>
+      <c r="O21">
+        <v>4515</v>
+      </c>
+      <c r="P21">
+        <v>12452</v>
+      </c>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="34"/>
+      <c r="S21" s="34"/>
+      <c r="T21" s="34"/>
+      <c r="U21" s="34"/>
+      <c r="V21" s="34"/>
+      <c r="W21" s="34"/>
+      <c r="X21" s="34"/>
+      <c r="Y21" s="34"/>
+      <c r="Z21" s="34"/>
+      <c r="AA21" s="34"/>
+      <c r="AB21" s="34"/>
+      <c r="AC21" s="34"/>
+      <c r="AD21" s="34"/>
+      <c r="AE21" s="34"/>
+      <c r="AF21" s="34"/>
+      <c r="AG21" s="34"/>
+      <c r="AH21" s="34"/>
+      <c r="AI21" s="34"/>
+      <c r="AJ21" s="34"/>
+      <c r="AK21" s="34"/>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2015</v>
+        <v>2000</v>
       </c>
       <c r="B22" s="21">
-        <v>64936</v>
+        <v>47640</v>
       </c>
       <c r="C22" s="21">
-        <v>63.7</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="D22" s="21">
-        <v>41343</v>
+        <v>30911</v>
       </c>
       <c r="E22" s="21">
-        <v>93.7</v>
+        <v>88.809808805926693</v>
       </c>
       <c r="F22" s="21">
-        <v>38741</v>
+        <v>27452</v>
       </c>
       <c r="G22" s="21">
-        <v>6.3</v>
+        <v>11.190191194073307</v>
       </c>
       <c r="H22" s="21">
-        <v>2602</v>
+        <v>3459</v>
       </c>
       <c r="I22" s="21">
-        <v>18.5</v>
-      </c>
-      <c r="K22" s="34">
-        <v>9972.65625</v>
-      </c>
-      <c r="L22" s="34">
-        <v>1320.9870000000001</v>
-      </c>
-      <c r="M22" s="34">
-        <v>234.51499999999999</v>
-      </c>
-      <c r="N22" s="34">
-        <v>3208.6109999999999</v>
-      </c>
-      <c r="O22" s="34">
-        <v>83.243750000000006</v>
-      </c>
-      <c r="P22" s="34">
-        <v>51.694249999999997</v>
-      </c>
-      <c r="Q22" s="34">
-        <v>2696.8139999999999</v>
-      </c>
-      <c r="R22" s="34">
-        <v>7312.9444999999996</v>
-      </c>
-      <c r="S22" s="34">
-        <v>2781.3657499999999</v>
-      </c>
-      <c r="T22" s="34">
-        <v>1716.2962500000001</v>
-      </c>
-      <c r="U22" s="34">
-        <v>381.00024999999999</v>
-      </c>
-      <c r="V22" s="34">
-        <v>497.56099999999998</v>
-      </c>
-      <c r="W22" s="34">
-        <v>184.10300000000001</v>
-      </c>
-      <c r="X22" s="34">
-        <v>208.47225</v>
-      </c>
-      <c r="Y22" s="34">
-        <v>1138.778</v>
-      </c>
-      <c r="Z22" s="34">
-        <v>2096.2435</v>
-      </c>
-      <c r="AA22" s="34">
-        <v>1282.1982499999999</v>
-      </c>
-      <c r="AB22" s="34">
-        <v>493.75175000000002</v>
-      </c>
-      <c r="AC22" s="34">
-        <v>343.154</v>
-      </c>
-      <c r="AD22" s="34">
-        <v>2733.1202499999999</v>
-      </c>
-      <c r="AE22" s="34">
-        <v>3.3242500000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+        <v>21.7</v>
+      </c>
+      <c r="L22" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M22" s="46"/>
+      <c r="N22" s="2">
+        <v>10181</v>
+      </c>
+      <c r="O22" s="2">
+        <v>4455</v>
+      </c>
+      <c r="P22" s="2">
+        <v>12817</v>
+      </c>
+      <c r="Q22" s="34"/>
+      <c r="R22" s="34"/>
+      <c r="S22" s="34"/>
+      <c r="T22" s="34"/>
+      <c r="U22" s="34"/>
+      <c r="V22" s="34"/>
+      <c r="W22" s="34"/>
+      <c r="X22" s="34"/>
+      <c r="Y22" s="34"/>
+      <c r="Z22" s="34"/>
+      <c r="AA22" s="34"/>
+      <c r="AB22" s="34"/>
+      <c r="AC22" s="34"/>
+      <c r="AD22" s="34"/>
+      <c r="AE22" s="34"/>
+      <c r="AF22" s="34"/>
+      <c r="AG22" s="34"/>
+      <c r="AH22" s="34"/>
+      <c r="AI22" s="34"/>
+      <c r="AJ22" s="34"/>
+      <c r="AK22" s="34"/>
+    </row>
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2016</v>
+        <v>2001</v>
       </c>
       <c r="B23" s="21">
-        <v>68311</v>
+        <v>48929</v>
       </c>
       <c r="C23" s="21">
-        <v>63.5</v>
+        <v>67.099999999999994</v>
       </c>
       <c r="D23" s="21">
-        <v>43361</v>
+        <v>32809</v>
       </c>
       <c r="E23" s="21">
-        <v>94.6</v>
+        <v>88.865859977445211</v>
       </c>
       <c r="F23" s="21">
-        <v>40998</v>
+        <v>29156</v>
       </c>
       <c r="G23" s="21">
-        <v>5.4</v>
+        <v>11.134140022554787</v>
       </c>
       <c r="H23" s="21">
-        <v>2363</v>
+        <v>3653</v>
       </c>
       <c r="I23" s="21">
-        <v>18.3</v>
-      </c>
-      <c r="K23" s="34">
-        <v>9801.11175</v>
-      </c>
-      <c r="L23" s="34">
-        <v>1262.58475</v>
-      </c>
-      <c r="M23" s="34">
-        <v>218.7765</v>
-      </c>
-      <c r="N23" s="34">
-        <v>3403.9629999999997</v>
-      </c>
-      <c r="O23" s="34">
-        <v>91.436499999999995</v>
-      </c>
-      <c r="P23" s="34">
-        <v>67.64425</v>
-      </c>
-      <c r="Q23" s="34">
-        <v>3377.6685000000002</v>
-      </c>
-      <c r="R23" s="34">
-        <v>8039.2467499999993</v>
-      </c>
-      <c r="S23" s="34">
-        <v>3037.8177500000002</v>
-      </c>
-      <c r="T23" s="34">
-        <v>1777.24</v>
-      </c>
-      <c r="U23" s="34">
-        <v>366.48975000000007</v>
-      </c>
-      <c r="V23" s="34">
-        <v>513.846</v>
-      </c>
-      <c r="W23" s="34">
-        <v>193.03750000000002</v>
-      </c>
-      <c r="X23" s="34">
-        <v>212.64449999999999</v>
-      </c>
-      <c r="Y23" s="34">
-        <v>1370.7760000000001</v>
-      </c>
-      <c r="Z23" s="34">
-        <v>2195.6932500000003</v>
-      </c>
-      <c r="AA23" s="34">
-        <v>1303.9195</v>
-      </c>
-      <c r="AB23" s="34">
-        <v>501.709</v>
-      </c>
-      <c r="AC23" s="34">
-        <v>361.28475000000003</v>
-      </c>
-      <c r="AD23" s="34">
-        <v>2897.7039999999997</v>
-      </c>
-      <c r="AE23" s="34">
-        <v>3.2734999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+        <v>17.2</v>
+      </c>
+      <c r="L23" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M23" s="46"/>
+      <c r="N23" s="2">
+        <v>10850</v>
+      </c>
+      <c r="O23" s="2">
+        <v>4712</v>
+      </c>
+      <c r="P23" s="2">
+        <v>13592</v>
+      </c>
+      <c r="Q23" s="34"/>
+      <c r="R23" s="34"/>
+      <c r="S23" s="34"/>
+      <c r="T23" s="34"/>
+      <c r="U23" s="34"/>
+      <c r="V23" s="34"/>
+      <c r="W23" s="34"/>
+      <c r="X23" s="34"/>
+      <c r="Y23" s="34"/>
+      <c r="Z23" s="34"/>
+      <c r="AA23" s="34"/>
+      <c r="AB23" s="34"/>
+      <c r="AC23" s="34"/>
+      <c r="AD23" s="34"/>
+      <c r="AE23" s="34"/>
+      <c r="AF23" s="34"/>
+      <c r="AG23" s="34"/>
+      <c r="AH23" s="34"/>
+      <c r="AI23" s="34"/>
+      <c r="AJ23" s="34"/>
+      <c r="AK23" s="34"/>
+    </row>
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2017</v>
+        <v>2002</v>
       </c>
       <c r="B24" s="21">
-        <v>69890.685750000004</v>
+        <v>50344</v>
       </c>
       <c r="C24" s="21">
-        <v>61.202718990348401</v>
+        <v>67.400000000000006</v>
       </c>
       <c r="D24" s="21">
-        <v>42775</v>
+        <v>33936</v>
       </c>
       <c r="E24" s="21">
-        <v>94.4</v>
+        <v>88.584394153701083</v>
       </c>
       <c r="F24" s="21">
-        <v>40334</v>
+        <v>30062</v>
       </c>
       <c r="G24" s="21">
-        <v>5.7</v>
+        <v>11.415605846298915</v>
       </c>
       <c r="H24" s="21">
-        <v>2441</v>
+        <v>3874</v>
       </c>
       <c r="I24" s="21">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="K24" s="34">
-        <v>9066.4807500000006</v>
-      </c>
-      <c r="L24" s="34">
-        <v>1194.38825</v>
-      </c>
-      <c r="M24" s="34">
-        <v>203.33250000000001</v>
-      </c>
-      <c r="N24" s="34">
-        <v>3481.2064999999998</v>
-      </c>
-      <c r="O24" s="34">
-        <v>79.866500000000002</v>
-      </c>
-      <c r="P24" s="34">
-        <v>68.668499999999995</v>
-      </c>
-      <c r="Q24" s="34">
-        <v>3536.8052499999999</v>
-      </c>
-      <c r="R24" s="34">
-        <v>7899.74125</v>
-      </c>
-      <c r="S24" s="34">
-        <v>3127.3642500000001</v>
-      </c>
-      <c r="T24" s="34">
-        <v>1739.6975</v>
-      </c>
-      <c r="U24" s="34">
-        <v>396.66750000000002</v>
-      </c>
-      <c r="V24" s="34">
-        <v>506.298</v>
-      </c>
-      <c r="W24" s="34">
-        <v>185.9965</v>
-      </c>
-      <c r="X24" s="34">
-        <v>247.29400000000001</v>
-      </c>
-      <c r="Y24" s="34">
-        <v>1474.9827499999999</v>
-      </c>
-      <c r="Z24" s="34">
-        <v>2408.2069999999999</v>
-      </c>
-      <c r="AA24" s="34">
-        <v>1204.4100000000001</v>
-      </c>
-      <c r="AB24" s="34">
-        <v>484.36750000000001</v>
-      </c>
-      <c r="AC24" s="34">
-        <v>325.40724999999998</v>
-      </c>
-      <c r="AD24" s="34">
-        <v>2701.0129999999999</v>
-      </c>
-      <c r="AE24" s="34">
-        <v>1.6074999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="L24" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M24" s="46"/>
+      <c r="N24" s="2">
+        <v>11122</v>
+      </c>
+      <c r="O24" s="2">
+        <v>4695</v>
+      </c>
+      <c r="P24" s="2">
+        <v>14246</v>
+      </c>
+      <c r="Q24" s="34"/>
+      <c r="R24" s="34"/>
+      <c r="S24" s="34"/>
+      <c r="T24" s="34"/>
+      <c r="U24" s="34"/>
+      <c r="V24" s="34"/>
+      <c r="W24" s="34"/>
+      <c r="X24" s="34"/>
+      <c r="Y24" s="34"/>
+      <c r="Z24" s="34"/>
+      <c r="AA24" s="34"/>
+      <c r="AB24" s="34"/>
+      <c r="AC24" s="34"/>
+      <c r="AD24" s="34"/>
+      <c r="AE24" s="34"/>
+      <c r="AF24" s="34"/>
+      <c r="AG24" s="34"/>
+      <c r="AH24" s="34"/>
+      <c r="AI24" s="34"/>
+      <c r="AJ24" s="34"/>
+      <c r="AK24" s="34"/>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2018</v>
+        <v>2003</v>
       </c>
       <c r="B25" s="21">
-        <v>71340</v>
+        <v>51793</v>
       </c>
       <c r="C25" s="21">
-        <v>60.9</v>
+        <v>66.7</v>
       </c>
       <c r="D25" s="21">
-        <v>43460</v>
+        <v>34571</v>
       </c>
       <c r="E25" s="21">
-        <v>94.7</v>
+        <v>88.614734893407771</v>
       </c>
       <c r="F25" s="21">
-        <v>41157</v>
+        <v>30635</v>
       </c>
       <c r="G25" s="21">
-        <v>5.3</v>
+        <v>11.385265106592231</v>
       </c>
       <c r="H25" s="21">
-        <v>2303</v>
+        <v>3936</v>
       </c>
       <c r="I25" s="21">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="K25" s="34">
-        <v>8872.2567500000005</v>
-      </c>
-      <c r="L25" s="34">
-        <v>1125.9902500000001</v>
-      </c>
-      <c r="M25" s="34">
-        <v>206.50450000000001</v>
-      </c>
-      <c r="N25" s="34">
-        <v>3625.2837500000001</v>
-      </c>
-      <c r="O25" s="34">
-        <v>87.583999999999989</v>
-      </c>
-      <c r="P25" s="34">
-        <v>61.377000000000002</v>
-      </c>
-      <c r="Q25" s="34">
-        <v>3865.4722499999998</v>
-      </c>
-      <c r="R25" s="34">
-        <v>7993.9129999999996</v>
-      </c>
-      <c r="S25" s="34">
-        <v>3220.1837500000001</v>
-      </c>
-      <c r="T25" s="34">
-        <v>1727.4402500000001</v>
-      </c>
-      <c r="U25" s="34">
-        <v>403.49475000000001</v>
-      </c>
-      <c r="V25" s="34">
-        <v>540.44375000000002</v>
-      </c>
-      <c r="W25" s="34">
-        <v>203.7055</v>
-      </c>
-      <c r="X25" s="34">
-        <v>274.62925000000001</v>
-      </c>
-      <c r="Y25" s="34">
-        <v>1583.8875</v>
-      </c>
-      <c r="Z25" s="34">
-        <v>2559.4537500000001</v>
-      </c>
-      <c r="AA25" s="34">
-        <v>1196.6400000000001</v>
-      </c>
-      <c r="AB25" s="34">
-        <v>517.58325000000002</v>
-      </c>
-      <c r="AC25" s="34">
-        <v>363.09724999999997</v>
-      </c>
-      <c r="AD25" s="34">
-        <v>2724.06475</v>
-      </c>
-      <c r="AE25" s="34">
-        <v>3.530250000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="L25" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M25" s="46"/>
+      <c r="N25" s="2">
+        <v>11220</v>
+      </c>
+      <c r="O25" s="2">
+        <v>4840</v>
+      </c>
+      <c r="P25" s="2">
+        <v>14577</v>
+      </c>
+      <c r="Q25" s="34"/>
+      <c r="R25" s="34"/>
+      <c r="S25" s="34"/>
+      <c r="T25" s="34"/>
+      <c r="U25" s="34"/>
+      <c r="V25" s="34"/>
+      <c r="W25" s="34"/>
+      <c r="X25" s="34"/>
+      <c r="Y25" s="34"/>
+      <c r="Z25" s="34"/>
+      <c r="AA25" s="34"/>
+      <c r="AB25" s="34"/>
+      <c r="AC25" s="34"/>
+      <c r="AD25" s="34"/>
+      <c r="AE25" s="34"/>
+      <c r="AF25" s="34"/>
+      <c r="AG25" s="34"/>
+      <c r="AH25" s="34"/>
+      <c r="AI25" s="34"/>
+      <c r="AJ25" s="34"/>
+      <c r="AK25" s="34"/>
+    </row>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>2019</v>
+        <v>2004</v>
       </c>
       <c r="B26" s="21">
-        <v>72143.458750000005</v>
+        <v>53144</v>
       </c>
       <c r="C26" s="21">
-        <v>61.262820579261316</v>
+        <v>67.5</v>
       </c>
       <c r="D26" s="21">
-        <v>44197.118000000002</v>
+        <v>35862</v>
       </c>
       <c r="E26" s="21">
-        <v>94.888568865508361</v>
+        <v>88.151804138084884</v>
       </c>
       <c r="F26" s="21">
-        <v>41938.012749999994</v>
+        <v>31613</v>
       </c>
       <c r="G26" s="21">
-        <v>5.1114317001393621</v>
+        <v>11.848195861915119</v>
       </c>
       <c r="H26" s="21">
-        <v>2259.1055000000001</v>
+        <v>4249</v>
       </c>
       <c r="I26" s="21">
-        <v>13.77815166027389</v>
-      </c>
-      <c r="K26" s="34">
-        <v>8070.0662499999999</v>
-      </c>
-      <c r="L26" s="34">
-        <v>1255.126</v>
-      </c>
-      <c r="M26" s="34">
-        <v>176.56825000000001</v>
-      </c>
-      <c r="N26" s="34">
-        <v>3650.78775</v>
-      </c>
-      <c r="O26" s="34">
-        <v>90.5595</v>
-      </c>
-      <c r="P26" s="34">
-        <v>64.483249999999998</v>
-      </c>
-      <c r="Q26" s="34">
-        <v>4123.3215</v>
-      </c>
-      <c r="R26" s="34">
-        <v>8368.490749999999</v>
-      </c>
-      <c r="S26" s="34">
-        <v>3424.13825</v>
-      </c>
-      <c r="T26" s="34">
-        <v>1932.9702500000001</v>
-      </c>
-      <c r="U26" s="34">
-        <v>433.09775000000002</v>
-      </c>
-      <c r="V26" s="34">
-        <v>585.54950000000008</v>
-      </c>
-      <c r="W26" s="34">
-        <v>236.70500000000001</v>
-      </c>
-      <c r="X26" s="34">
-        <v>309.97000000000003</v>
-      </c>
-      <c r="Y26" s="34">
-        <v>1692.36</v>
-      </c>
-      <c r="Z26" s="34">
-        <v>2723.6089999999999</v>
-      </c>
-      <c r="AA26" s="34">
-        <v>1266.97</v>
-      </c>
-      <c r="AB26" s="34">
-        <v>542.81275000000005</v>
-      </c>
-      <c r="AC26" s="34">
-        <v>401.74</v>
-      </c>
-      <c r="AD26" s="34">
-        <v>2588.1622499999999</v>
-      </c>
-      <c r="AE26" s="34">
-        <v>0.52550000000000008</v>
-      </c>
-    </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="L26" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M26" s="46"/>
+      <c r="N26" s="2">
+        <v>11381</v>
+      </c>
+      <c r="O26" s="2">
+        <v>4999</v>
+      </c>
+      <c r="P26" s="2">
+        <v>15237</v>
+      </c>
+      <c r="Q26" s="34"/>
+      <c r="R26" s="34"/>
+      <c r="S26" s="34"/>
+      <c r="T26" s="34"/>
+      <c r="U26" s="34"/>
+      <c r="V26" s="34"/>
+      <c r="W26" s="34"/>
+      <c r="X26" s="34"/>
+      <c r="Y26" s="34"/>
+      <c r="Z26" s="34"/>
+      <c r="AA26" s="34"/>
+      <c r="AB26" s="34"/>
+      <c r="AC26" s="34"/>
+      <c r="AD26" s="34"/>
+      <c r="AE26" s="34"/>
+      <c r="AF26" s="34"/>
+      <c r="AG26" s="34"/>
+      <c r="AH26" s="34"/>
+      <c r="AI26" s="34"/>
+      <c r="AJ26" s="34"/>
+      <c r="AK26" s="34"/>
+    </row>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2020</v>
+        <v>2005</v>
       </c>
       <c r="B27" s="21">
-        <v>73732.624500000005</v>
+        <v>54388</v>
       </c>
       <c r="C27" s="21">
-        <v>59.5</v>
+        <v>64.716310972814028</v>
       </c>
       <c r="D27" s="21">
-        <v>43878</v>
+        <v>35286</v>
       </c>
       <c r="E27" s="21">
-        <v>89.7</v>
+        <v>92.21337414156298</v>
       </c>
       <c r="F27" s="21">
-        <v>39378</v>
+        <v>32539</v>
       </c>
       <c r="G27" s="21">
-        <v>10.3</v>
+        <v>7.7866258584370058</v>
       </c>
       <c r="H27" s="21">
-        <v>4500</v>
+        <v>2747.6666666666665</v>
       </c>
       <c r="I27" s="21">
-        <v>16.2</v>
-      </c>
-      <c r="K27" s="34">
-        <v>8574.1839999999993</v>
-      </c>
-      <c r="L27" s="34">
-        <v>1179.499</v>
-      </c>
-      <c r="M27" s="34">
-        <v>184.001</v>
-      </c>
-      <c r="N27" s="34">
-        <v>3183.6959999999999</v>
-      </c>
-      <c r="O27" s="34">
-        <v>80.938999999999993</v>
-      </c>
-      <c r="P27" s="34">
-        <v>58.109000000000002</v>
-      </c>
-      <c r="Q27" s="34">
-        <v>3699.5619999999999</v>
-      </c>
-      <c r="R27" s="34">
-        <v>8081.0479999999998</v>
-      </c>
-      <c r="S27" s="34">
-        <v>2932.288</v>
-      </c>
-      <c r="T27" s="34">
-        <v>1468.16</v>
-      </c>
-      <c r="U27" s="34">
-        <v>349.64699999999999</v>
-      </c>
-      <c r="V27" s="34">
-        <v>555.76199999999994</v>
-      </c>
-      <c r="W27" s="34">
-        <v>191.977</v>
-      </c>
-      <c r="X27" s="34">
-        <v>260.32100000000003</v>
-      </c>
-      <c r="Y27" s="34">
-        <v>1608.915</v>
-      </c>
-      <c r="Z27" s="34">
-        <v>2563.3180000000002</v>
-      </c>
-      <c r="AA27" s="34">
-        <v>1286.059</v>
-      </c>
-      <c r="AB27" s="34">
-        <v>542.36599999999999</v>
-      </c>
-      <c r="AC27" s="34">
-        <v>230.41499999999999</v>
-      </c>
-      <c r="AD27" s="34">
-        <v>2345.681</v>
-      </c>
-      <c r="AE27" s="34">
-        <v>1.8979999999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L27" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M27" s="46"/>
+      <c r="N27" s="2">
+        <v>11718</v>
+      </c>
+      <c r="O27" s="2">
+        <v>5039</v>
+      </c>
+      <c r="P27" s="2">
+        <v>15785</v>
+      </c>
+      <c r="Q27" s="34"/>
+      <c r="R27" s="34"/>
+      <c r="S27" s="34"/>
+      <c r="T27" s="34"/>
+      <c r="U27" s="34"/>
+      <c r="V27" s="34"/>
+      <c r="W27" s="34"/>
+      <c r="X27" s="34"/>
+      <c r="Y27" s="34"/>
+      <c r="Z27" s="34"/>
+      <c r="AA27" s="34"/>
+      <c r="AB27" s="34"/>
+      <c r="AC27" s="34"/>
+      <c r="AD27" s="34"/>
+      <c r="AE27" s="34"/>
+      <c r="AF27" s="34"/>
+      <c r="AG27" s="34"/>
+      <c r="AH27" s="34"/>
+      <c r="AI27" s="34"/>
+      <c r="AJ27" s="34"/>
+      <c r="AK27" s="34"/>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2021</v>
+        <v>2006</v>
       </c>
       <c r="B28" s="21">
-        <v>75301.057289249497</v>
+        <v>55230</v>
       </c>
       <c r="C28" s="21">
-        <v>63.349976619962966</v>
+        <v>64.2</v>
       </c>
       <c r="D28" s="21">
-        <v>47703.202187324503</v>
+        <v>35464</v>
       </c>
       <c r="E28" s="21">
-        <v>92.212452153046868</v>
+        <v>92.02312138728324</v>
       </c>
       <c r="F28" s="21">
-        <v>43988.292492457811</v>
+        <v>32636</v>
       </c>
       <c r="G28" s="21">
-        <v>7.7875478469530783</v>
+        <v>7.9768786127167628</v>
       </c>
       <c r="H28" s="21">
-        <v>3714.9096948666634</v>
+        <v>2829</v>
       </c>
       <c r="I28" s="21">
-        <v>15.919764703947065</v>
-      </c>
-      <c r="K28" s="34">
-        <v>9352.7279999999992</v>
-      </c>
-      <c r="L28" s="34">
-        <v>1303.664</v>
-      </c>
-      <c r="M28" s="34">
-        <v>169.72300000000001</v>
-      </c>
-      <c r="N28" s="34">
-        <v>3453.009</v>
-      </c>
-      <c r="O28" s="34">
-        <v>75.843999999999994</v>
-      </c>
-      <c r="P28" s="34">
-        <v>74.724999999999994</v>
-      </c>
-      <c r="Q28" s="34">
-        <v>4319.1589999999997</v>
-      </c>
-      <c r="R28" s="34">
-        <v>9725.2090000000007</v>
-      </c>
-      <c r="S28" s="34">
-        <v>2938.85</v>
-      </c>
-      <c r="T28" s="34">
-        <v>1416.059</v>
-      </c>
-      <c r="U28" s="34">
-        <v>444.64499999999998</v>
-      </c>
-      <c r="V28" s="34">
-        <v>619.71799999999996</v>
-      </c>
-      <c r="W28" s="34">
-        <v>203.982</v>
-      </c>
-      <c r="X28" s="34">
-        <v>296.346</v>
-      </c>
-      <c r="Y28" s="34">
-        <v>1831.027</v>
-      </c>
-      <c r="Z28" s="34">
-        <v>2729.3069999999998</v>
-      </c>
-      <c r="AA28" s="34">
-        <v>1425.691</v>
-      </c>
-      <c r="AB28" s="34">
-        <v>658.19399999999996</v>
-      </c>
-      <c r="AC28" s="34">
-        <v>336.548</v>
-      </c>
-      <c r="AD28" s="34">
-        <v>2612.96</v>
-      </c>
-      <c r="AE28" s="34">
-        <v>0.90700000000000003</v>
-      </c>
-    </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
+        <v>22.6</v>
+      </c>
+      <c r="L28" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M28" s="46"/>
+      <c r="N28" s="2">
+        <v>11682</v>
+      </c>
+      <c r="O28" s="2">
+        <v>4997</v>
+      </c>
+      <c r="P28" s="2">
+        <v>15957</v>
+      </c>
+      <c r="Q28" s="34"/>
+      <c r="R28" s="34"/>
+      <c r="S28" s="34"/>
+      <c r="T28" s="34"/>
+      <c r="U28" s="34"/>
+      <c r="V28" s="34"/>
+      <c r="W28" s="34"/>
+      <c r="X28" s="34"/>
+      <c r="Y28" s="34"/>
+      <c r="Z28" s="34"/>
+      <c r="AA28" s="34"/>
+      <c r="AB28" s="34"/>
+      <c r="AC28" s="34"/>
+      <c r="AD28" s="34"/>
+      <c r="AE28" s="34"/>
+      <c r="AF28" s="34"/>
+      <c r="AG28" s="34"/>
+      <c r="AH28" s="34"/>
+      <c r="AI28" s="34"/>
+      <c r="AJ28" s="34"/>
+      <c r="AK28" s="34"/>
+    </row>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2022</v>
+        <v>2007</v>
       </c>
       <c r="B29" s="21">
-        <v>76598.736999999994</v>
+        <v>56565</v>
       </c>
       <c r="C29" s="21">
-        <v>64.7</v>
+        <v>64</v>
       </c>
       <c r="D29" s="21">
-        <v>49561.608999999997</v>
+        <v>36213</v>
       </c>
       <c r="E29" s="21">
-        <v>94.61</v>
+        <v>92.67390163753349</v>
       </c>
       <c r="F29" s="21">
-        <v>46890.39</v>
+        <v>33560</v>
       </c>
       <c r="G29" s="21">
-        <v>5.39</v>
+        <v>7.3260983624665172</v>
       </c>
       <c r="H29" s="21">
-        <v>2671.2190000000001</v>
+        <v>2653</v>
       </c>
       <c r="I29" s="21">
-        <v>14.24</v>
-      </c>
-      <c r="K29" s="34">
-        <v>9546.11</v>
-      </c>
-      <c r="L29" s="34">
-        <v>1289.6559999999999</v>
-      </c>
-      <c r="M29" s="34">
-        <v>221.846</v>
-      </c>
-      <c r="N29" s="34">
-        <v>3754.212</v>
-      </c>
-      <c r="O29" s="34">
-        <v>95.271000000000001</v>
-      </c>
-      <c r="P29" s="34">
-        <v>72.926000000000002</v>
-      </c>
-      <c r="Q29" s="34">
-        <v>4381.6570000000002</v>
-      </c>
-      <c r="R29" s="34">
-        <v>10392.92</v>
-      </c>
-      <c r="S29" s="34">
-        <v>3243.9560000000001</v>
-      </c>
-      <c r="T29" s="34">
-        <v>1812.557</v>
-      </c>
-      <c r="U29" s="34">
-        <v>483.87299999999999</v>
-      </c>
-      <c r="V29" s="34">
-        <v>645.24300000000005</v>
-      </c>
-      <c r="W29" s="34">
-        <v>238.16499999999999</v>
-      </c>
-      <c r="X29" s="34">
-        <v>344.74200000000002</v>
-      </c>
-      <c r="Y29" s="34">
-        <v>2185.5349999999999</v>
-      </c>
-      <c r="Z29" s="34">
-        <v>2842.9169999999999</v>
-      </c>
-      <c r="AA29" s="34">
-        <v>1463.85</v>
-      </c>
-      <c r="AB29" s="34">
-        <v>672.6</v>
-      </c>
-      <c r="AC29" s="34">
-        <v>410.27800000000002</v>
-      </c>
-      <c r="AD29" s="34">
-        <v>2790.3829999999998</v>
-      </c>
-      <c r="AE29" s="34">
-        <v>1.6950000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="L29" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M29" s="46"/>
+      <c r="N29" s="2">
+        <v>11786</v>
+      </c>
+      <c r="O29" s="2">
+        <v>5121</v>
+      </c>
+      <c r="P29" s="2">
+        <v>16654</v>
+      </c>
+      <c r="Q29" s="34"/>
+      <c r="R29" s="34"/>
+      <c r="S29" s="34"/>
+      <c r="T29" s="34"/>
+      <c r="U29" s="34"/>
+      <c r="V29" s="34"/>
+      <c r="W29" s="34"/>
+      <c r="X29" s="34"/>
+      <c r="Y29" s="34"/>
+      <c r="Z29" s="34"/>
+      <c r="AA29" s="34"/>
+      <c r="AB29" s="34"/>
+      <c r="AC29" s="34"/>
+      <c r="AD29" s="34"/>
+      <c r="AE29" s="34"/>
+      <c r="AF29" s="34"/>
+      <c r="AG29" s="34"/>
+      <c r="AH29" s="34"/>
+      <c r="AI29" s="34"/>
+      <c r="AJ29" s="34"/>
+      <c r="AK29" s="34"/>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>2023</v>
-      </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="K30" s="34"/>
-      <c r="L30" s="34"/>
-      <c r="M30" s="34"/>
-      <c r="N30" s="34"/>
-      <c r="O30" s="34"/>
-      <c r="P30" s="34"/>
+        <v>2008</v>
+      </c>
+      <c r="B30" s="21">
+        <v>57848</v>
+      </c>
+      <c r="C30" s="21">
+        <v>63.6</v>
+      </c>
+      <c r="D30" s="21">
+        <v>36805</v>
+      </c>
+      <c r="E30" s="21">
+        <v>92.620567857628046</v>
+      </c>
+      <c r="F30" s="21">
+        <v>34089</v>
+      </c>
+      <c r="G30" s="21">
+        <v>7.4</v>
+      </c>
+      <c r="H30" s="21">
+        <v>2716</v>
+      </c>
+      <c r="I30" s="21">
+        <v>19.3</v>
+      </c>
+      <c r="L30" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M30" s="46"/>
+      <c r="N30" s="2">
+        <v>12030</v>
+      </c>
+      <c r="O30" s="2">
+        <v>5048</v>
+      </c>
+      <c r="P30" s="2">
+        <v>17012</v>
+      </c>
       <c r="Q30" s="34"/>
       <c r="R30" s="34"/>
       <c r="S30" s="34"/>
@@ -18424,8 +18361,1409 @@
       <c r="AC30" s="34"/>
       <c r="AD30" s="34"/>
       <c r="AE30" s="34"/>
+      <c r="AF30" s="34"/>
+      <c r="AG30" s="34"/>
+      <c r="AH30" s="34"/>
+      <c r="AI30" s="34"/>
+      <c r="AJ30" s="34"/>
+      <c r="AK30" s="34"/>
+    </row>
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2009</v>
+      </c>
+      <c r="B31" s="21">
+        <v>59237</v>
+      </c>
+      <c r="C31" s="21">
+        <v>63.966355487279912</v>
+      </c>
+      <c r="D31" s="21">
+        <v>37891.75</v>
+      </c>
+      <c r="E31" s="21">
+        <v>92.530036221604973</v>
+      </c>
+      <c r="F31" s="21">
+        <v>35061.25</v>
+      </c>
+      <c r="G31" s="21">
+        <v>7.4699637783950337</v>
+      </c>
+      <c r="H31" s="21">
+        <v>2830.5</v>
+      </c>
+      <c r="I31" s="21">
+        <v>19.087311490605728</v>
+      </c>
+      <c r="L31" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M31" s="46"/>
+      <c r="N31" s="2">
+        <v>12043</v>
+      </c>
+      <c r="O31" s="2">
+        <v>5093</v>
+      </c>
+      <c r="P31" s="2">
+        <v>17925</v>
+      </c>
+      <c r="Q31" s="34"/>
+      <c r="R31" s="34"/>
+      <c r="S31" s="34"/>
+      <c r="T31" s="34"/>
+      <c r="U31" s="34"/>
+      <c r="V31" s="34"/>
+      <c r="W31" s="34"/>
+      <c r="X31" s="34"/>
+      <c r="Y31" s="34"/>
+      <c r="Z31" s="34"/>
+      <c r="AA31" s="34"/>
+      <c r="AB31" s="34"/>
+      <c r="AC31" s="34"/>
+      <c r="AD31" s="34"/>
+      <c r="AE31" s="34"/>
+      <c r="AF31" s="34"/>
+      <c r="AG31" s="34"/>
+      <c r="AH31" s="34"/>
+      <c r="AI31" s="34"/>
+      <c r="AJ31" s="34"/>
+      <c r="AK31" s="34"/>
+    </row>
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2010</v>
+      </c>
+      <c r="B32" s="21">
+        <v>60717</v>
+      </c>
+      <c r="C32" s="21">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="D32" s="21">
+        <v>38893</v>
+      </c>
+      <c r="E32" s="21">
+        <v>92.7</v>
+      </c>
+      <c r="F32" s="21">
+        <v>36035</v>
+      </c>
+      <c r="G32" s="21">
+        <v>7.3</v>
+      </c>
+      <c r="H32" s="21">
+        <v>2859</v>
+      </c>
+      <c r="I32" s="21">
+        <v>18.7</v>
+      </c>
+      <c r="L32" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M32" s="46"/>
+      <c r="N32" s="2">
+        <v>11956</v>
+      </c>
+      <c r="O32" s="2">
+        <v>5399</v>
+      </c>
+      <c r="P32" s="2">
+        <v>18682</v>
+      </c>
+      <c r="Q32" s="34"/>
+      <c r="R32" s="34"/>
+      <c r="S32" s="34"/>
+      <c r="T32" s="34"/>
+      <c r="U32" s="34"/>
+      <c r="V32" s="34"/>
+      <c r="W32" s="34"/>
+      <c r="X32" s="34"/>
+      <c r="Y32" s="34"/>
+      <c r="Z32" s="34"/>
+      <c r="AA32" s="34"/>
+      <c r="AB32" s="34"/>
+      <c r="AC32" s="34"/>
+      <c r="AD32" s="34"/>
+      <c r="AE32" s="34"/>
+      <c r="AF32" s="34"/>
+      <c r="AG32" s="34"/>
+      <c r="AH32" s="34"/>
+      <c r="AI32" s="34"/>
+      <c r="AJ32" s="34"/>
+      <c r="AK32" s="34"/>
+    </row>
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2011</v>
+      </c>
+      <c r="B33" s="21">
+        <v>61882.531999999999</v>
+      </c>
+      <c r="C33" s="21">
+        <v>64.647477174980494</v>
+      </c>
+      <c r="D33" s="21">
+        <v>40006.042999999998</v>
+      </c>
+      <c r="E33" s="21">
+        <v>92.967334369303501</v>
+      </c>
+      <c r="F33" s="21">
+        <v>37192.042999999998</v>
+      </c>
+      <c r="G33" s="21">
+        <v>7.0326656306965027</v>
+      </c>
+      <c r="H33" s="21">
+        <v>2814</v>
+      </c>
+      <c r="I33" s="21">
+        <v>19.260093482899016</v>
+      </c>
+      <c r="L33" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M33" s="46"/>
+      <c r="N33" s="2">
+        <v>12268</v>
+      </c>
+      <c r="O33" s="2">
+        <v>5530</v>
+      </c>
+      <c r="P33" s="2">
+        <v>19395</v>
+      </c>
+      <c r="Q33" s="34"/>
+      <c r="R33" s="34"/>
+      <c r="S33" s="34"/>
+      <c r="T33" s="34"/>
+      <c r="U33" s="34"/>
+      <c r="V33" s="34"/>
+      <c r="W33" s="34"/>
+      <c r="X33" s="34"/>
+      <c r="Y33" s="34"/>
+      <c r="Z33" s="34"/>
+      <c r="AA33" s="34"/>
+      <c r="AB33" s="34"/>
+      <c r="AC33" s="34"/>
+      <c r="AD33" s="34"/>
+      <c r="AE33" s="34"/>
+      <c r="AF33" s="34"/>
+      <c r="AG33" s="34"/>
+      <c r="AH33" s="34"/>
+      <c r="AI33" s="34"/>
+      <c r="AJ33" s="34"/>
+      <c r="AK33" s="34"/>
+    </row>
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2012</v>
+      </c>
+      <c r="B34" s="21">
+        <v>62985.349249999999</v>
+      </c>
+      <c r="C34" s="21">
+        <v>64.183842721170592</v>
+      </c>
+      <c r="D34" s="21">
+        <v>40426.417499999996</v>
+      </c>
+      <c r="E34" s="21">
+        <v>93.008986636028297</v>
+      </c>
+      <c r="F34" s="21">
+        <v>37600.201249999998</v>
+      </c>
+      <c r="G34" s="21">
+        <v>6.9910133639717156</v>
+      </c>
+      <c r="H34" s="21">
+        <v>2826.2162499999999</v>
+      </c>
+      <c r="I34" s="21">
+        <v>19.984181600623746</v>
+      </c>
+      <c r="L34" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M34" s="46"/>
+      <c r="N34" s="2">
+        <v>12092</v>
+      </c>
+      <c r="O34" s="2">
+        <v>5742</v>
+      </c>
+      <c r="P34" s="2">
+        <v>19764</v>
+      </c>
+      <c r="Q34" s="34">
+        <v>10660.443499999999</v>
+      </c>
+      <c r="R34" s="34">
+        <v>1432.2945</v>
+      </c>
+      <c r="S34" s="34">
+        <v>249.89350000000002</v>
+      </c>
+      <c r="T34" s="34">
+        <v>3112.3870000000002</v>
+      </c>
+      <c r="U34" s="34">
+        <v>89.460250000000002</v>
+      </c>
+      <c r="V34" s="34">
+        <v>59.448500000000003</v>
+      </c>
+      <c r="W34" s="34">
+        <v>2231.9047500000001</v>
+      </c>
+      <c r="X34" s="34">
+        <v>6863.9697500000002</v>
+      </c>
+      <c r="Y34" s="34">
+        <v>2616.8715000000002</v>
+      </c>
+      <c r="Z34" s="34">
+        <v>1571.3187500000001</v>
+      </c>
+      <c r="AA34" s="34">
+        <v>338.03375</v>
+      </c>
+      <c r="AB34" s="34">
+        <v>437.43799999999999</v>
+      </c>
+      <c r="AC34" s="34">
+        <v>170.4265</v>
+      </c>
+      <c r="AD34" s="34">
+        <v>188.90125</v>
+      </c>
+      <c r="AE34" s="34">
+        <v>936.55849999999998</v>
+      </c>
+      <c r="AF34" s="34">
+        <v>1957.98875</v>
+      </c>
+      <c r="AG34" s="34">
+        <v>1200.0219999999999</v>
+      </c>
+      <c r="AH34" s="34">
+        <v>437.64800000000002</v>
+      </c>
+      <c r="AI34" s="34">
+        <v>327.77875</v>
+      </c>
+      <c r="AJ34" s="34">
+        <v>2715.1417500000002</v>
+      </c>
+      <c r="AK34" s="34">
+        <v>2.2725</v>
+      </c>
+    </row>
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2013</v>
+      </c>
+      <c r="B35" s="21">
+        <v>64173.311000000002</v>
+      </c>
+      <c r="C35" s="21">
+        <v>63.92431465784896</v>
+      </c>
+      <c r="D35" s="21">
+        <v>41022.349249999999</v>
+      </c>
+      <c r="E35" s="21">
+        <v>92.919384059897538</v>
+      </c>
+      <c r="F35" s="21">
+        <v>38117.714249999997</v>
+      </c>
+      <c r="G35" s="21">
+        <v>7.0806159401024553</v>
+      </c>
+      <c r="H35" s="21">
+        <v>2904.6350000000002</v>
+      </c>
+      <c r="I35" s="21">
+        <v>19.338649090166786</v>
+      </c>
+      <c r="L35" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M35" s="46"/>
+      <c r="N35" s="2">
+        <v>11836</v>
+      </c>
+      <c r="O35" s="2">
+        <v>5936</v>
+      </c>
+      <c r="P35" s="2">
+        <v>20345</v>
+      </c>
+      <c r="Q35" s="34">
+        <v>10428.695750000001</v>
+      </c>
+      <c r="R35" s="34">
+        <v>1406.6915000000001</v>
+      </c>
+      <c r="S35" s="34">
+        <v>250.28675000000001</v>
+      </c>
+      <c r="T35" s="34">
+        <v>3159.3564999999999</v>
+      </c>
+      <c r="U35" s="34">
+        <v>94.4375</v>
+      </c>
+      <c r="V35" s="34">
+        <v>60.097000000000001</v>
+      </c>
+      <c r="W35" s="34">
+        <v>2372.7269999999999</v>
+      </c>
+      <c r="X35" s="34">
+        <v>7105.4902499999998</v>
+      </c>
+      <c r="Y35" s="34">
+        <v>2734.2240000000002</v>
+      </c>
+      <c r="Z35" s="34">
+        <v>1606.8902499999999</v>
+      </c>
+      <c r="AA35" s="34">
+        <v>344.45125000000002</v>
+      </c>
+      <c r="AB35" s="34">
+        <v>448.21800000000002</v>
+      </c>
+      <c r="AC35" s="34">
+        <v>172.61799999999999</v>
+      </c>
+      <c r="AD35" s="34">
+        <v>193.99700000000001</v>
+      </c>
+      <c r="AE35" s="34">
+        <v>1015.7535</v>
+      </c>
+      <c r="AF35" s="34">
+        <v>1965.4057500000001</v>
+      </c>
+      <c r="AG35" s="34">
+        <v>1225.6490000000001</v>
+      </c>
+      <c r="AH35" s="34">
+        <v>468.85025000000002</v>
+      </c>
+      <c r="AI35" s="34">
+        <v>347.25475</v>
+      </c>
+      <c r="AJ35" s="34">
+        <v>2712.7429999999999</v>
+      </c>
+      <c r="AK35" s="34">
+        <v>3.8767499999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2014</v>
+      </c>
+      <c r="B36" s="21">
+        <v>64033.078333333338</v>
+      </c>
+      <c r="C36" s="21">
+        <v>64.621820071277213</v>
+      </c>
+      <c r="D36" s="21">
+        <v>41379.340666666671</v>
+      </c>
+      <c r="E36" s="21">
+        <v>93.407133553328265</v>
+      </c>
+      <c r="F36" s="21">
+        <v>38651.256000000001</v>
+      </c>
+      <c r="G36" s="21">
+        <v>6.5928664466717537</v>
+      </c>
+      <c r="H36" s="21">
+        <v>2728.0846666666666</v>
+      </c>
+      <c r="I36" s="21">
+        <v>18.41672363764841</v>
+      </c>
+      <c r="L36" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M36" s="46"/>
+      <c r="N36" s="2">
+        <v>11801</v>
+      </c>
+      <c r="O36" s="2">
+        <v>6167</v>
+      </c>
+      <c r="P36" s="2">
+        <v>20683</v>
+      </c>
+      <c r="Q36" s="34">
+        <v>10404.944333333335</v>
+      </c>
+      <c r="R36" s="34">
+        <v>1396.4763333333333</v>
+      </c>
+      <c r="S36" s="34">
+        <v>239.42033333333336</v>
+      </c>
+      <c r="T36" s="34">
+        <v>3212.1773333333335</v>
+      </c>
+      <c r="U36" s="34">
+        <v>85.983666666666679</v>
+      </c>
+      <c r="V36" s="34">
+        <v>51.211333333333336</v>
+      </c>
+      <c r="W36" s="34">
+        <v>2578.3216666666667</v>
+      </c>
+      <c r="X36" s="34">
+        <v>7248.3973333333333</v>
+      </c>
+      <c r="Y36" s="34">
+        <v>2686.2336666666665</v>
+      </c>
+      <c r="Z36" s="34">
+        <v>1694.479</v>
+      </c>
+      <c r="AA36" s="34">
+        <v>352.0556666666667</v>
+      </c>
+      <c r="AB36" s="34">
+        <v>491.29066666666671</v>
+      </c>
+      <c r="AC36" s="34">
+        <v>167.55500000000001</v>
+      </c>
+      <c r="AD36" s="34">
+        <v>208.89333333333335</v>
+      </c>
+      <c r="AE36" s="34">
+        <v>1085.127</v>
+      </c>
+      <c r="AF36" s="34">
+        <v>1963.9393333333333</v>
+      </c>
+      <c r="AG36" s="34">
+        <v>1254.2953333333332</v>
+      </c>
+      <c r="AH36" s="34">
+        <v>480.31666666666672</v>
+      </c>
+      <c r="AI36" s="34">
+        <v>348.86966666666672</v>
+      </c>
+      <c r="AJ36" s="34">
+        <v>2694.3966666666665</v>
+      </c>
+      <c r="AK36" s="34">
+        <v>6.8713333333333333</v>
+      </c>
+    </row>
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2015</v>
+      </c>
+      <c r="B37" s="21">
+        <v>64936</v>
+      </c>
+      <c r="C37" s="21">
+        <v>63.7</v>
+      </c>
+      <c r="D37" s="21">
+        <v>41343</v>
+      </c>
+      <c r="E37" s="21">
+        <v>93.7</v>
+      </c>
+      <c r="F37" s="21">
+        <v>38741</v>
+      </c>
+      <c r="G37" s="21">
+        <v>6.3</v>
+      </c>
+      <c r="H37" s="21">
+        <v>2602</v>
+      </c>
+      <c r="I37" s="21">
+        <v>18.5</v>
+      </c>
+      <c r="L37" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M37" s="46"/>
+      <c r="N37" s="2">
+        <v>11294</v>
+      </c>
+      <c r="O37" s="2">
+        <v>6275</v>
+      </c>
+      <c r="P37" s="2">
+        <v>21172</v>
+      </c>
+      <c r="Q37" s="34">
+        <v>9972.65625</v>
+      </c>
+      <c r="R37" s="34">
+        <v>1320.9870000000001</v>
+      </c>
+      <c r="S37" s="34">
+        <v>234.51499999999999</v>
+      </c>
+      <c r="T37" s="34">
+        <v>3208.6109999999999</v>
+      </c>
+      <c r="U37" s="34">
+        <v>83.243750000000006</v>
+      </c>
+      <c r="V37" s="34">
+        <v>51.694249999999997</v>
+      </c>
+      <c r="W37" s="34">
+        <v>2696.8139999999999</v>
+      </c>
+      <c r="X37" s="34">
+        <v>7312.9444999999996</v>
+      </c>
+      <c r="Y37" s="34">
+        <v>2781.3657499999999</v>
+      </c>
+      <c r="Z37" s="34">
+        <v>1716.2962500000001</v>
+      </c>
+      <c r="AA37" s="34">
+        <v>381.00024999999999</v>
+      </c>
+      <c r="AB37" s="34">
+        <v>497.56099999999998</v>
+      </c>
+      <c r="AC37" s="34">
+        <v>184.10300000000001</v>
+      </c>
+      <c r="AD37" s="34">
+        <v>208.47225</v>
+      </c>
+      <c r="AE37" s="34">
+        <v>1138.778</v>
+      </c>
+      <c r="AF37" s="34">
+        <v>2096.2435</v>
+      </c>
+      <c r="AG37" s="34">
+        <v>1282.1982499999999</v>
+      </c>
+      <c r="AH37" s="34">
+        <v>493.75175000000002</v>
+      </c>
+      <c r="AI37" s="34">
+        <v>343.154</v>
+      </c>
+      <c r="AJ37" s="34">
+        <v>2733.1202499999999</v>
+      </c>
+      <c r="AK37" s="34">
+        <v>3.3242500000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2016</v>
+      </c>
+      <c r="B38" s="21">
+        <v>68311</v>
+      </c>
+      <c r="C38" s="21">
+        <v>63.5</v>
+      </c>
+      <c r="D38" s="21">
+        <v>43361</v>
+      </c>
+      <c r="E38" s="21">
+        <v>94.6</v>
+      </c>
+      <c r="F38" s="21">
+        <v>40998</v>
+      </c>
+      <c r="G38" s="21">
+        <v>5.4</v>
+      </c>
+      <c r="H38" s="21">
+        <v>2363</v>
+      </c>
+      <c r="I38" s="21">
+        <v>18.3</v>
+      </c>
+      <c r="L38" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M38" s="46"/>
+      <c r="N38" s="2">
+        <v>11064</v>
+      </c>
+      <c r="O38" s="2">
+        <v>7159</v>
+      </c>
+      <c r="P38" s="2">
+        <v>22775</v>
+      </c>
+      <c r="Q38" s="34">
+        <v>9801.11175</v>
+      </c>
+      <c r="R38" s="34">
+        <v>1262.58475</v>
+      </c>
+      <c r="S38" s="34">
+        <v>218.7765</v>
+      </c>
+      <c r="T38" s="34">
+        <v>3403.9629999999997</v>
+      </c>
+      <c r="U38" s="34">
+        <v>91.436499999999995</v>
+      </c>
+      <c r="V38" s="34">
+        <v>67.64425</v>
+      </c>
+      <c r="W38" s="34">
+        <v>3377.6685000000002</v>
+      </c>
+      <c r="X38" s="34">
+        <v>8039.2467499999993</v>
+      </c>
+      <c r="Y38" s="34">
+        <v>3037.8177500000002</v>
+      </c>
+      <c r="Z38" s="34">
+        <v>1777.24</v>
+      </c>
+      <c r="AA38" s="34">
+        <v>366.48975000000007</v>
+      </c>
+      <c r="AB38" s="34">
+        <v>513.846</v>
+      </c>
+      <c r="AC38" s="34">
+        <v>193.03750000000002</v>
+      </c>
+      <c r="AD38" s="34">
+        <v>212.64449999999999</v>
+      </c>
+      <c r="AE38" s="34">
+        <v>1370.7760000000001</v>
+      </c>
+      <c r="AF38" s="34">
+        <v>2195.6932500000003</v>
+      </c>
+      <c r="AG38" s="34">
+        <v>1303.9195</v>
+      </c>
+      <c r="AH38" s="34">
+        <v>501.709</v>
+      </c>
+      <c r="AI38" s="34">
+        <v>361.28475000000003</v>
+      </c>
+      <c r="AJ38" s="34">
+        <v>2897.7039999999997</v>
+      </c>
+      <c r="AK38" s="34">
+        <v>3.2734999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2017</v>
+      </c>
+      <c r="B39" s="21">
+        <v>69890.685750000004</v>
+      </c>
+      <c r="C39" s="21">
+        <v>61.202718990348401</v>
+      </c>
+      <c r="D39" s="21">
+        <v>42775</v>
+      </c>
+      <c r="E39" s="21">
+        <v>94.4</v>
+      </c>
+      <c r="F39" s="21">
+        <v>40334</v>
+      </c>
+      <c r="G39" s="21">
+        <v>5.7</v>
+      </c>
+      <c r="H39" s="21">
+        <v>2441</v>
+      </c>
+      <c r="I39" s="21">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="L39" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M39" s="46"/>
+      <c r="N39" s="2">
+        <v>10261</v>
+      </c>
+      <c r="O39" s="2">
+        <v>7371</v>
+      </c>
+      <c r="P39" s="2">
+        <v>22703</v>
+      </c>
+      <c r="Q39" s="34">
+        <v>9066.4807500000006</v>
+      </c>
+      <c r="R39" s="34">
+        <v>1194.38825</v>
+      </c>
+      <c r="S39" s="34">
+        <v>203.33250000000001</v>
+      </c>
+      <c r="T39" s="34">
+        <v>3481.2064999999998</v>
+      </c>
+      <c r="U39" s="34">
+        <v>79.866500000000002</v>
+      </c>
+      <c r="V39" s="34">
+        <v>68.668499999999995</v>
+      </c>
+      <c r="W39" s="34">
+        <v>3536.8052499999999</v>
+      </c>
+      <c r="X39" s="34">
+        <v>7899.74125</v>
+      </c>
+      <c r="Y39" s="34">
+        <v>3127.3642500000001</v>
+      </c>
+      <c r="Z39" s="34">
+        <v>1739.6975</v>
+      </c>
+      <c r="AA39" s="34">
+        <v>396.66750000000002</v>
+      </c>
+      <c r="AB39" s="34">
+        <v>506.298</v>
+      </c>
+      <c r="AC39" s="34">
+        <v>185.9965</v>
+      </c>
+      <c r="AD39" s="34">
+        <v>247.29400000000001</v>
+      </c>
+      <c r="AE39" s="34">
+        <v>1474.9827499999999</v>
+      </c>
+      <c r="AF39" s="34">
+        <v>2408.2069999999999</v>
+      </c>
+      <c r="AG39" s="34">
+        <v>1204.4100000000001</v>
+      </c>
+      <c r="AH39" s="34">
+        <v>484.36750000000001</v>
+      </c>
+      <c r="AI39" s="34">
+        <v>325.40724999999998</v>
+      </c>
+      <c r="AJ39" s="34">
+        <v>2701.0129999999999</v>
+      </c>
+      <c r="AK39" s="34">
+        <v>1.6074999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>2018</v>
+      </c>
+      <c r="B40" s="21">
+        <v>71340</v>
+      </c>
+      <c r="C40" s="21">
+        <v>60.9</v>
+      </c>
+      <c r="D40" s="21">
+        <v>43460</v>
+      </c>
+      <c r="E40" s="21">
+        <v>94.7</v>
+      </c>
+      <c r="F40" s="21">
+        <v>41157</v>
+      </c>
+      <c r="G40" s="21">
+        <v>5.3</v>
+      </c>
+      <c r="H40" s="21">
+        <v>2303</v>
+      </c>
+      <c r="I40" s="21">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="L40" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M40" s="46"/>
+      <c r="N40" s="2">
+        <v>9998</v>
+      </c>
+      <c r="O40" s="2">
+        <v>7846</v>
+      </c>
+      <c r="P40" s="2">
+        <v>23312</v>
+      </c>
+      <c r="Q40" s="34">
+        <v>8872.2567500000005</v>
+      </c>
+      <c r="R40" s="34">
+        <v>1125.9902500000001</v>
+      </c>
+      <c r="S40" s="34">
+        <v>206.50450000000001</v>
+      </c>
+      <c r="T40" s="34">
+        <v>3625.2837500000001</v>
+      </c>
+      <c r="U40" s="34">
+        <v>87.583999999999989</v>
+      </c>
+      <c r="V40" s="34">
+        <v>61.377000000000002</v>
+      </c>
+      <c r="W40" s="34">
+        <v>3865.4722499999998</v>
+      </c>
+      <c r="X40" s="34">
+        <v>7993.9129999999996</v>
+      </c>
+      <c r="Y40" s="34">
+        <v>3220.1837500000001</v>
+      </c>
+      <c r="Z40" s="34">
+        <v>1727.4402500000001</v>
+      </c>
+      <c r="AA40" s="34">
+        <v>403.49475000000001</v>
+      </c>
+      <c r="AB40" s="34">
+        <v>540.44375000000002</v>
+      </c>
+      <c r="AC40" s="34">
+        <v>203.7055</v>
+      </c>
+      <c r="AD40" s="34">
+        <v>274.62925000000001</v>
+      </c>
+      <c r="AE40" s="34">
+        <v>1583.8875</v>
+      </c>
+      <c r="AF40" s="34">
+        <v>2559.4537500000001</v>
+      </c>
+      <c r="AG40" s="34">
+        <v>1196.6400000000001</v>
+      </c>
+      <c r="AH40" s="34">
+        <v>517.58325000000002</v>
+      </c>
+      <c r="AI40" s="34">
+        <v>363.09724999999997</v>
+      </c>
+      <c r="AJ40" s="34">
+        <v>2724.06475</v>
+      </c>
+      <c r="AK40" s="34">
+        <v>3.530250000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>2019</v>
+      </c>
+      <c r="B41" s="21">
+        <v>72143.458750000005</v>
+      </c>
+      <c r="C41" s="21">
+        <v>61.262820579261316</v>
+      </c>
+      <c r="D41" s="21">
+        <v>44197.118000000002</v>
+      </c>
+      <c r="E41" s="21">
+        <v>94.888568865508361</v>
+      </c>
+      <c r="F41" s="21">
+        <v>41938.012749999994</v>
+      </c>
+      <c r="G41" s="21">
+        <v>5.1114317001393621</v>
+      </c>
+      <c r="H41" s="21">
+        <v>2259.1055000000001</v>
+      </c>
+      <c r="I41" s="21">
+        <v>13.77815166027389</v>
+      </c>
+      <c r="L41" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M41" s="46"/>
+      <c r="N41" s="2">
+        <v>9325</v>
+      </c>
+      <c r="O41" s="2">
+        <v>8106</v>
+      </c>
+      <c r="P41" s="2">
+        <v>24507</v>
+      </c>
+      <c r="Q41" s="34">
+        <v>8070.0662499999999</v>
+      </c>
+      <c r="R41" s="34">
+        <v>1255.126</v>
+      </c>
+      <c r="S41" s="34">
+        <v>176.56825000000001</v>
+      </c>
+      <c r="T41" s="34">
+        <v>3650.78775</v>
+      </c>
+      <c r="U41" s="34">
+        <v>90.5595</v>
+      </c>
+      <c r="V41" s="34">
+        <v>64.483249999999998</v>
+      </c>
+      <c r="W41" s="34">
+        <v>4123.3215</v>
+      </c>
+      <c r="X41" s="34">
+        <v>8368.490749999999</v>
+      </c>
+      <c r="Y41" s="34">
+        <v>3424.13825</v>
+      </c>
+      <c r="Z41" s="34">
+        <v>1932.9702500000001</v>
+      </c>
+      <c r="AA41" s="34">
+        <v>433.09775000000002</v>
+      </c>
+      <c r="AB41" s="34">
+        <v>585.54950000000008</v>
+      </c>
+      <c r="AC41" s="34">
+        <v>236.70500000000001</v>
+      </c>
+      <c r="AD41" s="34">
+        <v>309.97000000000003</v>
+      </c>
+      <c r="AE41" s="34">
+        <v>1692.36</v>
+      </c>
+      <c r="AF41" s="34">
+        <v>2723.6089999999999</v>
+      </c>
+      <c r="AG41" s="34">
+        <v>1266.97</v>
+      </c>
+      <c r="AH41" s="34">
+        <v>542.81275000000005</v>
+      </c>
+      <c r="AI41" s="34">
+        <v>401.74</v>
+      </c>
+      <c r="AJ41" s="34">
+        <v>2588.1622499999999</v>
+      </c>
+      <c r="AK41" s="34">
+        <v>0.52550000000000008</v>
+      </c>
+    </row>
+    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2020</v>
+      </c>
+      <c r="B42" s="21">
+        <v>73732.624500000005</v>
+      </c>
+      <c r="C42" s="21">
+        <v>59.5</v>
+      </c>
+      <c r="D42" s="21">
+        <v>43878</v>
+      </c>
+      <c r="E42" s="21">
+        <v>89.7</v>
+      </c>
+      <c r="F42" s="21">
+        <v>39378</v>
+      </c>
+      <c r="G42" s="21">
+        <v>10.3</v>
+      </c>
+      <c r="H42" s="21">
+        <v>4500</v>
+      </c>
+      <c r="I42" s="21">
+        <v>16.2</v>
+      </c>
+      <c r="L42" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M42" s="46"/>
+      <c r="N42" s="2">
+        <v>9754</v>
+      </c>
+      <c r="O42" s="2">
+        <v>7206</v>
+      </c>
+      <c r="P42" s="2">
+        <v>22418</v>
+      </c>
+      <c r="Q42" s="34">
+        <v>8574.1839999999993</v>
+      </c>
+      <c r="R42" s="34">
+        <v>1179.499</v>
+      </c>
+      <c r="S42" s="34">
+        <v>184.001</v>
+      </c>
+      <c r="T42" s="34">
+        <v>3183.6959999999999</v>
+      </c>
+      <c r="U42" s="34">
+        <v>80.938999999999993</v>
+      </c>
+      <c r="V42" s="34">
+        <v>58.109000000000002</v>
+      </c>
+      <c r="W42" s="34">
+        <v>3699.5619999999999</v>
+      </c>
+      <c r="X42" s="34">
+        <v>8081.0479999999998</v>
+      </c>
+      <c r="Y42" s="34">
+        <v>2932.288</v>
+      </c>
+      <c r="Z42" s="34">
+        <v>1468.16</v>
+      </c>
+      <c r="AA42" s="34">
+        <v>349.64699999999999</v>
+      </c>
+      <c r="AB42" s="34">
+        <v>555.76199999999994</v>
+      </c>
+      <c r="AC42" s="34">
+        <v>191.977</v>
+      </c>
+      <c r="AD42" s="34">
+        <v>260.32100000000003</v>
+      </c>
+      <c r="AE42" s="34">
+        <v>1608.915</v>
+      </c>
+      <c r="AF42" s="34">
+        <v>2563.3180000000002</v>
+      </c>
+      <c r="AG42" s="34">
+        <v>1286.059</v>
+      </c>
+      <c r="AH42" s="34">
+        <v>542.36599999999999</v>
+      </c>
+      <c r="AI42" s="34">
+        <v>230.41499999999999</v>
+      </c>
+      <c r="AJ42" s="34">
+        <v>2345.681</v>
+      </c>
+      <c r="AK42" s="34">
+        <v>1.8979999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>2021</v>
+      </c>
+      <c r="B43" s="21">
+        <v>75301.057289249497</v>
+      </c>
+      <c r="C43" s="21">
+        <v>63.349976619962966</v>
+      </c>
+      <c r="D43" s="21">
+        <v>47703.202187324503</v>
+      </c>
+      <c r="E43" s="21">
+        <v>92.212452153046868</v>
+      </c>
+      <c r="F43" s="21">
+        <v>43988.292492457811</v>
+      </c>
+      <c r="G43" s="21">
+        <v>7.7875478469530783</v>
+      </c>
+      <c r="H43" s="21">
+        <v>3714.9096948666634</v>
+      </c>
+      <c r="I43" s="21">
+        <v>15.919764703947065</v>
+      </c>
+      <c r="L43" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M43" s="46"/>
+      <c r="N43" s="2">
+        <v>10656</v>
+      </c>
+      <c r="O43" s="2">
+        <v>8092</v>
+      </c>
+      <c r="P43" s="2">
+        <v>25239</v>
+      </c>
+      <c r="Q43" s="34">
+        <v>9352.7279999999992</v>
+      </c>
+      <c r="R43" s="34">
+        <v>1303.664</v>
+      </c>
+      <c r="S43" s="34">
+        <v>169.72300000000001</v>
+      </c>
+      <c r="T43" s="34">
+        <v>3453.009</v>
+      </c>
+      <c r="U43" s="34">
+        <v>75.843999999999994</v>
+      </c>
+      <c r="V43" s="34">
+        <v>74.724999999999994</v>
+      </c>
+      <c r="W43" s="34">
+        <v>4319.1589999999997</v>
+      </c>
+      <c r="X43" s="34">
+        <v>9725.2090000000007</v>
+      </c>
+      <c r="Y43" s="34">
+        <v>2938.85</v>
+      </c>
+      <c r="Z43" s="34">
+        <v>1416.059</v>
+      </c>
+      <c r="AA43" s="34">
+        <v>444.64499999999998</v>
+      </c>
+      <c r="AB43" s="34">
+        <v>619.71799999999996</v>
+      </c>
+      <c r="AC43" s="34">
+        <v>203.982</v>
+      </c>
+      <c r="AD43" s="34">
+        <v>296.346</v>
+      </c>
+      <c r="AE43" s="34">
+        <v>1831.027</v>
+      </c>
+      <c r="AF43" s="34">
+        <v>2729.3069999999998</v>
+      </c>
+      <c r="AG43" s="34">
+        <v>1425.691</v>
+      </c>
+      <c r="AH43" s="34">
+        <v>658.19399999999996</v>
+      </c>
+      <c r="AI43" s="34">
+        <v>336.548</v>
+      </c>
+      <c r="AJ43" s="34">
+        <v>2612.96</v>
+      </c>
+      <c r="AK43" s="34">
+        <v>0.90700000000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>2022</v>
+      </c>
+      <c r="B44" s="21">
+        <v>76598.736999999994</v>
+      </c>
+      <c r="C44" s="21">
+        <v>64.7</v>
+      </c>
+      <c r="D44" s="21">
+        <v>49561.608999999997</v>
+      </c>
+      <c r="E44" s="21">
+        <v>94.61</v>
+      </c>
+      <c r="F44" s="21">
+        <v>46890.39</v>
+      </c>
+      <c r="G44" s="21">
+        <v>5.39</v>
+      </c>
+      <c r="H44" s="21">
+        <v>2671.2190000000001</v>
+      </c>
+      <c r="I44" s="21">
+        <v>14.24</v>
+      </c>
+      <c r="L44" s="46" t="s">
+        <v>813</v>
+      </c>
+      <c r="M44" s="46"/>
+      <c r="N44" s="2">
+        <v>10836</v>
+      </c>
+      <c r="O44" s="2">
+        <v>8526</v>
+      </c>
+      <c r="P44" s="2">
+        <v>27529</v>
+      </c>
+      <c r="Q44" s="34">
+        <v>9546.11</v>
+      </c>
+      <c r="R44" s="34">
+        <v>1289.6559999999999</v>
+      </c>
+      <c r="S44" s="34">
+        <v>221.846</v>
+      </c>
+      <c r="T44" s="34">
+        <v>3754.212</v>
+      </c>
+      <c r="U44" s="34">
+        <v>95.271000000000001</v>
+      </c>
+      <c r="V44" s="34">
+        <v>72.926000000000002</v>
+      </c>
+      <c r="W44" s="34">
+        <v>4381.6570000000002</v>
+      </c>
+      <c r="X44" s="34">
+        <v>10392.92</v>
+      </c>
+      <c r="Y44" s="34">
+        <v>3243.9560000000001</v>
+      </c>
+      <c r="Z44" s="34">
+        <v>1812.557</v>
+      </c>
+      <c r="AA44" s="34">
+        <v>483.87299999999999</v>
+      </c>
+      <c r="AB44" s="34">
+        <v>645.24300000000005</v>
+      </c>
+      <c r="AC44" s="34">
+        <v>238.16499999999999</v>
+      </c>
+      <c r="AD44" s="34">
+        <v>344.74200000000002</v>
+      </c>
+      <c r="AE44" s="34">
+        <v>2185.5349999999999</v>
+      </c>
+      <c r="AF44" s="34">
+        <v>2842.9169999999999</v>
+      </c>
+      <c r="AG44" s="34">
+        <v>1463.85</v>
+      </c>
+      <c r="AH44" s="34">
+        <v>672.6</v>
+      </c>
+      <c r="AI44" s="34">
+        <v>410.27800000000002</v>
+      </c>
+      <c r="AJ44" s="34">
+        <v>2790.3829999999998</v>
+      </c>
+      <c r="AK44" s="34">
+        <v>1.6950000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>2023</v>
+      </c>
+      <c r="B45" s="21">
+        <v>77613.256999999998</v>
+      </c>
+      <c r="C45" s="21">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="D45" s="21">
+        <v>50376.385999999999</v>
+      </c>
+      <c r="E45" s="21">
+        <v>95.7</v>
+      </c>
+      <c r="F45" s="21">
+        <v>48185.034</v>
+      </c>
+      <c r="G45" s="21">
+        <v>4.3</v>
+      </c>
+      <c r="H45" s="21">
+        <v>2191.3510000000001</v>
+      </c>
+      <c r="I45" s="21">
+        <v>12.3</v>
+      </c>
+      <c r="Q45" s="34"/>
+      <c r="R45" s="34"/>
+      <c r="S45" s="34"/>
+      <c r="T45" s="34"/>
+      <c r="U45" s="34"/>
+      <c r="V45" s="34"/>
+      <c r="W45" s="34"/>
+      <c r="X45" s="34"/>
+      <c r="Y45" s="34"/>
+      <c r="Z45" s="34"/>
+      <c r="AA45" s="34"/>
+      <c r="AB45" s="34"/>
+      <c r="AC45" s="34"/>
+      <c r="AD45" s="34"/>
+      <c r="AE45" s="34"/>
+      <c r="AF45" s="34"/>
+      <c r="AG45" s="34"/>
+      <c r="AH45" s="34"/>
+      <c r="AI45" s="34"/>
+      <c r="AJ45" s="34"/>
+      <c r="AK45" s="34"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -18433,23 +19771,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B3FDD3-8CAB-4986-8439-B73CD0CD9872}">
-  <dimension ref="A1:BS54"/>
+  <dimension ref="A1:BU54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="BO2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BT1" sqref="BT1"/>
+      <selection pane="bottomRight" activeCell="BT27" sqref="BT27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" style="24" customWidth="1"/>
     <col min="2" max="71" width="10.7109375" style="24" customWidth="1"/>
-    <col min="72" max="16384" width="9.140625" style="24"/>
+    <col min="72" max="72" width="9.140625" style="24"/>
+    <col min="73" max="73" width="10.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="74" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>685</v>
       </c>
@@ -18664,7 +20004,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>694</v>
       </c>
@@ -18846,8 +20186,10 @@
       <c r="BS2" s="26">
         <v>50185.470999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT2" s="26"/>
+      <c r="BU2" s="26"/>
+    </row>
+    <row r="3" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>691</v>
       </c>
@@ -18917,8 +20259,10 @@
       <c r="BQ3" s="26"/>
       <c r="BR3" s="26"/>
       <c r="BS3" s="26"/>
-    </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT3" s="26"/>
+      <c r="BU3" s="26"/>
+    </row>
+    <row r="4" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>693</v>
       </c>
@@ -19101,7 +20445,7 @@
         <v>9448.9699999999993</v>
       </c>
     </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>692</v>
       </c>
@@ -19284,7 +20628,7 @@
         <v>1223.2280000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>685</v>
       </c>
@@ -19352,8 +20696,10 @@
       <c r="BQ6" s="26"/>
       <c r="BR6" s="26"/>
       <c r="BS6" s="26"/>
-    </row>
-    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT6" s="26"/>
+      <c r="BU6" s="26"/>
+    </row>
+    <row r="7" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>690</v>
       </c>
@@ -19536,7 +20882,7 @@
         <v>291.67200000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>689</v>
       </c>
@@ -19719,7 +21065,7 @@
         <v>3405.971</v>
       </c>
     </row>
-    <row r="9" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>688</v>
       </c>
@@ -19902,7 +21248,7 @@
         <v>67.512</v>
       </c>
     </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>687</v>
       </c>
@@ -20085,7 +21431,7 @@
         <v>55.939</v>
       </c>
     </row>
-    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>686</v>
       </c>
@@ -20268,7 +21614,7 @@
         <v>5346.6750000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
         <v>669</v>
       </c>
@@ -20336,8 +21682,10 @@
       <c r="BQ12" s="26"/>
       <c r="BR12" s="26"/>
       <c r="BS12" s="26"/>
-    </row>
-    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT12" s="26"/>
+      <c r="BU12" s="26"/>
+    </row>
+    <row r="13" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>683</v>
       </c>
@@ -20520,7 +21868,7 @@
         <v>10180.915000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>682</v>
       </c>
@@ -20703,7 +22051,7 @@
         <v>4031.569</v>
       </c>
     </row>
-    <row r="15" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>681</v>
       </c>
@@ -20886,7 +22234,7 @@
         <v>2677.1469999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>680</v>
       </c>
@@ -45634,11 +46982,11 @@
   <dimension ref="A1:D191"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B175" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B173" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B153" sqref="B153"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B182" sqref="B182"/>
+      <selection pane="bottomRight" activeCell="B184" sqref="B184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47360,6 +48708,9 @@
       <c r="A183" s="1" t="s">
         <v>771</v>
       </c>
+      <c r="B183" t="s">
+        <v>820</v>
+      </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
@@ -47412,7 +48763,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47489,6 +48840,9 @@
       <c r="B10">
         <v>1</v>
       </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -47497,6 +48851,9 @@
       <c r="B11">
         <v>1</v>
       </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -47505,6 +48862,9 @@
       <c r="B12">
         <v>1</v>
       </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -47521,6 +48881,9 @@
       <c r="B14">
         <v>1</v>
       </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -47532,6 +48895,9 @@
       <c r="C15">
         <v>1</v>
       </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -47540,6 +48906,9 @@
       <c r="B16">
         <v>1</v>
       </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -47551,6 +48920,9 @@
       <c r="C17">
         <v>1</v>
       </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -47559,6 +48931,9 @@
       <c r="B18">
         <v>1</v>
       </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -47568,6 +48943,9 @@
         <v>1</v>
       </c>
       <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Monthly labor update - Jul 2025
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C3B3AE-5E22-4093-A21D-03051EE918ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E36C01-6426-4DC7-BEE3-B8865778D79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="855" yWindow="1365" windowWidth="14100" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2999" uniqueCount="821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3013" uniqueCount="834">
   <si>
     <t>LFS Round</t>
   </si>
@@ -2501,6 +2501,45 @@
   </si>
   <si>
     <t>https://psa.gov.ph/content/participation-labor-force-june-2025-increased-5242-million-filipinos-aged-15-years-and-over</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/participation-labor-force-july-2025-decreased-4864-million-filipinos-aged-15-years-and-over</t>
+  </si>
+  <si>
+    <t>2025Jan</t>
+  </si>
+  <si>
+    <t>2025Feb</t>
+  </si>
+  <si>
+    <t>2025Mar</t>
+  </si>
+  <si>
+    <t>2025Apr</t>
+  </si>
+  <si>
+    <t>2025May</t>
+  </si>
+  <si>
+    <t>2025Jun</t>
+  </si>
+  <si>
+    <t>2025Jul</t>
+  </si>
+  <si>
+    <t>2025Aug</t>
+  </si>
+  <si>
+    <t>2025Sep</t>
+  </si>
+  <si>
+    <t>2025Oct</t>
+  </si>
+  <si>
+    <t>2025Nov</t>
+  </si>
+  <si>
+    <t>2025Dec</t>
   </si>
 </sst>
 </file>
@@ -2513,11 +2552,18 @@
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2665,11 +2711,11 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2694,41 +2740,45 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2961,12 +3011,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P299"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D266" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D281" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F263" sqref="F263"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F293" sqref="F293"/>
+      <selection pane="bottomRight" activeCell="F294" sqref="F294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15455,7 +15505,7 @@
         <v>2157.422</v>
       </c>
       <c r="N274" s="2">
-        <f t="shared" ref="N274:N292" si="34">J274-K274</f>
+        <f t="shared" ref="N274:N293" si="34">J274-K274</f>
         <v>30572.822</v>
       </c>
       <c r="O274" s="2">
@@ -15737,43 +15787,40 @@
       <c r="D280" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E280" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F280" s="3">
         <f t="shared" ref="F280" si="37">K280/J280</f>
-        <v>0.63469480625870289</v>
+        <v>0.6345079922666238</v>
       </c>
       <c r="G280" s="3">
         <f t="shared" ref="G280" si="38">L280/K280</f>
-        <v>0.95256802192614232</v>
+        <v>0.95255090475919457</v>
       </c>
       <c r="H280" s="3">
         <f t="shared" ref="H280" si="39">M280/K280</f>
-        <v>4.7431978073857746E-2</v>
+        <v>4.7449095240805372E-2</v>
       </c>
       <c r="I280" s="3">
         <f t="shared" ref="I280" si="40">O280/L280</f>
-        <v>0.12110610167973515</v>
+        <v>0.12107203315603994</v>
       </c>
       <c r="J280" s="2">
-        <v>78893.918000000005</v>
+        <v>78894.39</v>
       </c>
       <c r="K280" s="2">
-        <v>50073.56</v>
+        <v>50059.120999999999</v>
       </c>
       <c r="L280" s="2">
-        <v>47698.472000000002</v>
+        <v>47683.860999999997</v>
       </c>
       <c r="M280" s="2">
-        <v>2375.0880000000002</v>
+        <v>2375.2600000000002</v>
       </c>
       <c r="N280" s="2">
         <f t="shared" si="34"/>
-        <v>28820.358000000007</v>
+        <v>28835.269</v>
       </c>
       <c r="O280" s="2">
-        <v>5776.576</v>
+        <v>5773.1819999999998</v>
       </c>
       <c r="P280" t="s">
         <v>663</v>
@@ -16364,19 +16411,19 @@
         <v>425</v>
       </c>
       <c r="F292" s="3">
-        <f t="shared" ref="F292" si="61">K292/J292</f>
+        <f t="shared" ref="F292:F293" si="61">K292/J292</f>
         <v>0.65710331091544816</v>
       </c>
       <c r="G292" s="3">
-        <f t="shared" ref="G292" si="62">L292/K292</f>
+        <f t="shared" ref="G292:G293" si="62">L292/K292</f>
         <v>0.96282180199484058</v>
       </c>
       <c r="H292" s="3">
-        <f t="shared" ref="H292" si="63">M292/K292</f>
+        <f t="shared" ref="H292:H293" si="63">M292/K292</f>
         <v>3.7178178929830163E-2</v>
       </c>
       <c r="I292" s="3">
-        <f t="shared" ref="I292" si="64">O292/L292</f>
+        <f t="shared" ref="I292:I293" si="64">O292/L292</f>
         <v>0.11416914389709779</v>
       </c>
       <c r="J292" s="2">
@@ -16415,7 +16462,47 @@
       <c r="D293" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="O293" s="2"/>
+      <c r="E293" s="49" t="s">
+        <v>425</v>
+      </c>
+      <c r="F293" s="3">
+        <f t="shared" si="61"/>
+        <v>0.60733264333125092</v>
+      </c>
+      <c r="G293" s="3">
+        <f t="shared" si="62"/>
+        <v>0.94668134653257563</v>
+      </c>
+      <c r="H293" s="3">
+        <f t="shared" si="63"/>
+        <v>5.3318653467424447E-2</v>
+      </c>
+      <c r="I293" s="3">
+        <f t="shared" si="64"/>
+        <v>0.14776248445292775</v>
+      </c>
+      <c r="J293" s="2">
+        <v>80087.680999999997</v>
+      </c>
+      <c r="K293" s="2">
+        <v>48639.862999999998</v>
+      </c>
+      <c r="L293" s="2">
+        <v>46046.451000000001</v>
+      </c>
+      <c r="M293" s="2">
+        <v>2593.4119999999998</v>
+      </c>
+      <c r="N293" s="2">
+        <f t="shared" si="34"/>
+        <v>31447.817999999999</v>
+      </c>
+      <c r="O293" s="2">
+        <v>6803.9380000000001</v>
+      </c>
+      <c r="P293" t="s">
+        <v>821</v>
+      </c>
     </row>
     <row r="294" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
@@ -19763,7 +19850,7 @@
       <c r="AK45" s="34"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -19771,25 +19858,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B3FDD3-8CAB-4986-8439-B73CD0CD9872}">
-  <dimension ref="A1:BU54"/>
+  <dimension ref="A1:CE54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="BO2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="BV2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BT27" sqref="BT27"/>
+      <selection pane="bottomRight" activeCell="BZ2" sqref="BZ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" style="24" customWidth="1"/>
     <col min="2" max="71" width="10.7109375" style="24" customWidth="1"/>
-    <col min="72" max="72" width="9.140625" style="24"/>
-    <col min="73" max="73" width="10.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="74" max="16384" width="9.140625" style="24"/>
+    <col min="72" max="83" width="10.7109375" style="26" customWidth="1"/>
+    <col min="84" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>685</v>
       </c>
@@ -19964,7 +20050,7 @@
       <c r="BF1" s="24" t="s">
         <v>706</v>
       </c>
-      <c r="BG1" s="31" t="s">
+      <c r="BG1" s="50" t="s">
         <v>705</v>
       </c>
       <c r="BH1" s="24" t="s">
@@ -19985,7 +20071,7 @@
       <c r="BM1" s="24" t="s">
         <v>699</v>
       </c>
-      <c r="BN1" s="24" t="s">
+      <c r="BN1" s="31" t="s">
         <v>698</v>
       </c>
       <c r="BO1" s="24" t="s">
@@ -20003,8 +20089,44 @@
       <c r="BS1" s="36" t="s">
         <v>766</v>
       </c>
-    </row>
-    <row r="2" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="BT1" s="26" t="s">
+        <v>822</v>
+      </c>
+      <c r="BU1" s="26" t="s">
+        <v>823</v>
+      </c>
+      <c r="BV1" s="26" t="s">
+        <v>824</v>
+      </c>
+      <c r="BW1" s="26" t="s">
+        <v>825</v>
+      </c>
+      <c r="BX1" s="26" t="s">
+        <v>826</v>
+      </c>
+      <c r="BY1" s="26" t="s">
+        <v>827</v>
+      </c>
+      <c r="BZ1" s="26" t="s">
+        <v>828</v>
+      </c>
+      <c r="CA1" s="26" t="s">
+        <v>829</v>
+      </c>
+      <c r="CB1" s="26" t="s">
+        <v>830</v>
+      </c>
+      <c r="CC1" s="26" t="s">
+        <v>831</v>
+      </c>
+      <c r="CD1" s="51" t="s">
+        <v>832</v>
+      </c>
+      <c r="CE1" s="52" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>694</v>
       </c>
@@ -20150,46 +20272,65 @@
       <c r="BG2" s="26">
         <v>50524.688000000002</v>
       </c>
-      <c r="BH2" s="26">
-        <v>45942.885999999999</v>
-      </c>
-      <c r="BI2" s="26">
+      <c r="BH2" s="34">
+        <v>45902.161</v>
+      </c>
+      <c r="BI2" s="34">
         <v>48950.548000000003</v>
       </c>
-      <c r="BJ2" s="26">
+      <c r="BJ2" s="34">
         <v>49152.983999999997</v>
       </c>
-      <c r="BK2" s="26">
-        <v>48355.254999999997</v>
-      </c>
-      <c r="BL2" s="26">
+      <c r="BK2" s="34">
+        <v>48354.356</v>
+      </c>
+      <c r="BL2" s="34">
         <v>48865.478000000003</v>
       </c>
-      <c r="BM2" s="26">
+      <c r="BM2" s="34">
         <v>50278.082000000002</v>
       </c>
-      <c r="BN2" s="26">
-        <v>47698.472000000002</v>
-      </c>
-      <c r="BO2" s="26">
+      <c r="BN2" s="34">
+        <v>47683.860999999997</v>
+      </c>
+      <c r="BO2" s="34">
         <v>49153.883000000002</v>
       </c>
-      <c r="BP2" s="26">
+      <c r="BP2" s="34">
         <v>49872.28</v>
       </c>
-      <c r="BQ2" s="26">
+      <c r="BQ2" s="34">
         <v>48156.966</v>
       </c>
-      <c r="BR2" s="26">
+      <c r="BR2" s="34">
         <v>49541.468999999997</v>
       </c>
-      <c r="BS2" s="26">
+      <c r="BS2" s="34">
         <v>50185.470999999998</v>
       </c>
-      <c r="BT2" s="26"/>
-      <c r="BU2" s="26"/>
-    </row>
-    <row r="3" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="BT2" s="34">
+        <v>48486.641000000003</v>
+      </c>
+      <c r="BU2" s="34">
+        <v>49154.667000000001</v>
+      </c>
+      <c r="BV2" s="34">
+        <v>48024.858</v>
+      </c>
+      <c r="BW2" s="34">
+        <v>48671.648000000001</v>
+      </c>
+      <c r="BX2" s="34">
+        <v>50289.760999999999</v>
+      </c>
+      <c r="BY2" s="34">
+        <v>50474.714999999997</v>
+      </c>
+      <c r="BZ2" s="34">
+        <v>46046.451000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>691</v>
       </c>
@@ -20259,10 +20400,8 @@
       <c r="BQ3" s="26"/>
       <c r="BR3" s="26"/>
       <c r="BS3" s="26"/>
-      <c r="BT3" s="26"/>
-      <c r="BU3" s="26"/>
-    </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>693</v>
       </c>
@@ -20409,25 +20548,25 @@
         <v>11007.349</v>
       </c>
       <c r="BH4" s="26">
-        <v>8327.1959999999999</v>
+        <v>8053.085</v>
       </c>
       <c r="BI4" s="26">
-        <v>9355.0630000000001</v>
+        <v>9365.4889999999996</v>
       </c>
       <c r="BJ4" s="26">
-        <v>9037.473</v>
+        <v>9079.9230000000007</v>
       </c>
       <c r="BK4" s="26">
-        <v>8353.2649999999994</v>
+        <v>8353.1270000000004</v>
       </c>
       <c r="BL4" s="26">
-        <v>8963.01</v>
+        <v>8962.4</v>
       </c>
       <c r="BM4" s="26">
-        <v>9534.3410000000003</v>
+        <v>9531.5619999999999</v>
       </c>
       <c r="BN4" s="26">
-        <v>8784.2950000000001</v>
+        <v>8756.9830000000002</v>
       </c>
       <c r="BO4" s="26">
         <v>8432.6589999999997</v>
@@ -20444,8 +20583,29 @@
       <c r="BS4" s="26">
         <v>9448.9699999999993</v>
       </c>
-    </row>
-    <row r="5" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="BT4" s="26">
+        <v>8936.34</v>
+      </c>
+      <c r="BU4" s="26">
+        <v>8415.9940000000006</v>
+      </c>
+      <c r="BV4" s="26">
+        <v>8470.4310000000005</v>
+      </c>
+      <c r="BW4" s="26">
+        <v>8612.8130000000001</v>
+      </c>
+      <c r="BX4" s="26">
+        <v>9431.5139999999992</v>
+      </c>
+      <c r="BY4" s="26">
+        <v>8951.8940000000002</v>
+      </c>
+      <c r="BZ4" s="26">
+        <v>7381.6890000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
         <v>692</v>
       </c>
@@ -20592,16 +20752,16 @@
         <v>1306.3240000000001</v>
       </c>
       <c r="BH5" s="26">
-        <v>1491.47</v>
+        <v>1315.279</v>
       </c>
       <c r="BI5" s="26">
         <v>1089.8810000000001</v>
       </c>
       <c r="BJ5" s="26">
-        <v>1031.0930000000001</v>
+        <v>1031.635</v>
       </c>
       <c r="BK5" s="26">
-        <v>1444.2560000000001</v>
+        <v>1445.0070000000001</v>
       </c>
       <c r="BL5" s="26">
         <v>1203.105</v>
@@ -20610,7 +20770,7 @@
         <v>1089.2</v>
       </c>
       <c r="BN5" s="26">
-        <v>1327.144</v>
+        <v>1323.8320000000001</v>
       </c>
       <c r="BO5" s="26">
         <v>1049.3320000000001</v>
@@ -20627,8 +20787,29 @@
       <c r="BS5" s="26">
         <v>1223.2280000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="BT5" s="26">
+        <v>1308.03</v>
+      </c>
+      <c r="BU5" s="26">
+        <v>1455.258</v>
+      </c>
+      <c r="BV5" s="26">
+        <v>1169.912</v>
+      </c>
+      <c r="BW5" s="26">
+        <v>1408.616</v>
+      </c>
+      <c r="BX5" s="26">
+        <v>1172.95</v>
+      </c>
+      <c r="BY5" s="26">
+        <v>1601.1949999999999</v>
+      </c>
+      <c r="BZ5" s="26">
+        <v>1151.009</v>
+      </c>
+    </row>
+    <row r="6" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>685</v>
       </c>
@@ -20696,10 +20877,8 @@
       <c r="BQ6" s="26"/>
       <c r="BR6" s="26"/>
       <c r="BS6" s="26"/>
-      <c r="BT6" s="26"/>
-      <c r="BU6" s="26"/>
-    </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>690</v>
       </c>
@@ -20846,7 +21025,7 @@
         <v>200.27199999999999</v>
       </c>
       <c r="BH7" s="26">
-        <v>227.578</v>
+        <v>215.55699999999999</v>
       </c>
       <c r="BI7" s="26">
         <v>233.07499999999999</v>
@@ -20855,16 +21034,16 @@
         <v>179.75</v>
       </c>
       <c r="BK7" s="26">
-        <v>243.74299999999999</v>
+        <v>243.76</v>
       </c>
       <c r="BL7" s="26">
-        <v>241.68</v>
+        <v>249.03200000000001</v>
       </c>
       <c r="BM7" s="26">
-        <v>283.59300000000002</v>
+        <v>279.82799999999997</v>
       </c>
       <c r="BN7" s="26">
-        <v>185.345</v>
+        <v>185.125</v>
       </c>
       <c r="BO7" s="26">
         <v>210.58099999999999</v>
@@ -20881,8 +21060,29 @@
       <c r="BS7" s="26">
         <v>291.67200000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="BT7" s="26">
+        <v>221.58500000000001</v>
+      </c>
+      <c r="BU7" s="26">
+        <v>231.15100000000001</v>
+      </c>
+      <c r="BV7" s="26">
+        <v>177.78700000000001</v>
+      </c>
+      <c r="BW7" s="26">
+        <v>188.47800000000001</v>
+      </c>
+      <c r="BX7" s="26">
+        <v>167.53</v>
+      </c>
+      <c r="BY7" s="26">
+        <v>183.52099999999999</v>
+      </c>
+      <c r="BZ7" s="26">
+        <v>245.18700000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>689</v>
       </c>
@@ -21029,25 +21229,25 @@
         <v>3792.8150000000001</v>
       </c>
       <c r="BH8" s="26">
-        <v>3520.1819999999998</v>
+        <v>3569.569</v>
       </c>
       <c r="BI8" s="26">
-        <v>3672.0070000000001</v>
+        <v>3646.84</v>
       </c>
       <c r="BJ8" s="26">
-        <v>4022.5309999999999</v>
+        <v>3981.3049999999998</v>
       </c>
       <c r="BK8" s="26">
-        <v>3738.4580000000001</v>
+        <v>3738.5929999999998</v>
       </c>
       <c r="BL8" s="26">
-        <v>3845.8180000000002</v>
+        <v>3887.5219999999999</v>
       </c>
       <c r="BM8" s="26">
-        <v>3929.9169999999999</v>
+        <v>3924.846</v>
       </c>
       <c r="BN8" s="26">
-        <v>3459.2739999999999</v>
+        <v>3453.3130000000001</v>
       </c>
       <c r="BO8" s="26">
         <v>3406.0970000000002</v>
@@ -21064,8 +21264,29 @@
       <c r="BS8" s="26">
         <v>3405.971</v>
       </c>
-    </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="BT8" s="26">
+        <v>3360.5790000000002</v>
+      </c>
+      <c r="BU8" s="26">
+        <v>3585.5050000000001</v>
+      </c>
+      <c r="BV8" s="26">
+        <v>3700.2350000000001</v>
+      </c>
+      <c r="BW8" s="26">
+        <v>3328.8119999999999</v>
+      </c>
+      <c r="BX8" s="26">
+        <v>3513.08</v>
+      </c>
+      <c r="BY8" s="26">
+        <v>3500.835</v>
+      </c>
+      <c r="BZ8" s="26">
+        <v>3561.9090000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
         <v>688</v>
       </c>
@@ -21212,7 +21433,7 @@
         <v>98.941999999999993</v>
       </c>
       <c r="BH9" s="26">
-        <v>87.903999999999996</v>
+        <v>90.087999999999994</v>
       </c>
       <c r="BI9" s="26">
         <v>94.751000000000005</v>
@@ -21221,16 +21442,16 @@
         <v>99.906999999999996</v>
       </c>
       <c r="BK9" s="26">
-        <v>70.477000000000004</v>
+        <v>70.134</v>
       </c>
       <c r="BL9" s="26">
-        <v>75.203000000000003</v>
+        <v>78.864000000000004</v>
       </c>
       <c r="BM9" s="26">
         <v>108.76300000000001</v>
       </c>
       <c r="BN9" s="26">
-        <v>97.334000000000003</v>
+        <v>93.182000000000002</v>
       </c>
       <c r="BO9" s="26">
         <v>92.911000000000001</v>
@@ -21247,8 +21468,29 @@
       <c r="BS9" s="26">
         <v>67.512</v>
       </c>
-    </row>
-    <row r="10" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="BT9" s="26">
+        <v>88.766999999999996</v>
+      </c>
+      <c r="BU9" s="26">
+        <v>94.613</v>
+      </c>
+      <c r="BV9" s="26">
+        <v>84.483000000000004</v>
+      </c>
+      <c r="BW9" s="26">
+        <v>112.11499999999999</v>
+      </c>
+      <c r="BX9" s="26">
+        <v>96.335999999999999</v>
+      </c>
+      <c r="BY9" s="26">
+        <v>103.614</v>
+      </c>
+      <c r="BZ9" s="26">
+        <v>97.754999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>687</v>
       </c>
@@ -21395,7 +21637,7 @@
         <v>73.010999999999996</v>
       </c>
       <c r="BH10" s="26">
-        <v>99.936000000000007</v>
+        <v>99.286000000000001</v>
       </c>
       <c r="BI10" s="26">
         <v>94.471000000000004</v>
@@ -21404,16 +21646,16 @@
         <v>65.700999999999993</v>
       </c>
       <c r="BK10" s="26">
-        <v>93.25</v>
+        <v>93.682000000000002</v>
       </c>
       <c r="BL10" s="26">
-        <v>83.394000000000005</v>
+        <v>108.48699999999999</v>
       </c>
       <c r="BM10" s="26">
         <v>47.353999999999999</v>
       </c>
       <c r="BN10" s="26">
-        <v>92.914000000000001</v>
+        <v>91.924000000000007</v>
       </c>
       <c r="BO10" s="26">
         <v>114.21</v>
@@ -21430,8 +21672,29 @@
       <c r="BS10" s="26">
         <v>55.939</v>
       </c>
-    </row>
-    <row r="11" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="BT10" s="26">
+        <v>90.847999999999999</v>
+      </c>
+      <c r="BU10" s="26">
+        <v>49.323</v>
+      </c>
+      <c r="BV10" s="26">
+        <v>67.367000000000004</v>
+      </c>
+      <c r="BW10" s="26">
+        <v>75.254000000000005</v>
+      </c>
+      <c r="BX10" s="26">
+        <v>58.371000000000002</v>
+      </c>
+      <c r="BY10" s="26">
+        <v>55.444000000000003</v>
+      </c>
+      <c r="BZ10" s="26">
+        <v>92.194000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>686</v>
       </c>
@@ -21578,25 +21841,25 @@
         <v>5083.8609999999999</v>
       </c>
       <c r="BH11" s="26">
-        <v>4534.4809999999998</v>
+        <v>4607.5039999999999</v>
       </c>
       <c r="BI11" s="26">
-        <v>4765.1819999999998</v>
+        <v>4772.66</v>
       </c>
       <c r="BJ11" s="26">
-        <v>4551.24</v>
+        <v>4554.5349999999999</v>
       </c>
       <c r="BK11" s="26">
-        <v>4697.7709999999997</v>
+        <v>4690.2550000000001</v>
       </c>
       <c r="BL11" s="26">
-        <v>5088.9709999999995</v>
+        <v>5083.0969999999998</v>
       </c>
       <c r="BM11" s="26">
         <v>5769.2190000000001</v>
       </c>
       <c r="BN11" s="26">
-        <v>4746.1880000000001</v>
+        <v>4751.4650000000001</v>
       </c>
       <c r="BO11" s="26">
         <v>4738.2860000000001</v>
@@ -21613,8 +21876,29 @@
       <c r="BS11" s="26">
         <v>5346.6750000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="BT11" s="26">
+        <v>4596.8190000000004</v>
+      </c>
+      <c r="BU11" s="26">
+        <v>5031.027</v>
+      </c>
+      <c r="BV11" s="26">
+        <v>4558.4160000000002</v>
+      </c>
+      <c r="BW11" s="26">
+        <v>4810.8779999999997</v>
+      </c>
+      <c r="BX11" s="26">
+        <v>4785.1679999999997</v>
+      </c>
+      <c r="BY11" s="26">
+        <v>5077.6289999999999</v>
+      </c>
+      <c r="BZ11" s="26">
+        <v>4604.7449999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
         <v>669</v>
       </c>
@@ -21682,10 +21966,8 @@
       <c r="BQ12" s="26"/>
       <c r="BR12" s="26"/>
       <c r="BS12" s="26"/>
-      <c r="BT12" s="26"/>
-      <c r="BU12" s="26"/>
-    </row>
-    <row r="13" spans="1:73" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>683</v>
       </c>
@@ -21832,25 +22114,25 @@
         <v>10287.226000000001</v>
       </c>
       <c r="BH13" s="26">
-        <v>9054.0400000000009</v>
+        <v>9141.7540000000008</v>
       </c>
       <c r="BI13" s="26">
-        <v>10662.749</v>
+        <v>10688.343999999999</v>
       </c>
       <c r="BJ13" s="26">
-        <v>10745.492</v>
+        <v>10348.145</v>
       </c>
       <c r="BK13" s="26">
-        <v>10143.936</v>
+        <v>10187.484</v>
       </c>
       <c r="BL13" s="26">
-        <v>10109.215</v>
+        <v>9451.2459999999992</v>
       </c>
       <c r="BM13" s="26">
-        <v>10599.304</v>
+        <v>10473.454</v>
       </c>
       <c r="BN13" s="26">
-        <v>9778.3979999999992</v>
+        <v>9738.1260000000002</v>
       </c>
       <c r="BO13" s="26">
         <v>10929.153</v>
@@ -21867,8 +22149,29 @@
       <c r="BS13" s="26">
         <v>10180.915000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="BT13" s="26">
+        <v>9991.3279999999995</v>
+      </c>
+      <c r="BU13" s="26">
+        <v>10611.763999999999</v>
+      </c>
+      <c r="BV13" s="26">
+        <v>10172.986000000001</v>
+      </c>
+      <c r="BW13" s="26">
+        <v>10130.905000000001</v>
+      </c>
+      <c r="BX13" s="26">
+        <v>9940.4140000000007</v>
+      </c>
+      <c r="BY13" s="26">
+        <v>10848.27</v>
+      </c>
+      <c r="BZ13" s="26">
+        <v>8841.4459999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>682</v>
       </c>
@@ -22015,25 +22318,25 @@
         <v>3476.6579999999999</v>
       </c>
       <c r="BH14" s="26">
-        <v>3648.047</v>
+        <v>3715.6219999999998</v>
       </c>
       <c r="BI14" s="26">
-        <v>3854.277</v>
+        <v>3839.395</v>
       </c>
       <c r="BJ14" s="26">
-        <v>3562.4650000000001</v>
+        <v>3556.1219999999998</v>
       </c>
       <c r="BK14" s="26">
-        <v>3754.4070000000002</v>
+        <v>3755.453</v>
       </c>
       <c r="BL14" s="26">
-        <v>3726.6930000000002</v>
+        <v>3753.0520000000001</v>
       </c>
       <c r="BM14" s="26">
-        <v>3574.6350000000002</v>
+        <v>3578.6869999999999</v>
       </c>
       <c r="BN14" s="26">
-        <v>3628.221</v>
+        <v>3628.5070000000001</v>
       </c>
       <c r="BO14" s="26">
         <v>3834.7220000000002</v>
@@ -22050,8 +22353,29 @@
       <c r="BS14" s="26">
         <v>4031.569</v>
       </c>
-    </row>
-    <row r="15" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="BT14" s="26">
+        <v>3856.989</v>
+      </c>
+      <c r="BU14" s="26">
+        <v>3680.9879999999998</v>
+      </c>
+      <c r="BV14" s="26">
+        <v>3544.52</v>
+      </c>
+      <c r="BW14" s="26">
+        <v>3768.9630000000002</v>
+      </c>
+      <c r="BX14" s="26">
+        <v>3746.1660000000002</v>
+      </c>
+      <c r="BY14" s="26">
+        <v>3789.3009999999999</v>
+      </c>
+      <c r="BZ14" s="26">
+        <v>3836.7649999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>681</v>
       </c>
@@ -22198,25 +22522,25 @@
         <v>2500.431</v>
       </c>
       <c r="BH15" s="26">
-        <v>2127.9870000000001</v>
+        <v>2165.5909999999999</v>
       </c>
       <c r="BI15" s="26">
-        <v>2452.759</v>
+        <v>2438.1120000000001</v>
       </c>
       <c r="BJ15" s="26">
-        <v>2562.4229999999998</v>
+        <v>2950.91</v>
       </c>
       <c r="BK15" s="26">
-        <v>2754.1840000000002</v>
+        <v>2708.7890000000002</v>
       </c>
       <c r="BL15" s="26">
-        <v>2431.864</v>
+        <v>2982.3690000000001</v>
       </c>
       <c r="BM15" s="26">
-        <v>2616.0450000000001</v>
+        <v>2670.8589999999999</v>
       </c>
       <c r="BN15" s="26">
-        <v>2557.1489999999999</v>
+        <v>2588.0880000000002</v>
       </c>
       <c r="BO15" s="26">
         <v>2517.9430000000002</v>
@@ -22233,8 +22557,29 @@
       <c r="BS15" s="26">
         <v>2677.1469999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:73" x14ac:dyDescent="0.25">
+      <c r="BT15" s="26">
+        <v>2698.9050000000002</v>
+      </c>
+      <c r="BU15" s="26">
+        <v>2815.482</v>
+      </c>
+      <c r="BV15" s="26">
+        <v>2913.1869999999999</v>
+      </c>
+      <c r="BW15" s="26">
+        <v>2567.8820000000001</v>
+      </c>
+      <c r="BX15" s="26">
+        <v>3347.152</v>
+      </c>
+      <c r="BY15" s="26">
+        <v>2785.1219999999998</v>
+      </c>
+      <c r="BZ15" s="26">
+        <v>2519.1410000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>680</v>
       </c>
@@ -22381,25 +22726,25 @@
         <v>558.91700000000003</v>
       </c>
       <c r="BH16" s="26">
-        <v>506.74900000000002</v>
+        <v>511.83499999999998</v>
       </c>
       <c r="BI16" s="26">
-        <v>370.13799999999998</v>
+        <v>369.76900000000001</v>
       </c>
       <c r="BJ16" s="26">
-        <v>529.33799999999997</v>
+        <v>530.63099999999997</v>
       </c>
       <c r="BK16" s="26">
-        <v>440.73700000000002</v>
+        <v>438.68400000000003</v>
       </c>
       <c r="BL16" s="26">
-        <v>443.76600000000002</v>
+        <v>443.49400000000003</v>
       </c>
       <c r="BM16" s="26">
-        <v>351.59399999999999</v>
+        <v>359.67700000000002</v>
       </c>
       <c r="BN16" s="26">
-        <v>466.791</v>
+        <v>459.96499999999997</v>
       </c>
       <c r="BO16" s="26">
         <v>430.78300000000002</v>
@@ -22416,8 +22761,29 @@
       <c r="BS16" s="26">
         <v>485.89</v>
       </c>
-    </row>
-    <row r="17" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT16" s="26">
+        <v>502.625</v>
+      </c>
+      <c r="BU16" s="26">
+        <v>413.47500000000002</v>
+      </c>
+      <c r="BV16" s="26">
+        <v>513.9</v>
+      </c>
+      <c r="BW16" s="26">
+        <v>454.27</v>
+      </c>
+      <c r="BX16" s="26">
+        <v>500.88</v>
+      </c>
+      <c r="BY16" s="26">
+        <v>487.84899999999999</v>
+      </c>
+      <c r="BZ16" s="26">
+        <v>511.774</v>
+      </c>
+    </row>
+    <row r="17" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>679</v>
       </c>
@@ -22564,25 +22930,25 @@
         <v>561.71299999999997</v>
       </c>
       <c r="BH17" s="26">
-        <v>641.48500000000001</v>
+        <v>648.24599999999998</v>
       </c>
       <c r="BI17" s="26">
-        <v>720.22</v>
+        <v>715.601</v>
       </c>
       <c r="BJ17" s="26">
-        <v>762.72500000000002</v>
+        <v>765.56399999999996</v>
       </c>
       <c r="BK17" s="26">
-        <v>652.08399999999995</v>
+        <v>648.649</v>
       </c>
       <c r="BL17" s="26">
-        <v>692.255</v>
+        <v>685.00400000000002</v>
       </c>
       <c r="BM17" s="26">
-        <v>568.55600000000004</v>
+        <v>557.06799999999998</v>
       </c>
       <c r="BN17" s="26">
-        <v>710.10799999999995</v>
+        <v>708.07100000000003</v>
       </c>
       <c r="BO17" s="26">
         <v>580.26599999999996</v>
@@ -22599,8 +22965,29 @@
       <c r="BS17" s="26">
         <v>757.32100000000003</v>
       </c>
-    </row>
-    <row r="18" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT17" s="26">
+        <v>742.65499999999997</v>
+      </c>
+      <c r="BU17" s="26">
+        <v>674.68499999999995</v>
+      </c>
+      <c r="BV17" s="26">
+        <v>687.39800000000002</v>
+      </c>
+      <c r="BW17" s="26">
+        <v>656.87800000000004</v>
+      </c>
+      <c r="BX17" s="26">
+        <v>636.30899999999997</v>
+      </c>
+      <c r="BY17" s="26">
+        <v>884.46400000000006</v>
+      </c>
+      <c r="BZ17" s="26">
+        <v>717.12599999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>678</v>
       </c>
@@ -22747,25 +23134,25 @@
         <v>243.08099999999999</v>
       </c>
       <c r="BH18" s="26">
-        <v>260.29000000000002</v>
+        <v>266.48700000000002</v>
       </c>
       <c r="BI18" s="26">
         <v>253.08099999999999</v>
       </c>
       <c r="BJ18" s="26">
-        <v>263.27999999999997</v>
+        <v>255.738</v>
       </c>
       <c r="BK18" s="26">
-        <v>229.82400000000001</v>
+        <v>231.58099999999999</v>
       </c>
       <c r="BL18" s="26">
-        <v>169.14099999999999</v>
+        <v>178.98</v>
       </c>
       <c r="BM18" s="26">
         <v>312.00200000000001</v>
       </c>
       <c r="BN18" s="26">
-        <v>292.77300000000002</v>
+        <v>292.05200000000002</v>
       </c>
       <c r="BO18" s="26">
         <v>328.76900000000001</v>
@@ -22782,8 +23169,29 @@
       <c r="BS18" s="26">
         <v>330.81799999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT18" s="26">
+        <v>282.58199999999999</v>
+      </c>
+      <c r="BU18" s="26">
+        <v>211.39699999999999</v>
+      </c>
+      <c r="BV18" s="26">
+        <v>268.63499999999999</v>
+      </c>
+      <c r="BW18" s="26">
+        <v>272.22199999999998</v>
+      </c>
+      <c r="BX18" s="26">
+        <v>351.471</v>
+      </c>
+      <c r="BY18" s="26">
+        <v>322.029</v>
+      </c>
+      <c r="BZ18" s="26">
+        <v>272.673</v>
+      </c>
+    </row>
+    <row r="19" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>677</v>
       </c>
@@ -22930,7 +23338,7 @@
         <v>309.233</v>
       </c>
       <c r="BH19" s="26">
-        <v>487.30399999999997</v>
+        <v>485.96699999999998</v>
       </c>
       <c r="BI19" s="26">
         <v>404.97699999999998</v>
@@ -22939,16 +23347,16 @@
         <v>371.79300000000001</v>
       </c>
       <c r="BK19" s="26">
-        <v>391.37200000000001</v>
+        <v>393.07</v>
       </c>
       <c r="BL19" s="26">
-        <v>290.18400000000003</v>
+        <v>298.30900000000003</v>
       </c>
       <c r="BM19" s="26">
         <v>417.33699999999999</v>
       </c>
       <c r="BN19" s="26">
-        <v>401.08100000000002</v>
+        <v>399.49700000000001</v>
       </c>
       <c r="BO19" s="26">
         <v>393.80599999999998</v>
@@ -22965,8 +23373,29 @@
       <c r="BS19" s="26">
         <v>438.92700000000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT19" s="26">
+        <v>427.60500000000002</v>
+      </c>
+      <c r="BU19" s="26">
+        <v>337.34399999999999</v>
+      </c>
+      <c r="BV19" s="26">
+        <v>271.33499999999998</v>
+      </c>
+      <c r="BW19" s="26">
+        <v>392.25</v>
+      </c>
+      <c r="BX19" s="26">
+        <v>465.33199999999999</v>
+      </c>
+      <c r="BY19" s="26">
+        <v>384.548</v>
+      </c>
+      <c r="BZ19" s="26">
+        <v>472.12900000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>676</v>
       </c>
@@ -23113,25 +23542,25 @@
         <v>2308.0479999999998</v>
       </c>
       <c r="BH20" s="26">
-        <v>2510.3220000000001</v>
+        <v>2550.4789999999998</v>
       </c>
       <c r="BI20" s="26">
-        <v>2515.8629999999998</v>
+        <v>2579.5410000000002</v>
       </c>
       <c r="BJ20" s="26">
-        <v>2398.1489999999999</v>
+        <v>2415.2570000000001</v>
       </c>
       <c r="BK20" s="26">
-        <v>2556.7860000000001</v>
+        <v>2612.0920000000001</v>
       </c>
       <c r="BL20" s="26">
-        <v>2422.2669999999998</v>
+        <v>2419.9490000000001</v>
       </c>
       <c r="BM20" s="26">
-        <v>2534.663</v>
+        <v>2636.895</v>
       </c>
       <c r="BN20" s="26">
-        <v>2530.73</v>
+        <v>2604.2179999999998</v>
       </c>
       <c r="BO20" s="26">
         <v>2568.1370000000002</v>
@@ -23148,8 +23577,29 @@
       <c r="BS20" s="26">
         <v>2531.3890000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT20" s="26">
+        <v>2686.248</v>
+      </c>
+      <c r="BU20" s="26">
+        <v>2378.7370000000001</v>
+      </c>
+      <c r="BV20" s="26">
+        <v>2560.5210000000002</v>
+      </c>
+      <c r="BW20" s="26">
+        <v>3005.9679999999998</v>
+      </c>
+      <c r="BX20" s="26">
+        <v>2791.047</v>
+      </c>
+      <c r="BY20" s="26">
+        <v>2769.3139999999999</v>
+      </c>
+      <c r="BZ20" s="26">
+        <v>2900.7130000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>675</v>
       </c>
@@ -23296,25 +23746,25 @@
         <v>2932.6950000000002</v>
       </c>
       <c r="BH21" s="26">
-        <v>2737.5479999999998</v>
+        <v>2787.28</v>
       </c>
       <c r="BI21" s="26">
-        <v>2683.7080000000001</v>
+        <v>2681.9119999999998</v>
       </c>
       <c r="BJ21" s="26">
-        <v>3289.4789999999998</v>
+        <v>3247.625</v>
       </c>
       <c r="BK21" s="26">
-        <v>2823.5920000000001</v>
+        <v>2801.538</v>
       </c>
       <c r="BL21" s="26">
-        <v>3133.0369999999998</v>
+        <v>3103.049</v>
       </c>
       <c r="BM21" s="26">
-        <v>2666.9879999999998</v>
+        <v>2639.2049999999999</v>
       </c>
       <c r="BN21" s="26">
-        <v>3010.627</v>
+        <v>2996.866</v>
       </c>
       <c r="BO21" s="26">
         <v>3361.7170000000001</v>
@@ -23331,8 +23781,29 @@
       <c r="BS21" s="26">
         <v>3143.31</v>
       </c>
-    </row>
-    <row r="22" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT21" s="26">
+        <v>2820.9369999999999</v>
+      </c>
+      <c r="BU21" s="26">
+        <v>3011.819</v>
+      </c>
+      <c r="BV21" s="26">
+        <v>2853.5650000000001</v>
+      </c>
+      <c r="BW21" s="26">
+        <v>3063.433</v>
+      </c>
+      <c r="BX21" s="26">
+        <v>3049.3209999999999</v>
+      </c>
+      <c r="BY21" s="26">
+        <v>2788.491</v>
+      </c>
+      <c r="BZ21" s="26">
+        <v>2991.5349999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>674</v>
       </c>
@@ -23479,25 +23950,25 @@
         <v>1641.2280000000001</v>
       </c>
       <c r="BH22" s="26">
-        <v>1544.279</v>
+        <v>1537.8920000000001</v>
       </c>
       <c r="BI22" s="26">
-        <v>1574.7940000000001</v>
+        <v>1569.0609999999999</v>
       </c>
       <c r="BJ22" s="26">
-        <v>1593.479</v>
+        <v>1615.288</v>
       </c>
       <c r="BK22" s="26">
-        <v>1580.818</v>
+        <v>1567.038</v>
       </c>
       <c r="BL22" s="26">
-        <v>1696.414</v>
+        <v>1743.3130000000001</v>
       </c>
       <c r="BM22" s="26">
-        <v>1512.856</v>
+        <v>1501.327</v>
       </c>
       <c r="BN22" s="26">
-        <v>1501.952</v>
+        <v>1513.9849999999999</v>
       </c>
       <c r="BO22" s="26">
         <v>1710.9680000000001</v>
@@ -23514,8 +23985,29 @@
       <c r="BS22" s="26">
         <v>1585.854</v>
       </c>
-    </row>
-    <row r="23" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT22" s="26">
+        <v>1585.1379999999999</v>
+      </c>
+      <c r="BU22" s="26">
+        <v>1668.931</v>
+      </c>
+      <c r="BV22" s="26">
+        <v>1825.681</v>
+      </c>
+      <c r="BW22" s="26">
+        <v>1632.9159999999999</v>
+      </c>
+      <c r="BX22" s="26">
+        <v>1783.15</v>
+      </c>
+      <c r="BY22" s="26">
+        <v>1528.117</v>
+      </c>
+      <c r="BZ22" s="26">
+        <v>1610.2719999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>673</v>
       </c>
@@ -23662,25 +24154,25 @@
         <v>641.74</v>
       </c>
       <c r="BH23" s="26">
-        <v>688.66700000000003</v>
+        <v>660.58299999999997</v>
       </c>
       <c r="BI23" s="26">
-        <v>755.298</v>
+        <v>734.51800000000003</v>
       </c>
       <c r="BJ23" s="26">
-        <v>680.00199999999995</v>
+        <v>678.75</v>
       </c>
       <c r="BK23" s="26">
-        <v>727.27300000000002</v>
+        <v>717.77700000000004</v>
       </c>
       <c r="BL23" s="26">
-        <v>702.93799999999999</v>
+        <v>705.39700000000005</v>
       </c>
       <c r="BM23" s="26">
-        <v>710.20299999999997</v>
+        <v>708.86199999999997</v>
       </c>
       <c r="BN23" s="26">
-        <v>669.02300000000002</v>
+        <v>637.46500000000003</v>
       </c>
       <c r="BO23" s="26">
         <v>835.30899999999997</v>
@@ -23697,8 +24189,29 @@
       <c r="BS23" s="26">
         <v>838.90499999999997</v>
       </c>
-    </row>
-    <row r="24" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT23" s="26">
+        <v>744.32100000000003</v>
+      </c>
+      <c r="BU23" s="26">
+        <v>739.54399999999998</v>
+      </c>
+      <c r="BV23" s="26">
+        <v>729.77099999999996</v>
+      </c>
+      <c r="BW23" s="26">
+        <v>779.73900000000003</v>
+      </c>
+      <c r="BX23" s="26">
+        <v>723.24400000000003</v>
+      </c>
+      <c r="BY23" s="26">
+        <v>887.57600000000002</v>
+      </c>
+      <c r="BZ23" s="26">
+        <v>806.16800000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>672</v>
       </c>
@@ -23845,25 +24358,25 @@
         <v>385.60199999999998</v>
       </c>
       <c r="BH24" s="26">
-        <v>468.93299999999999</v>
+        <v>471.32900000000001</v>
       </c>
       <c r="BI24" s="26">
-        <v>389.57400000000001</v>
+        <v>380.137</v>
       </c>
       <c r="BJ24" s="26">
-        <v>424.38</v>
+        <v>423.87599999999998</v>
       </c>
       <c r="BK24" s="26">
-        <v>511.041</v>
+        <v>509.44900000000001</v>
       </c>
       <c r="BL24" s="26">
-        <v>475.23099999999999</v>
+        <v>478.18200000000002</v>
       </c>
       <c r="BM24" s="26">
-        <v>490.24299999999999</v>
+        <v>509.327</v>
       </c>
       <c r="BN24" s="26">
-        <v>462.149</v>
+        <v>463.649</v>
       </c>
       <c r="BO24" s="26">
         <v>450.79</v>
@@ -23880,8 +24393,29 @@
       <c r="BS24" s="26">
         <v>406.45100000000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT24" s="26">
+        <v>442.35599999999999</v>
+      </c>
+      <c r="BU24" s="26">
+        <v>517.08199999999999</v>
+      </c>
+      <c r="BV24" s="26">
+        <v>514.57500000000005</v>
+      </c>
+      <c r="BW24" s="26">
+        <v>446.09800000000001</v>
+      </c>
+      <c r="BX24" s="26">
+        <v>504.75099999999998</v>
+      </c>
+      <c r="BY24" s="26">
+        <v>291.23099999999999</v>
+      </c>
+      <c r="BZ24" s="26">
+        <v>415.23500000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>671</v>
       </c>
@@ -24028,25 +24562,25 @@
         <v>3102.8890000000001</v>
       </c>
       <c r="BH25" s="26">
-        <v>2976.7910000000002</v>
+        <v>3006.89</v>
       </c>
       <c r="BI25" s="26">
-        <v>3008.683</v>
+        <v>2998.9349999999999</v>
       </c>
       <c r="BJ25" s="26">
-        <v>2982.2849999999999</v>
+        <v>3000.5279999999998</v>
       </c>
       <c r="BK25" s="26">
-        <v>3145.3270000000002</v>
+        <v>3145.5419999999999</v>
       </c>
       <c r="BL25" s="26">
-        <v>3071.29</v>
+        <v>3050.6280000000002</v>
       </c>
       <c r="BM25" s="26">
-        <v>3158.05</v>
+        <v>3159.3910000000001</v>
       </c>
       <c r="BN25" s="26">
-        <v>2995.91</v>
+        <v>2996.482</v>
       </c>
       <c r="BO25" s="26">
         <v>3167.444</v>
@@ -24063,8 +24597,29 @@
       <c r="BS25" s="26">
         <v>2937.009</v>
       </c>
-    </row>
-    <row r="26" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT25" s="26">
+        <v>3099.953</v>
+      </c>
+      <c r="BU25" s="26">
+        <v>3230.55</v>
+      </c>
+      <c r="BV25" s="26">
+        <v>2940.152</v>
+      </c>
+      <c r="BW25" s="26">
+        <v>2962.739</v>
+      </c>
+      <c r="BX25" s="26">
+        <v>3225.5749999999998</v>
+      </c>
+      <c r="BY25" s="26">
+        <v>3234.2719999999999</v>
+      </c>
+      <c r="BZ25" s="26">
+        <v>3016.4630000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>670</v>
       </c>
@@ -24211,7 +24766,7 @@
         <v>12.653</v>
       </c>
       <c r="BH26" s="26">
-        <v>1.6990000000000001</v>
+        <v>1.8380000000000001</v>
       </c>
       <c r="BI26" s="26">
         <v>0</v>
@@ -24246,8 +24801,29 @@
       <c r="BS26" s="26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="BT26" s="26">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="BU26" s="26">
+        <v>0</v>
+      </c>
+      <c r="BV26" s="26">
+        <v>0</v>
+      </c>
+      <c r="BW26" s="26">
+        <v>0.42</v>
+      </c>
+      <c r="BX26" s="26">
+        <v>0</v>
+      </c>
+      <c r="BY26" s="26">
+        <v>0</v>
+      </c>
+      <c r="BZ26" s="26">
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
         <v>694</v>
       </c>
@@ -24354,7 +24930,7 @@
       <c r="BR27" s="26"/>
       <c r="BS27" s="26"/>
     </row>
-    <row r="28" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
         <v>691</v>
       </c>
@@ -24433,7 +25009,7 @@
       <c r="BR28" s="26"/>
       <c r="BS28" s="26"/>
     </row>
-    <row r="29" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>693</v>
       </c>
@@ -24540,7 +25116,7 @@
       <c r="BR29" s="26"/>
       <c r="BS29" s="26"/>
     </row>
-    <row r="30" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>692</v>
       </c>
@@ -24647,7 +25223,7 @@
       <c r="BR30" s="26"/>
       <c r="BS30" s="26"/>
     </row>
-    <row r="31" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
         <v>685</v>
       </c>
@@ -24725,7 +25301,7 @@
       <c r="BR31" s="26"/>
       <c r="BS31" s="26"/>
     </row>
-    <row r="32" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>690</v>
       </c>
@@ -46986,7 +47562,7 @@
       <selection activeCell="B153" sqref="B153"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B184" sqref="B184"/>
+      <selection pane="bottomRight" activeCell="B185" sqref="B185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48715,6 +49291,9 @@
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>772</v>
+      </c>
+      <c r="B184" t="s">
+        <v>821</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Monthly labor update - Sep 2025
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E36C01-6426-4DC7-BEE3-B8865778D79E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F7A55A-53D6-45BD-9496-05BA9DC84443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="855" yWindow="1365" windowWidth="14100" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3013" uniqueCount="834">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3018" uniqueCount="836">
   <si>
     <t>LFS Round</t>
   </si>
@@ -2540,6 +2540,12 @@
   </si>
   <si>
     <t>2025Dec</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/participation-labor-force-august-2025-increase-5213-million-filipinos-aged-15-years-and</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/participation-labor-force-september-2025-decreased-5156-million-filipinos-aged-15-years-and</t>
   </si>
 </sst>
 </file>
@@ -2715,7 +2721,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2776,7 +2782,6 @@
     <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -3012,11 +3017,11 @@
   <dimension ref="A1:P299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D281" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D275" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F263" sqref="F263"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F294" sqref="F294"/>
+      <selection pane="bottomRight" activeCell="E297" sqref="E297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15505,7 +15510,7 @@
         <v>2157.422</v>
       </c>
       <c r="N274" s="2">
-        <f t="shared" ref="N274:N293" si="34">J274-K274</f>
+        <f t="shared" ref="N274:N295" si="34">J274-K274</f>
         <v>30572.822</v>
       </c>
       <c r="O274" s="2">
@@ -15839,9 +15844,6 @@
       <c r="D281" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E281" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F281" s="3">
         <f t="shared" ref="F281:F285" si="41">K281/J281</f>
         <v>0.64807383986548939</v>
@@ -15894,9 +15896,6 @@
       <c r="D282" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E282" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F282" s="3">
         <f t="shared" si="41"/>
         <v>0.65692169377521137</v>
@@ -16411,19 +16410,19 @@
         <v>425</v>
       </c>
       <c r="F292" s="3">
-        <f t="shared" ref="F292:F293" si="61">K292/J292</f>
+        <f t="shared" ref="F292:F295" si="61">K292/J292</f>
         <v>0.65710331091544816</v>
       </c>
       <c r="G292" s="3">
-        <f t="shared" ref="G292:G293" si="62">L292/K292</f>
+        <f t="shared" ref="G292:G295" si="62">L292/K292</f>
         <v>0.96282180199484058</v>
       </c>
       <c r="H292" s="3">
-        <f t="shared" ref="H292:H293" si="63">M292/K292</f>
+        <f t="shared" ref="H292:H295" si="63">M292/K292</f>
         <v>3.7178178929830163E-2</v>
       </c>
       <c r="I292" s="3">
-        <f t="shared" ref="I292:I293" si="64">O292/L292</f>
+        <f t="shared" ref="I292:I295" si="64">O292/L292</f>
         <v>0.11416914389709779</v>
       </c>
       <c r="J292" s="2">
@@ -16479,7 +16478,7 @@
       </c>
       <c r="I293" s="3">
         <f t="shared" si="64"/>
-        <v>0.14776248445292775</v>
+        <v>0.14774076725261628</v>
       </c>
       <c r="J293" s="2">
         <v>80087.680999999997</v>
@@ -16498,7 +16497,7 @@
         <v>31447.817999999999</v>
       </c>
       <c r="O293" s="2">
-        <v>6803.9380000000001</v>
+        <v>6802.9380000000001</v>
       </c>
       <c r="P293" t="s">
         <v>821</v>
@@ -16517,7 +16516,47 @@
       <c r="D294" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="O294" s="2"/>
+      <c r="E294" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F294" s="3">
+        <f t="shared" si="61"/>
+        <v>0.65059958154669972</v>
+      </c>
+      <c r="G294" s="3">
+        <f t="shared" si="62"/>
+        <v>0.96099154554045707</v>
+      </c>
+      <c r="H294" s="3">
+        <f t="shared" si="63"/>
+        <v>3.9008454459542867E-2</v>
+      </c>
+      <c r="I294" s="3">
+        <f t="shared" si="64"/>
+        <v>0.10740695427878283</v>
+      </c>
+      <c r="J294" s="2">
+        <v>80125.547999999995</v>
+      </c>
+      <c r="K294" s="2">
+        <v>52129.648000000001</v>
+      </c>
+      <c r="L294" s="2">
+        <v>50096.150999999998</v>
+      </c>
+      <c r="M294" s="2">
+        <v>2033.4970000000001</v>
+      </c>
+      <c r="N294" s="2">
+        <f t="shared" si="34"/>
+        <v>27995.899999999994</v>
+      </c>
+      <c r="O294" s="2">
+        <v>5380.6750000000002</v>
+      </c>
+      <c r="P294" t="s">
+        <v>834</v>
+      </c>
     </row>
     <row r="295" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
@@ -16532,7 +16571,47 @@
       <c r="D295" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="O295" s="2"/>
+      <c r="E295" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F295" s="3">
+        <f t="shared" si="61"/>
+        <v>0.64460489114467467</v>
+      </c>
+      <c r="G295" s="3">
+        <f t="shared" si="62"/>
+        <v>0.96206599107752477</v>
+      </c>
+      <c r="H295" s="3">
+        <f t="shared" si="63"/>
+        <v>3.7933989526717726E-2</v>
+      </c>
+      <c r="I295" s="3">
+        <f t="shared" si="64"/>
+        <v>0.11133747798823262</v>
+      </c>
+      <c r="J295" s="2">
+        <v>79983.362999999998</v>
+      </c>
+      <c r="K295" s="2">
+        <v>51557.667000000001</v>
+      </c>
+      <c r="L295" s="2">
+        <v>49601.877999999997</v>
+      </c>
+      <c r="M295" s="2">
+        <v>1955.788</v>
+      </c>
+      <c r="N295" s="2">
+        <f t="shared" si="34"/>
+        <v>28425.695999999996</v>
+      </c>
+      <c r="O295" s="2">
+        <v>5522.5479999999998</v>
+      </c>
+      <c r="P295" t="s">
+        <v>835</v>
+      </c>
     </row>
     <row r="296" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
@@ -20050,7 +20129,7 @@
       <c r="BF1" s="24" t="s">
         <v>706</v>
       </c>
-      <c r="BG1" s="50" t="s">
+      <c r="BG1" s="24" t="s">
         <v>705</v>
       </c>
       <c r="BH1" s="24" t="s">
@@ -20119,10 +20198,10 @@
       <c r="CC1" s="26" t="s">
         <v>831</v>
       </c>
-      <c r="CD1" s="51" t="s">
+      <c r="CD1" s="50" t="s">
         <v>832</v>
       </c>
-      <c r="CE1" s="52" t="s">
+      <c r="CE1" s="51" t="s">
         <v>833</v>
       </c>
     </row>
@@ -47562,7 +47641,7 @@
       <selection activeCell="B153" sqref="B153"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B185" sqref="B185"/>
+      <selection pane="bottomRight" activeCell="B186" sqref="B186:B187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49285,7 +49364,7 @@
         <v>771</v>
       </c>
       <c r="B183" t="s">
-        <v>820</v>
+        <v>809</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
@@ -49293,22 +49372,31 @@
         <v>772</v>
       </c>
       <c r="B184" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>773</v>
       </c>
+      <c r="B185" t="s">
+        <v>821</v>
+      </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>774</v>
       </c>
+      <c r="B186" t="s">
+        <v>834</v>
+      </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>775</v>
+      </c>
+      <c r="B187" t="s">
+        <v>835</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Monthly labor update - Nov 2025
</commit_message>
<xml_diff>
--- a/Data/Labor and Employment/Labor and Employment.xlsx
+++ b/Data/Labor and Employment/Labor and Employment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\GitHub Repositories\PH-Econ-Data\Data\Labor and Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F7A55A-53D6-45BD-9496-05BA9DC84443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DE202D-F5F5-4DE1-A722-8EE18371D011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2370" yWindow="1215" windowWidth="14715" windowHeight="13245" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3018" uniqueCount="836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3022" uniqueCount="838">
   <si>
     <t>LFS Round</t>
   </si>
@@ -2546,6 +2546,12 @@
   </si>
   <si>
     <t>https://psa.gov.ph/content/participation-labor-force-september-2025-decreased-5156-million-filipinos-aged-15-years-and</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/number-employed-persons-october-2025-increased-4862-million-filipinos-15-years-old-and-over</t>
+  </si>
+  <si>
+    <t>https://psa.gov.ph/content/participation-labor-force-november-2025-increased-5152-million-filipinos-aged-15-years-and</t>
   </si>
 </sst>
 </file>
@@ -2721,7 +2727,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2784,6 +2790,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -3016,12 +3023,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P299"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D275" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="E284" activePane="bottomRight" state="frozen"/>
       <selection activeCell="F263" sqref="F263"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E297" sqref="E297"/>
+      <selection pane="bottomRight" activeCell="E299" sqref="E299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15510,7 +15517,7 @@
         <v>2157.422</v>
       </c>
       <c r="N274" s="2">
-        <f t="shared" ref="N274:N295" si="34">J274-K274</f>
+        <f t="shared" ref="N274:N297" si="34">J274-K274</f>
         <v>30572.822</v>
       </c>
       <c r="O274" s="2">
@@ -15948,43 +15955,40 @@
       <c r="D283" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E283" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F283" s="3">
         <f t="shared" si="41"/>
-        <v>0.63269217517625431</v>
+        <v>0.63269996354087787</v>
       </c>
       <c r="G283" s="3">
         <f t="shared" si="42"/>
-        <v>0.96078319137977941</v>
+        <v>0.96078135236143614</v>
       </c>
       <c r="H283" s="3">
         <f t="shared" si="43"/>
-        <v>3.9216808620220631E-2</v>
+        <v>3.921864763856394E-2</v>
       </c>
       <c r="I283" s="3">
         <f t="shared" si="44"/>
-        <v>0.12631792459682778</v>
+        <v>0.12631803039456821</v>
       </c>
       <c r="J283" s="2">
-        <v>79221.171000000002</v>
+        <v>79220.229000000007</v>
       </c>
       <c r="K283" s="2">
-        <v>50122.614999999998</v>
+        <v>50122.635999999999</v>
       </c>
       <c r="L283" s="2">
-        <v>48156.966</v>
+        <v>48156.894</v>
       </c>
       <c r="M283" s="2">
-        <v>1965.6489999999999</v>
+        <v>1965.742</v>
       </c>
       <c r="N283" s="2">
         <f t="shared" si="34"/>
-        <v>29098.556000000004</v>
+        <v>29097.593000000008</v>
       </c>
       <c r="O283" s="2">
-        <v>6083.0879999999997</v>
+        <v>6083.0839999999998</v>
       </c>
       <c r="P283" t="s">
         <v>668</v>
@@ -16003,9 +16007,6 @@
       <c r="D284" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="E284" s="1" t="s">
-        <v>425</v>
-      </c>
       <c r="F284" s="3">
         <f t="shared" si="41"/>
         <v>0.64579733417179253</v>
@@ -16626,7 +16627,47 @@
       <c r="D296" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="O296" s="2"/>
+      <c r="E296" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F296" s="3">
+        <f t="shared" ref="F296" si="65">K296/J296</f>
+        <v>0.63560755079129783</v>
+      </c>
+      <c r="G296" s="3">
+        <f t="shared" ref="G296" si="66">L296/K296</f>
+        <v>0.95031294409585143</v>
+      </c>
+      <c r="H296" s="3">
+        <f t="shared" ref="H296" si="67">M296/K296</f>
+        <v>4.9687055904148611E-2</v>
+      </c>
+      <c r="I296" s="3">
+        <f t="shared" ref="I296" si="68">O296/L296</f>
+        <v>0.1195098432586716</v>
+      </c>
+      <c r="J296" s="2">
+        <v>80492.331999999995</v>
+      </c>
+      <c r="K296" s="2">
+        <v>51161.534</v>
+      </c>
+      <c r="L296" s="2">
+        <v>48619.468000000001</v>
+      </c>
+      <c r="M296" s="2">
+        <v>2542.0659999999998</v>
+      </c>
+      <c r="N296" s="2">
+        <f t="shared" si="34"/>
+        <v>29330.797999999995</v>
+      </c>
+      <c r="O296" s="2">
+        <v>5810.5050000000001</v>
+      </c>
+      <c r="P296" t="s">
+        <v>836</v>
+      </c>
     </row>
     <row r="297" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
@@ -16641,7 +16682,47 @@
       <c r="D297" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="O297" s="2"/>
+      <c r="E297" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F297" s="3">
+        <f t="shared" ref="F297" si="69">K297/J297</f>
+        <v>0.6401309260312904</v>
+      </c>
+      <c r="G297" s="3">
+        <f t="shared" ref="G297" si="70">L297/K297</f>
+        <v>0.95627988958077537</v>
+      </c>
+      <c r="H297" s="3">
+        <f t="shared" ref="H297" si="71">M297/K297</f>
+        <v>4.3720091008200068E-2</v>
+      </c>
+      <c r="I297" s="3">
+        <f t="shared" ref="I297" si="72">O297/L297</f>
+        <v>0.10373018599777829</v>
+      </c>
+      <c r="J297" s="2">
+        <v>80479.03</v>
+      </c>
+      <c r="K297" s="2">
+        <v>51517.116000000002</v>
+      </c>
+      <c r="L297" s="2">
+        <v>49264.781999999999</v>
+      </c>
+      <c r="M297" s="2">
+        <v>2252.3330000000001</v>
+      </c>
+      <c r="N297" s="2">
+        <f t="shared" si="34"/>
+        <v>28961.913999999997</v>
+      </c>
+      <c r="O297" s="2">
+        <v>5110.2449999999999</v>
+      </c>
+      <c r="P297" t="s">
+        <v>837</v>
+      </c>
     </row>
     <row r="298" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
@@ -16684,7 +16765,7 @@
   <dimension ref="A1:AK45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -19939,11 +20020,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B3FDD3-8CAB-4986-8439-B73CD0CD9872}">
   <dimension ref="A1:CE54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="BV2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="BP2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BZ2" sqref="BZ2"/>
+      <selection pane="bottomRight" activeCell="BQ1" sqref="BQ1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20150,7 +20231,7 @@
       <c r="BM1" s="24" t="s">
         <v>699</v>
       </c>
-      <c r="BN1" s="31" t="s">
+      <c r="BN1" s="52" t="s">
         <v>698</v>
       </c>
       <c r="BO1" s="24" t="s">
@@ -20159,7 +20240,7 @@
       <c r="BP1" s="24" t="s">
         <v>696</v>
       </c>
-      <c r="BQ1" s="24" t="s">
+      <c r="BQ1" s="31" t="s">
         <v>695</v>
       </c>
       <c r="BR1" s="35" t="s">
@@ -20379,7 +20460,7 @@
         <v>49872.28</v>
       </c>
       <c r="BQ2" s="34">
-        <v>48156.966</v>
+        <v>48156.894</v>
       </c>
       <c r="BR2" s="34">
         <v>49541.468999999997</v>
@@ -20407,6 +20488,18 @@
       </c>
       <c r="BZ2" s="34">
         <v>46046.451000000001</v>
+      </c>
+      <c r="CA2" s="26">
+        <v>50096.150999999998</v>
+      </c>
+      <c r="CB2" s="26">
+        <v>49601.877999999997</v>
+      </c>
+      <c r="CC2" s="26">
+        <v>48619.468000000001</v>
+      </c>
+      <c r="CD2" s="26">
+        <v>49264.781999999999</v>
       </c>
     </row>
     <row r="3" spans="1:83" x14ac:dyDescent="0.25">
@@ -20648,13 +20741,13 @@
         <v>8756.9830000000002</v>
       </c>
       <c r="BO4" s="26">
-        <v>8432.6589999999997</v>
+        <v>8433.3520000000008</v>
       </c>
       <c r="BP4" s="26">
-        <v>8726.4850000000006</v>
+        <v>8736.1970000000001</v>
       </c>
       <c r="BQ4" s="26">
-        <v>9049.2219999999998</v>
+        <v>9049.2170000000006</v>
       </c>
       <c r="BR4" s="26">
         <v>8714.152</v>
@@ -20682,6 +20775,18 @@
       </c>
       <c r="BZ4" s="26">
         <v>7381.6890000000003</v>
+      </c>
+      <c r="CA4" s="26">
+        <v>8732.8700000000008</v>
+      </c>
+      <c r="CB4" s="26">
+        <v>8861.9930000000004</v>
+      </c>
+      <c r="CC4" s="26">
+        <v>9217.4889999999996</v>
+      </c>
+      <c r="CD4" s="26">
+        <v>8700.8410000000003</v>
       </c>
     </row>
     <row r="5" spans="1:83" x14ac:dyDescent="0.25">
@@ -20886,6 +20991,18 @@
       </c>
       <c r="BZ5" s="26">
         <v>1151.009</v>
+      </c>
+      <c r="CA5" s="26">
+        <v>1497.403</v>
+      </c>
+      <c r="CB5" s="26">
+        <v>1490.702</v>
+      </c>
+      <c r="CC5" s="26">
+        <v>1225.366</v>
+      </c>
+      <c r="CD5" s="26">
+        <v>1147.6389999999999</v>
       </c>
     </row>
     <row r="6" spans="1:83" x14ac:dyDescent="0.25">
@@ -21131,7 +21248,7 @@
         <v>271.697</v>
       </c>
       <c r="BQ7" s="26">
-        <v>262.99700000000001</v>
+        <v>261.84100000000001</v>
       </c>
       <c r="BR7" s="26">
         <v>267.584</v>
@@ -21159,6 +21276,18 @@
       </c>
       <c r="BZ7" s="26">
         <v>245.18700000000001</v>
+      </c>
+      <c r="CA7" s="26">
+        <v>142.614</v>
+      </c>
+      <c r="CB7" s="26">
+        <v>256.08800000000002</v>
+      </c>
+      <c r="CC7" s="26">
+        <v>228.41800000000001</v>
+      </c>
+      <c r="CD7" s="26">
+        <v>242.04599999999999</v>
       </c>
     </row>
     <row r="8" spans="1:83" x14ac:dyDescent="0.25">
@@ -21329,16 +21458,16 @@
         <v>3453.3130000000001</v>
       </c>
       <c r="BO8" s="26">
-        <v>3406.0970000000002</v>
+        <v>3408.5340000000001</v>
       </c>
       <c r="BP8" s="26">
-        <v>3763.0160000000001</v>
+        <v>3752.7</v>
       </c>
       <c r="BQ8" s="26">
-        <v>3479.509</v>
+        <v>3482.886</v>
       </c>
       <c r="BR8" s="26">
-        <v>3710.7510000000002</v>
+        <v>3721.0889999999999</v>
       </c>
       <c r="BS8" s="26">
         <v>3405.971</v>
@@ -21363,6 +21492,18 @@
       </c>
       <c r="BZ8" s="26">
         <v>3561.9090000000001</v>
+      </c>
+      <c r="CA8" s="26">
+        <v>3492.2559999999999</v>
+      </c>
+      <c r="CB8" s="26">
+        <v>3451.0680000000002</v>
+      </c>
+      <c r="CC8" s="26">
+        <v>3635.1460000000002</v>
+      </c>
+      <c r="CD8" s="26">
+        <v>3571.4229999999998</v>
       </c>
     </row>
     <row r="9" spans="1:83" x14ac:dyDescent="0.25">
@@ -21539,10 +21680,10 @@
         <v>78.046999999999997</v>
       </c>
       <c r="BQ9" s="26">
-        <v>93.953999999999994</v>
+        <v>95.253</v>
       </c>
       <c r="BR9" s="26">
-        <v>70.995000000000005</v>
+        <v>73.866</v>
       </c>
       <c r="BS9" s="26">
         <v>67.512</v>
@@ -21567,6 +21708,18 @@
       </c>
       <c r="BZ9" s="26">
         <v>97.754999999999995</v>
+      </c>
+      <c r="CA9" s="26">
+        <v>91.498000000000005</v>
+      </c>
+      <c r="CB9" s="26">
+        <v>113.52</v>
+      </c>
+      <c r="CC9" s="26">
+        <v>95.936999999999998</v>
+      </c>
+      <c r="CD9" s="26">
+        <v>71.414000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:83" x14ac:dyDescent="0.25">
@@ -21737,7 +21890,7 @@
         <v>91.924000000000007</v>
       </c>
       <c r="BO10" s="26">
-        <v>114.21</v>
+        <v>133.65299999999999</v>
       </c>
       <c r="BP10" s="26">
         <v>86.849000000000004</v>
@@ -21746,7 +21899,7 @@
         <v>81.600999999999999</v>
       </c>
       <c r="BR10" s="26">
-        <v>53.923000000000002</v>
+        <v>51.725000000000001</v>
       </c>
       <c r="BS10" s="26">
         <v>55.939</v>
@@ -21771,6 +21924,18 @@
       </c>
       <c r="BZ10" s="26">
         <v>92.194000000000003</v>
+      </c>
+      <c r="CA10" s="26">
+        <v>75.697000000000003</v>
+      </c>
+      <c r="CB10" s="26">
+        <v>45.314999999999998</v>
+      </c>
+      <c r="CC10" s="26">
+        <v>60.319000000000003</v>
+      </c>
+      <c r="CD10" s="26">
+        <v>107.30500000000001</v>
       </c>
     </row>
     <row r="11" spans="1:83" x14ac:dyDescent="0.25">
@@ -21941,13 +22106,13 @@
         <v>4751.4650000000001</v>
       </c>
       <c r="BO11" s="26">
-        <v>4738.2860000000001</v>
+        <v>4735.8680000000004</v>
       </c>
       <c r="BP11" s="26">
         <v>4454.6549999999997</v>
       </c>
       <c r="BQ11" s="26">
-        <v>4688.4880000000003</v>
+        <v>4684.0680000000002</v>
       </c>
       <c r="BR11" s="26">
         <v>4763.9870000000001</v>
@@ -21975,6 +22140,18 @@
       </c>
       <c r="BZ11" s="26">
         <v>4604.7449999999999</v>
+      </c>
+      <c r="CA11" s="26">
+        <v>5276.3649999999998</v>
+      </c>
+      <c r="CB11" s="26">
+        <v>4968.3869999999997</v>
+      </c>
+      <c r="CC11" s="26">
+        <v>4706.9949999999999</v>
+      </c>
+      <c r="CD11" s="26">
+        <v>4850.0309999999999</v>
       </c>
     </row>
     <row r="12" spans="1:83" x14ac:dyDescent="0.25">
@@ -22214,16 +22391,16 @@
         <v>9738.1260000000002</v>
       </c>
       <c r="BO13" s="26">
-        <v>10929.153</v>
+        <v>10927.127</v>
       </c>
       <c r="BP13" s="26">
-        <v>10332.393</v>
+        <v>10246.115</v>
       </c>
       <c r="BQ13" s="26">
-        <v>9825.6129999999994</v>
+        <v>9787.4789999999994</v>
       </c>
       <c r="BR13" s="26">
-        <v>10571.767</v>
+        <v>10335.663</v>
       </c>
       <c r="BS13" s="26">
         <v>10180.915000000001</v>
@@ -22248,6 +22425,18 @@
       </c>
       <c r="BZ13" s="26">
         <v>8841.4459999999999</v>
+      </c>
+      <c r="CA13" s="26">
+        <v>10138.781000000001</v>
+      </c>
+      <c r="CB13" s="26">
+        <v>10207.099</v>
+      </c>
+      <c r="CC13" s="26">
+        <v>9721.6260000000002</v>
+      </c>
+      <c r="CD13" s="26">
+        <v>10077.5</v>
       </c>
     </row>
     <row r="14" spans="1:83" x14ac:dyDescent="0.25">
@@ -22424,10 +22613,10 @@
         <v>3874.2429999999999</v>
       </c>
       <c r="BQ14" s="26">
-        <v>3734.8620000000001</v>
+        <v>3737.6</v>
       </c>
       <c r="BR14" s="26">
-        <v>3848.0129999999999</v>
+        <v>3848.279</v>
       </c>
       <c r="BS14" s="26">
         <v>4031.569</v>
@@ -22452,6 +22641,18 @@
       </c>
       <c r="BZ14" s="26">
         <v>3836.7649999999999</v>
+      </c>
+      <c r="CA14" s="26">
+        <v>3887.9490000000001</v>
+      </c>
+      <c r="CB14" s="26">
+        <v>3641.4070000000002</v>
+      </c>
+      <c r="CC14" s="26">
+        <v>3809.569</v>
+      </c>
+      <c r="CD14" s="26">
+        <v>3866.884</v>
       </c>
     </row>
     <row r="15" spans="1:83" x14ac:dyDescent="0.25">
@@ -22622,16 +22823,16 @@
         <v>2588.0880000000002</v>
       </c>
       <c r="BO15" s="26">
-        <v>2517.9430000000002</v>
+        <v>2517.116</v>
       </c>
       <c r="BP15" s="26">
-        <v>2344.683</v>
+        <v>2413.998</v>
       </c>
       <c r="BQ15" s="26">
-        <v>2507.5239999999999</v>
+        <v>2534.1460000000002</v>
       </c>
       <c r="BR15" s="26">
-        <v>2896.1390000000001</v>
+        <v>3112.6680000000001</v>
       </c>
       <c r="BS15" s="26">
         <v>2677.1469999999999</v>
@@ -22656,6 +22857,18 @@
       </c>
       <c r="BZ15" s="26">
         <v>2519.1410000000001</v>
+      </c>
+      <c r="CA15" s="26">
+        <v>2635.8530000000001</v>
+      </c>
+      <c r="CB15" s="26">
+        <v>2721.1729999999998</v>
+      </c>
+      <c r="CC15" s="26">
+        <v>2713.84</v>
+      </c>
+      <c r="CD15" s="26">
+        <v>2804.1410000000001</v>
       </c>
     </row>
     <row r="16" spans="1:83" x14ac:dyDescent="0.25">
@@ -22829,13 +23042,13 @@
         <v>430.78300000000002</v>
       </c>
       <c r="BP16" s="26">
-        <v>492.86200000000002</v>
+        <v>491.10700000000003</v>
       </c>
       <c r="BQ16" s="26">
-        <v>541.06700000000001</v>
+        <v>540.11</v>
       </c>
       <c r="BR16" s="26">
-        <v>488.35</v>
+        <v>462.58800000000002</v>
       </c>
       <c r="BS16" s="26">
         <v>485.89</v>
@@ -22861,8 +23074,20 @@
       <c r="BZ16" s="26">
         <v>511.774</v>
       </c>
-    </row>
-    <row r="17" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="CA16" s="26">
+        <v>485.03800000000001</v>
+      </c>
+      <c r="CB16" s="26">
+        <v>549.59299999999996</v>
+      </c>
+      <c r="CC16" s="26">
+        <v>523.78399999999999</v>
+      </c>
+      <c r="CD16" s="26">
+        <v>544.56299999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>679</v>
       </c>
@@ -23030,16 +23255,16 @@
         <v>708.07100000000003</v>
       </c>
       <c r="BO17" s="26">
-        <v>580.26599999999996</v>
+        <v>576.21500000000003</v>
       </c>
       <c r="BP17" s="26">
         <v>706.26599999999996</v>
       </c>
       <c r="BQ17" s="26">
-        <v>714.04899999999998</v>
+        <v>713.68899999999996</v>
       </c>
       <c r="BR17" s="26">
-        <v>661.50599999999997</v>
+        <v>638.88800000000003</v>
       </c>
       <c r="BS17" s="26">
         <v>757.32100000000003</v>
@@ -23065,8 +23290,20 @@
       <c r="BZ17" s="26">
         <v>717.12599999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="CA17" s="26">
+        <v>776.69200000000001</v>
+      </c>
+      <c r="CB17" s="26">
+        <v>671.51</v>
+      </c>
+      <c r="CC17" s="26">
+        <v>763.92399999999998</v>
+      </c>
+      <c r="CD17" s="26">
+        <v>691.29399999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>678</v>
       </c>
@@ -23240,7 +23477,7 @@
         <v>299.40899999999999</v>
       </c>
       <c r="BQ18" s="26">
-        <v>236.655</v>
+        <v>237.46299999999999</v>
       </c>
       <c r="BR18" s="26">
         <v>242.67099999999999</v>
@@ -23269,8 +23506,20 @@
       <c r="BZ18" s="26">
         <v>272.673</v>
       </c>
-    </row>
-    <row r="19" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="CA18" s="26">
+        <v>253.90799999999999</v>
+      </c>
+      <c r="CB18" s="26">
+        <v>268.21899999999999</v>
+      </c>
+      <c r="CC18" s="26">
+        <v>324.90699999999998</v>
+      </c>
+      <c r="CD18" s="26">
+        <v>319.92599999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>677</v>
       </c>
@@ -23438,16 +23687,16 @@
         <v>399.49700000000001</v>
       </c>
       <c r="BO19" s="26">
-        <v>393.80599999999998</v>
+        <v>384.26100000000002</v>
       </c>
       <c r="BP19" s="26">
         <v>519.18499999999995</v>
       </c>
       <c r="BQ19" s="26">
-        <v>419.29399999999998</v>
+        <v>422.74900000000002</v>
       </c>
       <c r="BR19" s="26">
-        <v>370.48599999999999</v>
+        <v>363.98200000000003</v>
       </c>
       <c r="BS19" s="26">
         <v>438.92700000000002</v>
@@ -23473,8 +23722,20 @@
       <c r="BZ19" s="26">
         <v>472.12900000000002</v>
       </c>
-    </row>
-    <row r="20" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="CA19" s="26">
+        <v>369.64</v>
+      </c>
+      <c r="CB19" s="26">
+        <v>400.41</v>
+      </c>
+      <c r="CC19" s="26">
+        <v>376.24599999999998</v>
+      </c>
+      <c r="CD19" s="26">
+        <v>356.91800000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>676</v>
       </c>
@@ -23642,16 +23903,16 @@
         <v>2604.2179999999998</v>
       </c>
       <c r="BO20" s="26">
-        <v>2568.1370000000002</v>
+        <v>2631.9</v>
       </c>
       <c r="BP20" s="26">
-        <v>3210.212</v>
+        <v>3226.6350000000002</v>
       </c>
       <c r="BQ20" s="26">
-        <v>2790.6610000000001</v>
+        <v>2817.0839999999998</v>
       </c>
       <c r="BR20" s="26">
-        <v>2644.9749999999999</v>
+        <v>2751.6550000000002</v>
       </c>
       <c r="BS20" s="26">
         <v>2531.3890000000001</v>
@@ -23677,8 +23938,20 @@
       <c r="BZ20" s="26">
         <v>2900.7130000000002</v>
       </c>
-    </row>
-    <row r="21" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="CA20" s="26">
+        <v>2939.1419999999998</v>
+      </c>
+      <c r="CB20" s="26">
+        <v>2870.9229999999998</v>
+      </c>
+      <c r="CC20" s="26">
+        <v>2879.4830000000002</v>
+      </c>
+      <c r="CD20" s="26">
+        <v>2850.4360000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>675</v>
       </c>
@@ -23846,16 +24119,16 @@
         <v>2996.866</v>
       </c>
       <c r="BO21" s="26">
-        <v>3361.7170000000001</v>
+        <v>3282.8589999999999</v>
       </c>
       <c r="BP21" s="26">
-        <v>3236.3220000000001</v>
+        <v>3251.6770000000001</v>
       </c>
       <c r="BQ21" s="26">
-        <v>2878.7660000000001</v>
+        <v>2868.6790000000001</v>
       </c>
       <c r="BR21" s="26">
-        <v>2836.6239999999998</v>
+        <v>2819.174</v>
       </c>
       <c r="BS21" s="26">
         <v>3143.31</v>
@@ -23881,8 +24154,20 @@
       <c r="BZ21" s="26">
         <v>2991.5349999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="CA21" s="26">
+        <v>3062.3690000000001</v>
+      </c>
+      <c r="CB21" s="26">
+        <v>3031.9850000000001</v>
+      </c>
+      <c r="CC21" s="26">
+        <v>3125.3090000000002</v>
+      </c>
+      <c r="CD21" s="26">
+        <v>3004.3249999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>674</v>
       </c>
@@ -24050,16 +24335,16 @@
         <v>1513.9849999999999</v>
       </c>
       <c r="BO22" s="26">
-        <v>1710.9680000000001</v>
+        <v>1706.7149999999999</v>
       </c>
       <c r="BP22" s="26">
-        <v>1765.9259999999999</v>
+        <v>1768.9079999999999</v>
       </c>
       <c r="BQ22" s="26">
-        <v>1623.857</v>
+        <v>1627.4169999999999</v>
       </c>
       <c r="BR22" s="26">
-        <v>1635.202</v>
+        <v>1631.047</v>
       </c>
       <c r="BS22" s="26">
         <v>1585.854</v>
@@ -24085,8 +24370,20 @@
       <c r="BZ22" s="26">
         <v>1610.2719999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="CA22" s="26">
+        <v>1556.1289999999999</v>
+      </c>
+      <c r="CB22" s="26">
+        <v>1779.248</v>
+      </c>
+      <c r="CC22" s="26">
+        <v>1634.0840000000001</v>
+      </c>
+      <c r="CD22" s="26">
+        <v>1807.133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>673</v>
       </c>
@@ -24254,16 +24551,16 @@
         <v>637.46500000000003</v>
       </c>
       <c r="BO23" s="26">
-        <v>835.30899999999997</v>
+        <v>834.995</v>
       </c>
       <c r="BP23" s="26">
-        <v>658.43899999999996</v>
+        <v>635.5</v>
       </c>
       <c r="BQ23" s="26">
-        <v>792.34400000000005</v>
+        <v>778.27300000000002</v>
       </c>
       <c r="BR23" s="26">
-        <v>881.52300000000002</v>
+        <v>835.95600000000002</v>
       </c>
       <c r="BS23" s="26">
         <v>838.90499999999997</v>
@@ -24289,8 +24586,20 @@
       <c r="BZ23" s="26">
         <v>806.16800000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="CA23" s="26">
+        <v>701.37099999999998</v>
+      </c>
+      <c r="CB23" s="26">
+        <v>818.20699999999999</v>
+      </c>
+      <c r="CC23" s="26">
+        <v>793.55200000000002</v>
+      </c>
+      <c r="CD23" s="26">
+        <v>829.31600000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>672</v>
       </c>
@@ -24458,16 +24767,16 @@
         <v>463.649</v>
       </c>
       <c r="BO24" s="26">
-        <v>450.79</v>
+        <v>457.745</v>
       </c>
       <c r="BP24" s="26">
         <v>468.89699999999999</v>
       </c>
       <c r="BQ24" s="26">
-        <v>401.62</v>
+        <v>400.43200000000002</v>
       </c>
       <c r="BR24" s="26">
-        <v>450.57799999999997</v>
+        <v>450.27</v>
       </c>
       <c r="BS24" s="26">
         <v>406.45100000000002</v>
@@ -24493,8 +24802,20 @@
       <c r="BZ24" s="26">
         <v>415.23500000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="CA24" s="26">
+        <v>565.21500000000003</v>
+      </c>
+      <c r="CB24" s="26">
+        <v>538.09500000000003</v>
+      </c>
+      <c r="CC24" s="26">
+        <v>403.42700000000002</v>
+      </c>
+      <c r="CD24" s="26">
+        <v>421.74799999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>671</v>
       </c>
@@ -24662,16 +24983,16 @@
         <v>2996.482</v>
       </c>
       <c r="BO25" s="26">
-        <v>3167.444</v>
+        <v>3176.4450000000002</v>
       </c>
       <c r="BP25" s="26">
-        <v>3402.1950000000002</v>
+        <v>3409.6950000000002</v>
       </c>
       <c r="BQ25" s="26">
-        <v>2896.8890000000001</v>
+        <v>2898.9119999999998</v>
       </c>
       <c r="BR25" s="26">
-        <v>3225.143</v>
+        <v>3249.125</v>
       </c>
       <c r="BS25" s="26">
         <v>2937.009</v>
@@ -24697,8 +25018,20 @@
       <c r="BZ25" s="26">
         <v>3016.4630000000002</v>
       </c>
-    </row>
-    <row r="26" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="CA25" s="26">
+        <v>3415.3620000000001</v>
+      </c>
+      <c r="CB25" s="26">
+        <v>2916.9380000000001</v>
+      </c>
+      <c r="CC25" s="26">
+        <v>2378.4479999999999</v>
+      </c>
+      <c r="CD25" s="26">
+        <v>2999.1289999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>670</v>
       </c>
@@ -24901,8 +25234,20 @@
       <c r="BZ26" s="26">
         <v>0.52400000000000002</v>
       </c>
-    </row>
-    <row r="27" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="CA26" s="26">
+        <v>0</v>
+      </c>
+      <c r="CB26" s="26">
+        <v>0</v>
+      </c>
+      <c r="CC26" s="26">
+        <v>1.599</v>
+      </c>
+      <c r="CD26" s="26">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
         <v>694</v>
       </c>
@@ -25009,7 +25354,7 @@
       <c r="BR27" s="26"/>
       <c r="BS27" s="26"/>
     </row>
-    <row r="28" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
         <v>691</v>
       </c>
@@ -25088,7 +25433,7 @@
       <c r="BR28" s="26"/>
       <c r="BS28" s="26"/>
     </row>
-    <row r="29" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
         <v>693</v>
       </c>
@@ -25195,7 +25540,7 @@
       <c r="BR29" s="26"/>
       <c r="BS29" s="26"/>
     </row>
-    <row r="30" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>692</v>
       </c>
@@ -25302,7 +25647,7 @@
       <c r="BR30" s="26"/>
       <c r="BS30" s="26"/>
     </row>
-    <row r="31" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
         <v>685</v>
       </c>
@@ -25380,7 +25725,7 @@
       <c r="BR31" s="26"/>
       <c r="BS31" s="26"/>
     </row>
-    <row r="32" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
         <v>690</v>
       </c>
@@ -47641,7 +47986,7 @@
       <selection activeCell="B153" sqref="B153"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B186" sqref="B186:B187"/>
+      <selection pane="bottomRight" activeCell="B189" sqref="B189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49403,10 +49748,16 @@
       <c r="A188" s="1" t="s">
         <v>776</v>
       </c>
+      <c r="B188" t="s">
+        <v>836</v>
+      </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>777</v>
+      </c>
+      <c r="B189" t="s">
+        <v>837</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>